<commit_message>
RSD No Cooking constraint and Peat and Coal to decrease by at least 90% in 2050
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5F55C4-E72D-4AA4-9EF5-9918475A7D88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E8D3C4-0475-467C-8301-1CD3D6F1CAB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16020" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0" xr:uid="{9FF5C6AC-B75C-4529-857A-E9C78B6E0755}">
+    <comment ref="I35" authorId="0" shapeId="0" xr:uid="{9FF5C6AC-B75C-4529-857A-E9C78B6E0755}">
       <text>
         <r>
           <rPr>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="275">
   <si>
     <t>UC_N</t>
   </si>
@@ -12262,10 +12262,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:U183"/>
+  <dimension ref="A1:U185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12711,24 +12711,29 @@
       <c r="K26" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="27" spans="2:21">
-      <c r="C27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="M26" s="25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" s="44" customFormat="1">
+      <c r="C27" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>5</v>
-      </c>
-      <c r="I27">
-        <v>5</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="E27" s="44">
+        <v>2031</v>
+      </c>
+      <c r="H27" s="44">
+        <f>H25*M26</f>
+        <v>1.03</v>
+      </c>
+      <c r="I27" s="44">
+        <f>I25*M26</f>
+        <v>1.03</v>
+      </c>
+      <c r="K27" s="44" t="s">
         <v>228</v>
       </c>
     </row>
@@ -12740,16 +12745,16 @@
         <v>221</v>
       </c>
       <c r="E28">
-        <v>2020</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>8.3000000000000007</v>
+        <v>5</v>
       </c>
       <c r="I28">
-        <v>8.3000000000000007</v>
+        <v>5</v>
       </c>
       <c r="K28" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="2:21">
@@ -12760,15 +12765,13 @@
         <v>221</v>
       </c>
       <c r="E29">
-        <v>2030</v>
-      </c>
-      <c r="H29" s="44">
-        <f>H28*M25</f>
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="I29" s="44">
-        <f>I28*M25</f>
-        <v>4.1500000000000004</v>
+        <v>2020</v>
+      </c>
+      <c r="H29">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I29">
+        <v>8.3000000000000007</v>
       </c>
       <c r="K29" t="s">
         <v>237</v>
@@ -12782,109 +12785,110 @@
         <v>221</v>
       </c>
       <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>5</v>
-      </c>
-      <c r="I30">
-        <v>5</v>
+        <v>2030</v>
+      </c>
+      <c r="H30" s="44">
+        <f>H29*M25</f>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I30" s="44">
+        <f>I29*M25</f>
+        <v>4.1500000000000004</v>
       </c>
       <c r="K30" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="31" spans="2:21">
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
+    <row r="31" spans="2:21" s="44" customFormat="1">
+      <c r="C31" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="E31" s="44">
+        <v>2030</v>
+      </c>
+      <c r="H31" s="44">
+        <f>H29*M26</f>
+        <v>0.83000000000000007</v>
+      </c>
+      <c r="I31" s="44">
+        <f>I29*M26</f>
+        <v>0.83000000000000007</v>
+      </c>
+      <c r="K31" s="44" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="32" spans="2:21">
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" t="s">
+        <v>221</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="K32" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="7" t="s">
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+    </row>
+    <row r="34" spans="2:13">
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+    </row>
+    <row r="35" spans="2:13">
+      <c r="B35" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="I33" s="8"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-    </row>
-    <row r="34" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B34" s="10" t="s">
+      <c r="I35" s="8"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="2:13" ht="15.75" thickBot="1">
+      <c r="B36" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E36" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F36" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G36" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="11" t="str">
+      <c r="H36" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="I34" s="11" t="str">
+      <c r="I36" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="J34" s="12" t="s">
+      <c r="J36" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K34" s="12" t="s">
+      <c r="K36" s="12" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13">
-      <c r="C35" t="s">
-        <v>206</v>
-      </c>
-      <c r="D35" t="s">
-        <v>108</v>
-      </c>
-      <c r="H35">
-        <v>5</v>
-      </c>
-      <c r="I35">
-        <v>5</v>
-      </c>
-      <c r="J35" t="s">
-        <v>107</v>
-      </c>
-      <c r="K35" t="s">
-        <v>106</v>
-      </c>
-      <c r="M35" s="25">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13">
-      <c r="C36" t="s">
-        <v>206</v>
-      </c>
-      <c r="D36" t="s">
-        <v>108</v>
-      </c>
-      <c r="H36" s="26">
-        <f>RSDAFC!L2*$M$35</f>
-        <v>1.2406827591965401E-2</v>
-      </c>
-      <c r="I36" s="26">
-        <f>RSDAFC!M2*$M$35</f>
-        <v>1.2406827591965401E-2</v>
-      </c>
-      <c r="K36" t="str">
-        <f>RSDAFC!C2</f>
-        <v>R-HC_Apt_ELC_HPN1</v>
       </c>
     </row>
     <row r="37" spans="2:13">
@@ -12894,17 +12898,20 @@
       <c r="D37" t="s">
         <v>108</v>
       </c>
-      <c r="H37" s="26">
-        <f>RSDAFC!L3*$M$35</f>
-        <v>1.2406827591965401E-2</v>
-      </c>
-      <c r="I37" s="26">
-        <f>RSDAFC!M3*$M$35</f>
-        <v>1.2406827591965401E-2</v>
-      </c>
-      <c r="K37" t="str">
-        <f>RSDAFC!C3</f>
-        <v>R-HC_Apt_ELC_HPN1</v>
+      <c r="H37">
+        <v>5</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37" t="s">
+        <v>107</v>
+      </c>
+      <c r="K37" t="s">
+        <v>106</v>
+      </c>
+      <c r="M37" s="25">
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="2:13">
@@ -12915,16 +12922,16 @@
         <v>108</v>
       </c>
       <c r="H38" s="26">
-        <f>RSDAFC!L4*$M$35</f>
+        <f>RSDAFC!L2*$M$37</f>
         <v>1.2406827591965401E-2</v>
       </c>
       <c r="I38" s="26">
-        <f>RSDAFC!M4*$M$35</f>
+        <f>RSDAFC!M2*$M$37</f>
         <v>1.2406827591965401E-2</v>
       </c>
       <c r="K38" t="str">
-        <f>RSDAFC!C4</f>
-        <v>R-HC_Apt_ELC_HPN2</v>
+        <f>RSDAFC!C2</f>
+        <v>R-HC_Apt_ELC_HPN1</v>
       </c>
     </row>
     <row r="39" spans="2:13">
@@ -12935,16 +12942,16 @@
         <v>108</v>
       </c>
       <c r="H39" s="26">
-        <f>RSDAFC!L5*$M$35</f>
+        <f>RSDAFC!L3*$M$37</f>
         <v>1.2406827591965401E-2</v>
       </c>
       <c r="I39" s="26">
-        <f>RSDAFC!M5*$M$35</f>
+        <f>RSDAFC!M3*$M$37</f>
         <v>1.2406827591965401E-2</v>
       </c>
       <c r="K39" t="str">
-        <f>RSDAFC!C5</f>
-        <v>R-HC_Apt_ELC_HPN2</v>
+        <f>RSDAFC!C3</f>
+        <v>R-HC_Apt_ELC_HPN1</v>
       </c>
     </row>
     <row r="40" spans="2:13">
@@ -12955,16 +12962,16 @@
         <v>108</v>
       </c>
       <c r="H40" s="26">
-        <f>RSDAFC!L6*$M$35</f>
-        <v>8.6842891028111498E-3</v>
+        <f>RSDAFC!L4*$M$37</f>
+        <v>1.2406827591965401E-2</v>
       </c>
       <c r="I40" s="26">
-        <f>RSDAFC!M6*$M$35</f>
-        <v>8.6842891028111498E-3</v>
+        <f>RSDAFC!M4*$M$37</f>
+        <v>1.2406827591965401E-2</v>
       </c>
       <c r="K40" t="str">
-        <f>RSDAFC!C6</f>
-        <v>R-HC_Att_ELC_HPN1</v>
+        <f>RSDAFC!C4</f>
+        <v>R-HC_Apt_ELC_HPN2</v>
       </c>
     </row>
     <row r="41" spans="2:13">
@@ -12975,16 +12982,16 @@
         <v>108</v>
       </c>
       <c r="H41" s="26">
-        <f>RSDAFC!L7*$M$35</f>
-        <v>8.6842891028111498E-3</v>
+        <f>RSDAFC!L5*$M$37</f>
+        <v>1.2406827591965401E-2</v>
       </c>
       <c r="I41" s="26">
-        <f>RSDAFC!M7*$M$35</f>
-        <v>8.6842891028111498E-3</v>
+        <f>RSDAFC!M5*$M$37</f>
+        <v>1.2406827591965401E-2</v>
       </c>
       <c r="K41" t="str">
-        <f>RSDAFC!C7</f>
-        <v>R-HC_Att_ELC_HPN1</v>
+        <f>RSDAFC!C5</f>
+        <v>R-HC_Apt_ELC_HPN2</v>
       </c>
     </row>
     <row r="42" spans="2:13">
@@ -12995,16 +13002,16 @@
         <v>108</v>
       </c>
       <c r="H42" s="26">
-        <f>RSDAFC!L8*$M$35</f>
+        <f>RSDAFC!L6*$M$37</f>
         <v>8.6842891028111498E-3</v>
       </c>
       <c r="I42" s="26">
-        <f>RSDAFC!M8*$M$35</f>
+        <f>RSDAFC!M6*$M$37</f>
         <v>8.6842891028111498E-3</v>
       </c>
       <c r="K42" t="str">
-        <f>RSDAFC!C8</f>
-        <v>R-HC_Att_ELC_HPN2</v>
+        <f>RSDAFC!C6</f>
+        <v>R-HC_Att_ELC_HPN1</v>
       </c>
     </row>
     <row r="43" spans="2:13">
@@ -13015,16 +13022,16 @@
         <v>108</v>
       </c>
       <c r="H43" s="26">
-        <f>RSDAFC!L9*$M$35</f>
+        <f>RSDAFC!L7*$M$37</f>
         <v>8.6842891028111498E-3</v>
       </c>
       <c r="I43" s="26">
-        <f>RSDAFC!M9*$M$35</f>
+        <f>RSDAFC!M7*$M$37</f>
         <v>8.6842891028111498E-3</v>
       </c>
       <c r="K43" t="str">
-        <f>RSDAFC!C9</f>
-        <v>R-HC_Att_ELC_HPN2</v>
+        <f>RSDAFC!C7</f>
+        <v>R-HC_Att_ELC_HPN1</v>
       </c>
     </row>
     <row r="44" spans="2:13">
@@ -13035,16 +13042,16 @@
         <v>108</v>
       </c>
       <c r="H44" s="26">
-        <f>RSDAFC!L10*$M$35</f>
-        <v>1.58935057836939E-2</v>
+        <f>RSDAFC!L8*$M$37</f>
+        <v>8.6842891028111498E-3</v>
       </c>
       <c r="I44" s="26">
-        <f>RSDAFC!M10*$M$35</f>
-        <v>1.58935057836939E-2</v>
+        <f>RSDAFC!M8*$M$37</f>
+        <v>8.6842891028111498E-3</v>
       </c>
       <c r="K44" t="str">
-        <f>RSDAFC!C10</f>
-        <v>R-HC_Det_ELC_HPN1</v>
+        <f>RSDAFC!C8</f>
+        <v>R-HC_Att_ELC_HPN2</v>
       </c>
     </row>
     <row r="45" spans="2:13">
@@ -13055,16 +13062,16 @@
         <v>108</v>
       </c>
       <c r="H45" s="26">
-        <f>RSDAFC!L11*$M$35</f>
-        <v>1.58935057836939E-2</v>
+        <f>RSDAFC!L9*$M$37</f>
+        <v>8.6842891028111498E-3</v>
       </c>
       <c r="I45" s="26">
-        <f>RSDAFC!M11*$M$35</f>
-        <v>1.58935057836939E-2</v>
+        <f>RSDAFC!M9*$M$37</f>
+        <v>8.6842891028111498E-3</v>
       </c>
       <c r="K45" t="str">
-        <f>RSDAFC!C11</f>
-        <v>R-HC_Det_ELC_HPN1</v>
+        <f>RSDAFC!C9</f>
+        <v>R-HC_Att_ELC_HPN2</v>
       </c>
     </row>
     <row r="46" spans="2:13">
@@ -13075,16 +13082,16 @@
         <v>108</v>
       </c>
       <c r="H46" s="26">
-        <f>RSDAFC!L12*$M$35</f>
+        <f>RSDAFC!L10*$M$37</f>
         <v>1.58935057836939E-2</v>
       </c>
       <c r="I46" s="26">
-        <f>RSDAFC!M12*$M$35</f>
+        <f>RSDAFC!M10*$M$37</f>
         <v>1.58935057836939E-2</v>
       </c>
       <c r="K46" t="str">
-        <f>RSDAFC!C12</f>
-        <v>R-HC_Det_ELC_HPN2</v>
+        <f>RSDAFC!C10</f>
+        <v>R-HC_Det_ELC_HPN1</v>
       </c>
     </row>
     <row r="47" spans="2:13">
@@ -13095,16 +13102,16 @@
         <v>108</v>
       </c>
       <c r="H47" s="26">
-        <f>RSDAFC!L13*$M$35</f>
+        <f>RSDAFC!L11*$M$37</f>
         <v>1.58935057836939E-2</v>
       </c>
       <c r="I47" s="26">
-        <f>RSDAFC!M13*$M$35</f>
+        <f>RSDAFC!M11*$M$37</f>
         <v>1.58935057836939E-2</v>
       </c>
       <c r="K47" t="str">
-        <f>RSDAFC!C13</f>
-        <v>R-HC_Det_ELC_HPN2</v>
+        <f>RSDAFC!C11</f>
+        <v>R-HC_Det_ELC_HPN1</v>
       </c>
     </row>
     <row r="48" spans="2:13">
@@ -13115,16 +13122,16 @@
         <v>108</v>
       </c>
       <c r="H48" s="26">
-        <f>RSDAFC!L14*$M$35</f>
-        <v>1.04804159170382E-2</v>
+        <f>RSDAFC!L12*$M$37</f>
+        <v>1.58935057836939E-2</v>
       </c>
       <c r="I48" s="26">
-        <f>RSDAFC!M14*$M$35</f>
-        <v>1.04804159170382E-2</v>
+        <f>RSDAFC!M12*$M$37</f>
+        <v>1.58935057836939E-2</v>
       </c>
       <c r="K48" t="str">
-        <f>RSDAFC!C14</f>
-        <v>R-SW_Apt_ELC_HPN1</v>
+        <f>RSDAFC!C12</f>
+        <v>R-HC_Det_ELC_HPN2</v>
       </c>
     </row>
     <row r="49" spans="3:11">
@@ -13135,16 +13142,16 @@
         <v>108</v>
       </c>
       <c r="H49" s="26">
-        <f>RSDAFC!L15*$M$35</f>
-        <v>1.04804159170382E-2</v>
+        <f>RSDAFC!L13*$M$37</f>
+        <v>1.58935057836939E-2</v>
       </c>
       <c r="I49" s="26">
-        <f>RSDAFC!M15*$M$35</f>
-        <v>1.04804159170382E-2</v>
+        <f>RSDAFC!M13*$M$37</f>
+        <v>1.58935057836939E-2</v>
       </c>
       <c r="K49" t="str">
-        <f>RSDAFC!C15</f>
-        <v>R-SW_Apt_ELC_HPN1</v>
+        <f>RSDAFC!C13</f>
+        <v>R-HC_Det_ELC_HPN2</v>
       </c>
     </row>
     <row r="50" spans="3:11">
@@ -13155,16 +13162,16 @@
         <v>108</v>
       </c>
       <c r="H50" s="26">
-        <f>RSDAFC!L16*$M$35</f>
-        <v>4.7397506033708351E-3</v>
+        <f>RSDAFC!L14*$M$37</f>
+        <v>1.04804159170382E-2</v>
       </c>
       <c r="I50" s="26">
-        <f>RSDAFC!M16*$M$35</f>
-        <v>4.7397506033708351E-3</v>
+        <f>RSDAFC!M14*$M$37</f>
+        <v>1.04804159170382E-2</v>
       </c>
       <c r="K50" t="str">
-        <f>RSDAFC!C16</f>
-        <v>R-SW_Apt_GAS_HHPN1</v>
+        <f>RSDAFC!C14</f>
+        <v>R-SW_Apt_ELC_HPN1</v>
       </c>
     </row>
     <row r="51" spans="3:11">
@@ -13175,16 +13182,16 @@
         <v>108</v>
       </c>
       <c r="H51" s="26">
-        <f>RSDAFC!L17*$M$35</f>
-        <v>4.7397506033708351E-3</v>
+        <f>RSDAFC!L15*$M$37</f>
+        <v>1.04804159170382E-2</v>
       </c>
       <c r="I51" s="26">
-        <f>RSDAFC!M17*$M$35</f>
-        <v>4.7397506033708351E-3</v>
+        <f>RSDAFC!M15*$M$37</f>
+        <v>1.04804159170382E-2</v>
       </c>
       <c r="K51" t="str">
-        <f>RSDAFC!C17</f>
-        <v>R-SW_Apt_GAS_HHPN1</v>
+        <f>RSDAFC!C15</f>
+        <v>R-SW_Apt_ELC_HPN1</v>
       </c>
     </row>
     <row r="52" spans="3:11">
@@ -13195,16 +13202,16 @@
         <v>108</v>
       </c>
       <c r="H52" s="26">
-        <f>RSDAFC!L18*$M$35</f>
+        <f>RSDAFC!L16*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="I52" s="26">
-        <f>RSDAFC!M18*$M$35</f>
+        <f>RSDAFC!M16*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="K52" t="str">
-        <f>RSDAFC!C18</f>
-        <v>R-SW_Apt_GAS_HPN1</v>
+        <f>RSDAFC!C16</f>
+        <v>R-SW_Apt_GAS_HHPN1</v>
       </c>
     </row>
     <row r="53" spans="3:11">
@@ -13215,16 +13222,16 @@
         <v>108</v>
       </c>
       <c r="H53" s="26">
-        <f>RSDAFC!L19*$M$35</f>
+        <f>RSDAFC!L17*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="I53" s="26">
-        <f>RSDAFC!M19*$M$35</f>
+        <f>RSDAFC!M17*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="K53" t="str">
-        <f>RSDAFC!C19</f>
-        <v>R-SW_Apt_GAS_HPN1</v>
+        <f>RSDAFC!C17</f>
+        <v>R-SW_Apt_GAS_HHPN1</v>
       </c>
     </row>
     <row r="54" spans="3:11">
@@ -13235,16 +13242,16 @@
         <v>108</v>
       </c>
       <c r="H54" s="26">
-        <f>RSDAFC!L20*$M$35</f>
+        <f>RSDAFC!L18*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="I54" s="26">
-        <f>RSDAFC!M20*$M$35</f>
+        <f>RSDAFC!M18*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="K54" t="str">
-        <f>RSDAFC!C20</f>
-        <v>R-SW_Apt_GAS_HPN2</v>
+        <f>RSDAFC!C18</f>
+        <v>R-SW_Apt_GAS_HPN1</v>
       </c>
     </row>
     <row r="55" spans="3:11">
@@ -13255,16 +13262,16 @@
         <v>108</v>
       </c>
       <c r="H55" s="26">
-        <f>RSDAFC!L21*$M$35</f>
+        <f>RSDAFC!L19*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="I55" s="26">
-        <f>RSDAFC!M21*$M$35</f>
+        <f>RSDAFC!M19*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="K55" t="str">
-        <f>RSDAFC!C21</f>
-        <v>R-SW_Apt_GAS_HPN2</v>
+        <f>RSDAFC!C19</f>
+        <v>R-SW_Apt_GAS_HPN1</v>
       </c>
     </row>
     <row r="56" spans="3:11">
@@ -13275,16 +13282,16 @@
         <v>108</v>
       </c>
       <c r="H56" s="26">
-        <f>RSDAFC!L22*$M$35</f>
+        <f>RSDAFC!L20*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="I56" s="26">
-        <f>RSDAFC!M22*$M$35</f>
+        <f>RSDAFC!M20*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="K56" t="str">
-        <f>RSDAFC!C22</f>
-        <v>R-SW_Apt_GAS_N1</v>
+        <f>RSDAFC!C20</f>
+        <v>R-SW_Apt_GAS_HPN2</v>
       </c>
     </row>
     <row r="57" spans="3:11">
@@ -13295,16 +13302,16 @@
         <v>108</v>
       </c>
       <c r="H57" s="26">
-        <f>RSDAFC!L23*$M$35</f>
+        <f>RSDAFC!L21*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="I57" s="26">
-        <f>RSDAFC!M23*$M$35</f>
+        <f>RSDAFC!M21*$M$37</f>
         <v>4.7397506033708351E-3</v>
       </c>
       <c r="K57" t="str">
-        <f>RSDAFC!C23</f>
-        <v>R-SW_Apt_GAS_N1</v>
+        <f>RSDAFC!C21</f>
+        <v>R-SW_Apt_GAS_HPN2</v>
       </c>
     </row>
     <row r="58" spans="3:11">
@@ -13315,16 +13322,16 @@
         <v>108</v>
       </c>
       <c r="H58" s="26">
-        <f>RSDAFC!L24*$M$35</f>
-        <v>3.5434891836400251E-4</v>
+        <f>RSDAFC!L22*$M$37</f>
+        <v>4.7397506033708351E-3</v>
       </c>
       <c r="I58" s="26">
-        <f>RSDAFC!M24*$M$35</f>
-        <v>3.5434891836400251E-4</v>
+        <f>RSDAFC!M22*$M$37</f>
+        <v>4.7397506033708351E-3</v>
       </c>
       <c r="K58" t="str">
-        <f>RSDAFC!C24</f>
-        <v>R-SW_Apt_HET_N1</v>
+        <f>RSDAFC!C22</f>
+        <v>R-SW_Apt_GAS_N1</v>
       </c>
     </row>
     <row r="59" spans="3:11">
@@ -13335,16 +13342,16 @@
         <v>108</v>
       </c>
       <c r="H59" s="26">
-        <f>RSDAFC!L25*$M$35</f>
-        <v>3.5434891836400251E-4</v>
+        <f>RSDAFC!L23*$M$37</f>
+        <v>4.7397506033708351E-3</v>
       </c>
       <c r="I59" s="26">
-        <f>RSDAFC!M25*$M$35</f>
-        <v>3.5434891836400251E-4</v>
+        <f>RSDAFC!M23*$M$37</f>
+        <v>4.7397506033708351E-3</v>
       </c>
       <c r="K59" t="str">
-        <f>RSDAFC!C25</f>
-        <v>R-SW_Apt_HET_N1</v>
+        <f>RSDAFC!C23</f>
+        <v>R-SW_Apt_GAS_N1</v>
       </c>
     </row>
     <row r="60" spans="3:11">
@@ -13355,16 +13362,16 @@
         <v>108</v>
       </c>
       <c r="H60" s="26">
-        <f>RSDAFC!L26*$M$35</f>
+        <f>RSDAFC!L24*$M$37</f>
         <v>3.5434891836400251E-4</v>
       </c>
       <c r="I60" s="26">
-        <f>RSDAFC!M26*$M$35</f>
+        <f>RSDAFC!M24*$M$37</f>
         <v>3.5434891836400251E-4</v>
       </c>
       <c r="K60" t="str">
-        <f>RSDAFC!C26</f>
-        <v>R-SW_Apt_HET_N2</v>
+        <f>RSDAFC!C24</f>
+        <v>R-SW_Apt_HET_N1</v>
       </c>
     </row>
     <row r="61" spans="3:11">
@@ -13375,16 +13382,16 @@
         <v>108</v>
       </c>
       <c r="H61" s="26">
-        <f>RSDAFC!L27*$M$35</f>
+        <f>RSDAFC!L25*$M$37</f>
         <v>3.5434891836400251E-4</v>
       </c>
       <c r="I61" s="26">
-        <f>RSDAFC!M27*$M$35</f>
+        <f>RSDAFC!M25*$M$37</f>
         <v>3.5434891836400251E-4</v>
       </c>
       <c r="K61" t="str">
-        <f>RSDAFC!C27</f>
-        <v>R-SW_Apt_HET_N2</v>
+        <f>RSDAFC!C25</f>
+        <v>R-SW_Apt_HET_N1</v>
       </c>
     </row>
     <row r="62" spans="3:11">
@@ -13395,16 +13402,16 @@
         <v>108</v>
       </c>
       <c r="H62" s="26">
-        <f>RSDAFC!L28*$M$35</f>
-        <v>1.199300219050925E-2</v>
+        <f>RSDAFC!L26*$M$37</f>
+        <v>3.5434891836400251E-4</v>
       </c>
       <c r="I62" s="26">
-        <f>RSDAFC!M28*$M$35</f>
-        <v>1.199300219050925E-2</v>
+        <f>RSDAFC!M26*$M$37</f>
+        <v>3.5434891836400251E-4</v>
       </c>
       <c r="K62" t="str">
-        <f>RSDAFC!C28</f>
-        <v>R-SW_Apt_KER_N1</v>
+        <f>RSDAFC!C26</f>
+        <v>R-SW_Apt_HET_N2</v>
       </c>
     </row>
     <row r="63" spans="3:11">
@@ -13415,16 +13422,16 @@
         <v>108</v>
       </c>
       <c r="H63" s="26">
-        <f>RSDAFC!L29*$M$35</f>
-        <v>1.199300219050925E-2</v>
+        <f>RSDAFC!L27*$M$37</f>
+        <v>3.5434891836400251E-4</v>
       </c>
       <c r="I63" s="26">
-        <f>RSDAFC!M29*$M$35</f>
-        <v>1.199300219050925E-2</v>
+        <f>RSDAFC!M27*$M$37</f>
+        <v>3.5434891836400251E-4</v>
       </c>
       <c r="K63" t="str">
-        <f>RSDAFC!C29</f>
-        <v>R-SW_Apt_KER_N1</v>
+        <f>RSDAFC!C27</f>
+        <v>R-SW_Apt_HET_N2</v>
       </c>
     </row>
     <row r="64" spans="3:11">
@@ -13435,16 +13442,16 @@
         <v>108</v>
       </c>
       <c r="H64" s="26">
-        <f>RSDAFC!L30*$M$35</f>
-        <v>8.90395563099655E-3</v>
+        <f>RSDAFC!L28*$M$37</f>
+        <v>1.199300219050925E-2</v>
       </c>
       <c r="I64" s="26">
-        <f>RSDAFC!M30*$M$35</f>
-        <v>8.90395563099655E-3</v>
+        <f>RSDAFC!M28*$M$37</f>
+        <v>1.199300219050925E-2</v>
       </c>
       <c r="K64" t="str">
-        <f>RSDAFC!C30</f>
-        <v>R-SW_Apt_LPG_N1</v>
+        <f>RSDAFC!C28</f>
+        <v>R-SW_Apt_KER_N1</v>
       </c>
     </row>
     <row r="65" spans="3:11">
@@ -13455,16 +13462,16 @@
         <v>108</v>
       </c>
       <c r="H65" s="26">
-        <f>RSDAFC!L31*$M$35</f>
-        <v>8.90395563099655E-3</v>
+        <f>RSDAFC!L29*$M$37</f>
+        <v>1.199300219050925E-2</v>
       </c>
       <c r="I65" s="26">
-        <f>RSDAFC!M31*$M$35</f>
-        <v>8.90395563099655E-3</v>
+        <f>RSDAFC!M29*$M$37</f>
+        <v>1.199300219050925E-2</v>
       </c>
       <c r="K65" t="str">
-        <f>RSDAFC!C31</f>
-        <v>R-SW_Apt_LPG_N1</v>
+        <f>RSDAFC!C29</f>
+        <v>R-SW_Apt_KER_N1</v>
       </c>
     </row>
     <row r="66" spans="3:11">
@@ -13475,16 +13482,16 @@
         <v>108</v>
       </c>
       <c r="H66" s="26">
-        <f>RSDAFC!L32*$M$35</f>
-        <v>6.8519450639461001E-3</v>
+        <f>RSDAFC!L30*$M$37</f>
+        <v>8.90395563099655E-3</v>
       </c>
       <c r="I66" s="26">
-        <f>RSDAFC!M32*$M$35</f>
-        <v>6.8519450639461001E-3</v>
+        <f>RSDAFC!M30*$M$37</f>
+        <v>8.90395563099655E-3</v>
       </c>
       <c r="K66" t="str">
-        <f>RSDAFC!C32</f>
-        <v>R-SW_Apt_WOO_N1</v>
+        <f>RSDAFC!C30</f>
+        <v>R-SW_Apt_LPG_N1</v>
       </c>
     </row>
     <row r="67" spans="3:11">
@@ -13495,16 +13502,16 @@
         <v>108</v>
       </c>
       <c r="H67" s="26">
-        <f>RSDAFC!L33*$M$35</f>
-        <v>6.8519450639461001E-3</v>
+        <f>RSDAFC!L31*$M$37</f>
+        <v>8.90395563099655E-3</v>
       </c>
       <c r="I67" s="26">
-        <f>RSDAFC!M33*$M$35</f>
-        <v>6.8519450639461001E-3</v>
+        <f>RSDAFC!M31*$M$37</f>
+        <v>8.90395563099655E-3</v>
       </c>
       <c r="K67" t="str">
-        <f>RSDAFC!C33</f>
-        <v>R-SW_Apt_WOO_N1</v>
+        <f>RSDAFC!C31</f>
+        <v>R-SW_Apt_LPG_N1</v>
       </c>
     </row>
     <row r="68" spans="3:11">
@@ -13515,16 +13522,16 @@
         <v>108</v>
       </c>
       <c r="H68" s="26">
-        <f>RSDAFC!L34*$M$35</f>
-        <v>9.3952077625382002E-3</v>
+        <f>RSDAFC!L32*$M$37</f>
+        <v>6.8519450639461001E-3</v>
       </c>
       <c r="I68" s="26">
-        <f>RSDAFC!M34*$M$35</f>
-        <v>9.3952077625382002E-3</v>
+        <f>RSDAFC!M32*$M$37</f>
+        <v>6.8519450639461001E-3</v>
       </c>
       <c r="K68" t="str">
-        <f>RSDAFC!C34</f>
-        <v>R-SW_Att_ELC_HPN1</v>
+        <f>RSDAFC!C32</f>
+        <v>R-SW_Apt_WOO_N1</v>
       </c>
     </row>
     <row r="69" spans="3:11">
@@ -13535,16 +13542,16 @@
         <v>108</v>
       </c>
       <c r="H69" s="26">
-        <f>RSDAFC!L35*$M$35</f>
-        <v>9.3952077625382002E-3</v>
+        <f>RSDAFC!L33*$M$37</f>
+        <v>6.8519450639461001E-3</v>
       </c>
       <c r="I69" s="26">
-        <f>RSDAFC!M35*$M$35</f>
-        <v>9.3952077625382002E-3</v>
+        <f>RSDAFC!M33*$M$37</f>
+        <v>6.8519450639461001E-3</v>
       </c>
       <c r="K69" t="str">
-        <f>RSDAFC!C35</f>
-        <v>R-SW_Att_ELC_HPN1</v>
+        <f>RSDAFC!C33</f>
+        <v>R-SW_Apt_WOO_N1</v>
       </c>
     </row>
     <row r="70" spans="3:11">
@@ -13555,16 +13562,16 @@
         <v>108</v>
       </c>
       <c r="H70" s="26">
-        <f>RSDAFC!L36*$M$35</f>
+        <f>RSDAFC!L34*$M$37</f>
         <v>9.3952077625382002E-3</v>
       </c>
       <c r="I70" s="26">
-        <f>RSDAFC!M36*$M$35</f>
+        <f>RSDAFC!M34*$M$37</f>
         <v>9.3952077625382002E-3</v>
       </c>
       <c r="K70" t="str">
-        <f>RSDAFC!C36</f>
-        <v>R-SW_Att_ELC_HPN2</v>
+        <f>RSDAFC!C34</f>
+        <v>R-SW_Att_ELC_HPN1</v>
       </c>
     </row>
     <row r="71" spans="3:11">
@@ -13575,16 +13582,16 @@
         <v>108</v>
       </c>
       <c r="H71" s="26">
-        <f>RSDAFC!L37*$M$35</f>
+        <f>RSDAFC!L35*$M$37</f>
         <v>9.3952077625382002E-3</v>
       </c>
       <c r="I71" s="26">
-        <f>RSDAFC!M37*$M$35</f>
+        <f>RSDAFC!M35*$M$37</f>
         <v>9.3952077625382002E-3</v>
       </c>
       <c r="K71" t="str">
-        <f>RSDAFC!C37</f>
-        <v>R-SW_Att_ELC_HPN2</v>
+        <f>RSDAFC!C35</f>
+        <v>R-SW_Att_ELC_HPN1</v>
       </c>
     </row>
     <row r="72" spans="3:11">
@@ -13595,16 +13602,16 @@
         <v>108</v>
       </c>
       <c r="H72" s="26">
-        <f>RSDAFC!L38*$M$35</f>
-        <v>7.8256501810713003E-3</v>
+        <f>RSDAFC!L36*$M$37</f>
+        <v>9.3952077625382002E-3</v>
       </c>
       <c r="I72" s="26">
-        <f>RSDAFC!M38*$M$35</f>
-        <v>7.8256501810713003E-3</v>
+        <f>RSDAFC!M36*$M$37</f>
+        <v>9.3952077625382002E-3</v>
       </c>
       <c r="K72" t="str">
-        <f>RSDAFC!C38</f>
-        <v>R-SW_Att_GAS_HHPN1</v>
+        <f>RSDAFC!C36</f>
+        <v>R-SW_Att_ELC_HPN2</v>
       </c>
     </row>
     <row r="73" spans="3:11">
@@ -13615,16 +13622,16 @@
         <v>108</v>
       </c>
       <c r="H73" s="26">
-        <f>RSDAFC!L39*$M$35</f>
-        <v>7.8256501810713003E-3</v>
+        <f>RSDAFC!L37*$M$37</f>
+        <v>9.3952077625382002E-3</v>
       </c>
       <c r="I73" s="26">
-        <f>RSDAFC!M39*$M$35</f>
-        <v>7.8256501810713003E-3</v>
+        <f>RSDAFC!M37*$M$37</f>
+        <v>9.3952077625382002E-3</v>
       </c>
       <c r="K73" t="str">
-        <f>RSDAFC!C39</f>
-        <v>R-SW_Att_GAS_HHPN1</v>
+        <f>RSDAFC!C37</f>
+        <v>R-SW_Att_ELC_HPN2</v>
       </c>
     </row>
     <row r="74" spans="3:11">
@@ -13635,16 +13642,16 @@
         <v>108</v>
       </c>
       <c r="H74" s="26">
-        <f>RSDAFC!L40*$M$35</f>
+        <f>RSDAFC!L38*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I74" s="26">
-        <f>RSDAFC!M40*$M$35</f>
+        <f>RSDAFC!M38*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K74" t="str">
-        <f>RSDAFC!C40</f>
-        <v>R-SW_Att_GAS_HPN1</v>
+        <f>RSDAFC!C38</f>
+        <v>R-SW_Att_GAS_HHPN1</v>
       </c>
     </row>
     <row r="75" spans="3:11">
@@ -13655,16 +13662,16 @@
         <v>108</v>
       </c>
       <c r="H75" s="26">
-        <f>RSDAFC!L41*$M$35</f>
+        <f>RSDAFC!L39*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I75" s="26">
-        <f>RSDAFC!M41*$M$35</f>
+        <f>RSDAFC!M39*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K75" t="str">
-        <f>RSDAFC!C41</f>
-        <v>R-SW_Att_GAS_HPN1</v>
+        <f>RSDAFC!C39</f>
+        <v>R-SW_Att_GAS_HHPN1</v>
       </c>
     </row>
     <row r="76" spans="3:11">
@@ -13675,16 +13682,16 @@
         <v>108</v>
       </c>
       <c r="H76" s="26">
-        <f>RSDAFC!L42*$M$35</f>
+        <f>RSDAFC!L40*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I76" s="26">
-        <f>RSDAFC!M42*$M$35</f>
+        <f>RSDAFC!M40*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K76" t="str">
-        <f>RSDAFC!C42</f>
-        <v>R-SW_Att_GAS_HPN2</v>
+        <f>RSDAFC!C40</f>
+        <v>R-SW_Att_GAS_HPN1</v>
       </c>
     </row>
     <row r="77" spans="3:11">
@@ -13695,16 +13702,16 @@
         <v>108</v>
       </c>
       <c r="H77" s="26">
-        <f>RSDAFC!L43*$M$35</f>
+        <f>RSDAFC!L41*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I77" s="26">
-        <f>RSDAFC!M43*$M$35</f>
+        <f>RSDAFC!M41*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K77" t="str">
-        <f>RSDAFC!C43</f>
-        <v>R-SW_Att_GAS_HPN2</v>
+        <f>RSDAFC!C41</f>
+        <v>R-SW_Att_GAS_HPN1</v>
       </c>
     </row>
     <row r="78" spans="3:11">
@@ -13715,16 +13722,16 @@
         <v>108</v>
       </c>
       <c r="H78" s="26">
-        <f>RSDAFC!L44*$M$35</f>
+        <f>RSDAFC!L42*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I78" s="26">
-        <f>RSDAFC!M44*$M$35</f>
+        <f>RSDAFC!M42*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K78" t="str">
-        <f>RSDAFC!C44</f>
-        <v>R-SW_Att_GAS_N1</v>
+        <f>RSDAFC!C42</f>
+        <v>R-SW_Att_GAS_HPN2</v>
       </c>
     </row>
     <row r="79" spans="3:11">
@@ -13735,16 +13742,16 @@
         <v>108</v>
       </c>
       <c r="H79" s="26">
-        <f>RSDAFC!L45*$M$35</f>
+        <f>RSDAFC!L43*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I79" s="26">
-        <f>RSDAFC!M45*$M$35</f>
+        <f>RSDAFC!M43*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K79" t="str">
-        <f>RSDAFC!C45</f>
-        <v>R-SW_Att_GAS_N1</v>
+        <f>RSDAFC!C43</f>
+        <v>R-SW_Att_GAS_HPN2</v>
       </c>
     </row>
     <row r="80" spans="3:11">
@@ -13755,16 +13762,16 @@
         <v>108</v>
       </c>
       <c r="H80" s="26">
-        <f>RSDAFC!L46*$M$35</f>
+        <f>RSDAFC!L44*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I80" s="26">
-        <f>RSDAFC!M46*$M$35</f>
+        <f>RSDAFC!M44*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K80" t="str">
-        <f>RSDAFC!C46</f>
-        <v>R-SW_Att_GAS_N2</v>
+        <f>RSDAFC!C44</f>
+        <v>R-SW_Att_GAS_N1</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -13775,16 +13782,16 @@
         <v>108</v>
       </c>
       <c r="H81" s="26">
-        <f>RSDAFC!L47*$M$35</f>
+        <f>RSDAFC!L45*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I81" s="26">
-        <f>RSDAFC!M47*$M$35</f>
+        <f>RSDAFC!M45*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K81" t="str">
-        <f>RSDAFC!C47</f>
-        <v>R-SW_Att_GAS_N2</v>
+        <f>RSDAFC!C45</f>
+        <v>R-SW_Att_GAS_N1</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -13795,16 +13802,16 @@
         <v>108</v>
       </c>
       <c r="H82" s="26">
-        <f>RSDAFC!L48*$M$35</f>
+        <f>RSDAFC!L46*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I82" s="26">
-        <f>RSDAFC!M48*$M$35</f>
+        <f>RSDAFC!M46*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K82" t="str">
-        <f>RSDAFC!C48</f>
-        <v>R-SW_Att_GAS_N3</v>
+        <f>RSDAFC!C46</f>
+        <v>R-SW_Att_GAS_N2</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -13815,16 +13822,16 @@
         <v>108</v>
       </c>
       <c r="H83" s="26">
-        <f>RSDAFC!L49*$M$35</f>
+        <f>RSDAFC!L47*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="I83" s="26">
-        <f>RSDAFC!M49*$M$35</f>
+        <f>RSDAFC!M47*$M$37</f>
         <v>7.8256501810713003E-3</v>
       </c>
       <c r="K83" t="str">
-        <f>RSDAFC!C49</f>
-        <v>R-SW_Att_GAS_N3</v>
+        <f>RSDAFC!C47</f>
+        <v>R-SW_Att_GAS_N2</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -13835,16 +13842,16 @@
         <v>108</v>
       </c>
       <c r="H84" s="26">
-        <f>RSDAFC!L50*$M$35</f>
-        <v>3.7989460522007048E-3</v>
+        <f>RSDAFC!L48*$M$37</f>
+        <v>7.8256501810713003E-3</v>
       </c>
       <c r="I84" s="26">
-        <f>RSDAFC!M50*$M$35</f>
-        <v>3.7989460522007048E-3</v>
+        <f>RSDAFC!M48*$M$37</f>
+        <v>7.8256501810713003E-3</v>
       </c>
       <c r="K84" t="str">
-        <f>RSDAFC!C50</f>
-        <v>R-SW_Att_HET_N1</v>
+        <f>RSDAFC!C48</f>
+        <v>R-SW_Att_GAS_N3</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -13855,16 +13862,16 @@
         <v>108</v>
       </c>
       <c r="H85" s="26">
-        <f>RSDAFC!L51*$M$35</f>
-        <v>3.7989460522007048E-3</v>
+        <f>RSDAFC!L49*$M$37</f>
+        <v>7.8256501810713003E-3</v>
       </c>
       <c r="I85" s="26">
-        <f>RSDAFC!M51*$M$35</f>
-        <v>3.7989460522007048E-3</v>
+        <f>RSDAFC!M49*$M$37</f>
+        <v>7.8256501810713003E-3</v>
       </c>
       <c r="K85" t="str">
-        <f>RSDAFC!C51</f>
-        <v>R-SW_Att_HET_N1</v>
+        <f>RSDAFC!C49</f>
+        <v>R-SW_Att_GAS_N3</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -13875,16 +13882,16 @@
         <v>108</v>
       </c>
       <c r="H86" s="26">
-        <f>RSDAFC!L52*$M$35</f>
+        <f>RSDAFC!L50*$M$37</f>
         <v>3.7989460522007048E-3</v>
       </c>
       <c r="I86" s="26">
-        <f>RSDAFC!M52*$M$35</f>
+        <f>RSDAFC!M50*$M$37</f>
         <v>3.7989460522007048E-3</v>
       </c>
       <c r="K86" t="str">
-        <f>RSDAFC!C52</f>
-        <v>R-SW_Att_HET_N2</v>
+        <f>RSDAFC!C50</f>
+        <v>R-SW_Att_HET_N1</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -13895,16 +13902,16 @@
         <v>108</v>
       </c>
       <c r="H87" s="26">
-        <f>RSDAFC!L53*$M$35</f>
+        <f>RSDAFC!L51*$M$37</f>
         <v>3.7989460522007048E-3</v>
       </c>
       <c r="I87" s="26">
-        <f>RSDAFC!M53*$M$35</f>
+        <f>RSDAFC!M51*$M$37</f>
         <v>3.7989460522007048E-3</v>
       </c>
       <c r="K87" t="str">
-        <f>RSDAFC!C53</f>
-        <v>R-SW_Att_HET_N2</v>
+        <f>RSDAFC!C51</f>
+        <v>R-SW_Att_HET_N1</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -13915,16 +13922,16 @@
         <v>108</v>
       </c>
       <c r="H88" s="26">
-        <f>RSDAFC!L54*$M$35</f>
-        <v>9.8399724094370006E-3</v>
+        <f>RSDAFC!L52*$M$37</f>
+        <v>3.7989460522007048E-3</v>
       </c>
       <c r="I88" s="26">
-        <f>RSDAFC!M54*$M$35</f>
-        <v>9.8399724094370006E-3</v>
+        <f>RSDAFC!M52*$M$37</f>
+        <v>3.7989460522007048E-3</v>
       </c>
       <c r="K88" t="str">
-        <f>RSDAFC!C54</f>
-        <v>R-SW_Att_KER_N1</v>
+        <f>RSDAFC!C52</f>
+        <v>R-SW_Att_HET_N2</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -13935,16 +13942,16 @@
         <v>108</v>
       </c>
       <c r="H89" s="26">
-        <f>RSDAFC!L55*$M$35</f>
-        <v>9.8399724094370006E-3</v>
+        <f>RSDAFC!L53*$M$37</f>
+        <v>3.7989460522007048E-3</v>
       </c>
       <c r="I89" s="26">
-        <f>RSDAFC!M55*$M$35</f>
-        <v>9.8399724094370006E-3</v>
+        <f>RSDAFC!M53*$M$37</f>
+        <v>3.7989460522007048E-3</v>
       </c>
       <c r="K89" t="str">
-        <f>RSDAFC!C55</f>
-        <v>R-SW_Att_KER_N1</v>
+        <f>RSDAFC!C53</f>
+        <v>R-SW_Att_HET_N2</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -13955,16 +13962,16 @@
         <v>108</v>
       </c>
       <c r="H90" s="26">
-        <f>RSDAFC!L56*$M$35</f>
+        <f>RSDAFC!L54*$M$37</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="I90" s="26">
-        <f>RSDAFC!M56*$M$35</f>
+        <f>RSDAFC!M54*$M$37</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="K90" t="str">
-        <f>RSDAFC!C56</f>
-        <v>R-SW_Att_KER_N2</v>
+        <f>RSDAFC!C54</f>
+        <v>R-SW_Att_KER_N1</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -13975,16 +13982,16 @@
         <v>108</v>
       </c>
       <c r="H91" s="26">
-        <f>RSDAFC!L57*$M$35</f>
+        <f>RSDAFC!L55*$M$37</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="I91" s="26">
-        <f>RSDAFC!M57*$M$35</f>
+        <f>RSDAFC!M55*$M$37</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="K91" t="str">
-        <f>RSDAFC!C57</f>
-        <v>R-SW_Att_KER_N2</v>
+        <f>RSDAFC!C55</f>
+        <v>R-SW_Att_KER_N1</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -13995,16 +14002,16 @@
         <v>108</v>
       </c>
       <c r="H92" s="26">
-        <f>RSDAFC!L58*$M$35</f>
+        <f>RSDAFC!L56*$M$37</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="I92" s="26">
-        <f>RSDAFC!M58*$M$35</f>
+        <f>RSDAFC!M56*$M$37</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="K92" t="str">
-        <f>RSDAFC!C58</f>
-        <v>R-SW_Att_KER_N3</v>
+        <f>RSDAFC!C56</f>
+        <v>R-SW_Att_KER_N2</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -14015,66 +14022,56 @@
         <v>108</v>
       </c>
       <c r="H93" s="26">
-        <f>RSDAFC!L59*$M$35</f>
+        <f>RSDAFC!L57*$M$37</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="I93" s="26">
-        <f>RSDAFC!M59*$M$35</f>
+        <f>RSDAFC!M57*$M$37</f>
         <v>9.8399724094370006E-3</v>
       </c>
       <c r="K93" t="str">
+        <f>RSDAFC!C57</f>
+        <v>R-SW_Att_KER_N2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="C94" t="s">
+        <v>206</v>
+      </c>
+      <c r="D94" t="s">
+        <v>108</v>
+      </c>
+      <c r="H94" s="26">
+        <f>RSDAFC!L58*$M$37</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="I94" s="26">
+        <f>RSDAFC!M58*$M$37</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="K94" t="str">
+        <f>RSDAFC!C58</f>
+        <v>R-SW_Att_KER_N3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="C95" t="s">
+        <v>206</v>
+      </c>
+      <c r="D95" t="s">
+        <v>108</v>
+      </c>
+      <c r="H95" s="26">
+        <f>RSDAFC!L59*$M$37</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="I95" s="26">
+        <f>RSDAFC!M59*$M$37</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="K95" t="str">
         <f>RSDAFC!C59</f>
         <v>R-SW_Att_KER_N3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11">
-      <c r="A94" s="30"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="D94" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E94" s="30"/>
-      <c r="F94" s="30"/>
-      <c r="G94" s="30"/>
-      <c r="H94" s="31">
-        <f>H100</f>
-        <v>2.14779508723714E-2</v>
-      </c>
-      <c r="I94" s="31">
-        <f>I100</f>
-        <v>2.14779508723714E-2</v>
-      </c>
-      <c r="J94" s="30"/>
-      <c r="K94" s="30" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11">
-      <c r="A95" s="30"/>
-      <c r="B95" s="30"/>
-      <c r="C95" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="D95" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E95" s="30"/>
-      <c r="F95" s="30"/>
-      <c r="G95" s="30"/>
-      <c r="H95" s="31">
-        <f>H101</f>
-        <v>2.14779508723714E-2</v>
-      </c>
-      <c r="I95" s="31">
-        <f>I101</f>
-        <v>2.14779508723714E-2</v>
-      </c>
-      <c r="J95" s="30"/>
-      <c r="K95" s="30" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -14090,16 +14087,16 @@
       <c r="F96" s="30"/>
       <c r="G96" s="30"/>
       <c r="H96" s="31">
-        <f>H93</f>
-        <v>9.8399724094370006E-3</v>
+        <f>H102</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="I96" s="31">
-        <f>I93</f>
-        <v>9.8399724094370006E-3</v>
+        <f>I102</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="J96" s="30"/>
       <c r="K96" s="30" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -14115,56 +14112,66 @@
       <c r="F97" s="30"/>
       <c r="G97" s="30"/>
       <c r="H97" s="31">
-        <f>H96</f>
-        <v>9.8399724094370006E-3</v>
+        <f>H103</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="I97" s="31">
-        <f>I96</f>
-        <v>9.8399724094370006E-3</v>
+        <f>I103</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="J97" s="30"/>
       <c r="K97" s="30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="30"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E98" s="30"/>
+      <c r="F98" s="30"/>
+      <c r="G98" s="30"/>
+      <c r="H98" s="31">
+        <f>H95</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="I98" s="31">
+        <f>I95</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="J98" s="30"/>
+      <c r="K98" s="30" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" s="30"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E99" s="30"/>
+      <c r="F99" s="30"/>
+      <c r="G99" s="30"/>
+      <c r="H99" s="31">
+        <f>H98</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="I99" s="31">
+        <f>I98</f>
+        <v>9.8399724094370006E-3</v>
+      </c>
+      <c r="J99" s="30"/>
+      <c r="K99" s="30" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11">
-      <c r="C98" t="s">
-        <v>206</v>
-      </c>
-      <c r="D98" t="s">
-        <v>108</v>
-      </c>
-      <c r="H98" s="26">
-        <f>RSDAFC!L60*$M$35</f>
-        <v>1.1698585866472801E-2</v>
-      </c>
-      <c r="I98" s="26">
-        <f>RSDAFC!M60*$M$35</f>
-        <v>1.1698585866472801E-2</v>
-      </c>
-      <c r="K98" t="str">
-        <f>RSDAFC!C60</f>
-        <v>R-SW_Att_LPG_N1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11">
-      <c r="C99" t="s">
-        <v>206</v>
-      </c>
-      <c r="D99" t="s">
-        <v>108</v>
-      </c>
-      <c r="H99" s="26">
-        <f>RSDAFC!L61*$M$35</f>
-        <v>1.1698585866472801E-2</v>
-      </c>
-      <c r="I99" s="26">
-        <f>RSDAFC!M61*$M$35</f>
-        <v>1.1698585866472801E-2</v>
-      </c>
-      <c r="K99" t="str">
-        <f>RSDAFC!C61</f>
-        <v>R-SW_Att_LPG_N1</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -14175,16 +14182,16 @@
         <v>108</v>
       </c>
       <c r="H100" s="26">
-        <f>RSDAFC!L62*$M$35</f>
-        <v>2.14779508723714E-2</v>
+        <f>RSDAFC!L60*$M$37</f>
+        <v>1.1698585866472801E-2</v>
       </c>
       <c r="I100" s="26">
-        <f>RSDAFC!M62*$M$35</f>
-        <v>2.14779508723714E-2</v>
+        <f>RSDAFC!M60*$M$37</f>
+        <v>1.1698585866472801E-2</v>
       </c>
       <c r="K100" t="str">
-        <f>RSDAFC!C62</f>
-        <v>R-SW_Att_WOO_N1</v>
+        <f>RSDAFC!C60</f>
+        <v>R-SW_Att_LPG_N1</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -14195,16 +14202,16 @@
         <v>108</v>
       </c>
       <c r="H101" s="26">
-        <f>RSDAFC!L63*$M$35</f>
-        <v>2.14779508723714E-2</v>
+        <f>RSDAFC!L61*$M$37</f>
+        <v>1.1698585866472801E-2</v>
       </c>
       <c r="I101" s="26">
-        <f>RSDAFC!M63*$M$35</f>
-        <v>2.14779508723714E-2</v>
+        <f>RSDAFC!M61*$M$37</f>
+        <v>1.1698585866472801E-2</v>
       </c>
       <c r="K101" t="str">
-        <f>RSDAFC!C63</f>
-        <v>R-SW_Att_WOO_N1</v>
+        <f>RSDAFC!C61</f>
+        <v>R-SW_Att_LPG_N1</v>
       </c>
     </row>
     <row r="102" spans="1:11">
@@ -14215,16 +14222,16 @@
         <v>108</v>
       </c>
       <c r="H102" s="26">
-        <f>RSDAFC!L64*$M$35</f>
-        <v>1.3735723758749249E-2</v>
+        <f>RSDAFC!L62*$M$37</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="I102" s="26">
-        <f>RSDAFC!M64*$M$35</f>
-        <v>1.3735723758749249E-2</v>
+        <f>RSDAFC!M62*$M$37</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="K102" t="str">
-        <f>RSDAFC!C64</f>
-        <v>R-SW_Det_ELC_HPN1</v>
+        <f>RSDAFC!C62</f>
+        <v>R-SW_Att_WOO_N1</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -14235,16 +14242,16 @@
         <v>108</v>
       </c>
       <c r="H103" s="26">
-        <f>RSDAFC!L65*$M$35</f>
-        <v>1.3735723758749249E-2</v>
+        <f>RSDAFC!L63*$M$37</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="I103" s="26">
-        <f>RSDAFC!M65*$M$35</f>
-        <v>1.3735723758749249E-2</v>
+        <f>RSDAFC!M63*$M$37</f>
+        <v>2.14779508723714E-2</v>
       </c>
       <c r="K103" t="str">
-        <f>RSDAFC!C65</f>
-        <v>R-SW_Det_ELC_HPN1</v>
+        <f>RSDAFC!C63</f>
+        <v>R-SW_Att_WOO_N1</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -14255,16 +14262,16 @@
         <v>108</v>
       </c>
       <c r="H104" s="26">
-        <f>RSDAFC!L66*$M$35</f>
+        <f>RSDAFC!L64*$M$37</f>
         <v>1.3735723758749249E-2</v>
       </c>
       <c r="I104" s="26">
-        <f>RSDAFC!M66*$M$35</f>
+        <f>RSDAFC!M64*$M$37</f>
         <v>1.3735723758749249E-2</v>
       </c>
       <c r="K104" t="str">
-        <f>RSDAFC!C66</f>
-        <v>R-SW_Det_ELC_HPN2</v>
+        <f>RSDAFC!C64</f>
+        <v>R-SW_Det_ELC_HPN1</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -14275,16 +14282,16 @@
         <v>108</v>
       </c>
       <c r="H105" s="26">
-        <f>RSDAFC!L67*$M$35</f>
+        <f>RSDAFC!L65*$M$37</f>
         <v>1.3735723758749249E-2</v>
       </c>
       <c r="I105" s="26">
-        <f>RSDAFC!M67*$M$35</f>
+        <f>RSDAFC!M65*$M$37</f>
         <v>1.3735723758749249E-2</v>
       </c>
       <c r="K105" t="str">
-        <f>RSDAFC!C67</f>
-        <v>R-SW_Det_ELC_HPN2</v>
+        <f>RSDAFC!C65</f>
+        <v>R-SW_Det_ELC_HPN1</v>
       </c>
     </row>
     <row r="106" spans="1:11">
@@ -14295,16 +14302,16 @@
         <v>108</v>
       </c>
       <c r="H106" s="26">
-        <f>RSDAFC!L68*$M$35</f>
-        <v>1.222361012943445E-2</v>
+        <f>RSDAFC!L66*$M$37</f>
+        <v>1.3735723758749249E-2</v>
       </c>
       <c r="I106" s="26">
-        <f>RSDAFC!M68*$M$35</f>
-        <v>1.222361012943445E-2</v>
+        <f>RSDAFC!M66*$M$37</f>
+        <v>1.3735723758749249E-2</v>
       </c>
       <c r="K106" t="str">
-        <f>RSDAFC!C68</f>
-        <v>R-SW_Det_GAS_HHPN1</v>
+        <f>RSDAFC!C66</f>
+        <v>R-SW_Det_ELC_HPN2</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -14315,16 +14322,16 @@
         <v>108</v>
       </c>
       <c r="H107" s="26">
-        <f>RSDAFC!L69*$M$35</f>
-        <v>1.222361012943445E-2</v>
+        <f>RSDAFC!L67*$M$37</f>
+        <v>1.3735723758749249E-2</v>
       </c>
       <c r="I107" s="26">
-        <f>RSDAFC!M69*$M$35</f>
-        <v>1.222361012943445E-2</v>
+        <f>RSDAFC!M67*$M$37</f>
+        <v>1.3735723758749249E-2</v>
       </c>
       <c r="K107" t="str">
-        <f>RSDAFC!C69</f>
-        <v>R-SW_Det_GAS_HHPN1</v>
+        <f>RSDAFC!C67</f>
+        <v>R-SW_Det_ELC_HPN2</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -14335,16 +14342,16 @@
         <v>108</v>
       </c>
       <c r="H108" s="26">
-        <f>RSDAFC!L70*$M$35</f>
+        <f>RSDAFC!L68*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="I108" s="26">
-        <f>RSDAFC!M70*$M$35</f>
+        <f>RSDAFC!M68*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="K108" t="str">
-        <f>RSDAFC!C70</f>
-        <v>R-SW_Det_GAS_HPN1</v>
+        <f>RSDAFC!C68</f>
+        <v>R-SW_Det_GAS_HHPN1</v>
       </c>
     </row>
     <row r="109" spans="1:11">
@@ -14355,16 +14362,16 @@
         <v>108</v>
       </c>
       <c r="H109" s="26">
-        <f>RSDAFC!L71*$M$35</f>
+        <f>RSDAFC!L69*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="I109" s="26">
-        <f>RSDAFC!M71*$M$35</f>
+        <f>RSDAFC!M69*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="K109" t="str">
-        <f>RSDAFC!C71</f>
-        <v>R-SW_Det_GAS_HPN1</v>
+        <f>RSDAFC!C69</f>
+        <v>R-SW_Det_GAS_HHPN1</v>
       </c>
     </row>
     <row r="110" spans="1:11">
@@ -14375,16 +14382,16 @@
         <v>108</v>
       </c>
       <c r="H110" s="26">
-        <f>RSDAFC!L72*$M$35</f>
+        <f>RSDAFC!L70*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="I110" s="26">
-        <f>RSDAFC!M72*$M$35</f>
+        <f>RSDAFC!M70*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="K110" t="str">
-        <f>RSDAFC!C72</f>
-        <v>R-SW_Det_GAS_HPN2</v>
+        <f>RSDAFC!C70</f>
+        <v>R-SW_Det_GAS_HPN1</v>
       </c>
     </row>
     <row r="111" spans="1:11">
@@ -14395,16 +14402,16 @@
         <v>108</v>
       </c>
       <c r="H111" s="26">
-        <f>RSDAFC!L73*$M$35</f>
+        <f>RSDAFC!L71*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="I111" s="26">
-        <f>RSDAFC!M73*$M$35</f>
+        <f>RSDAFC!M71*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="K111" t="str">
-        <f>RSDAFC!C73</f>
-        <v>R-SW_Det_GAS_HPN2</v>
+        <f>RSDAFC!C71</f>
+        <v>R-SW_Det_GAS_HPN1</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -14415,366 +14422,356 @@
         <v>108</v>
       </c>
       <c r="H112" s="26">
-        <f>RSDAFC!L74*$M$35</f>
+        <f>RSDAFC!L72*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="I112" s="26">
-        <f>RSDAFC!M74*$M$35</f>
+        <f>RSDAFC!M72*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
       <c r="K112" t="str">
+        <f>RSDAFC!C72</f>
+        <v>R-SW_Det_GAS_HPN2</v>
+      </c>
+    </row>
+    <row r="113" spans="3:11">
+      <c r="C113" t="s">
+        <v>206</v>
+      </c>
+      <c r="D113" t="s">
+        <v>108</v>
+      </c>
+      <c r="H113" s="26">
+        <f>RSDAFC!L73*$M$37</f>
+        <v>1.222361012943445E-2</v>
+      </c>
+      <c r="I113" s="26">
+        <f>RSDAFC!M73*$M$37</f>
+        <v>1.222361012943445E-2</v>
+      </c>
+      <c r="K113" t="str">
+        <f>RSDAFC!C73</f>
+        <v>R-SW_Det_GAS_HPN2</v>
+      </c>
+    </row>
+    <row r="114" spans="3:11">
+      <c r="C114" t="s">
+        <v>206</v>
+      </c>
+      <c r="D114" t="s">
+        <v>108</v>
+      </c>
+      <c r="H114" s="26">
+        <f>RSDAFC!L74*$M$37</f>
+        <v>1.222361012943445E-2</v>
+      </c>
+      <c r="I114" s="26">
+        <f>RSDAFC!M74*$M$37</f>
+        <v>1.222361012943445E-2</v>
+      </c>
+      <c r="K114" t="str">
         <f>RSDAFC!C74</f>
         <v>R-SW_Det_GAS_N1</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
-      <c r="C113" t="s">
+    <row r="115" spans="3:11">
+      <c r="C115" t="s">
         <v>206</v>
       </c>
-      <c r="D113" t="s">
-        <v>108</v>
-      </c>
-      <c r="H113" s="26">
-        <f>RSDAFC!L75*$M$35</f>
+      <c r="D115" t="s">
+        <v>108</v>
+      </c>
+      <c r="H115" s="26">
+        <f>RSDAFC!L75*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I113" s="26">
-        <f>RSDAFC!M75*$M$35</f>
+      <c r="I115" s="26">
+        <f>RSDAFC!M75*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K113" t="str">
+      <c r="K115" t="str">
         <f>RSDAFC!C75</f>
         <v>R-SW_Det_GAS_N1</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
-      <c r="C114" t="s">
+    <row r="116" spans="3:11">
+      <c r="C116" t="s">
         <v>206</v>
       </c>
-      <c r="D114" t="s">
-        <v>108</v>
-      </c>
-      <c r="H114" s="26">
-        <f>RSDAFC!L76*$M$35</f>
+      <c r="D116" t="s">
+        <v>108</v>
+      </c>
+      <c r="H116" s="26">
+        <f>RSDAFC!L76*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I114" s="26">
-        <f>RSDAFC!M76*$M$35</f>
+      <c r="I116" s="26">
+        <f>RSDAFC!M76*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K114" t="str">
+      <c r="K116" t="str">
         <f>RSDAFC!C76</f>
         <v>R-SW_Det_GAS_N2</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
-      <c r="C115" t="s">
+    <row r="117" spans="3:11">
+      <c r="C117" t="s">
         <v>206</v>
       </c>
-      <c r="D115" t="s">
-        <v>108</v>
-      </c>
-      <c r="H115" s="26">
-        <f>RSDAFC!L77*$M$35</f>
+      <c r="D117" t="s">
+        <v>108</v>
+      </c>
+      <c r="H117" s="26">
+        <f>RSDAFC!L77*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I115" s="26">
-        <f>RSDAFC!M77*$M$35</f>
+      <c r="I117" s="26">
+        <f>RSDAFC!M77*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K115" t="str">
+      <c r="K117" t="str">
         <f>RSDAFC!C77</f>
         <v>R-SW_Det_GAS_N2</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
-      <c r="C116" t="s">
+    <row r="118" spans="3:11">
+      <c r="C118" t="s">
         <v>206</v>
       </c>
-      <c r="D116" t="s">
-        <v>108</v>
-      </c>
-      <c r="H116" s="26">
-        <f>RSDAFC!L78*$M$35</f>
+      <c r="D118" t="s">
+        <v>108</v>
+      </c>
+      <c r="H118" s="26">
+        <f>RSDAFC!L78*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I116" s="26">
-        <f>RSDAFC!M78*$M$35</f>
+      <c r="I118" s="26">
+        <f>RSDAFC!M78*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K116" t="str">
+      <c r="K118" t="str">
         <f>RSDAFC!C78</f>
         <v>R-SW_Det_GAS_N3</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
-      <c r="C117" t="s">
+    <row r="119" spans="3:11">
+      <c r="C119" t="s">
         <v>206</v>
       </c>
-      <c r="D117" t="s">
-        <v>108</v>
-      </c>
-      <c r="H117" s="26">
-        <f>RSDAFC!L79*$M$35</f>
+      <c r="D119" t="s">
+        <v>108</v>
+      </c>
+      <c r="H119" s="26">
+        <f>RSDAFC!L79*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="I117" s="26">
-        <f>RSDAFC!M79*$M$35</f>
+      <c r="I119" s="26">
+        <f>RSDAFC!M79*$M$37</f>
         <v>1.222361012943445E-2</v>
       </c>
-      <c r="K117" t="str">
+      <c r="K119" t="str">
         <f>RSDAFC!C79</f>
         <v>R-SW_Det_GAS_N3</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
-      <c r="C118" t="s">
+    <row r="120" spans="3:11">
+      <c r="C120" t="s">
         <v>206</v>
       </c>
-      <c r="D118" t="s">
-        <v>108</v>
-      </c>
-      <c r="H118" s="26">
-        <f>RSDAFC!L80*$M$35</f>
+      <c r="D120" t="s">
+        <v>108</v>
+      </c>
+      <c r="H120" s="26">
+        <f>RSDAFC!L80*$M$37</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="I118" s="26">
-        <f>RSDAFC!M80*$M$35</f>
+      <c r="I120" s="26">
+        <f>RSDAFC!M80*$M$37</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="K118" t="str">
+      <c r="K120" t="str">
         <f>RSDAFC!C80</f>
         <v>R-SW_Det_HET_N1</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
-      <c r="C119" t="s">
+    <row r="121" spans="3:11">
+      <c r="C121" t="s">
         <v>206</v>
       </c>
-      <c r="D119" t="s">
-        <v>108</v>
-      </c>
-      <c r="H119" s="26">
-        <f>RSDAFC!L81*$M$35</f>
+      <c r="D121" t="s">
+        <v>108</v>
+      </c>
+      <c r="H121" s="26">
+        <f>RSDAFC!L81*$M$37</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="I119" s="26">
-        <f>RSDAFC!M81*$M$35</f>
+      <c r="I121" s="26">
+        <f>RSDAFC!M81*$M$37</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="K119" t="str">
+      <c r="K121" t="str">
         <f>RSDAFC!C81</f>
         <v>R-SW_Det_HET_N1</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
-      <c r="C120" t="s">
+    <row r="122" spans="3:11">
+      <c r="C122" t="s">
         <v>206</v>
       </c>
-      <c r="D120" t="s">
-        <v>108</v>
-      </c>
-      <c r="H120" s="26">
-        <f>RSDAFC!L82*$M$35</f>
+      <c r="D122" t="s">
+        <v>108</v>
+      </c>
+      <c r="H122" s="26">
+        <f>RSDAFC!L82*$M$37</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="I120" s="26">
-        <f>RSDAFC!M82*$M$35</f>
+      <c r="I122" s="26">
+        <f>RSDAFC!M82*$M$37</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="K120" t="str">
+      <c r="K122" t="str">
         <f>RSDAFC!C82</f>
         <v>R-SW_Det_HET_N2</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
-      <c r="C121" t="s">
+    <row r="123" spans="3:11">
+      <c r="C123" t="s">
         <v>206</v>
       </c>
-      <c r="D121" t="s">
-        <v>108</v>
-      </c>
-      <c r="H121" s="26">
-        <f>RSDAFC!L83*$M$35</f>
+      <c r="D123" t="s">
+        <v>108</v>
+      </c>
+      <c r="H123" s="26">
+        <f>RSDAFC!L83*$M$37</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="I121" s="26">
-        <f>RSDAFC!M83*$M$35</f>
+      <c r="I123" s="26">
+        <f>RSDAFC!M83*$M$37</f>
         <v>4.782102180462415E-2</v>
       </c>
-      <c r="K121" t="str">
+      <c r="K123" t="str">
         <f>RSDAFC!C83</f>
         <v>R-SW_Det_HET_N2</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
-      <c r="C122" t="s">
+    <row r="124" spans="3:11">
+      <c r="C124" t="s">
         <v>206</v>
       </c>
-      <c r="D122" t="s">
-        <v>108</v>
-      </c>
-      <c r="H122" s="26">
-        <f>RSDAFC!L84*$M$35</f>
+      <c r="D124" t="s">
+        <v>108</v>
+      </c>
+      <c r="H124" s="26">
+        <f>RSDAFC!L84*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I122" s="26">
-        <f>RSDAFC!M84*$M$35</f>
+      <c r="I124" s="26">
+        <f>RSDAFC!M84*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K122" t="str">
+      <c r="K124" t="str">
         <f>RSDAFC!C84</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
-      <c r="C123" t="s">
+    <row r="125" spans="3:11">
+      <c r="C125" t="s">
         <v>206</v>
       </c>
-      <c r="D123" t="s">
-        <v>108</v>
-      </c>
-      <c r="H123" s="26">
-        <f>RSDAFC!L85*$M$35</f>
+      <c r="D125" t="s">
+        <v>108</v>
+      </c>
+      <c r="H125" s="26">
+        <f>RSDAFC!L85*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I123" s="26">
-        <f>RSDAFC!M85*$M$35</f>
+      <c r="I125" s="26">
+        <f>RSDAFC!M85*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K123" t="str">
+      <c r="K125" t="str">
         <f>RSDAFC!C85</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
-      <c r="C124" t="s">
+    <row r="126" spans="3:11">
+      <c r="C126" t="s">
         <v>206</v>
       </c>
-      <c r="D124" t="s">
-        <v>108</v>
-      </c>
-      <c r="H124" s="26">
-        <f>RSDAFC!L86*$M$35</f>
+      <c r="D126" t="s">
+        <v>108</v>
+      </c>
+      <c r="H126" s="26">
+        <f>RSDAFC!L86*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I124" s="26">
-        <f>RSDAFC!M86*$M$35</f>
+      <c r="I126" s="26">
+        <f>RSDAFC!M86*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K124" t="str">
+      <c r="K126" t="str">
         <f>RSDAFC!C86</f>
         <v>R-SW_Det_KER_N2</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
-      <c r="C125" t="s">
+    <row r="127" spans="3:11">
+      <c r="C127" t="s">
         <v>206</v>
       </c>
-      <c r="D125" t="s">
-        <v>108</v>
-      </c>
-      <c r="H125" s="26">
-        <f>RSDAFC!L87*$M$35</f>
+      <c r="D127" t="s">
+        <v>108</v>
+      </c>
+      <c r="H127" s="26">
+        <f>RSDAFC!L87*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I125" s="26">
-        <f>RSDAFC!M87*$M$35</f>
+      <c r="I127" s="26">
+        <f>RSDAFC!M87*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K125" t="str">
+      <c r="K127" t="str">
         <f>RSDAFC!C87</f>
         <v>R-SW_Det_KER_N2</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
-      <c r="C126" t="s">
+    <row r="128" spans="3:11">
+      <c r="C128" t="s">
         <v>206</v>
       </c>
-      <c r="D126" t="s">
-        <v>108</v>
-      </c>
-      <c r="H126" s="26">
-        <f>RSDAFC!L88*$M$35</f>
+      <c r="D128" t="s">
+        <v>108</v>
+      </c>
+      <c r="H128" s="26">
+        <f>RSDAFC!L88*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I126" s="26">
-        <f>RSDAFC!M88*$M$35</f>
+      <c r="I128" s="26">
+        <f>RSDAFC!M88*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K126" t="str">
+      <c r="K128" t="str">
         <f>RSDAFC!C88</f>
         <v>R-SW_Det_KER_N3</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
-      <c r="C127" t="s">
+    <row r="129" spans="1:11">
+      <c r="C129" t="s">
         <v>206</v>
       </c>
-      <c r="D127" t="s">
-        <v>108</v>
-      </c>
-      <c r="H127" s="26">
-        <f>RSDAFC!L89*$M$35</f>
+      <c r="D129" t="s">
+        <v>108</v>
+      </c>
+      <c r="H129" s="26">
+        <f>RSDAFC!L89*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="I127" s="26">
-        <f>RSDAFC!M89*$M$35</f>
+      <c r="I129" s="26">
+        <f>RSDAFC!M89*$M$37</f>
         <v>1.5039738210625601E-2</v>
       </c>
-      <c r="K127" t="str">
+      <c r="K129" t="str">
         <f>RSDAFC!C89</f>
         <v>R-SW_Det_KER_N3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11">
-      <c r="A128" s="30"/>
-      <c r="B128" s="30"/>
-      <c r="C128" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="D128" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E128" s="30"/>
-      <c r="F128" s="30"/>
-      <c r="G128" s="30"/>
-      <c r="H128" s="31">
-        <f>H134</f>
-        <v>2.6433948538654248E-2</v>
-      </c>
-      <c r="I128" s="31">
-        <f>I134</f>
-        <v>2.6433948538654248E-2</v>
-      </c>
-      <c r="J128" s="30"/>
-      <c r="K128" s="30" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11">
-      <c r="A129" s="30"/>
-      <c r="B129" s="30"/>
-      <c r="C129" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="D129" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E129" s="30"/>
-      <c r="F129" s="30"/>
-      <c r="G129" s="30"/>
-      <c r="H129" s="31">
-        <f>H135</f>
-        <v>2.6433948538654248E-2</v>
-      </c>
-      <c r="I129" s="31">
-        <f>I135</f>
-        <v>2.6433948538654248E-2</v>
-      </c>
-      <c r="J129" s="30"/>
-      <c r="K129" s="30" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="130" spans="1:11">
@@ -14790,16 +14787,16 @@
       <c r="F130" s="30"/>
       <c r="G130" s="30"/>
       <c r="H130" s="31">
-        <f>H127</f>
-        <v>1.5039738210625601E-2</v>
+        <f>H136</f>
+        <v>2.6433948538654248E-2</v>
       </c>
       <c r="I130" s="31">
-        <f>I127</f>
-        <v>1.5039738210625601E-2</v>
+        <f>I136</f>
+        <v>2.6433948538654248E-2</v>
       </c>
       <c r="J130" s="30"/>
       <c r="K130" s="30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="131" spans="1:11">
@@ -14815,56 +14812,66 @@
       <c r="F131" s="30"/>
       <c r="G131" s="30"/>
       <c r="H131" s="31">
-        <f>H130</f>
-        <v>1.5039738210625601E-2</v>
+        <f>H137</f>
+        <v>2.6433948538654248E-2</v>
       </c>
       <c r="I131" s="31">
-        <f>I130</f>
-        <v>1.5039738210625601E-2</v>
+        <f>I137</f>
+        <v>2.6433948538654248E-2</v>
       </c>
       <c r="J131" s="30"/>
       <c r="K131" s="30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="30"/>
+      <c r="B132" s="30"/>
+      <c r="C132" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D132" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E132" s="30"/>
+      <c r="F132" s="30"/>
+      <c r="G132" s="30"/>
+      <c r="H132" s="31">
+        <f>H129</f>
+        <v>1.5039738210625601E-2</v>
+      </c>
+      <c r="I132" s="31">
+        <f>I129</f>
+        <v>1.5039738210625601E-2</v>
+      </c>
+      <c r="J132" s="30"/>
+      <c r="K132" s="30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="A133" s="30"/>
+      <c r="B133" s="30"/>
+      <c r="C133" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D133" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E133" s="30"/>
+      <c r="F133" s="30"/>
+      <c r="G133" s="30"/>
+      <c r="H133" s="31">
+        <f>H132</f>
+        <v>1.5039738210625601E-2</v>
+      </c>
+      <c r="I133" s="31">
+        <f>I132</f>
+        <v>1.5039738210625601E-2</v>
+      </c>
+      <c r="J133" s="30"/>
+      <c r="K133" s="30" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11">
-      <c r="C132" t="s">
-        <v>206</v>
-      </c>
-      <c r="D132" t="s">
-        <v>108</v>
-      </c>
-      <c r="H132" s="26">
-        <f>RSDAFC!L90*$M$35</f>
-        <v>2.10969847812758E-2</v>
-      </c>
-      <c r="I132" s="26">
-        <f>RSDAFC!M90*$M$35</f>
-        <v>2.10969847812758E-2</v>
-      </c>
-      <c r="K132" t="str">
-        <f>RSDAFC!C90</f>
-        <v>R-SW_Det_LPG_N1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11">
-      <c r="C133" t="s">
-        <v>206</v>
-      </c>
-      <c r="D133" t="s">
-        <v>108</v>
-      </c>
-      <c r="H133" s="26">
-        <f>RSDAFC!L91*$M$35</f>
-        <v>2.10969847812758E-2</v>
-      </c>
-      <c r="I133" s="26">
-        <f>RSDAFC!M91*$M$35</f>
-        <v>2.10969847812758E-2</v>
-      </c>
-      <c r="K133" t="str">
-        <f>RSDAFC!C91</f>
-        <v>R-SW_Det_LPG_N1</v>
       </c>
     </row>
     <row r="134" spans="1:11">
@@ -14875,16 +14882,16 @@
         <v>108</v>
       </c>
       <c r="H134" s="26">
-        <f>RSDAFC!L92*$M$35</f>
-        <v>2.6433948538654248E-2</v>
+        <f>RSDAFC!L90*$M$37</f>
+        <v>2.10969847812758E-2</v>
       </c>
       <c r="I134" s="26">
-        <f>RSDAFC!M92*$M$35</f>
-        <v>2.6433948538654248E-2</v>
+        <f>RSDAFC!M90*$M$37</f>
+        <v>2.10969847812758E-2</v>
       </c>
       <c r="K134" t="str">
-        <f>RSDAFC!C92</f>
-        <v>R-SW_Det_WOO_N1</v>
+        <f>RSDAFC!C90</f>
+        <v>R-SW_Det_LPG_N1</v>
       </c>
     </row>
     <row r="135" spans="1:11">
@@ -14895,16 +14902,16 @@
         <v>108</v>
       </c>
       <c r="H135" s="26">
-        <f>RSDAFC!L93*$M$35</f>
-        <v>2.6433948538654248E-2</v>
+        <f>RSDAFC!L91*$M$37</f>
+        <v>2.10969847812758E-2</v>
       </c>
       <c r="I135" s="26">
-        <f>RSDAFC!M93*$M$35</f>
-        <v>2.6433948538654248E-2</v>
+        <f>RSDAFC!M91*$M$37</f>
+        <v>2.10969847812758E-2</v>
       </c>
       <c r="K135" t="str">
-        <f>RSDAFC!C93</f>
-        <v>R-SW_Det_WOO_N1</v>
+        <f>RSDAFC!C91</f>
+        <v>R-SW_Det_LPG_N1</v>
       </c>
     </row>
     <row r="136" spans="1:11">
@@ -14915,16 +14922,16 @@
         <v>108</v>
       </c>
       <c r="H136" s="26">
-        <f>RSDAFA!L2*$M$35</f>
-        <v>9.59298200649405E-3</v>
+        <f>RSDAFC!L92*$M$37</f>
+        <v>2.6433948538654248E-2</v>
       </c>
       <c r="I136" s="26">
-        <f>RSDAFA!M2*$M$35</f>
-        <v>9.59298200649405E-3</v>
-      </c>
-      <c r="K136" s="26" t="str">
-        <f>RSDAFA!C2</f>
-        <v>R-SH_Apt_ELC_HPN1</v>
+        <f>RSDAFC!M92*$M$37</f>
+        <v>2.6433948538654248E-2</v>
+      </c>
+      <c r="K136" t="str">
+        <f>RSDAFC!C92</f>
+        <v>R-SW_Det_WOO_N1</v>
       </c>
     </row>
     <row r="137" spans="1:11">
@@ -14935,16 +14942,16 @@
         <v>108</v>
       </c>
       <c r="H137" s="26">
-        <f>RSDAFA!L3*$M$35</f>
-        <v>9.59298200649405E-3</v>
+        <f>RSDAFC!L93*$M$37</f>
+        <v>2.6433948538654248E-2</v>
       </c>
       <c r="I137" s="26">
-        <f>RSDAFA!M3*$M$35</f>
-        <v>9.59298200649405E-3</v>
-      </c>
-      <c r="K137" s="26" t="str">
-        <f>RSDAFA!C3</f>
-        <v>R-SH_Apt_ELC_HPN2</v>
+        <f>RSDAFC!M93*$M$37</f>
+        <v>2.6433948538654248E-2</v>
+      </c>
+      <c r="K137" t="str">
+        <f>RSDAFC!C93</f>
+        <v>R-SW_Det_WOO_N1</v>
       </c>
     </row>
     <row r="138" spans="1:11">
@@ -14955,16 +14962,16 @@
         <v>108</v>
       </c>
       <c r="H138" s="26">
-        <f>RSDAFA!L4*$M$35</f>
+        <f>RSDAFA!L2*$M$37</f>
         <v>9.59298200649405E-3</v>
       </c>
       <c r="I138" s="26">
-        <f>RSDAFA!M4*$M$35</f>
+        <f>RSDAFA!M2*$M$37</f>
         <v>9.59298200649405E-3</v>
       </c>
       <c r="K138" s="26" t="str">
-        <f>RSDAFA!C4</f>
-        <v>R-SH_Apt_ELC_HPN3</v>
+        <f>RSDAFA!C2</f>
+        <v>R-SH_Apt_ELC_HPN1</v>
       </c>
     </row>
     <row r="139" spans="1:11">
@@ -14975,16 +14982,16 @@
         <v>108</v>
       </c>
       <c r="H139" s="26">
-        <f>RSDAFA!L5*$M$35</f>
+        <f>RSDAFA!L3*$M$37</f>
         <v>9.59298200649405E-3</v>
       </c>
       <c r="I139" s="26">
-        <f>RSDAFA!M5*$M$35</f>
+        <f>RSDAFA!M3*$M$37</f>
         <v>9.59298200649405E-3</v>
       </c>
       <c r="K139" s="26" t="str">
-        <f>RSDAFA!C5</f>
-        <v>R-SH_Apt_ELC_N1</v>
+        <f>RSDAFA!C3</f>
+        <v>R-SH_Apt_ELC_HPN2</v>
       </c>
     </row>
     <row r="140" spans="1:11">
@@ -14995,16 +15002,16 @@
         <v>108</v>
       </c>
       <c r="H140" s="26">
-        <f>RSDAFA!L6*$M$35</f>
-        <v>5.9295434183648001E-3</v>
+        <f>RSDAFA!L4*$M$37</f>
+        <v>9.59298200649405E-3</v>
       </c>
       <c r="I140" s="26">
-        <f>RSDAFA!M6*$M$35</f>
-        <v>5.9295434183648001E-3</v>
+        <f>RSDAFA!M4*$M$37</f>
+        <v>9.59298200649405E-3</v>
       </c>
       <c r="K140" s="26" t="str">
-        <f>RSDAFA!C6</f>
-        <v>R-SH_Apt_GAS_N1</v>
+        <f>RSDAFA!C4</f>
+        <v>R-SH_Apt_ELC_HPN3</v>
       </c>
     </row>
     <row r="141" spans="1:11">
@@ -15015,16 +15022,16 @@
         <v>108</v>
       </c>
       <c r="H141" s="26">
-        <f>RSDAFA!L7*$M$35</f>
-        <v>1.8679913115832E-2</v>
+        <f>RSDAFA!L5*$M$37</f>
+        <v>9.59298200649405E-3</v>
       </c>
       <c r="I141" s="26">
-        <f>RSDAFA!M7*$M$35</f>
-        <v>1.8679913115832E-2</v>
+        <f>RSDAFA!M5*$M$37</f>
+        <v>9.59298200649405E-3</v>
       </c>
       <c r="K141" s="26" t="str">
-        <f>RSDAFA!C7</f>
-        <v>R-SH_Apt_KER_N1</v>
+        <f>RSDAFA!C5</f>
+        <v>R-SH_Apt_ELC_N1</v>
       </c>
     </row>
     <row r="142" spans="1:11">
@@ -15035,16 +15042,16 @@
         <v>108</v>
       </c>
       <c r="H142" s="26">
-        <f>RSDAFA!L8*$M$35</f>
-        <v>1.1539296595339751E-2</v>
+        <f>RSDAFA!L6*$M$37</f>
+        <v>5.9295434183648001E-3</v>
       </c>
       <c r="I142" s="26">
-        <f>RSDAFA!M8*$M$35</f>
-        <v>1.1539296595339751E-2</v>
+        <f>RSDAFA!M6*$M$37</f>
+        <v>5.9295434183648001E-3</v>
       </c>
       <c r="K142" s="26" t="str">
-        <f>RSDAFA!C8</f>
-        <v>R-SH_Apt_LPG_N1</v>
+        <f>RSDAFA!C6</f>
+        <v>R-SH_Apt_GAS_N1</v>
       </c>
     </row>
     <row r="143" spans="1:11">
@@ -15055,16 +15062,16 @@
         <v>108</v>
       </c>
       <c r="H143" s="26">
-        <f>RSDAFA!L9*$M$35</f>
-        <v>8.8239524029044506E-3</v>
+        <f>RSDAFA!L7*$M$37</f>
+        <v>1.8679913115832E-2</v>
       </c>
       <c r="I143" s="26">
-        <f>RSDAFA!M9*$M$35</f>
-        <v>8.8239524029044506E-3</v>
+        <f>RSDAFA!M7*$M$37</f>
+        <v>1.8679913115832E-2</v>
       </c>
       <c r="K143" s="26" t="str">
-        <f>RSDAFA!C9</f>
-        <v>R-SH_Apt_WOO_N1</v>
+        <f>RSDAFA!C7</f>
+        <v>R-SH_Apt_KER_N1</v>
       </c>
     </row>
     <row r="144" spans="1:11">
@@ -15075,16 +15082,16 @@
         <v>108</v>
       </c>
       <c r="H144" s="26">
-        <f>RSDAFA!L10*$M$35</f>
-        <v>1.2326631289923951E-2</v>
+        <f>RSDAFA!L8*$M$37</f>
+        <v>1.1539296595339751E-2</v>
       </c>
       <c r="I144" s="26">
-        <f>RSDAFA!M10*$M$35</f>
-        <v>1.2326631289923951E-2</v>
+        <f>RSDAFA!M8*$M$37</f>
+        <v>1.1539296595339751E-2</v>
       </c>
       <c r="K144" s="26" t="str">
-        <f>RSDAFA!C10</f>
-        <v>R-SH_Att_ELC_HPN1</v>
+        <f>RSDAFA!C8</f>
+        <v>R-SH_Apt_LPG_N1</v>
       </c>
     </row>
     <row r="145" spans="3:11">
@@ -15095,16 +15102,16 @@
         <v>108</v>
       </c>
       <c r="H145" s="26">
-        <f>RSDAFA!L11*$M$35</f>
-        <v>1.2326631289923951E-2</v>
+        <f>RSDAFA!L9*$M$37</f>
+        <v>8.8239524029044506E-3</v>
       </c>
       <c r="I145" s="26">
-        <f>RSDAFA!M11*$M$35</f>
-        <v>1.2326631289923951E-2</v>
+        <f>RSDAFA!M9*$M$37</f>
+        <v>8.8239524029044506E-3</v>
       </c>
       <c r="K145" s="26" t="str">
-        <f>RSDAFA!C11</f>
-        <v>R-SH_Att_ELC_HPN2</v>
+        <f>RSDAFA!C9</f>
+        <v>R-SH_Apt_WOO_N1</v>
       </c>
     </row>
     <row r="146" spans="3:11">
@@ -15115,16 +15122,16 @@
         <v>108</v>
       </c>
       <c r="H146" s="26">
-        <f>RSDAFA!L12*$M$35</f>
+        <f>RSDAFA!L10*$M$37</f>
         <v>1.2326631289923951E-2</v>
       </c>
       <c r="I146" s="26">
-        <f>RSDAFA!M12*$M$35</f>
+        <f>RSDAFA!M10*$M$37</f>
         <v>1.2326631289923951E-2</v>
       </c>
       <c r="K146" s="26" t="str">
-        <f>RSDAFA!C12</f>
-        <v>R-SH_Att_ELC_HPN3</v>
+        <f>RSDAFA!C10</f>
+        <v>R-SH_Att_ELC_HPN1</v>
       </c>
     </row>
     <row r="147" spans="3:11">
@@ -15135,16 +15142,16 @@
         <v>108</v>
       </c>
       <c r="H147" s="26">
-        <f>RSDAFA!L13*$M$35</f>
+        <f>RSDAFA!L11*$M$37</f>
         <v>1.2326631289923951E-2</v>
       </c>
       <c r="I147" s="26">
-        <f>RSDAFA!M13*$M$35</f>
+        <f>RSDAFA!M11*$M$37</f>
         <v>1.2326631289923951E-2</v>
       </c>
       <c r="K147" s="26" t="str">
-        <f>RSDAFA!C13</f>
-        <v>R-SH_Att_ELC_N1</v>
+        <f>RSDAFA!C11</f>
+        <v>R-SH_Att_ELC_HPN2</v>
       </c>
     </row>
     <row r="148" spans="3:11">
@@ -15155,16 +15162,16 @@
         <v>108</v>
       </c>
       <c r="H148" s="26">
-        <f>RSDAFA!L14*$M$35</f>
-        <v>1.10479456620104E-2</v>
+        <f>RSDAFA!L12*$M$37</f>
+        <v>1.2326631289923951E-2</v>
       </c>
       <c r="I148" s="26">
-        <f>RSDAFA!M14*$M$35</f>
-        <v>1.10479456620104E-2</v>
+        <f>RSDAFA!M12*$M$37</f>
+        <v>1.2326631289923951E-2</v>
       </c>
       <c r="K148" s="26" t="str">
-        <f>RSDAFA!C14</f>
-        <v>R-SH_Att_GAS_N1</v>
+        <f>RSDAFA!C12</f>
+        <v>R-SH_Att_ELC_HPN3</v>
       </c>
     </row>
     <row r="149" spans="3:11">
@@ -15175,16 +15182,16 @@
         <v>108</v>
       </c>
       <c r="H149" s="26">
-        <f>RSDAFA!L15*$M$35</f>
-        <v>1.418438071184145E-2</v>
+        <f>RSDAFA!L13*$M$37</f>
+        <v>1.2326631289923951E-2</v>
       </c>
       <c r="I149" s="26">
-        <f>RSDAFA!M15*$M$35</f>
-        <v>1.418438071184145E-2</v>
+        <f>RSDAFA!M13*$M$37</f>
+        <v>1.2326631289923951E-2</v>
       </c>
       <c r="K149" s="26" t="str">
-        <f>RSDAFA!C15</f>
-        <v>R-SH_Att_KER_N1</v>
+        <f>RSDAFA!C13</f>
+        <v>R-SH_Att_ELC_N1</v>
       </c>
     </row>
     <row r="150" spans="3:11">
@@ -15195,16 +15202,16 @@
         <v>108</v>
       </c>
       <c r="H150" s="26">
-        <f>RSDAFA!L16*$M$35</f>
-        <v>1.5468436444358601E-2</v>
+        <f>RSDAFA!L14*$M$37</f>
+        <v>1.10479456620104E-2</v>
       </c>
       <c r="I150" s="26">
-        <f>RSDAFA!M16*$M$35</f>
-        <v>1.5468436444358601E-2</v>
+        <f>RSDAFA!M14*$M$37</f>
+        <v>1.10479456620104E-2</v>
       </c>
       <c r="K150" s="26" t="str">
-        <f>RSDAFA!C16</f>
-        <v>R-SH_Att_LPG_N1</v>
+        <f>RSDAFA!C14</f>
+        <v>R-SH_Att_GAS_N1</v>
       </c>
     </row>
     <row r="151" spans="3:11">
@@ -15215,16 +15222,16 @@
         <v>108</v>
       </c>
       <c r="H151" s="26">
-        <f>RSDAFA!L17*$M$35</f>
-        <v>3.7533433216504153E-2</v>
+        <f>RSDAFA!L15*$M$37</f>
+        <v>1.418438071184145E-2</v>
       </c>
       <c r="I151" s="26">
-        <f>RSDAFA!M17*$M$35</f>
-        <v>3.7533433216504153E-2</v>
+        <f>RSDAFA!M15*$M$37</f>
+        <v>1.418438071184145E-2</v>
       </c>
       <c r="K151" s="26" t="str">
-        <f>RSDAFA!C17</f>
-        <v>R-SH_Att_WOO_N1</v>
+        <f>RSDAFA!C15</f>
+        <v>R-SH_Att_KER_N1</v>
       </c>
     </row>
     <row r="152" spans="3:11">
@@ -15235,16 +15242,16 @@
         <v>108</v>
       </c>
       <c r="H152" s="26">
-        <f>RSDAFA!L18*$M$35</f>
-        <v>2.08072041359634E-2</v>
+        <f>RSDAFA!L16*$M$37</f>
+        <v>1.5468436444358601E-2</v>
       </c>
       <c r="I152" s="26">
-        <f>RSDAFA!M18*$M$35</f>
-        <v>2.08072041359634E-2</v>
+        <f>RSDAFA!M16*$M$37</f>
+        <v>1.5468436444358601E-2</v>
       </c>
       <c r="K152" s="26" t="str">
-        <f>RSDAFA!C18</f>
-        <v>R-SH_Det_ELC_HPN1</v>
+        <f>RSDAFA!C16</f>
+        <v>R-SH_Att_LPG_N1</v>
       </c>
     </row>
     <row r="153" spans="3:11">
@@ -15255,16 +15262,16 @@
         <v>108</v>
       </c>
       <c r="H153" s="26">
-        <f>RSDAFA!L19*$M$35</f>
-        <v>2.08072041359634E-2</v>
+        <f>RSDAFA!L17*$M$37</f>
+        <v>3.7533433216504153E-2</v>
       </c>
       <c r="I153" s="26">
-        <f>RSDAFA!M19*$M$35</f>
-        <v>2.08072041359634E-2</v>
+        <f>RSDAFA!M17*$M$37</f>
+        <v>3.7533433216504153E-2</v>
       </c>
       <c r="K153" s="26" t="str">
-        <f>RSDAFA!C19</f>
-        <v>R-SH_Det_ELC_HPN2</v>
+        <f>RSDAFA!C17</f>
+        <v>R-SH_Att_WOO_N1</v>
       </c>
     </row>
     <row r="154" spans="3:11">
@@ -15275,16 +15282,16 @@
         <v>108</v>
       </c>
       <c r="H154" s="26">
-        <f>RSDAFA!L20*$M$35</f>
+        <f>RSDAFA!L18*$M$37</f>
         <v>2.08072041359634E-2</v>
       </c>
       <c r="I154" s="26">
-        <f>RSDAFA!M20*$M$35</f>
+        <f>RSDAFA!M18*$M$37</f>
         <v>2.08072041359634E-2</v>
       </c>
       <c r="K154" s="26" t="str">
-        <f>RSDAFA!C20</f>
-        <v>R-SH_Det_ELC_HPN3</v>
+        <f>RSDAFA!C18</f>
+        <v>R-SH_Det_ELC_HPN1</v>
       </c>
     </row>
     <row r="155" spans="3:11">
@@ -15295,16 +15302,16 @@
         <v>108</v>
       </c>
       <c r="H155" s="26">
-        <f>RSDAFA!L21*$M$35</f>
+        <f>RSDAFA!L19*$M$37</f>
         <v>2.08072041359634E-2</v>
       </c>
       <c r="I155" s="26">
-        <f>RSDAFA!M21*$M$35</f>
+        <f>RSDAFA!M19*$M$37</f>
         <v>2.08072041359634E-2</v>
       </c>
       <c r="K155" s="26" t="str">
-        <f>RSDAFA!C21</f>
-        <v>R-SH_Det_ELC_N1</v>
+        <f>RSDAFA!C19</f>
+        <v>R-SH_Det_ELC_HPN2</v>
       </c>
     </row>
     <row r="156" spans="3:11">
@@ -15315,16 +15322,16 @@
         <v>108</v>
       </c>
       <c r="H156" s="26">
-        <f>RSDAFA!L22*$M$35</f>
-        <v>1.852031558004625E-2</v>
+        <f>RSDAFA!L20*$M$37</f>
+        <v>2.08072041359634E-2</v>
       </c>
       <c r="I156" s="26">
-        <f>RSDAFA!M22*$M$35</f>
-        <v>1.852031558004625E-2</v>
+        <f>RSDAFA!M20*$M$37</f>
+        <v>2.08072041359634E-2</v>
       </c>
       <c r="K156" s="26" t="str">
-        <f>RSDAFA!C22</f>
-        <v>R-SH_Det_GAS_N1</v>
+        <f>RSDAFA!C20</f>
+        <v>R-SH_Det_ELC_HPN3</v>
       </c>
     </row>
     <row r="157" spans="3:11">
@@ -15335,16 +15342,16 @@
         <v>108</v>
       </c>
       <c r="H157" s="26">
-        <f>RSDAFA!L23*$M$35</f>
-        <v>2.3310863988210799E-2</v>
+        <f>RSDAFA!L21*$M$37</f>
+        <v>2.08072041359634E-2</v>
       </c>
       <c r="I157" s="26">
-        <f>RSDAFA!M23*$M$35</f>
-        <v>2.3310863988210799E-2</v>
+        <f>RSDAFA!M21*$M$37</f>
+        <v>2.08072041359634E-2</v>
       </c>
       <c r="K157" s="26" t="str">
-        <f>RSDAFA!C23</f>
-        <v>R-SH_Det_KER_N1</v>
+        <f>RSDAFA!C21</f>
+        <v>R-SH_Det_ELC_N1</v>
       </c>
     </row>
     <row r="158" spans="3:11">
@@ -15355,16 +15362,16 @@
         <v>108</v>
       </c>
       <c r="H158" s="26">
-        <f>RSDAFA!L24*$M$35</f>
-        <v>3.3516837935026751E-2</v>
+        <f>RSDAFA!L22*$M$37</f>
+        <v>1.852031558004625E-2</v>
       </c>
       <c r="I158" s="26">
-        <f>RSDAFA!M24*$M$35</f>
-        <v>3.3516837935026751E-2</v>
+        <f>RSDAFA!M22*$M$37</f>
+        <v>1.852031558004625E-2</v>
       </c>
       <c r="K158" s="26" t="str">
-        <f>RSDAFA!C24</f>
-        <v>R-SH_Det_LPG_N1</v>
+        <f>RSDAFA!C22</f>
+        <v>R-SH_Det_GAS_N1</v>
       </c>
     </row>
     <row r="159" spans="3:11">
@@ -15375,16 +15382,16 @@
         <v>108</v>
       </c>
       <c r="H159" s="26">
-        <f>RSDAFA!L25*$M$35</f>
-        <v>4.5576915292050248E-2</v>
+        <f>RSDAFA!L23*$M$37</f>
+        <v>2.3310863988210799E-2</v>
       </c>
       <c r="I159" s="26">
-        <f>RSDAFA!M25*$M$35</f>
-        <v>4.5576915292050248E-2</v>
+        <f>RSDAFA!M23*$M$37</f>
+        <v>2.3310863988210799E-2</v>
       </c>
       <c r="K159" s="26" t="str">
-        <f>RSDAFA!C25</f>
-        <v>R-SH_Det_WOO_N1</v>
+        <f>RSDAFA!C23</f>
+        <v>R-SH_Det_KER_N1</v>
       </c>
     </row>
     <row r="160" spans="3:11">
@@ -15395,16 +15402,16 @@
         <v>108</v>
       </c>
       <c r="H160" s="26">
-        <f>RSDAFA!L26*$M$35</f>
-        <v>1.1367849827582301E-2</v>
+        <f>RSDAFA!L24*$M$37</f>
+        <v>3.3516837935026751E-2</v>
       </c>
       <c r="I160" s="26">
-        <f>RSDAFA!M26*$M$35</f>
-        <v>1.1367849827582301E-2</v>
+        <f>RSDAFA!M24*$M$37</f>
+        <v>3.3516837935026751E-2</v>
       </c>
       <c r="K160" s="26" t="str">
-        <f>RSDAFA!C26</f>
-        <v>R-WH_Apt_ELC_N1</v>
+        <f>RSDAFA!C24</f>
+        <v>R-SH_Det_LPG_N1</v>
       </c>
     </row>
     <row r="161" spans="3:11">
@@ -15415,16 +15422,16 @@
         <v>108</v>
       </c>
       <c r="H161" s="26">
-        <f>RSDAFA!L27*$M$35</f>
-        <v>4.3149364997261599E-3</v>
+        <f>RSDAFA!L25*$M$37</f>
+        <v>4.5576915292050248E-2</v>
       </c>
       <c r="I161" s="26">
-        <f>RSDAFA!M27*$M$35</f>
-        <v>4.3149364997261599E-3</v>
+        <f>RSDAFA!M25*$M$37</f>
+        <v>4.5576915292050248E-2</v>
       </c>
       <c r="K161" s="26" t="str">
-        <f>RSDAFA!C27</f>
-        <v>R-WH_Apt_SOL_N1</v>
+        <f>RSDAFA!C25</f>
+        <v>R-SH_Det_WOO_N1</v>
       </c>
     </row>
     <row r="162" spans="3:11">
@@ -15435,16 +15442,16 @@
         <v>108</v>
       </c>
       <c r="H162" s="26">
-        <f>RSDAFA!L28*$M$35</f>
-        <v>6.4637842351524498E-3</v>
+        <f>RSDAFA!L26*$M$37</f>
+        <v>1.1367849827582301E-2</v>
       </c>
       <c r="I162" s="26">
-        <f>RSDAFA!M28*$M$35</f>
-        <v>6.4637842351524498E-3</v>
+        <f>RSDAFA!M26*$M$37</f>
+        <v>1.1367849827582301E-2</v>
       </c>
       <c r="K162" s="26" t="str">
-        <f>RSDAFA!C28</f>
-        <v>R-WH_Att_ELC_N1</v>
+        <f>RSDAFA!C26</f>
+        <v>R-WH_Apt_ELC_N1</v>
       </c>
     </row>
     <row r="163" spans="3:11">
@@ -15455,16 +15462,16 @@
         <v>108</v>
       </c>
       <c r="H163" s="26">
-        <f>RSDAFA!L29*$M$35</f>
-        <v>1.72048031425758E-2</v>
+        <f>RSDAFA!L27*$M$37</f>
+        <v>4.3149364997261599E-3</v>
       </c>
       <c r="I163" s="26">
-        <f>RSDAFA!M29*$M$35</f>
-        <v>1.72048031425758E-2</v>
+        <f>RSDAFA!M27*$M$37</f>
+        <v>4.3149364997261599E-3</v>
       </c>
       <c r="K163" s="26" t="str">
-        <f>RSDAFA!C29</f>
-        <v>R-WH_Att_SOL_N1</v>
+        <f>RSDAFA!C27</f>
+        <v>R-WH_Apt_SOL_N1</v>
       </c>
     </row>
     <row r="164" spans="3:11">
@@ -15475,16 +15482,16 @@
         <v>108</v>
       </c>
       <c r="H164" s="26">
-        <f>RSDAFA!L30*$M$35</f>
-        <v>6.6642433815351501E-3</v>
+        <f>RSDAFA!L28*$M$37</f>
+        <v>6.4637842351524498E-3</v>
       </c>
       <c r="I164" s="26">
-        <f>RSDAFA!M30*$M$35</f>
-        <v>6.6642433815351501E-3</v>
+        <f>RSDAFA!M28*$M$37</f>
+        <v>6.4637842351524498E-3</v>
       </c>
       <c r="K164" s="26" t="str">
-        <f>RSDAFA!C30</f>
-        <v>R-WH_Det_ELC_N1</v>
+        <f>RSDAFA!C28</f>
+        <v>R-WH_Att_ELC_N1</v>
       </c>
     </row>
     <row r="165" spans="3:11">
@@ -15495,27 +15502,57 @@
         <v>108</v>
       </c>
       <c r="H165" s="26">
-        <f>RSDAFA!L31*$M$35</f>
+        <f>RSDAFA!L29*$M$37</f>
+        <v>1.72048031425758E-2</v>
+      </c>
+      <c r="I165" s="26">
+        <f>RSDAFA!M29*$M$37</f>
+        <v>1.72048031425758E-2</v>
+      </c>
+      <c r="K165" s="26" t="str">
+        <f>RSDAFA!C29</f>
+        <v>R-WH_Att_SOL_N1</v>
+      </c>
+    </row>
+    <row r="166" spans="3:11">
+      <c r="C166" t="s">
+        <v>206</v>
+      </c>
+      <c r="D166" t="s">
+        <v>108</v>
+      </c>
+      <c r="H166" s="26">
+        <f>RSDAFA!L30*$M$37</f>
+        <v>6.6642433815351501E-3</v>
+      </c>
+      <c r="I166" s="26">
+        <f>RSDAFA!M30*$M$37</f>
+        <v>6.6642433815351501E-3</v>
+      </c>
+      <c r="K166" s="26" t="str">
+        <f>RSDAFA!C30</f>
+        <v>R-WH_Det_ELC_N1</v>
+      </c>
+    </row>
+    <row r="167" spans="3:11">
+      <c r="C167" t="s">
+        <v>206</v>
+      </c>
+      <c r="D167" t="s">
+        <v>108</v>
+      </c>
+      <c r="H167" s="26">
+        <f>RSDAFA!L31*$M$37</f>
         <v>5.6525755788417502E-2</v>
       </c>
-      <c r="I165" s="26">
-        <f>RSDAFA!M31*$M$35</f>
+      <c r="I167" s="26">
+        <f>RSDAFA!M31*$M$37</f>
         <v>5.6525755788417502E-2</v>
       </c>
-      <c r="K165" s="26" t="str">
+      <c r="K167" s="26" t="str">
         <f>RSDAFA!C31</f>
         <v>R-WH_Det_SOL_N1</v>
       </c>
-    </row>
-    <row r="166" spans="3:11">
-      <c r="H166" s="26"/>
-      <c r="I166" s="26"/>
-      <c r="K166" s="26"/>
-    </row>
-    <row r="167" spans="3:11">
-      <c r="H167" s="26"/>
-      <c r="I167" s="26"/>
-      <c r="K167" s="26"/>
     </row>
     <row r="168" spans="3:11">
       <c r="H168" s="26"/>
@@ -15596,6 +15633,16 @@
       <c r="H183" s="26"/>
       <c r="I183" s="26"/>
       <c r="K183" s="26"/>
+    </row>
+    <row r="184" spans="8:11">
+      <c r="H184" s="26"/>
+      <c r="I184" s="26"/>
+      <c r="K184" s="26"/>
+    </row>
+    <row r="185" spans="8:11">
+      <c r="H185" s="26"/>
+      <c r="I185" s="26"/>
+      <c r="K185" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correct 2050 Peat and Coal maximum amounts
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E8D3C4-0475-467C-8301-1CD3D6F1CAB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E9EDCE-05D9-49FF-A9F7-8ECEF8C4FF37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16020" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12265,7 +12265,7 @@
   <dimension ref="A1:U185"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12723,7 +12723,7 @@
         <v>221</v>
       </c>
       <c r="E27" s="44">
-        <v>2031</v>
+        <v>2050</v>
       </c>
       <c r="H27" s="44">
         <f>H25*M26</f>
@@ -12807,7 +12807,7 @@
         <v>221</v>
       </c>
       <c r="E31" s="44">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="H31" s="44">
         <f>H29*M26</f>

</xml_diff>

<commit_message>
Update HP constraint per EPC
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA6B741-B8B8-4332-99EB-A17096269507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968263B1-F117-4CC7-8AF3-77769B36F549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1350,7 +1350,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1450,6 +1450,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1774,7 +1780,7 @@
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2010,6 +2016,9 @@
     </xf>
     <xf numFmtId="166" fontId="21" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="18" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -13012,7 +13021,7 @@
   <dimension ref="A1:AM200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13285,8 +13294,8 @@
       </c>
       <c r="I7" s="27"/>
       <c r="J7" s="93">
-        <f>-(1-T33)</f>
-        <v>-0.23317382384900065</v>
+        <f>-(T33)</f>
+        <v>-0.76682617615099935</v>
       </c>
       <c r="K7" s="27"/>
       <c r="L7" s="27"/>
@@ -13358,8 +13367,8 @@
       </c>
       <c r="I8" s="27"/>
       <c r="J8" s="93">
-        <f t="shared" ref="J8:J12" si="0">-(1-T34)</f>
-        <v>-0.4861092956738583</v>
+        <f>-(T34)</f>
+        <v>-0.5138907043261417</v>
       </c>
       <c r="K8" s="27"/>
       <c r="L8" s="27"/>
@@ -13421,8 +13430,8 @@
       </c>
       <c r="I9" s="27"/>
       <c r="J9" s="93">
-        <f t="shared" si="0"/>
-        <v>-0.62415466320972102</v>
+        <f>-(T35)</f>
+        <v>-0.37584533679027893</v>
       </c>
       <c r="K9" s="27"/>
       <c r="L9" s="27"/>
@@ -13484,8 +13493,8 @@
       </c>
       <c r="I10" s="27"/>
       <c r="J10" s="93">
-        <f t="shared" si="0"/>
-        <v>-0.83447193865632041</v>
+        <f>-(T36)</f>
+        <v>-0.16552806134367962</v>
       </c>
       <c r="K10" s="27"/>
       <c r="L10" s="27"/>
@@ -13547,8 +13556,8 @@
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="93">
-        <f t="shared" si="0"/>
-        <v>-0.90850781306873241</v>
+        <f>-(T37)</f>
+        <v>-9.1492186931267622E-2</v>
       </c>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
@@ -13610,8 +13619,8 @@
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="93">
-        <f t="shared" si="0"/>
-        <v>-0.69865557579959314</v>
+        <f>-(T38)</f>
+        <v>-3.6630747396996691E-2</v>
       </c>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
@@ -13862,8 +13871,9 @@
         <v>6.0039999999999996</v>
       </c>
       <c r="AC15" s="44"/>
-      <c r="AD15" s="84">
-        <v>5.3559999999999999</v>
+      <c r="AD15" s="101">
+        <f>AVERAGE(AE15:AF15)</f>
+        <v>1.5565</v>
       </c>
       <c r="AE15" s="84">
         <v>1.6439999999999999</v>
@@ -13893,8 +13903,8 @@
       </c>
       <c r="I16" s="27"/>
       <c r="J16" s="93">
-        <f>-(1-AA33)</f>
-        <v>-0.51397876029532341</v>
+        <f>-(AA33)</f>
+        <v>-0.48602123970467664</v>
       </c>
       <c r="K16" s="27"/>
       <c r="L16" s="27"/>
@@ -13957,8 +13967,8 @@
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="93">
-        <f t="shared" ref="J17:J21" si="1">-(1-AA34)</f>
-        <v>-0.74619914743826954</v>
+        <f>-(AA34)</f>
+        <v>-0.25380085256173046</v>
       </c>
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
@@ -14011,8 +14021,8 @@
       </c>
       <c r="I18" s="27"/>
       <c r="J18" s="93">
-        <f t="shared" si="1"/>
-        <v>-0.91024597615670111</v>
+        <f>-(AA35)</f>
+        <v>-8.9754023843298891E-2</v>
       </c>
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
@@ -14065,8 +14075,8 @@
       </c>
       <c r="I19" s="27"/>
       <c r="J19" s="93">
-        <f t="shared" si="1"/>
-        <v>-0.94948839539857766</v>
+        <f>-(AA36)</f>
+        <v>-5.0511604601422351E-2</v>
       </c>
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
@@ -14113,8 +14123,8 @@
       </c>
       <c r="I20" s="27"/>
       <c r="J20" s="93">
-        <f t="shared" si="1"/>
-        <v>-0.96778950270909458</v>
+        <f>-(AA37)</f>
+        <v>-3.2210497290905374E-2</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
@@ -14157,8 +14167,8 @@
       </c>
       <c r="I21" s="27"/>
       <c r="J21" s="93">
-        <f t="shared" si="1"/>
-        <v>-0.96945690287072717</v>
+        <f>-(AA38)</f>
+        <v>-3.054309712927282E-2</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
@@ -14342,8 +14352,8 @@
       </c>
       <c r="I25" s="27"/>
       <c r="J25" s="93">
-        <f>-(1-AH33)</f>
-        <v>-0.85016985557165992</v>
+        <f>-(AH33)</f>
+        <v>-0.14983014442834014</v>
       </c>
       <c r="K25" s="27"/>
       <c r="L25" s="27"/>
@@ -14389,8 +14399,8 @@
       </c>
       <c r="I26" s="27"/>
       <c r="J26" s="93">
-        <f t="shared" ref="J26:J30" si="2">-(1-AH34)</f>
-        <v>-0.93398859506903908</v>
+        <f>-(AH34)</f>
+        <v>-6.6011404930960929E-2</v>
       </c>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
@@ -14436,8 +14446,8 @@
       </c>
       <c r="I27" s="27"/>
       <c r="J27" s="93">
-        <f t="shared" si="2"/>
-        <v>-0.9430204031826559</v>
+        <f>-(AH35)</f>
+        <v>-5.6979596817344061E-2</v>
       </c>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
@@ -14483,8 +14493,8 @@
       </c>
       <c r="I28" s="27"/>
       <c r="J28" s="93">
-        <f t="shared" si="2"/>
-        <v>-0.97114354960585436</v>
+        <f>-(AH36)</f>
+        <v>-2.8856450394145666E-2</v>
       </c>
       <c r="K28" s="27"/>
       <c r="L28" s="27"/>
@@ -14535,8 +14545,8 @@
       </c>
       <c r="I29" s="27"/>
       <c r="J29" s="93">
-        <f t="shared" si="2"/>
-        <v>-0.99266745705794235</v>
+        <f>-(AH37)</f>
+        <v>-7.3325429420576533E-3</v>
       </c>
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
@@ -14611,8 +14621,8 @@
       </c>
       <c r="I30" s="27"/>
       <c r="J30" s="93">
-        <f t="shared" si="2"/>
-        <v>-0.99679138287567692</v>
+        <f>-(AH38)</f>
+        <v>-3.2086171243230267E-3</v>
       </c>
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
@@ -14625,23 +14635,23 @@
         <v>287</v>
       </c>
       <c r="T30" s="88">
-        <f t="shared" ref="T30:T38" si="3">_xlfn.NORM.DIST(2,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="T30:T38" si="0">_xlfn.NORM.DIST(2,Z7,AD7,TRUE)</f>
         <v>0.99986614214614677</v>
       </c>
       <c r="U30" s="88">
-        <f t="shared" ref="U30:U38" si="4">_xlfn.NORM.DIST(2.3,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="U30:U38" si="1">_xlfn.NORM.DIST(2.3,Z7,AD7,TRUE)</f>
         <v>0.99999895018069218</v>
       </c>
       <c r="V30" s="88">
-        <f t="shared" ref="V30:V38" si="5">_xlfn.NORM.DIST(2.5,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="V30:V38" si="2">_xlfn.NORM.DIST(2.5,Z7,AD7,TRUE)</f>
         <v>0.99999997827100517</v>
       </c>
       <c r="W30" s="88">
-        <f t="shared" ref="W30:W38" si="6">_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="W30:W38" si="3">_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
         <v>0.99999999973303144</v>
       </c>
       <c r="X30" s="88">
-        <f t="shared" ref="X30:X38" si="7">1-_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="X30:X38" si="4">1-_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
         <v>2.6696855837116118E-10</v>
       </c>
       <c r="Y30" s="44"/>
@@ -14649,23 +14659,23 @@
         <v>287</v>
       </c>
       <c r="AA30" s="88">
-        <f t="shared" ref="AA30:AA38" si="8">_xlfn.NORM.DIST(2,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AA30:AA38" si="5">_xlfn.NORM.DIST(2,AA7,AE7,TRUE)</f>
         <v>0.99358230344905218</v>
       </c>
       <c r="AB30" s="88">
-        <f t="shared" ref="AB30:AB38" si="9">_xlfn.NORM.DIST(2.3,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AB30:AB38" si="6">_xlfn.NORM.DIST(2.3,AA7,AE7,TRUE)</f>
         <v>0.99961797061500135</v>
       </c>
       <c r="AC30" s="88">
-        <f t="shared" ref="AC30:AC38" si="10">_xlfn.NORM.DIST(2.5,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AC30:AC38" si="7">_xlfn.NORM.DIST(2.5,AA7,AE7,TRUE)</f>
         <v>0.99996097211163748</v>
       </c>
       <c r="AD30" s="88">
-        <f t="shared" ref="AD30:AD38" si="11">_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AD30:AD38" si="8">_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
         <v>0.99999712102252392</v>
       </c>
       <c r="AE30" s="88">
-        <f t="shared" ref="AE30:AE38" si="12">1-_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AE30:AE38" si="9">1-_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
         <v>2.8789774760840103E-6</v>
       </c>
       <c r="AF30" s="44"/>
@@ -14673,23 +14683,23 @@
         <v>287</v>
       </c>
       <c r="AH30" s="44">
-        <f t="shared" ref="AH30:AH38" si="13">_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AH30:AH38" si="10">_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
         <v>0.99867076285153633</v>
       </c>
       <c r="AI30" s="44">
-        <f t="shared" ref="AI30:AI38" si="14">_xlfn.NORM.DIST(2.3,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AI30:AI38" si="11">_xlfn.NORM.DIST(2.3,AB7,AF7,TRUE)</f>
         <v>0.99999490602709384</v>
       </c>
       <c r="AJ30" s="44">
-        <f t="shared" ref="AJ30:AJ38" si="15">_xlfn.NORM.DIST(2.5,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AJ30:AJ38" si="12">_xlfn.NORM.DIST(2.5,AB7,AF7,TRUE)</f>
         <v>0.99999995653338158</v>
       </c>
       <c r="AK30" s="44">
-        <f t="shared" ref="AK30:AK38" si="16">_xlfn.NORM.DIST(2.7,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AK30:AK38" si="13">_xlfn.NORM.DIST(2.7,AB7,AF7,TRUE)</f>
         <v>0.99999999984236743</v>
       </c>
       <c r="AL30" s="44">
-        <f t="shared" ref="AL30:AL38" si="17">1-_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AL30:AL38" si="14">1-_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
         <v>1.3292371484636689E-3</v>
       </c>
       <c r="AM30" s="44"/>
@@ -14720,23 +14730,23 @@
         <v>289</v>
       </c>
       <c r="T31" s="88">
+        <f t="shared" si="0"/>
+        <v>0.96885301500182108</v>
+      </c>
+      <c r="U31" s="88">
+        <f t="shared" si="1"/>
+        <v>0.99736560266376562</v>
+      </c>
+      <c r="V31" s="88">
+        <f t="shared" si="2"/>
+        <v>0.99967208422117826</v>
+      </c>
+      <c r="W31" s="88">
         <f t="shared" si="3"/>
-        <v>0.96885301500182108</v>
-      </c>
-      <c r="U31" s="88">
+        <v>0.99997147495584515</v>
+      </c>
+      <c r="X31" s="88">
         <f t="shared" si="4"/>
-        <v>0.99736560266376562</v>
-      </c>
-      <c r="V31" s="88">
-        <f t="shared" si="5"/>
-        <v>0.99967208422117826</v>
-      </c>
-      <c r="W31" s="88">
-        <f t="shared" si="6"/>
-        <v>0.99997147495584515</v>
-      </c>
-      <c r="X31" s="88">
-        <f t="shared" si="7"/>
         <v>2.8525044154847912E-5</v>
       </c>
       <c r="Y31" s="44"/>
@@ -14744,23 +14754,23 @@
         <v>289</v>
       </c>
       <c r="AA31" s="88">
+        <f t="shared" si="5"/>
+        <v>0.7694627396275191</v>
+      </c>
+      <c r="AB31" s="88">
+        <f t="shared" si="6"/>
+        <v>0.92091247414921895</v>
+      </c>
+      <c r="AC31" s="88">
+        <f t="shared" si="7"/>
+        <v>0.96860489728090593</v>
+      </c>
+      <c r="AD31" s="88">
         <f t="shared" si="8"/>
-        <v>0.7694627396275191</v>
-      </c>
-      <c r="AB31" s="88">
+        <v>0.98955903282288238</v>
+      </c>
+      <c r="AE31" s="88">
         <f t="shared" si="9"/>
-        <v>0.92091247414921895</v>
-      </c>
-      <c r="AC31" s="88">
-        <f t="shared" si="10"/>
-        <v>0.96860489728090593</v>
-      </c>
-      <c r="AD31" s="88">
-        <f t="shared" si="11"/>
-        <v>0.98955903282288238</v>
-      </c>
-      <c r="AE31" s="88">
-        <f t="shared" si="12"/>
         <v>1.0440967177117622E-2</v>
       </c>
       <c r="AF31" s="44"/>
@@ -14768,23 +14778,23 @@
         <v>289</v>
       </c>
       <c r="AH31" s="44">
+        <f t="shared" si="10"/>
+        <v>0.6130931526036395</v>
+      </c>
+      <c r="AI31" s="44">
+        <f t="shared" si="11"/>
+        <v>0.87842619586393023</v>
+      </c>
+      <c r="AJ31" s="44">
+        <f t="shared" si="12"/>
+        <v>0.9602560960127382</v>
+      </c>
+      <c r="AK31" s="44">
         <f t="shared" si="13"/>
-        <v>0.6130931526036395</v>
-      </c>
-      <c r="AI31" s="44">
+        <v>0.99036267162555125</v>
+      </c>
+      <c r="AL31" s="44">
         <f t="shared" si="14"/>
-        <v>0.87842619586393023</v>
-      </c>
-      <c r="AJ31" s="44">
-        <f t="shared" si="15"/>
-        <v>0.9602560960127382</v>
-      </c>
-      <c r="AK31" s="44">
-        <f t="shared" si="16"/>
-        <v>0.99036267162555125</v>
-      </c>
-      <c r="AL31" s="44">
-        <f t="shared" si="17"/>
         <v>0.3869068473963605</v>
       </c>
       <c r="AM31" s="44"/>
@@ -14812,69 +14822,69 @@
         <v>291</v>
       </c>
       <c r="T32" s="88">
+        <f t="shared" si="0"/>
+        <v>0.93969745300565943</v>
+      </c>
+      <c r="U32" s="88">
+        <f t="shared" si="1"/>
+        <v>0.99622594121059427</v>
+      </c>
+      <c r="V32" s="88">
+        <f t="shared" si="2"/>
+        <v>0.99968448066910742</v>
+      </c>
+      <c r="W32" s="88">
         <f t="shared" si="3"/>
-        <v>0.93969745300565943</v>
-      </c>
-      <c r="U32" s="88">
+        <v>0.99998437626199244</v>
+      </c>
+      <c r="X32" s="88">
         <f t="shared" si="4"/>
-        <v>0.99622594121059427</v>
-      </c>
-      <c r="V32" s="88">
-        <f t="shared" si="5"/>
-        <v>0.99968448066910742</v>
-      </c>
-      <c r="W32" s="88">
-        <f t="shared" si="6"/>
-        <v>0.99998437626199244</v>
-      </c>
-      <c r="X32" s="88">
-        <f t="shared" si="7"/>
         <v>1.5623738007564114E-5</v>
       </c>
       <c r="Z32" s="76" t="s">
         <v>291</v>
       </c>
       <c r="AA32" s="88">
+        <f t="shared" si="5"/>
+        <v>0.63358245624321075</v>
+      </c>
+      <c r="AB32" s="88">
+        <f t="shared" si="6"/>
+        <v>0.84081469035187228</v>
+      </c>
+      <c r="AC32" s="88">
+        <f t="shared" si="7"/>
+        <v>0.92442034414706997</v>
+      </c>
+      <c r="AD32" s="88">
         <f t="shared" si="8"/>
-        <v>0.63358245624321075</v>
-      </c>
-      <c r="AB32" s="88">
+        <v>0.9694716992391359</v>
+      </c>
+      <c r="AE32" s="88">
         <f t="shared" si="9"/>
-        <v>0.84081469035187228</v>
-      </c>
-      <c r="AC32" s="88">
-        <f t="shared" si="10"/>
-        <v>0.92442034414706997</v>
-      </c>
-      <c r="AD32" s="88">
-        <f t="shared" si="11"/>
-        <v>0.9694716992391359</v>
-      </c>
-      <c r="AE32" s="88">
-        <f t="shared" si="12"/>
         <v>3.0528300760864102E-2</v>
       </c>
       <c r="AG32" s="76" t="s">
         <v>291</v>
       </c>
       <c r="AH32" s="44">
+        <f t="shared" si="10"/>
+        <v>0.34194299028735675</v>
+      </c>
+      <c r="AI32" s="44">
+        <f t="shared" si="11"/>
+        <v>0.71567219724569331</v>
+      </c>
+      <c r="AJ32" s="44">
+        <f t="shared" si="12"/>
+        <v>0.88905130905570107</v>
+      </c>
+      <c r="AK32" s="44">
         <f t="shared" si="13"/>
-        <v>0.34194299028735675</v>
-      </c>
-      <c r="AI32" s="44">
+        <v>0.9694633335110785</v>
+      </c>
+      <c r="AL32" s="44">
         <f t="shared" si="14"/>
-        <v>0.71567219724569331</v>
-      </c>
-      <c r="AJ32" s="44">
-        <f t="shared" si="15"/>
-        <v>0.88905130905570107</v>
-      </c>
-      <c r="AK32" s="44">
-        <f t="shared" si="16"/>
-        <v>0.9694633335110785</v>
-      </c>
-      <c r="AL32" s="44">
-        <f t="shared" si="17"/>
         <v>0.65805700971264325</v>
       </c>
     </row>
@@ -14887,23 +14897,23 @@
         <v>293</v>
       </c>
       <c r="T33" s="88">
+        <f t="shared" si="0"/>
+        <v>0.76682617615099935</v>
+      </c>
+      <c r="U33" s="88">
+        <f t="shared" si="1"/>
+        <v>0.95418880111755022</v>
+      </c>
+      <c r="V33" s="88">
+        <f t="shared" si="2"/>
+        <v>0.98998748585906793</v>
+      </c>
+      <c r="W33" s="88">
         <f t="shared" si="3"/>
-        <v>0.76682617615099935</v>
-      </c>
-      <c r="U33" s="88">
+        <v>0.99848587792694921</v>
+      </c>
+      <c r="X33" s="88">
         <f t="shared" si="4"/>
-        <v>0.95418880111755022</v>
-      </c>
-      <c r="V33" s="88">
-        <f t="shared" si="5"/>
-        <v>0.98998748585906793</v>
-      </c>
-      <c r="W33" s="88">
-        <f t="shared" si="6"/>
-        <v>0.99848587792694921</v>
-      </c>
-      <c r="X33" s="88">
-        <f t="shared" si="7"/>
         <v>1.5141220730507943E-3</v>
       </c>
       <c r="Y33" s="44"/>
@@ -14911,23 +14921,23 @@
         <v>293</v>
       </c>
       <c r="AA33" s="88">
+        <f t="shared" si="5"/>
+        <v>0.48602123970467664</v>
+      </c>
+      <c r="AB33" s="88">
+        <f t="shared" si="6"/>
+        <v>0.74725860659793841</v>
+      </c>
+      <c r="AC33" s="88">
+        <f t="shared" si="7"/>
+        <v>0.87143015426775872</v>
+      </c>
+      <c r="AD33" s="88">
         <f t="shared" si="8"/>
-        <v>0.48602123970467664</v>
-      </c>
-      <c r="AB33" s="88">
+        <v>0.94525252109261237</v>
+      </c>
+      <c r="AE33" s="88">
         <f t="shared" si="9"/>
-        <v>0.74725860659793841</v>
-      </c>
-      <c r="AC33" s="88">
-        <f t="shared" si="10"/>
-        <v>0.87143015426775872</v>
-      </c>
-      <c r="AD33" s="88">
-        <f t="shared" si="11"/>
-        <v>0.94525252109261237</v>
-      </c>
-      <c r="AE33" s="88">
-        <f t="shared" si="12"/>
         <v>5.4747478907387626E-2</v>
       </c>
       <c r="AF33" s="44"/>
@@ -14935,23 +14945,23 @@
         <v>293</v>
       </c>
       <c r="AH33" s="44">
+        <f t="shared" si="10"/>
+        <v>0.14983014442834014</v>
+      </c>
+      <c r="AI33" s="44">
+        <f t="shared" si="11"/>
+        <v>0.49056643348839696</v>
+      </c>
+      <c r="AJ33" s="44">
+        <f t="shared" si="12"/>
+        <v>0.74280813134921952</v>
+      </c>
+      <c r="AK33" s="44">
         <f t="shared" si="13"/>
-        <v>0.14983014442834014</v>
-      </c>
-      <c r="AI33" s="44">
+        <v>0.90786182982277952</v>
+      </c>
+      <c r="AL33" s="44">
         <f t="shared" si="14"/>
-        <v>0.49056643348839696</v>
-      </c>
-      <c r="AJ33" s="44">
-        <f t="shared" si="15"/>
-        <v>0.74280813134921952</v>
-      </c>
-      <c r="AK33" s="44">
-        <f t="shared" si="16"/>
-        <v>0.90786182982277952</v>
-      </c>
-      <c r="AL33" s="44">
-        <f t="shared" si="17"/>
         <v>0.85016985557165992</v>
       </c>
       <c r="AM33" s="44"/>
@@ -14966,23 +14976,23 @@
         <v>295</v>
       </c>
       <c r="T34" s="88">
+        <f t="shared" si="0"/>
+        <v>0.5138907043261417</v>
+      </c>
+      <c r="U34" s="88">
+        <f t="shared" si="1"/>
+        <v>0.70275414783970647</v>
+      </c>
+      <c r="V34" s="88">
+        <f t="shared" si="2"/>
+        <v>0.80620969874302539</v>
+      </c>
+      <c r="W34" s="88">
         <f t="shared" si="3"/>
-        <v>0.5138907043261417</v>
-      </c>
-      <c r="U34" s="88">
+        <v>0.88409087605518322</v>
+      </c>
+      <c r="X34" s="88">
         <f t="shared" si="4"/>
-        <v>0.70275414783970647</v>
-      </c>
-      <c r="V34" s="88">
-        <f t="shared" si="5"/>
-        <v>0.80620969874302539</v>
-      </c>
-      <c r="W34" s="88">
-        <f t="shared" si="6"/>
-        <v>0.88409087605518322</v>
-      </c>
-      <c r="X34" s="88">
-        <f t="shared" si="7"/>
         <v>0.11590912394481678</v>
       </c>
       <c r="Y34" s="44"/>
@@ -14990,23 +15000,23 @@
         <v>295</v>
       </c>
       <c r="AA34" s="88">
+        <f t="shared" si="5"/>
+        <v>0.25380085256173046</v>
+      </c>
+      <c r="AB34" s="88">
+        <f t="shared" si="6"/>
+        <v>0.48042786872418958</v>
+      </c>
+      <c r="AC34" s="88">
+        <f t="shared" si="7"/>
+        <v>0.64054584703308814</v>
+      </c>
+      <c r="AD34" s="88">
         <f t="shared" si="8"/>
-        <v>0.25380085256173046</v>
-      </c>
-      <c r="AB34" s="88">
+        <v>0.77902845692514355</v>
+      </c>
+      <c r="AE34" s="88">
         <f t="shared" si="9"/>
-        <v>0.48042786872418958</v>
-      </c>
-      <c r="AC34" s="88">
-        <f t="shared" si="10"/>
-        <v>0.64054584703308814</v>
-      </c>
-      <c r="AD34" s="88">
-        <f t="shared" si="11"/>
-        <v>0.77902845692514355</v>
-      </c>
-      <c r="AE34" s="88">
-        <f t="shared" si="12"/>
         <v>0.22097154307485645</v>
       </c>
       <c r="AF34" s="44"/>
@@ -15014,23 +15024,23 @@
         <v>295</v>
       </c>
       <c r="AH34" s="44">
+        <f t="shared" si="10"/>
+        <v>6.6011404930960929E-2</v>
+      </c>
+      <c r="AI34" s="44">
+        <f t="shared" si="11"/>
+        <v>0.22200714259760385</v>
+      </c>
+      <c r="AJ34" s="44">
+        <f t="shared" si="12"/>
+        <v>0.39296290098211079</v>
+      </c>
+      <c r="AK34" s="44">
         <f t="shared" si="13"/>
-        <v>6.6011404930960929E-2</v>
-      </c>
-      <c r="AI34" s="44">
+        <v>0.58792955212905773</v>
+      </c>
+      <c r="AL34" s="44">
         <f t="shared" si="14"/>
-        <v>0.22200714259760385</v>
-      </c>
-      <c r="AJ34" s="44">
-        <f t="shared" si="15"/>
-        <v>0.39296290098211079</v>
-      </c>
-      <c r="AK34" s="44">
-        <f t="shared" si="16"/>
-        <v>0.58792955212905773</v>
-      </c>
-      <c r="AL34" s="44">
-        <f t="shared" si="17"/>
         <v>0.93398859506903908</v>
       </c>
       <c r="AM34" s="44"/>
@@ -15045,23 +15055,23 @@
         <v>297</v>
       </c>
       <c r="T35" s="88">
+        <f t="shared" si="0"/>
+        <v>0.37584533679027893</v>
+      </c>
+      <c r="U35" s="88">
+        <f t="shared" si="1"/>
+        <v>0.51506861469064869</v>
+      </c>
+      <c r="V35" s="88">
+        <f t="shared" si="2"/>
+        <v>0.60792230376456446</v>
+      </c>
+      <c r="W35" s="88">
         <f t="shared" si="3"/>
-        <v>0.37584533679027893</v>
-      </c>
-      <c r="U35" s="88">
+        <v>0.69498667602271957</v>
+      </c>
+      <c r="X35" s="88">
         <f t="shared" si="4"/>
-        <v>0.51506861469064869</v>
-      </c>
-      <c r="V35" s="88">
-        <f t="shared" si="5"/>
-        <v>0.60792230376456446</v>
-      </c>
-      <c r="W35" s="88">
-        <f t="shared" si="6"/>
-        <v>0.69498667602271957</v>
-      </c>
-      <c r="X35" s="88">
-        <f t="shared" si="7"/>
         <v>0.30501332397728043</v>
       </c>
       <c r="Y35" s="44"/>
@@ -15069,23 +15079,23 @@
         <v>297</v>
       </c>
       <c r="AA35" s="88">
+        <f t="shared" si="5"/>
+        <v>8.9754023843298891E-2</v>
+      </c>
+      <c r="AB35" s="88">
+        <f t="shared" si="6"/>
+        <v>0.19240027281705166</v>
+      </c>
+      <c r="AC35" s="88">
+        <f t="shared" si="7"/>
+        <v>0.28991681177663592</v>
+      </c>
+      <c r="AD35" s="88">
         <f t="shared" si="8"/>
-        <v>8.9754023843298891E-2</v>
-      </c>
-      <c r="AB35" s="88">
+        <v>0.40587448754231226</v>
+      </c>
+      <c r="AE35" s="88">
         <f t="shared" si="9"/>
-        <v>0.19240027281705166</v>
-      </c>
-      <c r="AC35" s="88">
-        <f t="shared" si="10"/>
-        <v>0.28991681177663592</v>
-      </c>
-      <c r="AD35" s="88">
-        <f t="shared" si="11"/>
-        <v>0.40587448754231226</v>
-      </c>
-      <c r="AE35" s="88">
-        <f t="shared" si="12"/>
         <v>0.59412551245768774</v>
       </c>
       <c r="AF35" s="44"/>
@@ -15093,23 +15103,23 @@
         <v>297</v>
       </c>
       <c r="AH35" s="44">
+        <f t="shared" si="10"/>
+        <v>5.6979596817344061E-2</v>
+      </c>
+      <c r="AI35" s="44">
+        <f t="shared" si="11"/>
+        <v>0.12698439253107691</v>
+      </c>
+      <c r="AJ35" s="44">
+        <f t="shared" si="12"/>
+        <v>0.19835620119859471</v>
+      </c>
+      <c r="AK35" s="44">
         <f t="shared" si="13"/>
-        <v>5.6979596817344061E-2</v>
-      </c>
-      <c r="AI35" s="44">
+        <v>0.28970312941742804</v>
+      </c>
+      <c r="AL35" s="44">
         <f t="shared" si="14"/>
-        <v>0.12698439253107691</v>
-      </c>
-      <c r="AJ35" s="44">
-        <f t="shared" si="15"/>
-        <v>0.19835620119859471</v>
-      </c>
-      <c r="AK35" s="44">
-        <f t="shared" si="16"/>
-        <v>0.28970312941742804</v>
-      </c>
-      <c r="AL35" s="44">
-        <f t="shared" si="17"/>
         <v>0.9430204031826559</v>
       </c>
       <c r="AM35" s="44"/>
@@ -15129,69 +15139,69 @@
         <v>301</v>
       </c>
       <c r="T36" s="88">
+        <f t="shared" si="0"/>
+        <v>0.16552806134367962</v>
+      </c>
+      <c r="U36" s="88">
+        <f t="shared" si="1"/>
+        <v>0.29053559209062707</v>
+      </c>
+      <c r="V36" s="88">
+        <f t="shared" si="2"/>
+        <v>0.39292301197938029</v>
+      </c>
+      <c r="W36" s="88">
         <f t="shared" si="3"/>
-        <v>0.16552806134367962</v>
-      </c>
-      <c r="U36" s="88">
+        <v>0.50335241668180219</v>
+      </c>
+      <c r="X36" s="88">
         <f t="shared" si="4"/>
-        <v>0.29053559209062707</v>
-      </c>
-      <c r="V36" s="88">
-        <f t="shared" si="5"/>
-        <v>0.39292301197938029</v>
-      </c>
-      <c r="W36" s="88">
-        <f t="shared" si="6"/>
-        <v>0.50335241668180219</v>
-      </c>
-      <c r="X36" s="88">
-        <f t="shared" si="7"/>
         <v>0.49664758331819781</v>
       </c>
       <c r="Z36" s="76" t="s">
         <v>301</v>
       </c>
       <c r="AA36" s="88">
+        <f t="shared" si="5"/>
+        <v>5.0511604601422351E-2</v>
+      </c>
+      <c r="AB36" s="88">
+        <f t="shared" si="6"/>
+        <v>9.4333345509310967E-2</v>
+      </c>
+      <c r="AC36" s="88">
+        <f t="shared" si="7"/>
+        <v>0.13618656405660809</v>
+      </c>
+      <c r="AD36" s="88">
         <f t="shared" si="8"/>
-        <v>5.0511604601422351E-2</v>
-      </c>
-      <c r="AB36" s="88">
+        <v>0.18924169383003042</v>
+      </c>
+      <c r="AE36" s="88">
         <f t="shared" si="9"/>
-        <v>9.4333345509310967E-2</v>
-      </c>
-      <c r="AC36" s="88">
-        <f t="shared" si="10"/>
-        <v>0.13618656405660809</v>
-      </c>
-      <c r="AD36" s="88">
-        <f t="shared" si="11"/>
-        <v>0.18924169383003042</v>
-      </c>
-      <c r="AE36" s="88">
-        <f t="shared" si="12"/>
         <v>0.81075830616996958</v>
       </c>
       <c r="AG36" s="76" t="s">
         <v>301</v>
       </c>
       <c r="AH36" s="44">
+        <f t="shared" si="10"/>
+        <v>2.8856450394145666E-2</v>
+      </c>
+      <c r="AI36" s="44">
+        <f t="shared" si="11"/>
+        <v>5.7199757058308189E-2</v>
+      </c>
+      <c r="AJ36" s="44">
+        <f t="shared" si="12"/>
+        <v>8.5976160021217857E-2</v>
+      </c>
+      <c r="AK36" s="44">
         <f t="shared" si="13"/>
-        <v>2.8856450394145666E-2</v>
-      </c>
-      <c r="AI36" s="44">
+        <v>0.12441589797637952</v>
+      </c>
+      <c r="AL36" s="44">
         <f t="shared" si="14"/>
-        <v>5.7199757058308189E-2</v>
-      </c>
-      <c r="AJ36" s="44">
-        <f t="shared" si="15"/>
-        <v>8.5976160021217857E-2</v>
-      </c>
-      <c r="AK36" s="44">
-        <f t="shared" si="16"/>
-        <v>0.12441589797637952</v>
-      </c>
-      <c r="AL36" s="44">
-        <f t="shared" si="17"/>
         <v>0.97114354960585436</v>
       </c>
     </row>
@@ -15206,23 +15216,23 @@
         <v>302</v>
       </c>
       <c r="T37" s="88">
+        <f t="shared" si="0"/>
+        <v>9.1492186931267622E-2</v>
+      </c>
+      <c r="U37" s="88">
+        <f t="shared" si="1"/>
+        <v>0.15300882371326033</v>
+      </c>
+      <c r="V37" s="88">
+        <f t="shared" si="2"/>
+        <v>0.20660004501142309</v>
+      </c>
+      <c r="W37" s="88">
         <f t="shared" si="3"/>
-        <v>9.1492186931267622E-2</v>
-      </c>
-      <c r="U37" s="88">
+        <v>0.26995921510986137</v>
+      </c>
+      <c r="X37" s="88">
         <f t="shared" si="4"/>
-        <v>0.15300882371326033</v>
-      </c>
-      <c r="V37" s="88">
-        <f t="shared" si="5"/>
-        <v>0.20660004501142309</v>
-      </c>
-      <c r="W37" s="88">
-        <f t="shared" si="6"/>
-        <v>0.26995921510986137</v>
-      </c>
-      <c r="X37" s="88">
-        <f t="shared" si="7"/>
         <v>0.73004078489013868</v>
       </c>
       <c r="Y37" s="44"/>
@@ -15230,23 +15240,23 @@
         <v>302</v>
       </c>
       <c r="AA37" s="88">
+        <f t="shared" si="5"/>
+        <v>3.2210497290905374E-2</v>
+      </c>
+      <c r="AB37" s="88">
+        <f t="shared" si="6"/>
+        <v>5.6332486553475364E-2</v>
+      </c>
+      <c r="AC37" s="88">
+        <f t="shared" si="7"/>
+        <v>7.9115975834815E-2</v>
+      </c>
+      <c r="AD37" s="88">
         <f t="shared" si="8"/>
-        <v>3.2210497290905374E-2</v>
-      </c>
-      <c r="AB37" s="88">
+        <v>0.10827424567922854</v>
+      </c>
+      <c r="AE37" s="88">
         <f t="shared" si="9"/>
-        <v>5.6332486553475364E-2</v>
-      </c>
-      <c r="AC37" s="88">
-        <f t="shared" si="10"/>
-        <v>7.9115975834815E-2</v>
-      </c>
-      <c r="AD37" s="88">
-        <f t="shared" si="11"/>
-        <v>0.10827424567922854</v>
-      </c>
-      <c r="AE37" s="88">
-        <f t="shared" si="12"/>
         <v>0.8917257543207715</v>
       </c>
       <c r="AF37" s="44"/>
@@ -15254,23 +15264,23 @@
         <v>302</v>
       </c>
       <c r="AH37" s="44">
+        <f t="shared" si="10"/>
+        <v>7.3325429420576533E-3</v>
+      </c>
+      <c r="AI37" s="44">
+        <f t="shared" si="11"/>
+        <v>1.5850994164039133E-2</v>
+      </c>
+      <c r="AJ37" s="44">
+        <f t="shared" si="12"/>
+        <v>2.5396980814932565E-2</v>
+      </c>
+      <c r="AK37" s="44">
         <f t="shared" si="13"/>
-        <v>7.3325429420576533E-3</v>
-      </c>
-      <c r="AI37" s="44">
+        <v>3.9349548301286723E-2</v>
+      </c>
+      <c r="AL37" s="44">
         <f t="shared" si="14"/>
-        <v>1.5850994164039133E-2</v>
-      </c>
-      <c r="AJ37" s="44">
-        <f t="shared" si="15"/>
-        <v>2.5396980814932565E-2</v>
-      </c>
-      <c r="AK37" s="44">
-        <f t="shared" si="16"/>
-        <v>3.9349548301286723E-2</v>
-      </c>
-      <c r="AL37" s="44">
-        <f t="shared" si="17"/>
         <v>0.99266745705794235</v>
       </c>
       <c r="AM37" s="44"/>
@@ -15291,47 +15301,47 @@
         <v>303</v>
       </c>
       <c r="T38" s="88">
+        <f t="shared" si="0"/>
+        <v>3.6630747396996691E-2</v>
+      </c>
+      <c r="U38" s="88">
+        <f t="shared" si="1"/>
+        <v>5.4970533940220757E-2</v>
+      </c>
+      <c r="V38" s="88">
+        <f t="shared" si="2"/>
+        <v>7.0785662206478708E-2</v>
+      </c>
+      <c r="W38" s="88">
         <f t="shared" si="3"/>
-        <v>0.30134442420040691</v>
-      </c>
-      <c r="U38" s="88">
+        <v>8.9883749084018569E-2</v>
+      </c>
+      <c r="X38" s="88">
         <f t="shared" si="4"/>
-        <v>0.32113555204517064</v>
-      </c>
-      <c r="V38" s="88">
-        <f t="shared" si="5"/>
-        <v>0.33462248738956413</v>
-      </c>
-      <c r="W38" s="88">
-        <f t="shared" si="6"/>
-        <v>0.34832626090830937</v>
-      </c>
-      <c r="X38" s="88">
-        <f t="shared" si="7"/>
-        <v>0.65167373909169068</v>
+        <v>0.91011625091598147</v>
       </c>
       <c r="Y38" s="44"/>
       <c r="Z38" s="82" t="s">
         <v>303</v>
       </c>
       <c r="AA38" s="88">
+        <f t="shared" si="5"/>
+        <v>3.054309712927282E-2</v>
+      </c>
+      <c r="AB38" s="88">
+        <f t="shared" si="6"/>
+        <v>4.54767509141593E-2</v>
+      </c>
+      <c r="AC38" s="88">
+        <f t="shared" si="7"/>
+        <v>5.8354873920238394E-2</v>
+      </c>
+      <c r="AD38" s="88">
         <f t="shared" si="8"/>
-        <v>3.054309712927282E-2</v>
-      </c>
-      <c r="AB38" s="88">
+        <v>7.3937218528355567E-2</v>
+      </c>
+      <c r="AE38" s="88">
         <f t="shared" si="9"/>
-        <v>4.54767509141593E-2</v>
-      </c>
-      <c r="AC38" s="88">
-        <f t="shared" si="10"/>
-        <v>5.8354873920238394E-2</v>
-      </c>
-      <c r="AD38" s="88">
-        <f t="shared" si="11"/>
-        <v>7.3937218528355567E-2</v>
-      </c>
-      <c r="AE38" s="88">
-        <f t="shared" si="12"/>
         <v>0.92606278147164445</v>
       </c>
       <c r="AF38" s="44"/>
@@ -15339,23 +15349,23 @@
         <v>303</v>
       </c>
       <c r="AH38" s="44">
+        <f t="shared" si="10"/>
+        <v>3.2086171243230267E-3</v>
+      </c>
+      <c r="AI38" s="44">
+        <f t="shared" si="11"/>
+        <v>5.8437278169573741E-3</v>
+      </c>
+      <c r="AJ38" s="44">
+        <f t="shared" si="12"/>
+        <v>8.5326893308700167E-3</v>
+      </c>
+      <c r="AK38" s="44">
         <f t="shared" si="13"/>
-        <v>3.2086171243230267E-3</v>
-      </c>
-      <c r="AI38" s="44">
+        <v>1.2251506395051929E-2</v>
+      </c>
+      <c r="AL38" s="44">
         <f t="shared" si="14"/>
-        <v>5.8437278169573741E-3</v>
-      </c>
-      <c r="AJ38" s="44">
-        <f t="shared" si="15"/>
-        <v>8.5326893308700167E-3</v>
-      </c>
-      <c r="AK38" s="44">
-        <f t="shared" si="16"/>
-        <v>1.2251506395051929E-2</v>
-      </c>
-      <c r="AL38" s="44">
-        <f t="shared" si="17"/>
         <v>0.99679138287567692</v>
       </c>
       <c r="AM38" s="44"/>
@@ -15673,15 +15683,15 @@
         <v>287</v>
       </c>
       <c r="T44" s="68">
-        <f t="shared" ref="T44:T52" si="18">U7*T30</f>
+        <f t="shared" ref="T44:T52" si="15">U7*T30</f>
         <v>9417.6380632201017</v>
       </c>
       <c r="U44" s="68">
-        <f t="shared" ref="U44:U52" si="19">V7*AA30</f>
+        <f t="shared" ref="U44:U52" si="16">V7*AA30</f>
         <v>15372.778652981828</v>
       </c>
       <c r="V44" s="68">
-        <f t="shared" ref="V44:V52" si="20">W7*AH30</f>
+        <f t="shared" ref="V44:V52" si="17">W7*AH30</f>
         <v>20351.618204054608</v>
       </c>
       <c r="W44" s="44"/>
@@ -15689,15 +15699,15 @@
         <v>287</v>
       </c>
       <c r="Y44" s="68">
-        <f t="shared" ref="Y44:Y52" si="21">U7*U30</f>
+        <f t="shared" ref="Y44:Y52" si="18">U7*U30</f>
         <v>9418.8889686648563</v>
       </c>
       <c r="Z44" s="68">
-        <f t="shared" ref="Z44:Z52" si="22">V7*AB30</f>
+        <f t="shared" ref="Z44:Z52" si="19">V7*AB30</f>
         <v>15466.162940366092</v>
       </c>
       <c r="AA44" s="68">
-        <f t="shared" ref="AA44:AA52" si="23">W7*AI30</f>
+        <f t="shared" ref="AA44:AA52" si="20">W7*AI30</f>
         <v>20378.602528978172</v>
       </c>
       <c r="AB44" s="44"/>
@@ -15705,15 +15715,15 @@
         <v>287</v>
       </c>
       <c r="AD44" s="68">
-        <f t="shared" ref="AD44:AD52" si="24">U7*V30</f>
+        <f t="shared" ref="AD44:AD52" si="21">U7*V30</f>
         <v>9418.898652143529</v>
       </c>
       <c r="AE44" s="68">
-        <f t="shared" ref="AE44:AE52" si="25">V7*AC30</f>
+        <f t="shared" ref="AE44:AE52" si="22">V7*AC30</f>
         <v>15471.469884810578</v>
       </c>
       <c r="AF44" s="68">
-        <f t="shared" ref="AF44:AF52" si="26">W7*AJ30</f>
+        <f t="shared" ref="AF44:AF52" si="23">W7*AJ30</f>
         <v>20378.705451762668</v>
       </c>
       <c r="AG44" s="44"/>
@@ -15753,15 +15763,15 @@
         <v>289</v>
       </c>
       <c r="T45" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>7226.9569082675025</v>
       </c>
       <c r="U45" s="73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>7338.965095745436</v>
       </c>
       <c r="V45" s="73">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>5783.8602283503142</v>
       </c>
       <c r="W45" s="44"/>
@@ -15769,15 +15779,15 @@
         <v>289</v>
       </c>
       <c r="Y45" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>7439.6406066050522</v>
       </c>
       <c r="Z45" s="73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>8783.4591019824566</v>
       </c>
       <c r="AA45" s="73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>8286.9859436891857</v>
       </c>
       <c r="AB45" s="44"/>
@@ -15785,15 +15795,15 @@
         <v>289</v>
       </c>
       <c r="AD45" s="73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>7456.845324521013</v>
       </c>
       <c r="AE45" s="73">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>9238.3388650550733</v>
       </c>
       <c r="AF45" s="73">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>9058.9611369377526</v>
       </c>
       <c r="AG45" s="44"/>
@@ -15838,15 +15848,15 @@
         <v>291</v>
       </c>
       <c r="T46" s="78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>13195.088262110432</v>
       </c>
       <c r="U46" s="78">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>11116.263088697284</v>
       </c>
       <c r="V46" s="78">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>6869.9592457318131</v>
       </c>
       <c r="W46" s="44"/>
@@ -15854,15 +15864,15 @@
         <v>291</v>
       </c>
       <c r="Y46" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>13988.85266873088</v>
       </c>
       <c r="Z46" s="78">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>14752.17189916172</v>
       </c>
       <c r="AA46" s="78">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>14378.533755727773</v>
       </c>
       <c r="AB46" s="44"/>
@@ -15870,15 +15880,15 @@
         <v>291</v>
       </c>
       <c r="AD46" s="78">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>14037.41695212561</v>
       </c>
       <c r="AE46" s="78">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>16219.040866463431</v>
       </c>
       <c r="AF46" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>17861.884682719923</v>
       </c>
       <c r="AG46" s="44"/>
@@ -15916,15 +15926,15 @@
         <v>293</v>
       </c>
       <c r="T47" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>15278.613097799687</v>
       </c>
       <c r="U47" s="73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>24188.71802303115</v>
       </c>
       <c r="V47" s="73">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>8010.8499729257437</v>
       </c>
       <c r="W47" s="44"/>
@@ -15932,15 +15942,15 @@
         <v>293</v>
       </c>
       <c r="Y47" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>19011.716041964675</v>
       </c>
       <c r="Z47" s="73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>37190.201268289908</v>
       </c>
       <c r="AA47" s="73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>26228.727973417597</v>
       </c>
       <c r="AB47" s="44"/>
@@ -15948,15 +15958,15 @@
         <v>293</v>
       </c>
       <c r="AD47" s="73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>19724.986233549855</v>
       </c>
       <c r="AE47" s="73">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>43370.07635953842</v>
       </c>
       <c r="AF47" s="73">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>39715.1355730949</v>
       </c>
       <c r="AG47" s="44"/>
@@ -15979,15 +15989,15 @@
         <v>295</v>
       </c>
       <c r="T48" s="78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>30270.630926141846</v>
       </c>
       <c r="U48" s="78">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>71610.298224913975</v>
       </c>
       <c r="V48" s="78">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>16589.915893594109</v>
       </c>
       <c r="W48" s="44"/>
@@ -15995,15 +16005,15 @@
         <v>295</v>
       </c>
       <c r="Y48" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>41395.59494263638</v>
       </c>
       <c r="Z48" s="78">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>135553.45700240019</v>
       </c>
       <c r="AA48" s="78">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>55794.598332264082</v>
       </c>
       <c r="AB48" s="44"/>
@@ -16011,15 +16021,15 @@
         <v>295</v>
       </c>
       <c r="AD48" s="78">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>47489.623833004342</v>
       </c>
       <c r="AE48" s="78">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>180730.98915856858</v>
       </c>
       <c r="AF48" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>98759.017224587151</v>
       </c>
       <c r="AG48" s="44"/>
@@ -16041,15 +16051,15 @@
         <v>297</v>
       </c>
       <c r="T49" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>16439.227593093379</v>
       </c>
       <c r="U49" s="73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>16840.280240037471</v>
       </c>
       <c r="V49" s="73">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>9496.663557138043</v>
       </c>
       <c r="W49" s="44"/>
@@ -16057,15 +16067,15 @@
         <v>297</v>
       </c>
       <c r="Y49" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>22528.762110686101</v>
       </c>
       <c r="Z49" s="73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>36099.49029311091</v>
       </c>
       <c r="AA49" s="73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>21164.20824704953</v>
       </c>
       <c r="AB49" s="44"/>
@@ -16073,15 +16083,15 @@
         <v>297</v>
       </c>
       <c r="AD49" s="73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>26590.121340469981</v>
       </c>
       <c r="AE49" s="73">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>54396.228130570431</v>
       </c>
       <c r="AF49" s="73">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>33059.589966801032</v>
       </c>
       <c r="AG49" s="44"/>
@@ -16107,15 +16117,15 @@
         <v>301</v>
       </c>
       <c r="T50" s="78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>4265.3066374795972</v>
       </c>
       <c r="U50" s="78">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>5122.8311719375915</v>
       </c>
       <c r="V50" s="78">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>2348.819777782865</v>
       </c>
       <c r="W50" s="44"/>
@@ -16123,15 +16133,15 @@
         <v>301</v>
       </c>
       <c r="Y50" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>7486.4852479318533</v>
       </c>
       <c r="Z50" s="78">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>9567.1837539417502</v>
       </c>
       <c r="AA50" s="78">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>4655.871350351058</v>
       </c>
       <c r="AB50" s="44"/>
@@ -16139,15 +16149,15 @@
         <v>301</v>
       </c>
       <c r="AD50" s="78">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>10124.791635989994</v>
       </c>
       <c r="AE50" s="78">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>13811.89097145851</v>
       </c>
       <c r="AF50" s="78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>6998.1755315487662</v>
       </c>
       <c r="AG50" s="44"/>
@@ -16199,15 +16209,15 @@
         <v>302</v>
       </c>
       <c r="T51" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>1128.2060059559165</v>
       </c>
       <c r="U51" s="73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>1614.512718252895</v>
       </c>
       <c r="V51" s="73">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>317.06653161471883</v>
       </c>
       <c r="W51" s="44"/>
@@ -16215,15 +16225,15 @@
         <v>302</v>
       </c>
       <c r="Y51" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>1886.7783104499745</v>
       </c>
       <c r="Z51" s="73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>2823.5986290430769</v>
       </c>
       <c r="AA51" s="73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>685.4129299959742</v>
       </c>
       <c r="AB51" s="44"/>
@@ -16231,15 +16241,15 @@
         <v>302</v>
       </c>
       <c r="AD51" s="73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>2547.6209437178968</v>
       </c>
       <c r="AE51" s="73">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>3965.5938264064957</v>
       </c>
       <c r="AF51" s="73">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>1098.1909937804644</v>
       </c>
       <c r="AG51" s="44"/>
@@ -16277,15 +16287,15 @@
         <v>303</v>
       </c>
       <c r="T52" s="83">
-        <f t="shared" si="18"/>
-        <v>4583.8019318404531</v>
+        <f t="shared" si="15"/>
+        <v>557.19660693455216</v>
       </c>
       <c r="U52" s="83">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v>1609.8250753795896</v>
       </c>
       <c r="V52" s="83">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v>251.66959576095758</v>
       </c>
       <c r="W52" s="44"/>
@@ -16293,15 +16303,15 @@
         <v>303</v>
       </c>
       <c r="Y52" s="83">
-        <f t="shared" si="21"/>
-        <v>4884.8481857701345</v>
+        <f t="shared" si="18"/>
+        <v>836.16625838715231</v>
       </c>
       <c r="Z52" s="83">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>2396.928302933643</v>
       </c>
       <c r="AA52" s="83">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>458.35590861936208</v>
       </c>
       <c r="AB52" s="44"/>
@@ -16309,15 +16319,15 @@
         <v>303</v>
       </c>
       <c r="AD52" s="83">
-        <f t="shared" si="24"/>
-        <v>5090.0002819148576</v>
+        <f t="shared" si="21"/>
+        <v>1076.7328980106768</v>
       </c>
       <c r="AE52" s="83">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>3075.6913390220689</v>
       </c>
       <c r="AF52" s="83">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>669.26603937107893</v>
       </c>
       <c r="AG52" s="44"/>
@@ -16356,14 +16366,14 @@
       </c>
       <c r="T53" s="86">
         <f>SUM(T44:T52)</f>
-        <v>101805.46942590893</v>
+        <v>97778.864101003026</v>
       </c>
       <c r="U53" s="86">
-        <f t="shared" ref="U53:V53" si="27">SUM(U44:U52)</f>
+        <f t="shared" ref="U53:V53" si="24">SUM(U44:U52)</f>
         <v>154814.47229097722</v>
       </c>
       <c r="V53" s="86">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>70020.423006953177</v>
       </c>
       <c r="W53" s="44"/>
@@ -16372,14 +16382,14 @@
       </c>
       <c r="Y53" s="86">
         <f>SUM(Y44:Y52)</f>
-        <v>128041.56708343991</v>
+        <v>123992.88515605692</v>
       </c>
       <c r="Z53" s="86">
-        <f t="shared" ref="Z53:AA53" si="28">SUM(Z44:Z52)</f>
+        <f t="shared" ref="Z53:AA53" si="25">SUM(Z44:Z52)</f>
         <v>262632.65319122979</v>
       </c>
       <c r="AA53" s="86">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v>152031.29697009272</v>
       </c>
       <c r="AB53" s="44"/>
@@ -16388,14 +16398,14 @@
       </c>
       <c r="AD53" s="86">
         <f>SUM(AD44:AD52)</f>
-        <v>142480.30519743709</v>
+        <v>138467.03781353289</v>
       </c>
       <c r="AE53" s="86">
-        <f t="shared" ref="AE53:AF53" si="29">SUM(AE44:AE52)</f>
+        <f t="shared" ref="AE53:AF53" si="26">SUM(AE44:AE52)</f>
         <v>340279.31940189365</v>
       </c>
       <c r="AF53" s="86">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>227598.92660060374</v>
       </c>
       <c r="AG53" s="44"/>
@@ -16435,7 +16445,7 @@
       <c r="S54" s="44"/>
       <c r="T54" s="89">
         <f>T53/U16</f>
-        <v>0.49229215827691208</v>
+        <v>0.47282104108541512</v>
       </c>
       <c r="U54" s="89">
         <f>U53/V16</f>
@@ -16449,7 +16459,7 @@
       <c r="X54" s="44"/>
       <c r="Y54" s="89">
         <f>Y53/U16</f>
-        <v>0.61915985225664982</v>
+        <v>0.59958198109267813</v>
       </c>
       <c r="Z54" s="89">
         <f>Z53/V16</f>
@@ -16463,7 +16473,7 @@
       <c r="AC54" s="44"/>
       <c r="AD54" s="89">
         <f>AD53/U16</f>
-        <v>0.68898004550380965</v>
+        <v>0.66957342547341547</v>
       </c>
       <c r="AE54" s="89">
         <f>AE53/V16</f>
@@ -16557,11 +16567,11 @@
         <v>96093.46148811256</v>
       </c>
       <c r="U56" s="90">
-        <f t="shared" ref="U56:V56" si="30">SUM(U44:U50)</f>
+        <f t="shared" ref="U56:V56" si="27">SUM(U44:U50)</f>
         <v>151590.13449734473</v>
       </c>
       <c r="V56" s="90">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>69451.686879577494</v>
       </c>
       <c r="W56" s="44"/>
@@ -16571,11 +16581,11 @@
         <v>121269.9405872198</v>
       </c>
       <c r="Z56" s="90">
-        <f t="shared" ref="Z56:AA56" si="31">SUM(Z44:Z50)</f>
+        <f t="shared" ref="Z56:AA56" si="28">SUM(Z44:Z50)</f>
         <v>257412.12625925304</v>
       </c>
       <c r="AA56" s="90">
-        <f t="shared" si="31"/>
+        <f t="shared" si="28"/>
         <v>150887.52813147739</v>
       </c>
       <c r="AB56" s="44"/>
@@ -16585,11 +16595,11 @@
         <v>134842.68397180433</v>
       </c>
       <c r="AE56" s="90">
-        <f t="shared" ref="AE56:AF56" si="32">SUM(AE44:AE50)</f>
+        <f t="shared" ref="AE56:AF56" si="29">SUM(AE44:AE50)</f>
         <v>333238.03423646506</v>
       </c>
       <c r="AF56" s="90">
-        <f t="shared" si="32"/>
+        <f t="shared" si="29"/>
         <v>225831.46956745218</v>
       </c>
       <c r="AG56" s="44"/>

</xml_diff>

<commit_message>
No F and G rated to have HP without fabric upgrade
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968263B1-F117-4CC7-8AF3-77769B36F549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA867F63-ED17-4DB3-A0A0-98E8FC2B5E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1996,6 +1996,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="12" fillId="18" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2016,9 +2019,6 @@
     </xf>
     <xf numFmtId="166" fontId="21" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="18" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3415,12 +3415,12 @@
       <c r="Z15" s="46"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="96" t="s">
         <v>253</v>
       </c>
-      <c r="B16" s="95"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
       <c r="E16" s="47"/>
       <c r="F16" s="47"/>
       <c r="G16" s="48"/>
@@ -3504,11 +3504,11 @@
       <c r="A19" s="52" t="s">
         <v>254</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
       <c r="E19" s="53"/>
       <c r="F19" s="53"/>
       <c r="G19" s="54"/>
@@ -3536,11 +3536,11 @@
       <c r="A20" s="52" t="s">
         <v>255</v>
       </c>
-      <c r="B20" s="94" t="s">
+      <c r="B20" s="95" t="s">
         <v>266</v>
       </c>
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
       <c r="E20" s="53"/>
       <c r="F20" s="53"/>
       <c r="G20" s="54"/>
@@ -3628,11 +3628,11 @@
       <c r="A23" s="52" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="94" t="s">
+      <c r="B23" s="95" t="s">
         <v>265</v>
       </c>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
       <c r="E23" s="46"/>
       <c r="F23" s="46"/>
       <c r="G23" s="46"/>
@@ -3718,11 +3718,11 @@
       <c r="A26" s="52" t="s">
         <v>258</v>
       </c>
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="95" t="s">
         <v>265</v>
       </c>
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
       <c r="E26" s="46"/>
       <c r="F26" s="46"/>
       <c r="G26" s="46"/>
@@ -3838,11 +3838,11 @@
       <c r="A30" s="52" t="s">
         <v>260</v>
       </c>
-      <c r="B30" s="96" t="s">
+      <c r="B30" s="97" t="s">
         <v>261</v>
       </c>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="95"/>
       <c r="E30" s="57"/>
       <c r="F30" s="57"/>
       <c r="G30" s="46"/>
@@ -3870,11 +3870,11 @@
       <c r="A31" s="52" t="s">
         <v>262</v>
       </c>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="95" t="s">
         <v>263</v>
       </c>
-      <c r="C31" s="94"/>
-      <c r="D31" s="94"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="95"/>
       <c r="E31" s="57"/>
       <c r="F31" s="57"/>
       <c r="G31" s="46"/>
@@ -13021,7 +13021,7 @@
   <dimension ref="A1:AM200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13170,31 +13170,31 @@
         <v>11</v>
       </c>
       <c r="O5" s="44"/>
-      <c r="P5" s="99" t="s">
+      <c r="P5" s="100" t="s">
         <v>277</v>
       </c>
-      <c r="Q5" s="99"/>
-      <c r="R5" s="99"/>
+      <c r="Q5" s="100"/>
+      <c r="R5" s="100"/>
       <c r="S5" s="44"/>
-      <c r="T5" s="99" t="s">
+      <c r="T5" s="100" t="s">
         <v>278</v>
       </c>
-      <c r="U5" s="99"/>
-      <c r="V5" s="99"/>
-      <c r="W5" s="99"/>
-      <c r="X5" s="99"/>
+      <c r="U5" s="100"/>
+      <c r="V5" s="100"/>
+      <c r="W5" s="100"/>
+      <c r="X5" s="100"/>
       <c r="Y5" s="44"/>
-      <c r="Z5" s="99" t="s">
+      <c r="Z5" s="100" t="s">
         <v>279</v>
       </c>
-      <c r="AA5" s="99"/>
-      <c r="AB5" s="99"/>
+      <c r="AA5" s="100"/>
+      <c r="AB5" s="100"/>
       <c r="AC5" s="44"/>
-      <c r="AD5" s="99" t="s">
+      <c r="AD5" s="100" t="s">
         <v>280</v>
       </c>
-      <c r="AE5" s="99"/>
-      <c r="AF5" s="99"/>
+      <c r="AE5" s="100"/>
+      <c r="AF5" s="100"/>
       <c r="AG5" s="44"/>
       <c r="AH5" s="44"/>
       <c r="AI5" s="44"/>
@@ -13294,7 +13294,7 @@
       </c>
       <c r="I7" s="27"/>
       <c r="J7" s="93">
-        <f>-(T33)</f>
+        <f t="shared" ref="J7:J12" si="0">-(T33)</f>
         <v>-0.76682617615099935</v>
       </c>
       <c r="K7" s="27"/>
@@ -13367,7 +13367,7 @@
       </c>
       <c r="I8" s="27"/>
       <c r="J8" s="93">
-        <f>-(T34)</f>
+        <f t="shared" si="0"/>
         <v>-0.5138907043261417</v>
       </c>
       <c r="K8" s="27"/>
@@ -13430,7 +13430,7 @@
       </c>
       <c r="I9" s="27"/>
       <c r="J9" s="93">
-        <f>-(T35)</f>
+        <f t="shared" si="0"/>
         <v>-0.37584533679027893</v>
       </c>
       <c r="K9" s="27"/>
@@ -13493,7 +13493,7 @@
       </c>
       <c r="I10" s="27"/>
       <c r="J10" s="93">
-        <f>-(T36)</f>
+        <f t="shared" si="0"/>
         <v>-0.16552806134367962</v>
       </c>
       <c r="K10" s="27"/>
@@ -13556,8 +13556,7 @@
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="93">
-        <f>-(T37)</f>
-        <v>-9.1492186931267622E-2</v>
+        <v>0</v>
       </c>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
@@ -13619,16 +13618,15 @@
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="93">
-        <f>-(T38)</f>
-        <v>-3.6630747396996691E-2</v>
+        <v>0</v>
       </c>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
-      <c r="P12" s="100" t="s">
+      <c r="P12" s="101" t="s">
         <v>296</v>
       </c>
-      <c r="Q12" s="100"/>
-      <c r="R12" s="100"/>
+      <c r="Q12" s="101"/>
+      <c r="R12" s="101"/>
       <c r="T12" s="71" t="s">
         <v>297</v>
       </c>
@@ -13871,7 +13869,7 @@
         <v>6.0039999999999996</v>
       </c>
       <c r="AC15" s="44"/>
-      <c r="AD15" s="101">
+      <c r="AD15" s="94">
         <f>AVERAGE(AE15:AF15)</f>
         <v>1.5565</v>
       </c>
@@ -13903,7 +13901,7 @@
       </c>
       <c r="I16" s="27"/>
       <c r="J16" s="93">
-        <f>-(AA33)</f>
+        <f t="shared" ref="J16:J21" si="1">-(AA33)</f>
         <v>-0.48602123970467664</v>
       </c>
       <c r="K16" s="27"/>
@@ -13967,7 +13965,7 @@
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="93">
-        <f>-(AA34)</f>
+        <f t="shared" si="1"/>
         <v>-0.25380085256173046</v>
       </c>
       <c r="K17" s="27"/>
@@ -14021,7 +14019,7 @@
       </c>
       <c r="I18" s="27"/>
       <c r="J18" s="93">
-        <f>-(AA35)</f>
+        <f t="shared" si="1"/>
         <v>-8.9754023843298891E-2</v>
       </c>
       <c r="K18" s="27"/>
@@ -14075,7 +14073,7 @@
       </c>
       <c r="I19" s="27"/>
       <c r="J19" s="93">
-        <f>-(AA36)</f>
+        <f t="shared" si="1"/>
         <v>-5.0511604601422351E-2</v>
       </c>
       <c r="K19" s="27"/>
@@ -14123,8 +14121,7 @@
       </c>
       <c r="I20" s="27"/>
       <c r="J20" s="93">
-        <f>-(AA37)</f>
-        <v>-3.2210497290905374E-2</v>
+        <v>0</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
@@ -14167,8 +14164,7 @@
       </c>
       <c r="I21" s="27"/>
       <c r="J21" s="93">
-        <f>-(AA38)</f>
-        <v>-3.054309712927282E-2</v>
+        <v>0</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
@@ -14352,7 +14348,7 @@
       </c>
       <c r="I25" s="27"/>
       <c r="J25" s="93">
-        <f>-(AH33)</f>
+        <f t="shared" ref="J25:J30" si="2">-(AH33)</f>
         <v>-0.14983014442834014</v>
       </c>
       <c r="K25" s="27"/>
@@ -14399,7 +14395,7 @@
       </c>
       <c r="I26" s="27"/>
       <c r="J26" s="93">
-        <f>-(AH34)</f>
+        <f t="shared" si="2"/>
         <v>-6.6011404930960929E-2</v>
       </c>
       <c r="K26" s="27"/>
@@ -14446,7 +14442,7 @@
       </c>
       <c r="I27" s="27"/>
       <c r="J27" s="93">
-        <f>-(AH35)</f>
+        <f t="shared" si="2"/>
         <v>-5.6979596817344061E-2</v>
       </c>
       <c r="K27" s="27"/>
@@ -14493,7 +14489,7 @@
       </c>
       <c r="I28" s="27"/>
       <c r="J28" s="93">
-        <f>-(AH36)</f>
+        <f t="shared" si="2"/>
         <v>-2.8856450394145666E-2</v>
       </c>
       <c r="K28" s="27"/>
@@ -14504,31 +14500,31 @@
       <c r="Q28" s="44"/>
       <c r="R28" s="44"/>
       <c r="S28" s="44"/>
-      <c r="T28" s="97" t="s">
+      <c r="T28" s="98" t="s">
         <v>281</v>
       </c>
-      <c r="U28" s="98"/>
-      <c r="V28" s="98"/>
-      <c r="W28" s="98"/>
-      <c r="X28" s="98"/>
+      <c r="U28" s="99"/>
+      <c r="V28" s="99"/>
+      <c r="W28" s="99"/>
+      <c r="X28" s="99"/>
       <c r="Y28" s="44"/>
       <c r="Z28" s="44"/>
-      <c r="AA28" s="97" t="s">
+      <c r="AA28" s="98" t="s">
         <v>282</v>
       </c>
-      <c r="AB28" s="98"/>
-      <c r="AC28" s="98"/>
-      <c r="AD28" s="98"/>
-      <c r="AE28" s="98"/>
+      <c r="AB28" s="99"/>
+      <c r="AC28" s="99"/>
+      <c r="AD28" s="99"/>
+      <c r="AE28" s="99"/>
       <c r="AF28" s="44"/>
       <c r="AG28" s="44"/>
-      <c r="AH28" s="97" t="s">
+      <c r="AH28" s="98" t="s">
         <v>283</v>
       </c>
-      <c r="AI28" s="98"/>
-      <c r="AJ28" s="98"/>
-      <c r="AK28" s="98"/>
-      <c r="AL28" s="98"/>
+      <c r="AI28" s="99"/>
+      <c r="AJ28" s="99"/>
+      <c r="AK28" s="99"/>
+      <c r="AL28" s="99"/>
       <c r="AM28" s="44"/>
     </row>
     <row r="29" spans="2:39" ht="15.75" thickBot="1">
@@ -14545,8 +14541,7 @@
       </c>
       <c r="I29" s="27"/>
       <c r="J29" s="93">
-        <f>-(AH37)</f>
-        <v>-7.3325429420576533E-3</v>
+        <v>0</v>
       </c>
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
@@ -14621,8 +14616,7 @@
       </c>
       <c r="I30" s="27"/>
       <c r="J30" s="93">
-        <f>-(AH38)</f>
-        <v>-3.2086171243230267E-3</v>
+        <v>0</v>
       </c>
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
@@ -14635,23 +14629,23 @@
         <v>287</v>
       </c>
       <c r="T30" s="88">
-        <f t="shared" ref="T30:T38" si="0">_xlfn.NORM.DIST(2,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="T30:T38" si="3">_xlfn.NORM.DIST(2,Z7,AD7,TRUE)</f>
         <v>0.99986614214614677</v>
       </c>
       <c r="U30" s="88">
-        <f t="shared" ref="U30:U38" si="1">_xlfn.NORM.DIST(2.3,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="U30:U38" si="4">_xlfn.NORM.DIST(2.3,Z7,AD7,TRUE)</f>
         <v>0.99999895018069218</v>
       </c>
       <c r="V30" s="88">
-        <f t="shared" ref="V30:V38" si="2">_xlfn.NORM.DIST(2.5,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="V30:V38" si="5">_xlfn.NORM.DIST(2.5,Z7,AD7,TRUE)</f>
         <v>0.99999997827100517</v>
       </c>
       <c r="W30" s="88">
-        <f t="shared" ref="W30:W38" si="3">_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="W30:W38" si="6">_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
         <v>0.99999999973303144</v>
       </c>
       <c r="X30" s="88">
-        <f t="shared" ref="X30:X38" si="4">1-_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
+        <f t="shared" ref="X30:X38" si="7">1-_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
         <v>2.6696855837116118E-10</v>
       </c>
       <c r="Y30" s="44"/>
@@ -14659,23 +14653,23 @@
         <v>287</v>
       </c>
       <c r="AA30" s="88">
-        <f t="shared" ref="AA30:AA38" si="5">_xlfn.NORM.DIST(2,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AA30:AA38" si="8">_xlfn.NORM.DIST(2,AA7,AE7,TRUE)</f>
         <v>0.99358230344905218</v>
       </c>
       <c r="AB30" s="88">
-        <f t="shared" ref="AB30:AB38" si="6">_xlfn.NORM.DIST(2.3,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AB30:AB38" si="9">_xlfn.NORM.DIST(2.3,AA7,AE7,TRUE)</f>
         <v>0.99961797061500135</v>
       </c>
       <c r="AC30" s="88">
-        <f t="shared" ref="AC30:AC38" si="7">_xlfn.NORM.DIST(2.5,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AC30:AC38" si="10">_xlfn.NORM.DIST(2.5,AA7,AE7,TRUE)</f>
         <v>0.99996097211163748</v>
       </c>
       <c r="AD30" s="88">
-        <f t="shared" ref="AD30:AD38" si="8">_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AD30:AD38" si="11">_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
         <v>0.99999712102252392</v>
       </c>
       <c r="AE30" s="88">
-        <f t="shared" ref="AE30:AE38" si="9">1-_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
+        <f t="shared" ref="AE30:AE38" si="12">1-_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
         <v>2.8789774760840103E-6</v>
       </c>
       <c r="AF30" s="44"/>
@@ -14683,23 +14677,23 @@
         <v>287</v>
       </c>
       <c r="AH30" s="44">
-        <f t="shared" ref="AH30:AH38" si="10">_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AH30:AH38" si="13">_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
         <v>0.99867076285153633</v>
       </c>
       <c r="AI30" s="44">
-        <f t="shared" ref="AI30:AI38" si="11">_xlfn.NORM.DIST(2.3,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AI30:AI38" si="14">_xlfn.NORM.DIST(2.3,AB7,AF7,TRUE)</f>
         <v>0.99999490602709384</v>
       </c>
       <c r="AJ30" s="44">
-        <f t="shared" ref="AJ30:AJ38" si="12">_xlfn.NORM.DIST(2.5,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AJ30:AJ38" si="15">_xlfn.NORM.DIST(2.5,AB7,AF7,TRUE)</f>
         <v>0.99999995653338158</v>
       </c>
       <c r="AK30" s="44">
-        <f t="shared" ref="AK30:AK38" si="13">_xlfn.NORM.DIST(2.7,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AK30:AK38" si="16">_xlfn.NORM.DIST(2.7,AB7,AF7,TRUE)</f>
         <v>0.99999999984236743</v>
       </c>
       <c r="AL30" s="44">
-        <f t="shared" ref="AL30:AL38" si="14">1-_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
+        <f t="shared" ref="AL30:AL38" si="17">1-_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
         <v>1.3292371484636689E-3</v>
       </c>
       <c r="AM30" s="44"/>
@@ -14730,23 +14724,23 @@
         <v>289</v>
       </c>
       <c r="T31" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.96885301500182108</v>
       </c>
       <c r="U31" s="88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.99736560266376562</v>
       </c>
       <c r="V31" s="88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.99967208422117826</v>
       </c>
       <c r="W31" s="88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99997147495584515</v>
       </c>
       <c r="X31" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.8525044154847912E-5</v>
       </c>
       <c r="Y31" s="44"/>
@@ -14754,23 +14748,23 @@
         <v>289</v>
       </c>
       <c r="AA31" s="88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.7694627396275191</v>
       </c>
       <c r="AB31" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.92091247414921895</v>
       </c>
       <c r="AC31" s="88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.96860489728090593</v>
       </c>
       <c r="AD31" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.98955903282288238</v>
       </c>
       <c r="AE31" s="88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.0440967177117622E-2</v>
       </c>
       <c r="AF31" s="44"/>
@@ -14778,23 +14772,23 @@
         <v>289</v>
       </c>
       <c r="AH31" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.6130931526036395</v>
       </c>
       <c r="AI31" s="44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.87842619586393023</v>
       </c>
       <c r="AJ31" s="44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.9602560960127382</v>
       </c>
       <c r="AK31" s="44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.99036267162555125</v>
       </c>
       <c r="AL31" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.3869068473963605</v>
       </c>
       <c r="AM31" s="44"/>
@@ -14822,69 +14816,69 @@
         <v>291</v>
       </c>
       <c r="T32" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.93969745300565943</v>
       </c>
       <c r="U32" s="88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.99622594121059427</v>
       </c>
       <c r="V32" s="88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.99968448066910742</v>
       </c>
       <c r="W32" s="88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99998437626199244</v>
       </c>
       <c r="X32" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.5623738007564114E-5</v>
       </c>
       <c r="Z32" s="76" t="s">
         <v>291</v>
       </c>
       <c r="AA32" s="88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.63358245624321075</v>
       </c>
       <c r="AB32" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.84081469035187228</v>
       </c>
       <c r="AC32" s="88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.92442034414706997</v>
       </c>
       <c r="AD32" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.9694716992391359</v>
       </c>
       <c r="AE32" s="88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>3.0528300760864102E-2</v>
       </c>
       <c r="AG32" s="76" t="s">
         <v>291</v>
       </c>
       <c r="AH32" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.34194299028735675</v>
       </c>
       <c r="AI32" s="44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.71567219724569331</v>
       </c>
       <c r="AJ32" s="44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.88905130905570107</v>
       </c>
       <c r="AK32" s="44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.9694633335110785</v>
       </c>
       <c r="AL32" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.65805700971264325</v>
       </c>
     </row>
@@ -14897,23 +14891,23 @@
         <v>293</v>
       </c>
       <c r="T33" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.76682617615099935</v>
       </c>
       <c r="U33" s="88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.95418880111755022</v>
       </c>
       <c r="V33" s="88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.98998748585906793</v>
       </c>
       <c r="W33" s="88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.99848587792694921</v>
       </c>
       <c r="X33" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.5141220730507943E-3</v>
       </c>
       <c r="Y33" s="44"/>
@@ -14921,23 +14915,23 @@
         <v>293</v>
       </c>
       <c r="AA33" s="88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.48602123970467664</v>
       </c>
       <c r="AB33" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.74725860659793841</v>
       </c>
       <c r="AC33" s="88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.87143015426775872</v>
       </c>
       <c r="AD33" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.94525252109261237</v>
       </c>
       <c r="AE33" s="88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>5.4747478907387626E-2</v>
       </c>
       <c r="AF33" s="44"/>
@@ -14945,23 +14939,23 @@
         <v>293</v>
       </c>
       <c r="AH33" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.14983014442834014</v>
       </c>
       <c r="AI33" s="44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.49056643348839696</v>
       </c>
       <c r="AJ33" s="44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.74280813134921952</v>
       </c>
       <c r="AK33" s="44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.90786182982277952</v>
       </c>
       <c r="AL33" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.85016985557165992</v>
       </c>
       <c r="AM33" s="44"/>
@@ -14976,23 +14970,23 @@
         <v>295</v>
       </c>
       <c r="T34" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5138907043261417</v>
       </c>
       <c r="U34" s="88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.70275414783970647</v>
       </c>
       <c r="V34" s="88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.80620969874302539</v>
       </c>
       <c r="W34" s="88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.88409087605518322</v>
       </c>
       <c r="X34" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.11590912394481678</v>
       </c>
       <c r="Y34" s="44"/>
@@ -15000,23 +14994,23 @@
         <v>295</v>
       </c>
       <c r="AA34" s="88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.25380085256173046</v>
       </c>
       <c r="AB34" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.48042786872418958</v>
       </c>
       <c r="AC34" s="88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.64054584703308814</v>
       </c>
       <c r="AD34" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.77902845692514355</v>
       </c>
       <c r="AE34" s="88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.22097154307485645</v>
       </c>
       <c r="AF34" s="44"/>
@@ -15024,23 +15018,23 @@
         <v>295</v>
       </c>
       <c r="AH34" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>6.6011404930960929E-2</v>
       </c>
       <c r="AI34" s="44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.22200714259760385</v>
       </c>
       <c r="AJ34" s="44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.39296290098211079</v>
       </c>
       <c r="AK34" s="44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.58792955212905773</v>
       </c>
       <c r="AL34" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.93398859506903908</v>
       </c>
       <c r="AM34" s="44"/>
@@ -15055,23 +15049,23 @@
         <v>297</v>
       </c>
       <c r="T35" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.37584533679027893</v>
       </c>
       <c r="U35" s="88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.51506861469064869</v>
       </c>
       <c r="V35" s="88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.60792230376456446</v>
       </c>
       <c r="W35" s="88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.69498667602271957</v>
       </c>
       <c r="X35" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.30501332397728043</v>
       </c>
       <c r="Y35" s="44"/>
@@ -15079,23 +15073,23 @@
         <v>297</v>
       </c>
       <c r="AA35" s="88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.9754023843298891E-2</v>
       </c>
       <c r="AB35" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.19240027281705166</v>
       </c>
       <c r="AC35" s="88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.28991681177663592</v>
       </c>
       <c r="AD35" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.40587448754231226</v>
       </c>
       <c r="AE35" s="88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.59412551245768774</v>
       </c>
       <c r="AF35" s="44"/>
@@ -15103,23 +15097,23 @@
         <v>297</v>
       </c>
       <c r="AH35" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>5.6979596817344061E-2</v>
       </c>
       <c r="AI35" s="44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.12698439253107691</v>
       </c>
       <c r="AJ35" s="44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.19835620119859471</v>
       </c>
       <c r="AK35" s="44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.28970312941742804</v>
       </c>
       <c r="AL35" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.9430204031826559</v>
       </c>
       <c r="AM35" s="44"/>
@@ -15139,69 +15133,69 @@
         <v>301</v>
       </c>
       <c r="T36" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.16552806134367962</v>
       </c>
       <c r="U36" s="88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.29053559209062707</v>
       </c>
       <c r="V36" s="88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.39292301197938029</v>
       </c>
       <c r="W36" s="88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.50335241668180219</v>
       </c>
       <c r="X36" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.49664758331819781</v>
       </c>
       <c r="Z36" s="76" t="s">
         <v>301</v>
       </c>
       <c r="AA36" s="88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.0511604601422351E-2</v>
       </c>
       <c r="AB36" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9.4333345509310967E-2</v>
       </c>
       <c r="AC36" s="88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.13618656405660809</v>
       </c>
       <c r="AD36" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.18924169383003042</v>
       </c>
       <c r="AE36" s="88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.81075830616996958</v>
       </c>
       <c r="AG36" s="76" t="s">
         <v>301</v>
       </c>
       <c r="AH36" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.8856450394145666E-2</v>
       </c>
       <c r="AI36" s="44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>5.7199757058308189E-2</v>
       </c>
       <c r="AJ36" s="44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>8.5976160021217857E-2</v>
       </c>
       <c r="AK36" s="44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.12441589797637952</v>
       </c>
       <c r="AL36" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.97114354960585436</v>
       </c>
     </row>
@@ -15216,23 +15210,23 @@
         <v>302</v>
       </c>
       <c r="T37" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.1492186931267622E-2</v>
       </c>
       <c r="U37" s="88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.15300882371326033</v>
       </c>
       <c r="V37" s="88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.20660004501142309</v>
       </c>
       <c r="W37" s="88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.26995921510986137</v>
       </c>
       <c r="X37" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.73004078489013868</v>
       </c>
       <c r="Y37" s="44"/>
@@ -15240,23 +15234,23 @@
         <v>302</v>
       </c>
       <c r="AA37" s="88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.2210497290905374E-2</v>
       </c>
       <c r="AB37" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5.6332486553475364E-2</v>
       </c>
       <c r="AC37" s="88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>7.9115975834815E-2</v>
       </c>
       <c r="AD37" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.10827424567922854</v>
       </c>
       <c r="AE37" s="88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.8917257543207715</v>
       </c>
       <c r="AF37" s="44"/>
@@ -15264,23 +15258,23 @@
         <v>302</v>
       </c>
       <c r="AH37" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>7.3325429420576533E-3</v>
       </c>
       <c r="AI37" s="44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.5850994164039133E-2</v>
       </c>
       <c r="AJ37" s="44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>2.5396980814932565E-2</v>
       </c>
       <c r="AK37" s="44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>3.9349548301286723E-2</v>
       </c>
       <c r="AL37" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.99266745705794235</v>
       </c>
       <c r="AM37" s="44"/>
@@ -15301,23 +15295,23 @@
         <v>303</v>
       </c>
       <c r="T38" s="88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.6630747396996691E-2</v>
       </c>
       <c r="U38" s="88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.4970533940220757E-2</v>
       </c>
       <c r="V38" s="88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.0785662206478708E-2</v>
       </c>
       <c r="W38" s="88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>8.9883749084018569E-2</v>
       </c>
       <c r="X38" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.91011625091598147</v>
       </c>
       <c r="Y38" s="44"/>
@@ -15325,23 +15319,23 @@
         <v>303</v>
       </c>
       <c r="AA38" s="88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.054309712927282E-2</v>
       </c>
       <c r="AB38" s="88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4.54767509141593E-2</v>
       </c>
       <c r="AC38" s="88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.8354873920238394E-2</v>
       </c>
       <c r="AD38" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>7.3937218528355567E-2</v>
       </c>
       <c r="AE38" s="88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.92606278147164445</v>
       </c>
       <c r="AF38" s="44"/>
@@ -15349,23 +15343,23 @@
         <v>303</v>
       </c>
       <c r="AH38" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3.2086171243230267E-3</v>
       </c>
       <c r="AI38" s="44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>5.8437278169573741E-3</v>
       </c>
       <c r="AJ38" s="44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>8.5326893308700167E-3</v>
       </c>
       <c r="AK38" s="44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1.2251506395051929E-2</v>
       </c>
       <c r="AL38" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.99679138287567692</v>
       </c>
       <c r="AM38" s="44"/>
@@ -15555,26 +15549,26 @@
       <c r="P42" s="44"/>
       <c r="Q42" s="44"/>
       <c r="R42" s="44"/>
-      <c r="S42" s="99" t="s">
+      <c r="S42" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="T42" s="99"/>
-      <c r="U42" s="99"/>
-      <c r="V42" s="99"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
+      <c r="V42" s="100"/>
       <c r="W42" s="44"/>
-      <c r="X42" s="99" t="s">
+      <c r="X42" s="100" t="s">
         <v>308</v>
       </c>
-      <c r="Y42" s="99"/>
-      <c r="Z42" s="99"/>
-      <c r="AA42" s="99"/>
+      <c r="Y42" s="100"/>
+      <c r="Z42" s="100"/>
+      <c r="AA42" s="100"/>
       <c r="AB42" s="44"/>
-      <c r="AC42" s="99" t="s">
+      <c r="AC42" s="100" t="s">
         <v>309</v>
       </c>
-      <c r="AD42" s="99"/>
-      <c r="AE42" s="99"/>
-      <c r="AF42" s="99"/>
+      <c r="AD42" s="100"/>
+      <c r="AE42" s="100"/>
+      <c r="AF42" s="100"/>
       <c r="AG42" s="44"/>
       <c r="AH42" s="44"/>
       <c r="AI42" s="44"/>
@@ -15683,15 +15677,15 @@
         <v>287</v>
       </c>
       <c r="T44" s="68">
-        <f t="shared" ref="T44:T52" si="15">U7*T30</f>
+        <f t="shared" ref="T44:T52" si="18">U7*T30</f>
         <v>9417.6380632201017</v>
       </c>
       <c r="U44" s="68">
-        <f t="shared" ref="U44:U52" si="16">V7*AA30</f>
+        <f t="shared" ref="U44:U52" si="19">V7*AA30</f>
         <v>15372.778652981828</v>
       </c>
       <c r="V44" s="68">
-        <f t="shared" ref="V44:V52" si="17">W7*AH30</f>
+        <f t="shared" ref="V44:V52" si="20">W7*AH30</f>
         <v>20351.618204054608</v>
       </c>
       <c r="W44" s="44"/>
@@ -15699,15 +15693,15 @@
         <v>287</v>
       </c>
       <c r="Y44" s="68">
-        <f t="shared" ref="Y44:Y52" si="18">U7*U30</f>
+        <f t="shared" ref="Y44:Y52" si="21">U7*U30</f>
         <v>9418.8889686648563</v>
       </c>
       <c r="Z44" s="68">
-        <f t="shared" ref="Z44:Z52" si="19">V7*AB30</f>
+        <f t="shared" ref="Z44:Z52" si="22">V7*AB30</f>
         <v>15466.162940366092</v>
       </c>
       <c r="AA44" s="68">
-        <f t="shared" ref="AA44:AA52" si="20">W7*AI30</f>
+        <f t="shared" ref="AA44:AA52" si="23">W7*AI30</f>
         <v>20378.602528978172</v>
       </c>
       <c r="AB44" s="44"/>
@@ -15715,15 +15709,15 @@
         <v>287</v>
       </c>
       <c r="AD44" s="68">
-        <f t="shared" ref="AD44:AD52" si="21">U7*V30</f>
+        <f t="shared" ref="AD44:AD52" si="24">U7*V30</f>
         <v>9418.898652143529</v>
       </c>
       <c r="AE44" s="68">
-        <f t="shared" ref="AE44:AE52" si="22">V7*AC30</f>
+        <f t="shared" ref="AE44:AE52" si="25">V7*AC30</f>
         <v>15471.469884810578</v>
       </c>
       <c r="AF44" s="68">
-        <f t="shared" ref="AF44:AF52" si="23">W7*AJ30</f>
+        <f t="shared" ref="AF44:AF52" si="26">W7*AJ30</f>
         <v>20378.705451762668</v>
       </c>
       <c r="AG44" s="44"/>
@@ -15763,15 +15757,15 @@
         <v>289</v>
       </c>
       <c r="T45" s="73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>7226.9569082675025</v>
       </c>
       <c r="U45" s="73">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>7338.965095745436</v>
       </c>
       <c r="V45" s="73">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5783.8602283503142</v>
       </c>
       <c r="W45" s="44"/>
@@ -15779,15 +15773,15 @@
         <v>289</v>
       </c>
       <c r="Y45" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>7439.6406066050522</v>
       </c>
       <c r="Z45" s="73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>8783.4591019824566</v>
       </c>
       <c r="AA45" s="73">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>8286.9859436891857</v>
       </c>
       <c r="AB45" s="44"/>
@@ -15795,15 +15789,15 @@
         <v>289</v>
       </c>
       <c r="AD45" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>7456.845324521013</v>
       </c>
       <c r="AE45" s="73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>9238.3388650550733</v>
       </c>
       <c r="AF45" s="73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>9058.9611369377526</v>
       </c>
       <c r="AG45" s="44"/>
@@ -15848,15 +15842,15 @@
         <v>291</v>
       </c>
       <c r="T46" s="78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>13195.088262110432</v>
       </c>
       <c r="U46" s="78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11116.263088697284</v>
       </c>
       <c r="V46" s="78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>6869.9592457318131</v>
       </c>
       <c r="W46" s="44"/>
@@ -15864,15 +15858,15 @@
         <v>291</v>
       </c>
       <c r="Y46" s="78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>13988.85266873088</v>
       </c>
       <c r="Z46" s="78">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>14752.17189916172</v>
       </c>
       <c r="AA46" s="78">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>14378.533755727773</v>
       </c>
       <c r="AB46" s="44"/>
@@ -15880,15 +15874,15 @@
         <v>291</v>
       </c>
       <c r="AD46" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>14037.41695212561</v>
       </c>
       <c r="AE46" s="78">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>16219.040866463431</v>
       </c>
       <c r="AF46" s="78">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>17861.884682719923</v>
       </c>
       <c r="AG46" s="44"/>
@@ -15926,15 +15920,15 @@
         <v>293</v>
       </c>
       <c r="T47" s="73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>15278.613097799687</v>
       </c>
       <c r="U47" s="73">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>24188.71802303115</v>
       </c>
       <c r="V47" s="73">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>8010.8499729257437</v>
       </c>
       <c r="W47" s="44"/>
@@ -15942,15 +15936,15 @@
         <v>293</v>
       </c>
       <c r="Y47" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>19011.716041964675</v>
       </c>
       <c r="Z47" s="73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>37190.201268289908</v>
       </c>
       <c r="AA47" s="73">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>26228.727973417597</v>
       </c>
       <c r="AB47" s="44"/>
@@ -15958,15 +15952,15 @@
         <v>293</v>
       </c>
       <c r="AD47" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>19724.986233549855</v>
       </c>
       <c r="AE47" s="73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>43370.07635953842</v>
       </c>
       <c r="AF47" s="73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>39715.1355730949</v>
       </c>
       <c r="AG47" s="44"/>
@@ -15989,15 +15983,15 @@
         <v>295</v>
       </c>
       <c r="T48" s="78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>30270.630926141846</v>
       </c>
       <c r="U48" s="78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>71610.298224913975</v>
       </c>
       <c r="V48" s="78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>16589.915893594109</v>
       </c>
       <c r="W48" s="44"/>
@@ -16005,15 +15999,15 @@
         <v>295</v>
       </c>
       <c r="Y48" s="78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>41395.59494263638</v>
       </c>
       <c r="Z48" s="78">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>135553.45700240019</v>
       </c>
       <c r="AA48" s="78">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>55794.598332264082</v>
       </c>
       <c r="AB48" s="44"/>
@@ -16021,15 +16015,15 @@
         <v>295</v>
       </c>
       <c r="AD48" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>47489.623833004342</v>
       </c>
       <c r="AE48" s="78">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>180730.98915856858</v>
       </c>
       <c r="AF48" s="78">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>98759.017224587151</v>
       </c>
       <c r="AG48" s="44"/>
@@ -16051,15 +16045,15 @@
         <v>297</v>
       </c>
       <c r="T49" s="73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>16439.227593093379</v>
       </c>
       <c r="U49" s="73">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>16840.280240037471</v>
       </c>
       <c r="V49" s="73">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9496.663557138043</v>
       </c>
       <c r="W49" s="44"/>
@@ -16067,15 +16061,15 @@
         <v>297</v>
       </c>
       <c r="Y49" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>22528.762110686101</v>
       </c>
       <c r="Z49" s="73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>36099.49029311091</v>
       </c>
       <c r="AA49" s="73">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>21164.20824704953</v>
       </c>
       <c r="AB49" s="44"/>
@@ -16083,15 +16077,15 @@
         <v>297</v>
       </c>
       <c r="AD49" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>26590.121340469981</v>
       </c>
       <c r="AE49" s="73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>54396.228130570431</v>
       </c>
       <c r="AF49" s="73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>33059.589966801032</v>
       </c>
       <c r="AG49" s="44"/>
@@ -16117,15 +16111,15 @@
         <v>301</v>
       </c>
       <c r="T50" s="78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>4265.3066374795972</v>
       </c>
       <c r="U50" s="78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5122.8311719375915</v>
       </c>
       <c r="V50" s="78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>2348.819777782865</v>
       </c>
       <c r="W50" s="44"/>
@@ -16133,15 +16127,15 @@
         <v>301</v>
       </c>
       <c r="Y50" s="78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>7486.4852479318533</v>
       </c>
       <c r="Z50" s="78">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>9567.1837539417502</v>
       </c>
       <c r="AA50" s="78">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>4655.871350351058</v>
       </c>
       <c r="AB50" s="44"/>
@@ -16149,15 +16143,15 @@
         <v>301</v>
       </c>
       <c r="AD50" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>10124.791635989994</v>
       </c>
       <c r="AE50" s="78">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>13811.89097145851</v>
       </c>
       <c r="AF50" s="78">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>6998.1755315487662</v>
       </c>
       <c r="AG50" s="44"/>
@@ -16209,15 +16203,15 @@
         <v>302</v>
       </c>
       <c r="T51" s="73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1128.2060059559165</v>
       </c>
       <c r="U51" s="73">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1614.512718252895</v>
       </c>
       <c r="V51" s="73">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>317.06653161471883</v>
       </c>
       <c r="W51" s="44"/>
@@ -16225,15 +16219,15 @@
         <v>302</v>
       </c>
       <c r="Y51" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1886.7783104499745</v>
       </c>
       <c r="Z51" s="73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2823.5986290430769</v>
       </c>
       <c r="AA51" s="73">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>685.4129299959742</v>
       </c>
       <c r="AB51" s="44"/>
@@ -16241,15 +16235,15 @@
         <v>302</v>
       </c>
       <c r="AD51" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>2547.6209437178968</v>
       </c>
       <c r="AE51" s="73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>3965.5938264064957</v>
       </c>
       <c r="AF51" s="73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>1098.1909937804644</v>
       </c>
       <c r="AG51" s="44"/>
@@ -16287,15 +16281,15 @@
         <v>303</v>
       </c>
       <c r="T52" s="83">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>557.19660693455216</v>
       </c>
       <c r="U52" s="83">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1609.8250753795896</v>
       </c>
       <c r="V52" s="83">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>251.66959576095758</v>
       </c>
       <c r="W52" s="44"/>
@@ -16303,15 +16297,15 @@
         <v>303</v>
       </c>
       <c r="Y52" s="83">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>836.16625838715231</v>
       </c>
       <c r="Z52" s="83">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2396.928302933643</v>
       </c>
       <c r="AA52" s="83">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>458.35590861936208</v>
       </c>
       <c r="AB52" s="44"/>
@@ -16319,15 +16313,15 @@
         <v>303</v>
       </c>
       <c r="AD52" s="83">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>1076.7328980106768</v>
       </c>
       <c r="AE52" s="83">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>3075.6913390220689</v>
       </c>
       <c r="AF52" s="83">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>669.26603937107893</v>
       </c>
       <c r="AG52" s="44"/>
@@ -16369,11 +16363,11 @@
         <v>97778.864101003026</v>
       </c>
       <c r="U53" s="86">
-        <f t="shared" ref="U53:V53" si="24">SUM(U44:U52)</f>
+        <f t="shared" ref="U53:V53" si="27">SUM(U44:U52)</f>
         <v>154814.47229097722</v>
       </c>
       <c r="V53" s="86">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>70020.423006953177</v>
       </c>
       <c r="W53" s="44"/>
@@ -16385,11 +16379,11 @@
         <v>123992.88515605692</v>
       </c>
       <c r="Z53" s="86">
-        <f t="shared" ref="Z53:AA53" si="25">SUM(Z44:Z52)</f>
+        <f t="shared" ref="Z53:AA53" si="28">SUM(Z44:Z52)</f>
         <v>262632.65319122979</v>
       </c>
       <c r="AA53" s="86">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>152031.29697009272</v>
       </c>
       <c r="AB53" s="44"/>
@@ -16401,11 +16395,11 @@
         <v>138467.03781353289</v>
       </c>
       <c r="AE53" s="86">
-        <f t="shared" ref="AE53:AF53" si="26">SUM(AE44:AE52)</f>
+        <f t="shared" ref="AE53:AF53" si="29">SUM(AE44:AE52)</f>
         <v>340279.31940189365</v>
       </c>
       <c r="AF53" s="86">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>227598.92660060374</v>
       </c>
       <c r="AG53" s="44"/>
@@ -16567,11 +16561,11 @@
         <v>96093.46148811256</v>
       </c>
       <c r="U56" s="90">
-        <f t="shared" ref="U56:V56" si="27">SUM(U44:U50)</f>
+        <f t="shared" ref="U56:V56" si="30">SUM(U44:U50)</f>
         <v>151590.13449734473</v>
       </c>
       <c r="V56" s="90">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>69451.686879577494</v>
       </c>
       <c r="W56" s="44"/>
@@ -16581,11 +16575,11 @@
         <v>121269.9405872198</v>
       </c>
       <c r="Z56" s="90">
-        <f t="shared" ref="Z56:AA56" si="28">SUM(Z44:Z50)</f>
+        <f t="shared" ref="Z56:AA56" si="31">SUM(Z44:Z50)</f>
         <v>257412.12625925304</v>
       </c>
       <c r="AA56" s="90">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>150887.52813147739</v>
       </c>
       <c r="AB56" s="44"/>
@@ -16595,11 +16589,11 @@
         <v>134842.68397180433</v>
       </c>
       <c r="AE56" s="90">
-        <f t="shared" ref="AE56:AF56" si="29">SUM(AE44:AE50)</f>
+        <f t="shared" ref="AE56:AF56" si="32">SUM(AE44:AE50)</f>
         <v>333238.03423646506</v>
       </c>
       <c r="AF56" s="90">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>225831.46956745218</v>
       </c>
       <c r="AG56" s="44"/>

</xml_diff>

<commit_message>
Upper GAS UC and F and G rated exceptions in HP
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA867F63-ED17-4DB3-A0A0-98E8FC2B5E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3B7A07-C1E6-46E5-AA12-D7E62454153D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13556,7 +13556,8 @@
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="93">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-9.1492186931267622E-2</v>
       </c>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
@@ -13618,7 +13619,8 @@
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="93">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-3.6630747396996691E-2</v>
       </c>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
@@ -14121,7 +14123,8 @@
       </c>
       <c r="I20" s="27"/>
       <c r="J20" s="93">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>-3.2210497290905374E-2</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
@@ -14164,7 +14167,8 @@
       </c>
       <c r="I21" s="27"/>
       <c r="J21" s="93">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>-3.054309712927282E-2</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
@@ -14541,7 +14545,8 @@
       </c>
       <c r="I29" s="27"/>
       <c r="J29" s="93">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-7.3325429420576533E-3</v>
       </c>
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
@@ -14616,7 +14621,8 @@
       </c>
       <c r="I30" s="27"/>
       <c r="J30" s="93">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-3.2086171243230267E-3</v>
       </c>
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>

</xml_diff>

<commit_message>
Update HLI 3.5 limits
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4ED4CB5-F7EF-400B-8D2C-3CEB88439AB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15E77F3-8935-4FD2-B638-C31373A21C05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="333">
   <si>
     <t>UC_N</t>
   </si>
@@ -1188,7 +1188,19 @@
     <t>RSDSH_Det-AB,RSDSH_Det-C,RSDSH_Det-D,RSDSH_Det-E,RSDSH_Det-F,RSDSH_Det-G</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>&lt;3.5</t>
+  </si>
+  <si>
+    <t>&lt;4</t>
+  </si>
+  <si>
+    <t>&lt;4.5</t>
+  </si>
+  <si>
+    <t>&lt;3</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1216,7 @@
     <numFmt numFmtId="168" formatCode="0.000"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1357,6 +1369,12 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1996,7 +2014,6 @@
     <xf numFmtId="3" fontId="8" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="14" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2023,15 +2040,16 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="21" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -2555,16 +2573,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>132292</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>79376</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>153458</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>445558</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>105229</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>392642</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>136979</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2594,8 +2612,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="29688367" y="3101975"/>
-          <a:ext cx="2142066" cy="2089604"/>
+          <a:off x="33099376" y="2756958"/>
+          <a:ext cx="2154766" cy="2100188"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3427,12 +3445,12 @@
       <c r="Z15" s="46"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="96" t="s">
+      <c r="A16" s="95" t="s">
         <v>253</v>
       </c>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
       <c r="E16" s="47"/>
       <c r="F16" s="47"/>
       <c r="G16" s="48"/>
@@ -3516,11 +3534,11 @@
       <c r="A19" s="52" t="s">
         <v>254</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="94" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
       <c r="E19" s="53"/>
       <c r="F19" s="53"/>
       <c r="G19" s="54"/>
@@ -3548,11 +3566,11 @@
       <c r="A20" s="52" t="s">
         <v>255</v>
       </c>
-      <c r="B20" s="95" t="s">
+      <c r="B20" s="94" t="s">
         <v>266</v>
       </c>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
       <c r="E20" s="53"/>
       <c r="F20" s="53"/>
       <c r="G20" s="54"/>
@@ -3640,11 +3658,11 @@
       <c r="A23" s="52" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="95" t="s">
+      <c r="B23" s="94" t="s">
         <v>265</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
       <c r="E23" s="46"/>
       <c r="F23" s="46"/>
       <c r="G23" s="46"/>
@@ -3730,11 +3748,11 @@
       <c r="A26" s="52" t="s">
         <v>258</v>
       </c>
-      <c r="B26" s="95" t="s">
+      <c r="B26" s="94" t="s">
         <v>265</v>
       </c>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
       <c r="E26" s="46"/>
       <c r="F26" s="46"/>
       <c r="G26" s="46"/>
@@ -3850,11 +3868,11 @@
       <c r="A30" s="52" t="s">
         <v>260</v>
       </c>
-      <c r="B30" s="97" t="s">
+      <c r="B30" s="96" t="s">
         <v>261</v>
       </c>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
       <c r="E30" s="57"/>
       <c r="F30" s="57"/>
       <c r="G30" s="46"/>
@@ -3882,11 +3900,11 @@
       <c r="A31" s="52" t="s">
         <v>262</v>
       </c>
-      <c r="B31" s="95" t="s">
+      <c r="B31" s="94" t="s">
         <v>263</v>
       </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="94"/>
       <c r="E31" s="57"/>
       <c r="F31" s="57"/>
       <c r="G31" s="46"/>
@@ -13030,10 +13048,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:AM200"/>
+  <dimension ref="A1:AU200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K172" sqref="K172"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13182,31 +13200,31 @@
         <v>11</v>
       </c>
       <c r="O5" s="44"/>
-      <c r="P5" s="100" t="s">
+      <c r="P5" s="98" t="s">
         <v>277</v>
       </c>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
       <c r="S5" s="44"/>
-      <c r="T5" s="100" t="s">
+      <c r="T5" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="U5" s="100"/>
-      <c r="V5" s="100"/>
-      <c r="W5" s="100"/>
-      <c r="X5" s="100"/>
+      <c r="U5" s="98"/>
+      <c r="V5" s="98"/>
+      <c r="W5" s="98"/>
+      <c r="X5" s="98"/>
       <c r="Y5" s="44"/>
-      <c r="Z5" s="100" t="s">
+      <c r="Z5" s="98" t="s">
         <v>279</v>
       </c>
-      <c r="AA5" s="100"/>
-      <c r="AB5" s="100"/>
+      <c r="AA5" s="98"/>
+      <c r="AB5" s="98"/>
       <c r="AC5" s="44"/>
-      <c r="AD5" s="100" t="s">
+      <c r="AD5" s="98" t="s">
         <v>280</v>
       </c>
-      <c r="AE5" s="100"/>
-      <c r="AF5" s="100"/>
+      <c r="AE5" s="98"/>
+      <c r="AF5" s="98"/>
       <c r="AG5" s="44"/>
       <c r="AH5" s="44"/>
       <c r="AI5" s="44"/>
@@ -13305,15 +13323,13 @@
         <v>2019</v>
       </c>
       <c r="I7" s="27"/>
-      <c r="J7" s="93">
-        <f>IF(N7="Y",0,-(T33))</f>
-        <v>0</v>
+      <c r="J7" s="92">
+        <f>IF(N7="Y",0,-(X33))</f>
+        <v>-0.99999998312382343</v>
       </c>
       <c r="K7" s="27"/>
       <c r="L7" s="27"/>
-      <c r="N7" t="s">
-        <v>328</v>
-      </c>
+      <c r="N7" s="44"/>
       <c r="O7" s="66" t="s">
         <v>286</v>
       </c>
@@ -13381,15 +13397,12 @@
         <v>2019</v>
       </c>
       <c r="I8" s="27"/>
-      <c r="J8" s="93">
-        <f t="shared" ref="J8:J12" si="0">IF(N8="Y",0,-(T34))</f>
-        <v>0</v>
+      <c r="J8" s="92">
+        <f t="shared" ref="J8:J12" si="0">IF(N8="Y",0,-(X34))</f>
+        <v>-0.99417194789886376</v>
       </c>
       <c r="K8" s="27"/>
       <c r="L8" s="27"/>
-      <c r="N8" s="44" t="s">
-        <v>328</v>
-      </c>
       <c r="O8" s="71" t="s">
         <v>288</v>
       </c>
@@ -13447,15 +13460,12 @@
         <v>2019</v>
       </c>
       <c r="I9" s="27"/>
-      <c r="J9" s="93">
+      <c r="J9" s="92">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.92710242952401201</v>
       </c>
       <c r="K9" s="27"/>
       <c r="L9" s="27"/>
-      <c r="N9" s="44" t="s">
-        <v>328</v>
-      </c>
       <c r="O9" s="76" t="s">
         <v>290</v>
       </c>
@@ -13513,15 +13523,12 @@
         <v>2019</v>
       </c>
       <c r="I10" s="27"/>
-      <c r="J10" s="93">
+      <c r="J10" s="92">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.87051976694100974</v>
       </c>
       <c r="K10" s="27"/>
       <c r="L10" s="27"/>
-      <c r="N10" s="44" t="s">
-        <v>328</v>
-      </c>
       <c r="O10" s="71" t="s">
         <v>292</v>
       </c>
@@ -13579,15 +13586,12 @@
         <v>2019</v>
       </c>
       <c r="I11" s="27"/>
-      <c r="J11" s="93">
+      <c r="J11" s="92">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.58254904641534866</v>
       </c>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
-      <c r="N11" s="44" t="s">
-        <v>328</v>
-      </c>
       <c r="O11" s="76" t="s">
         <v>294</v>
       </c>
@@ -13645,20 +13649,17 @@
         <v>2019</v>
       </c>
       <c r="I12" s="27"/>
-      <c r="J12" s="93">
+      <c r="J12" s="92">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.20397754353748057</v>
       </c>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
-      <c r="N12" s="44" t="s">
-        <v>328</v>
-      </c>
-      <c r="P12" s="101" t="s">
+      <c r="P12" s="99" t="s">
         <v>296</v>
       </c>
-      <c r="Q12" s="101"/>
-      <c r="R12" s="101"/>
+      <c r="Q12" s="99"/>
+      <c r="R12" s="99"/>
       <c r="T12" s="71" t="s">
         <v>297</v>
       </c>
@@ -13901,7 +13902,7 @@
         <v>6.0039999999999996</v>
       </c>
       <c r="AC15" s="44"/>
-      <c r="AD15" s="94">
+      <c r="AD15" s="93">
         <f>AVERAGE(AE15:AF15)</f>
         <v>1.5565</v>
       </c>
@@ -13932,16 +13933,14 @@
         <v>2019</v>
       </c>
       <c r="I16" s="27"/>
-      <c r="J16" s="93">
-        <f>IF(N7="Y",0,-(AA33))</f>
-        <v>0</v>
+      <c r="J16" s="92">
+        <f>IF(N16="Y",0,-(AH33))</f>
+        <v>-0.99973940839121955</v>
       </c>
       <c r="K16" s="27"/>
       <c r="L16" s="27"/>
       <c r="M16" s="44"/>
-      <c r="N16" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N16" s="44"/>
       <c r="O16" s="76" t="s">
         <v>290</v>
       </c>
@@ -13986,7 +13985,7 @@
       <c r="AL16" s="44"/>
       <c r="AM16" s="44"/>
     </row>
-    <row r="17" spans="2:39">
+    <row r="17" spans="2:47">
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
       <c r="D17" s="27" t="s">
@@ -13999,16 +13998,14 @@
         <v>2019</v>
       </c>
       <c r="I17" s="27"/>
-      <c r="J17" s="93">
-        <f t="shared" ref="J17:J21" si="1">IF(N8="Y",0,-(AA34))</f>
-        <v>0</v>
+      <c r="J17" s="92">
+        <f>IF(N17="Y",0,-(AH34))</f>
+        <v>-0.99191173064402915</v>
       </c>
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
       <c r="M17" s="44"/>
-      <c r="N17" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N17" s="44"/>
       <c r="O17" s="71" t="s">
         <v>292</v>
       </c>
@@ -14043,7 +14040,7 @@
       <c r="AL17" s="44"/>
       <c r="AM17" s="44"/>
     </row>
-    <row r="18" spans="2:39">
+    <row r="18" spans="2:47">
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
       <c r="D18" s="27" t="s">
@@ -14056,16 +14053,14 @@
         <v>2019</v>
       </c>
       <c r="I18" s="27"/>
-      <c r="J18" s="93">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="J18" s="92">
+        <f t="shared" ref="J17:J21" si="1">IF(N18="Y",0,-(AH35))</f>
+        <v>-0.8470018886690438</v>
       </c>
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
       <c r="M18" s="44"/>
-      <c r="N18" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N18" s="44"/>
       <c r="O18" s="76" t="s">
         <v>294</v>
       </c>
@@ -14100,7 +14095,7 @@
       <c r="AL18" s="44"/>
       <c r="AM18" s="44"/>
     </row>
-    <row r="19" spans="2:39">
+    <row r="19" spans="2:47">
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
       <c r="D19" s="27" t="s">
@@ -14113,16 +14108,14 @@
         <v>2019</v>
       </c>
       <c r="I19" s="27"/>
-      <c r="J19" s="93">
+      <c r="J19" s="92">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.49480783925100147</v>
       </c>
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
       <c r="M19" s="44"/>
-      <c r="N19" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N19" s="44"/>
       <c r="O19" s="44"/>
       <c r="P19" s="44"/>
       <c r="Q19" s="44"/>
@@ -14151,7 +14144,7 @@
       <c r="AL19" s="44"/>
       <c r="AM19" s="44"/>
     </row>
-    <row r="20" spans="2:39">
+    <row r="20" spans="2:47">
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
       <c r="D20" s="27" t="s">
@@ -14164,16 +14157,14 @@
         <v>2019</v>
       </c>
       <c r="I20" s="27"/>
-      <c r="J20" s="93">
+      <c r="J20" s="92">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.29645675583092174</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
       <c r="M20" s="44"/>
-      <c r="N20" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N20" s="44"/>
       <c r="O20" s="44"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
@@ -14200,7 +14191,7 @@
       <c r="AL20" s="44"/>
       <c r="AM20" s="44"/>
     </row>
-    <row r="21" spans="2:39">
+    <row r="21" spans="2:47">
       <c r="D21" s="27" t="s">
         <v>317</v>
       </c>
@@ -14211,16 +14202,14 @@
         <v>2019</v>
       </c>
       <c r="I21" s="27"/>
-      <c r="J21" s="93">
+      <c r="J21" s="92">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.16841130134712209</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
       <c r="M21" s="44"/>
-      <c r="N21" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N21" s="44"/>
       <c r="O21" s="44"/>
       <c r="P21" s="44"/>
       <c r="Q21" s="44"/>
@@ -14249,7 +14238,7 @@
       <c r="AL21" s="44"/>
       <c r="AM21" s="44"/>
     </row>
-    <row r="22" spans="2:39">
+    <row r="22" spans="2:47">
       <c r="D22" s="27" t="s">
         <v>206</v>
       </c>
@@ -14293,7 +14282,7 @@
       <c r="AL22" s="44"/>
       <c r="AM22" s="44"/>
     </row>
-    <row r="23" spans="2:39">
+    <row r="23" spans="2:47">
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
@@ -14334,7 +14323,7 @@
       <c r="AL23" s="44"/>
       <c r="AM23" s="44"/>
     </row>
-    <row r="24" spans="2:39">
+    <row r="24" spans="2:47">
       <c r="B24" t="s">
         <v>93</v>
       </c>
@@ -14386,7 +14375,7 @@
       <c r="AL24" s="44"/>
       <c r="AM24" s="44"/>
     </row>
-    <row r="25" spans="2:39">
+    <row r="25" spans="2:47">
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="27" t="s">
@@ -14399,16 +14388,14 @@
         <v>2019</v>
       </c>
       <c r="I25" s="27"/>
-      <c r="J25" s="93">
-        <f>IF(N7="Y",0,-(AH33))</f>
-        <v>0</v>
+      <c r="J25" s="92">
+        <f>IF(N25="Y",0,-(AR33))</f>
+        <v>-0.99997215963294783</v>
       </c>
       <c r="K25" s="27"/>
       <c r="L25" s="27"/>
       <c r="M25" s="44"/>
-      <c r="N25" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N25" s="44"/>
       <c r="O25" s="44"/>
       <c r="P25" s="44"/>
       <c r="Q25" s="44"/>
@@ -14435,7 +14422,7 @@
       <c r="AL25" s="44"/>
       <c r="AM25" s="44"/>
     </row>
-    <row r="26" spans="2:39">
+    <row r="26" spans="2:47">
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
       <c r="D26" s="27" t="s">
@@ -14448,16 +14435,14 @@
         <v>2019</v>
       </c>
       <c r="I26" s="27"/>
-      <c r="J26" s="93">
-        <f t="shared" ref="J26:J30" si="2">IF(N8="Y",0,-(AH34))</f>
-        <v>0</v>
+      <c r="J26" s="92">
+        <f t="shared" ref="J26:J30" si="2">IF(N26="Y",0,-(AR34))</f>
+        <v>-0.98600872265415918</v>
       </c>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
       <c r="M26" s="44"/>
-      <c r="N26" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N26" s="44"/>
       <c r="O26" s="44"/>
       <c r="P26" s="44"/>
       <c r="Q26" s="44"/>
@@ -14484,7 +14469,7 @@
       <c r="AL26" s="44"/>
       <c r="AM26" s="44"/>
     </row>
-    <row r="27" spans="2:39">
+    <row r="27" spans="2:47">
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
       <c r="D27" s="27" t="s">
@@ -14497,43 +14482,97 @@
         <v>2019</v>
       </c>
       <c r="I27" s="27"/>
-      <c r="J27" s="93">
+      <c r="J27" s="92">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.73196550526672355</v>
       </c>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
       <c r="M27" s="44"/>
-      <c r="N27" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N27" s="44"/>
       <c r="O27" s="44"/>
       <c r="P27" s="44"/>
       <c r="Q27" s="44"/>
       <c r="R27" s="44"/>
       <c r="S27" s="44"/>
-      <c r="T27" s="44"/>
-      <c r="U27" s="44"/>
-      <c r="V27" s="44"/>
-      <c r="W27" s="44"/>
-      <c r="X27" s="44"/>
-      <c r="Y27" s="44"/>
-      <c r="Z27" s="44"/>
-      <c r="AA27" s="44"/>
+      <c r="T27" s="44">
+        <v>2</v>
+      </c>
+      <c r="U27" s="44">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V27" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="W27" s="44">
+        <v>3</v>
+      </c>
+      <c r="X27" s="44">
+        <v>3.5</v>
+      </c>
+      <c r="Y27" s="44">
+        <v>4</v>
+      </c>
+      <c r="Z27" s="44">
+        <v>4.5</v>
+      </c>
+      <c r="AA27" s="44">
+        <v>0</v>
+      </c>
       <c r="AB27" s="44"/>
       <c r="AC27" s="44"/>
-      <c r="AD27" s="44"/>
-      <c r="AE27" s="44"/>
-      <c r="AF27" s="44"/>
-      <c r="AG27" s="44"/>
-      <c r="AH27" s="44"/>
-      <c r="AI27" s="44"/>
-      <c r="AJ27" s="44"/>
-      <c r="AK27" s="44"/>
+      <c r="AD27" s="44">
+        <v>2</v>
+      </c>
+      <c r="AE27" s="44">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AF27" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="AG27" s="44">
+        <v>3</v>
+      </c>
+      <c r="AH27" s="44">
+        <v>3.5</v>
+      </c>
+      <c r="AI27" s="44">
+        <v>4</v>
+      </c>
+      <c r="AJ27" s="44">
+        <v>4.5</v>
+      </c>
+      <c r="AK27" s="44">
+        <v>0</v>
+      </c>
       <c r="AL27" s="44"/>
       <c r="AM27" s="44"/>
-    </row>
-    <row r="28" spans="2:39" ht="15.75" thickBot="1">
+      <c r="AN27" s="44">
+        <v>2</v>
+      </c>
+      <c r="AO27" s="44">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AP27" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="AQ27" s="44">
+        <v>3</v>
+      </c>
+      <c r="AR27" s="44">
+        <v>3.5</v>
+      </c>
+      <c r="AS27" s="44">
+        <v>4</v>
+      </c>
+      <c r="AT27" s="44">
+        <v>4.5</v>
+      </c>
+      <c r="AU27" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:47" ht="15.75" thickBot="1">
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
       <c r="D28" s="27" t="s">
@@ -14546,49 +14585,55 @@
         <v>2019</v>
       </c>
       <c r="I28" s="27"/>
-      <c r="J28" s="93">
+      <c r="J28" s="92">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.38127737390844418</v>
       </c>
       <c r="K28" s="27"/>
       <c r="L28" s="27"/>
       <c r="M28" s="44"/>
-      <c r="N28" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N28" s="44"/>
       <c r="O28" s="44"/>
       <c r="P28" s="44"/>
       <c r="Q28" s="44"/>
       <c r="R28" s="44"/>
       <c r="S28" s="44"/>
-      <c r="T28" s="98" t="s">
+      <c r="T28" s="97" t="s">
         <v>281</v>
       </c>
-      <c r="U28" s="99"/>
-      <c r="V28" s="99"/>
-      <c r="W28" s="99"/>
-      <c r="X28" s="99"/>
-      <c r="Y28" s="44"/>
-      <c r="Z28" s="44"/>
-      <c r="AA28" s="98" t="s">
+      <c r="U28" s="100"/>
+      <c r="V28" s="100"/>
+      <c r="W28" s="100"/>
+      <c r="X28" s="100"/>
+      <c r="Y28" s="100"/>
+      <c r="Z28" s="100"/>
+      <c r="AA28" s="100"/>
+      <c r="AB28" s="44"/>
+      <c r="AC28" s="100" t="s">
         <v>282</v>
       </c>
-      <c r="AB28" s="99"/>
-      <c r="AC28" s="99"/>
-      <c r="AD28" s="99"/>
-      <c r="AE28" s="99"/>
-      <c r="AF28" s="44"/>
-      <c r="AG28" s="44"/>
-      <c r="AH28" s="98" t="s">
+      <c r="AD28" s="100"/>
+      <c r="AE28" s="100"/>
+      <c r="AF28" s="100"/>
+      <c r="AG28" s="100"/>
+      <c r="AH28" s="100"/>
+      <c r="AI28" s="100"/>
+      <c r="AJ28" s="100"/>
+      <c r="AK28" s="100"/>
+      <c r="AL28" s="44"/>
+      <c r="AM28" s="97" t="s">
         <v>283</v>
       </c>
-      <c r="AI28" s="99"/>
-      <c r="AJ28" s="99"/>
-      <c r="AK28" s="99"/>
-      <c r="AL28" s="99"/>
-      <c r="AM28" s="44"/>
-    </row>
-    <row r="29" spans="2:39" ht="15.75" thickBot="1">
+      <c r="AN28" s="100"/>
+      <c r="AO28" s="100"/>
+      <c r="AP28" s="100"/>
+      <c r="AQ28" s="100"/>
+      <c r="AR28" s="100"/>
+      <c r="AS28" s="100"/>
+      <c r="AT28" s="100"/>
+      <c r="AU28" s="100"/>
+    </row>
+    <row r="29" spans="2:47" ht="15.75" thickBot="1">
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
       <c r="D29" s="27" t="s">
@@ -14601,16 +14646,14 @@
         <v>2019</v>
       </c>
       <c r="I29" s="27"/>
-      <c r="J29" s="93">
+      <c r="J29" s="92">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.16389933245411942</v>
       </c>
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
       <c r="M29" s="44"/>
-      <c r="N29" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N29" s="44"/>
       <c r="O29" s="44"/>
       <c r="P29" s="44"/>
       <c r="Q29" s="44"/>
@@ -14626,48 +14669,73 @@
         <v>290</v>
       </c>
       <c r="W29" s="71" t="s">
-        <v>292</v>
-      </c>
-      <c r="X29" s="76" t="s">
-        <v>294</v>
-      </c>
-      <c r="Y29" s="44"/>
-      <c r="Z29" s="44"/>
-      <c r="AA29" s="66" t="s">
+        <v>331</v>
+      </c>
+      <c r="X29" s="71" t="s">
+        <v>328</v>
+      </c>
+      <c r="Y29" s="71" t="s">
+        <v>329</v>
+      </c>
+      <c r="Z29" s="71" t="s">
+        <v>330</v>
+      </c>
+      <c r="AA29" s="71" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB29" s="44"/>
+      <c r="AC29" s="44"/>
+      <c r="AD29" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="AB29" s="71" t="s">
+      <c r="AE29" s="71" t="s">
         <v>288</v>
       </c>
-      <c r="AC29" s="76" t="s">
+      <c r="AF29" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="AD29" s="71" t="s">
-        <v>292</v>
-      </c>
-      <c r="AE29" s="76" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF29" s="44"/>
-      <c r="AG29" s="44"/>
-      <c r="AH29" s="66" t="s">
+      <c r="AG29" s="71" t="s">
+        <v>331</v>
+      </c>
+      <c r="AH29" s="71" t="s">
+        <v>328</v>
+      </c>
+      <c r="AI29" s="71" t="s">
+        <v>329</v>
+      </c>
+      <c r="AJ29" s="71" t="s">
+        <v>330</v>
+      </c>
+      <c r="AK29" s="71" t="s">
+        <v>332</v>
+      </c>
+      <c r="AM29" s="44"/>
+      <c r="AN29" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="AI29" s="71" t="s">
+      <c r="AO29" s="71" t="s">
         <v>288</v>
       </c>
-      <c r="AJ29" s="76" t="s">
+      <c r="AP29" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="AK29" s="71" t="s">
-        <v>292</v>
-      </c>
-      <c r="AL29" s="76" t="s">
-        <v>294</v>
-      </c>
-      <c r="AM29" s="44"/>
-    </row>
-    <row r="30" spans="2:39">
+      <c r="AQ29" s="71" t="s">
+        <v>331</v>
+      </c>
+      <c r="AR29" s="71" t="s">
+        <v>328</v>
+      </c>
+      <c r="AS29" s="71" t="s">
+        <v>329</v>
+      </c>
+      <c r="AT29" s="71" t="s">
+        <v>330</v>
+      </c>
+      <c r="AU29" s="71" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30" spans="2:47">
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
       <c r="D30" s="27" t="s">
@@ -14680,16 +14748,14 @@
         <v>2019</v>
       </c>
       <c r="I30" s="27"/>
-      <c r="J30" s="93">
+      <c r="J30" s="92">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-4.4138172035112347E-2</v>
       </c>
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
       <c r="M30" s="44"/>
-      <c r="N30" s="44" t="s">
-        <v>328</v>
-      </c>
+      <c r="N30" s="44"/>
       <c r="O30" s="44"/>
       <c r="P30" s="44"/>
       <c r="Q30" s="44"/>
@@ -14697,77 +14763,109 @@
       <c r="S30" s="66" t="s">
         <v>287</v>
       </c>
-      <c r="T30" s="88">
-        <f t="shared" ref="T30:T38" si="3">_xlfn.NORM.DIST(2,Z7,AD7,TRUE)</f>
+      <c r="T30" s="101">
+        <f>_xlfn.NORM.DIST($T$27,Z7,AD7,TRUE)</f>
         <v>0.99986614214614677</v>
       </c>
-      <c r="U30" s="88">
-        <f t="shared" ref="U30:U38" si="4">_xlfn.NORM.DIST(2.3,Z7,AD7,TRUE)</f>
+      <c r="U30" s="101">
+        <f>_xlfn.NORM.DIST($U$27,Z7,AD7,TRUE)</f>
         <v>0.99999895018069218</v>
       </c>
-      <c r="V30" s="88">
-        <f t="shared" ref="V30:V38" si="5">_xlfn.NORM.DIST(2.5,Z7,AD7,TRUE)</f>
+      <c r="V30" s="101">
+        <f>_xlfn.NORM.DIST($V$27,Z7,AD7,TRUE)</f>
         <v>0.99999997827100517</v>
       </c>
-      <c r="W30" s="88">
-        <f t="shared" ref="W30:W38" si="6">_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
-        <v>0.99999999973303144</v>
-      </c>
-      <c r="X30" s="88">
-        <f t="shared" ref="X30:X38" si="7">1-_xlfn.NORM.DIST(2.7,Z7,AD7,TRUE)</f>
-        <v>2.6696855837116118E-10</v>
-      </c>
-      <c r="Y30" s="44"/>
-      <c r="Z30" s="66" t="s">
+      <c r="W30" s="101">
+        <f>_xlfn.NORM.DIST($W$27,Z7,AD7,TRUE)</f>
+        <v>0.99999999999986411</v>
+      </c>
+      <c r="X30" s="101">
+        <f>_xlfn.NORM.DIST($X$27,Z7,AD7,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="Y30" s="101">
+        <f>_xlfn.NORM.DIST($Y$27,Z7,AD7,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="Z30" s="101">
+        <f>_xlfn.NORM.DIST($Z$27,Z7,AD7,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="AA30" s="101">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="44"/>
+      <c r="AC30" s="66" t="s">
         <v>287</v>
       </c>
-      <c r="AA30" s="88">
-        <f t="shared" ref="AA30:AA38" si="8">_xlfn.NORM.DIST(2,AA7,AE7,TRUE)</f>
+      <c r="AD30" s="101">
+        <f>_xlfn.NORM.DIST($AD$27,AA7,AE7,TRUE)</f>
         <v>0.99358230344905218</v>
       </c>
-      <c r="AB30" s="88">
-        <f t="shared" ref="AB30:AB38" si="9">_xlfn.NORM.DIST(2.3,AA7,AE7,TRUE)</f>
+      <c r="AE30" s="101">
+        <f>_xlfn.NORM.DIST($AE$27,AA7,AE7,TRUE)</f>
         <v>0.99961797061500135</v>
       </c>
-      <c r="AC30" s="88">
-        <f t="shared" ref="AC30:AC38" si="10">_xlfn.NORM.DIST(2.5,AA7,AE7,TRUE)</f>
+      <c r="AF30" s="101">
+        <f>_xlfn.NORM.DIST($AF$27,AA7,AE7,TRUE)</f>
         <v>0.99996097211163748</v>
       </c>
-      <c r="AD30" s="88">
-        <f t="shared" ref="AD30:AD38" si="11">_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
-        <v>0.99999712102252392</v>
-      </c>
-      <c r="AE30" s="88">
-        <f t="shared" ref="AE30:AE38" si="12">1-_xlfn.NORM.DIST(2.7,AA7,AE7,TRUE)</f>
-        <v>2.8789774760840103E-6</v>
-      </c>
-      <c r="AF30" s="44"/>
-      <c r="AG30" s="66" t="s">
+      <c r="AG30" s="101">
+        <f>_xlfn.NORM.DIST($AG$27,AA7,AE7,TRUE)</f>
+        <v>0.99999996888648002</v>
+      </c>
+      <c r="AH30" s="101">
+        <f>_xlfn.NORM.DIST($AH$27,AA7,AE7,TRUE)</f>
+        <v>0.9999999999968846</v>
+      </c>
+      <c r="AI30" s="101">
+        <f>_xlfn.NORM.DIST($AI$27,AA7,AE7,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ30" s="101">
+        <f>_xlfn.NORM.DIST($AJ$27,AA7,AE7,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="AK30" s="101">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="44"/>
+      <c r="AM30" s="66" t="s">
         <v>287</v>
       </c>
-      <c r="AH30" s="44">
-        <f t="shared" ref="AH30:AH38" si="13">_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
+      <c r="AN30" s="101">
+        <f>_xlfn.NORM.DIST($AN$27,AB7,AF7,TRUE)</f>
         <v>0.99867076285153633</v>
       </c>
-      <c r="AI30" s="44">
-        <f t="shared" ref="AI30:AI38" si="14">_xlfn.NORM.DIST(2.3,AB7,AF7,TRUE)</f>
+      <c r="AO30" s="101">
+        <f>_xlfn.NORM.DIST($AO$27,AB7,AF7,TRUE)</f>
         <v>0.99999490602709384</v>
       </c>
-      <c r="AJ30" s="44">
-        <f t="shared" ref="AJ30:AJ38" si="15">_xlfn.NORM.DIST(2.5,AB7,AF7,TRUE)</f>
+      <c r="AP30" s="101">
+        <f>_xlfn.NORM.DIST($AP$27,AB7,AF7,TRUE)</f>
         <v>0.99999995653338158</v>
       </c>
-      <c r="AK30" s="44">
-        <f t="shared" ref="AK30:AK38" si="16">_xlfn.NORM.DIST(2.7,AB7,AF7,TRUE)</f>
-        <v>0.99999999984236743</v>
-      </c>
-      <c r="AL30" s="44">
-        <f t="shared" ref="AL30:AL38" si="17">1-_xlfn.NORM.DIST(2,AB7,AF7,TRUE)</f>
-        <v>1.3292371484636689E-3</v>
-      </c>
-      <c r="AM30" s="44"/>
-    </row>
-    <row r="31" spans="2:39">
+      <c r="AQ30" s="101">
+        <f>_xlfn.NORM.DIST($AQ$27,AB7,AF7,TRUE)</f>
+        <v>0.99999999999999312</v>
+      </c>
+      <c r="AR30" s="101">
+        <f>_xlfn.NORM.DIST($AR$27,AB7,AF7,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="AS30" s="101">
+        <f>_xlfn.NORM.DIST($AS$27,AB7,AF7,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="AT30" s="101">
+        <f>_xlfn.NORM.DIST($AT$27,AB7,AF7,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="AU30" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:47">
       <c r="D31" s="27" t="s">
         <v>206</v>
       </c>
@@ -14792,77 +14890,109 @@
       <c r="S31" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="T31" s="88">
-        <f t="shared" si="3"/>
+      <c r="T31" s="101">
+        <f t="shared" ref="T31:T38" si="3">_xlfn.NORM.DIST($T$27,Z8,AD8,TRUE)</f>
         <v>0.96885301500182108</v>
       </c>
-      <c r="U31" s="88">
-        <f t="shared" si="4"/>
+      <c r="U31" s="101">
+        <f t="shared" ref="U31:U38" si="4">_xlfn.NORM.DIST($U$27,Z8,AD8,TRUE)</f>
         <v>0.99736560266376562</v>
       </c>
-      <c r="V31" s="88">
-        <f t="shared" si="5"/>
+      <c r="V31" s="101">
+        <f t="shared" ref="V31:V38" si="5">_xlfn.NORM.DIST($V$27,Z8,AD8,TRUE)</f>
         <v>0.99967208422117826</v>
       </c>
-      <c r="W31" s="88">
-        <f t="shared" si="6"/>
-        <v>0.99997147495584515</v>
-      </c>
-      <c r="X31" s="88">
-        <f t="shared" si="7"/>
-        <v>2.8525044154847912E-5</v>
-      </c>
-      <c r="Y31" s="44"/>
-      <c r="Z31" s="71" t="s">
+      <c r="W31" s="101">
+        <f t="shared" ref="W31:W38" si="6">_xlfn.NORM.DIST($W$27,Z8,AD8,TRUE)</f>
+        <v>0.99999963010770987</v>
+      </c>
+      <c r="X31" s="101">
+        <f t="shared" ref="X31:X38" si="7">_xlfn.NORM.DIST($X$27,Z8,AD8,TRUE)</f>
+        <v>0.99999999995815858</v>
+      </c>
+      <c r="Y31" s="101">
+        <f t="shared" ref="Y31:Y38" si="8">_xlfn.NORM.DIST($Y$27,Z8,AD8,TRUE)</f>
+        <v>0.99999999999999956</v>
+      </c>
+      <c r="Z31" s="101">
+        <f t="shared" ref="Z31:Z38" si="9">_xlfn.NORM.DIST($Z$27,Z8,AD8,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="AA31" s="101">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="44"/>
+      <c r="AC31" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="AA31" s="88">
-        <f t="shared" si="8"/>
+      <c r="AD31" s="101">
+        <f t="shared" ref="AD31:AD38" si="10">_xlfn.NORM.DIST($AD$27,AA8,AE8,TRUE)</f>
         <v>0.7694627396275191</v>
       </c>
-      <c r="AB31" s="88">
-        <f t="shared" si="9"/>
+      <c r="AE31" s="101">
+        <f t="shared" ref="AE31:AE38" si="11">_xlfn.NORM.DIST($AE$27,AA8,AE8,TRUE)</f>
         <v>0.92091247414921895</v>
       </c>
-      <c r="AC31" s="88">
-        <f t="shared" si="10"/>
+      <c r="AF31" s="101">
+        <f t="shared" ref="AF31:AF38" si="12">_xlfn.NORM.DIST($AF$27,AA8,AE8,TRUE)</f>
         <v>0.96860489728090593</v>
       </c>
-      <c r="AD31" s="88">
-        <f t="shared" si="11"/>
-        <v>0.98955903282288238</v>
-      </c>
-      <c r="AE31" s="88">
-        <f t="shared" si="12"/>
-        <v>1.0440967177117622E-2</v>
-      </c>
-      <c r="AF31" s="44"/>
-      <c r="AG31" s="71" t="s">
+      <c r="AG31" s="101">
+        <f t="shared" ref="AG31:AG38" si="13">_xlfn.NORM.DIST($AG$27,AA8,AE8,TRUE)</f>
+        <v>0.99857871934570608</v>
+      </c>
+      <c r="AH31" s="101">
+        <f t="shared" ref="AH31:AH38" si="14">_xlfn.NORM.DIST($AH$27,AA8,AE8,TRUE)</f>
+        <v>0.99998003334500252</v>
+      </c>
+      <c r="AI31" s="101">
+        <f t="shared" ref="AI31:AI38" si="15">_xlfn.NORM.DIST($AI$27,AA8,AE8,TRUE)</f>
+        <v>0.99999991591209203</v>
+      </c>
+      <c r="AJ31" s="101">
+        <f t="shared" ref="AJ31:AJ38" si="16">_xlfn.NORM.DIST($AJ$27,AA8,AE8,TRUE)</f>
+        <v>0.99999999989582478</v>
+      </c>
+      <c r="AK31" s="101">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="44"/>
+      <c r="AM31" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="AH31" s="44">
-        <f t="shared" si="13"/>
+      <c r="AN31" s="101">
+        <f t="shared" ref="AN31:AN38" si="17">_xlfn.NORM.DIST($AN$27,AB8,AF8,TRUE)</f>
         <v>0.6130931526036395</v>
       </c>
-      <c r="AI31" s="44">
-        <f t="shared" si="14"/>
+      <c r="AO31" s="101">
+        <f t="shared" ref="AO31:AO38" si="18">_xlfn.NORM.DIST($AO$27,AB8,AF8,TRUE)</f>
         <v>0.87842619586393023</v>
       </c>
-      <c r="AJ31" s="44">
-        <f t="shared" si="15"/>
+      <c r="AP31" s="101">
+        <f t="shared" ref="AP31:AP38" si="19">_xlfn.NORM.DIST($AP$27,AB8,AF8,TRUE)</f>
         <v>0.9602560960127382</v>
       </c>
-      <c r="AK31" s="44">
-        <f t="shared" si="16"/>
-        <v>0.99036267162555125</v>
-      </c>
-      <c r="AL31" s="44">
-        <f t="shared" si="17"/>
-        <v>0.3869068473963605</v>
-      </c>
-      <c r="AM31" s="44"/>
-    </row>
-    <row r="32" spans="2:39" s="44" customFormat="1">
+      <c r="AQ31" s="101">
+        <f t="shared" ref="AQ31:AQ38" si="20">_xlfn.NORM.DIST($AQ$27,AB8,AF8,TRUE)</f>
+        <v>0.99935891586967851</v>
+      </c>
+      <c r="AR31" s="101">
+        <f t="shared" ref="AR31:AR38" si="21">_xlfn.NORM.DIST($AR$27,AB8,AF8,TRUE)</f>
+        <v>0.99999860849411715</v>
+      </c>
+      <c r="AS31" s="101">
+        <f t="shared" ref="AS31:AS38" si="22">_xlfn.NORM.DIST($AS$27,AB8,AF8,TRUE)</f>
+        <v>0.99999999961862751</v>
+      </c>
+      <c r="AT31" s="101">
+        <f t="shared" ref="AT31:AT38" si="23">_xlfn.NORM.DIST($AT$27,AB8,AF8,TRUE)</f>
+        <v>0.99999999999998723</v>
+      </c>
+      <c r="AU31" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:47" s="44" customFormat="1">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32" s="28"/>
@@ -14884,74 +15014,107 @@
       <c r="S32" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="T32" s="88">
+      <c r="T32" s="101">
         <f t="shared" si="3"/>
         <v>0.93969745300565943</v>
       </c>
-      <c r="U32" s="88">
+      <c r="U32" s="101">
         <f t="shared" si="4"/>
         <v>0.99622594121059427</v>
       </c>
-      <c r="V32" s="88">
+      <c r="V32" s="101">
         <f t="shared" si="5"/>
         <v>0.99968448066910742</v>
       </c>
-      <c r="W32" s="88">
+      <c r="W32" s="101">
         <f t="shared" si="6"/>
-        <v>0.99998437626199244</v>
-      </c>
-      <c r="X32" s="88">
+        <v>0.99999993665897058</v>
+      </c>
+      <c r="X32" s="101">
         <f t="shared" si="7"/>
-        <v>1.5623738007564114E-5</v>
-      </c>
-      <c r="Z32" s="76" t="s">
+        <v>0.99999999999956379</v>
+      </c>
+      <c r="Y32" s="101">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="Z32" s="101">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="AA32" s="101">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="AA32" s="88">
-        <f t="shared" si="8"/>
+      <c r="AD32" s="101">
+        <f t="shared" si="10"/>
         <v>0.63358245624321075</v>
       </c>
-      <c r="AB32" s="88">
-        <f t="shared" si="9"/>
+      <c r="AE32" s="101">
+        <f t="shared" si="11"/>
         <v>0.84081469035187228</v>
       </c>
-      <c r="AC32" s="88">
-        <f t="shared" si="10"/>
+      <c r="AF32" s="101">
+        <f t="shared" si="12"/>
         <v>0.92442034414706997</v>
       </c>
-      <c r="AD32" s="88">
-        <f t="shared" si="11"/>
-        <v>0.9694716992391359</v>
-      </c>
-      <c r="AE32" s="88">
-        <f t="shared" si="12"/>
-        <v>3.0528300760864102E-2</v>
-      </c>
-      <c r="AG32" s="76" t="s">
+      <c r="AG32" s="101">
+        <f t="shared" si="13"/>
+        <v>0.99428940010152511</v>
+      </c>
+      <c r="AH32" s="101">
+        <f t="shared" si="14"/>
+        <v>0.99985475279512115</v>
+      </c>
+      <c r="AI32" s="101">
+        <f t="shared" si="15"/>
+        <v>0.99999880751297388</v>
+      </c>
+      <c r="AJ32" s="101">
+        <f t="shared" si="16"/>
+        <v>0.99999999691006625</v>
+      </c>
+      <c r="AK32" s="101">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="AH32" s="44">
-        <f t="shared" si="13"/>
+      <c r="AN32" s="101">
+        <f t="shared" si="17"/>
         <v>0.34194299028735675</v>
       </c>
-      <c r="AI32" s="44">
-        <f t="shared" si="14"/>
+      <c r="AO32" s="101">
+        <f t="shared" si="18"/>
         <v>0.71567219724569331</v>
       </c>
-      <c r="AJ32" s="44">
-        <f t="shared" si="15"/>
+      <c r="AP32" s="101">
+        <f t="shared" si="19"/>
         <v>0.88905130905570107</v>
       </c>
-      <c r="AK32" s="44">
-        <f t="shared" si="16"/>
-        <v>0.9694633335110785</v>
-      </c>
-      <c r="AL32" s="44">
-        <f t="shared" si="17"/>
-        <v>0.65805700971264325</v>
-      </c>
-    </row>
-    <row r="33" spans="2:39">
+      <c r="AQ32" s="101">
+        <f t="shared" si="20"/>
+        <v>0.99781515762844886</v>
+      </c>
+      <c r="AR32" s="101">
+        <f t="shared" si="21"/>
+        <v>0.99999624728992065</v>
+      </c>
+      <c r="AS32" s="101">
+        <f t="shared" si="22"/>
+        <v>0.99999999949395513</v>
+      </c>
+      <c r="AT32" s="101">
+        <f t="shared" si="23"/>
+        <v>0.99999999999999489</v>
+      </c>
+      <c r="AU32" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:47">
       <c r="O33" s="44"/>
       <c r="P33" s="44"/>
       <c r="Q33" s="44"/>
@@ -14959,77 +15122,109 @@
       <c r="S33" s="71" t="s">
         <v>293</v>
       </c>
-      <c r="T33" s="88">
+      <c r="T33" s="101">
         <f t="shared" si="3"/>
         <v>0.76682617615099935</v>
       </c>
-      <c r="U33" s="88">
+      <c r="U33" s="101">
         <f t="shared" si="4"/>
         <v>0.95418880111755022</v>
       </c>
-      <c r="V33" s="88">
+      <c r="V33" s="101">
         <f t="shared" si="5"/>
         <v>0.98998748585906793</v>
       </c>
-      <c r="W33" s="88">
+      <c r="W33" s="101">
         <f t="shared" si="6"/>
-        <v>0.99848587792694921</v>
-      </c>
-      <c r="X33" s="88">
+        <v>0.99995633197497646</v>
+      </c>
+      <c r="X33" s="101">
         <f t="shared" si="7"/>
-        <v>1.5141220730507943E-3</v>
-      </c>
-      <c r="Y33" s="44"/>
-      <c r="Z33" s="71" t="s">
+        <v>0.99999998312382343</v>
+      </c>
+      <c r="Y33" s="101">
+        <f t="shared" si="8"/>
+        <v>0.99999999999945333</v>
+      </c>
+      <c r="Z33" s="101">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="AA33" s="101">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="44"/>
+      <c r="AC33" s="71" t="s">
         <v>293</v>
       </c>
-      <c r="AA33" s="88">
-        <f t="shared" si="8"/>
+      <c r="AD33" s="101">
+        <f t="shared" si="10"/>
         <v>0.48602123970467664</v>
       </c>
-      <c r="AB33" s="88">
-        <f t="shared" si="9"/>
+      <c r="AE33" s="101">
+        <f t="shared" si="11"/>
         <v>0.74725860659793841</v>
       </c>
-      <c r="AC33" s="88">
-        <f t="shared" si="10"/>
+      <c r="AF33" s="101">
+        <f t="shared" si="12"/>
         <v>0.87143015426775872</v>
       </c>
-      <c r="AD33" s="88">
-        <f t="shared" si="11"/>
-        <v>0.94525252109261237</v>
-      </c>
-      <c r="AE33" s="88">
-        <f t="shared" si="12"/>
-        <v>5.4747478907387626E-2</v>
-      </c>
-      <c r="AF33" s="44"/>
-      <c r="AG33" s="71" t="s">
+      <c r="AG33" s="101">
+        <f t="shared" si="13"/>
+        <v>0.98931553681492335</v>
+      </c>
+      <c r="AH33" s="101">
+        <f t="shared" si="14"/>
+        <v>0.99973940839121955</v>
+      </c>
+      <c r="AI33" s="101">
+        <f t="shared" si="15"/>
+        <v>0.99999823974334678</v>
+      </c>
+      <c r="AJ33" s="101">
+        <f t="shared" si="16"/>
+        <v>0.99999999680227936</v>
+      </c>
+      <c r="AK33" s="101">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="44"/>
+      <c r="AM33" s="71" t="s">
         <v>293</v>
       </c>
-      <c r="AH33" s="44">
-        <f t="shared" si="13"/>
+      <c r="AN33" s="101">
+        <f t="shared" si="17"/>
         <v>0.14983014442834014</v>
       </c>
-      <c r="AI33" s="44">
-        <f t="shared" si="14"/>
+      <c r="AO33" s="101">
+        <f t="shared" si="18"/>
         <v>0.49056643348839696</v>
       </c>
-      <c r="AJ33" s="44">
-        <f t="shared" si="15"/>
+      <c r="AP33" s="101">
+        <f t="shared" si="19"/>
         <v>0.74280813134921952</v>
       </c>
-      <c r="AK33" s="44">
-        <f t="shared" si="16"/>
-        <v>0.90786182982277952</v>
-      </c>
-      <c r="AL33" s="44">
-        <f t="shared" si="17"/>
-        <v>0.85016985557165992</v>
-      </c>
-      <c r="AM33" s="44"/>
-    </row>
-    <row r="34" spans="2:39">
+      <c r="AQ33" s="101">
+        <f t="shared" si="20"/>
+        <v>0.9903894839477374</v>
+      </c>
+      <c r="AR33" s="101">
+        <f t="shared" si="21"/>
+        <v>0.99997215963294783</v>
+      </c>
+      <c r="AS33" s="101">
+        <f t="shared" si="22"/>
+        <v>0.99999999466107425</v>
+      </c>
+      <c r="AT33" s="101">
+        <f t="shared" si="23"/>
+        <v>0.99999999999993627</v>
+      </c>
+      <c r="AU33" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:47">
       <c r="L34" s="44"/>
       <c r="O34" s="44"/>
       <c r="P34" s="44"/>
@@ -15038,77 +15233,109 @@
       <c r="S34" s="76" t="s">
         <v>295</v>
       </c>
-      <c r="T34" s="88">
+      <c r="T34" s="101">
         <f t="shared" si="3"/>
         <v>0.5138907043261417</v>
       </c>
-      <c r="U34" s="88">
+      <c r="U34" s="101">
         <f t="shared" si="4"/>
         <v>0.70275414783970647</v>
       </c>
-      <c r="V34" s="88">
+      <c r="V34" s="101">
         <f t="shared" si="5"/>
         <v>0.80620969874302539</v>
       </c>
-      <c r="W34" s="88">
+      <c r="W34" s="101">
         <f t="shared" si="6"/>
-        <v>0.88409087605518322</v>
-      </c>
-      <c r="X34" s="88">
+        <v>0.95479136080813631</v>
+      </c>
+      <c r="X34" s="101">
         <f t="shared" si="7"/>
-        <v>0.11590912394481678</v>
-      </c>
-      <c r="Y34" s="44"/>
-      <c r="Z34" s="76" t="s">
+        <v>0.99417194789886376</v>
+      </c>
+      <c r="Y34" s="101">
+        <f t="shared" si="8"/>
+        <v>0.99959823430951478</v>
+      </c>
+      <c r="Z34" s="101">
+        <f t="shared" si="9"/>
+        <v>0.99998547336263233</v>
+      </c>
+      <c r="AA34" s="101">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="44"/>
+      <c r="AC34" s="76" t="s">
         <v>295</v>
       </c>
-      <c r="AA34" s="88">
-        <f t="shared" si="8"/>
+      <c r="AD34" s="101">
+        <f t="shared" si="10"/>
         <v>0.25380085256173046</v>
       </c>
-      <c r="AB34" s="88">
-        <f t="shared" si="9"/>
+      <c r="AE34" s="101">
+        <f t="shared" si="11"/>
         <v>0.48042786872418958</v>
       </c>
-      <c r="AC34" s="88">
-        <f t="shared" si="10"/>
+      <c r="AF34" s="101">
+        <f t="shared" si="12"/>
         <v>0.64054584703308814</v>
       </c>
-      <c r="AD34" s="88">
-        <f t="shared" si="11"/>
-        <v>0.77902845692514355</v>
-      </c>
-      <c r="AE34" s="88">
-        <f t="shared" si="12"/>
-        <v>0.22097154307485645</v>
-      </c>
-      <c r="AF34" s="44"/>
-      <c r="AG34" s="76" t="s">
+      <c r="AG34" s="101">
+        <f t="shared" si="13"/>
+        <v>0.91657755012121211</v>
+      </c>
+      <c r="AH34" s="101">
+        <f t="shared" si="14"/>
+        <v>0.99191173064402915</v>
+      </c>
+      <c r="AI34" s="101">
+        <f t="shared" si="15"/>
+        <v>0.99969530786128746</v>
+      </c>
+      <c r="AJ34" s="101">
+        <f t="shared" si="16"/>
+        <v>0.9999957044409139</v>
+      </c>
+      <c r="AK34" s="101">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="44"/>
+      <c r="AM34" s="76" t="s">
         <v>295</v>
       </c>
-      <c r="AH34" s="44">
-        <f t="shared" si="13"/>
+      <c r="AN34" s="101">
+        <f t="shared" si="17"/>
         <v>6.6011404930960929E-2</v>
       </c>
-      <c r="AI34" s="44">
-        <f t="shared" si="14"/>
+      <c r="AO34" s="101">
+        <f t="shared" si="18"/>
         <v>0.22200714259760385</v>
       </c>
-      <c r="AJ34" s="44">
-        <f t="shared" si="15"/>
+      <c r="AP34" s="101">
+        <f t="shared" si="19"/>
         <v>0.39296290098211079</v>
       </c>
-      <c r="AK34" s="44">
-        <f t="shared" si="16"/>
-        <v>0.58792955212905773</v>
-      </c>
-      <c r="AL34" s="44">
-        <f t="shared" si="17"/>
-        <v>0.93398859506903908</v>
-      </c>
-      <c r="AM34" s="44"/>
-    </row>
-    <row r="35" spans="2:39">
+      <c r="AQ34" s="101">
+        <f t="shared" si="20"/>
+        <v>0.83221694488457221</v>
+      </c>
+      <c r="AR34" s="101">
+        <f t="shared" si="21"/>
+        <v>0.98600872265415918</v>
+      </c>
+      <c r="AS34" s="101">
+        <f t="shared" si="22"/>
+        <v>0.99970053530100189</v>
+      </c>
+      <c r="AT34" s="101">
+        <f t="shared" si="23"/>
+        <v>0.99999846937326342</v>
+      </c>
+      <c r="AU34" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:47">
       <c r="L35" s="44"/>
       <c r="O35" s="44"/>
       <c r="P35" s="44"/>
@@ -15117,77 +15344,109 @@
       <c r="S35" s="71" t="s">
         <v>297</v>
       </c>
-      <c r="T35" s="88">
-        <f t="shared" si="3"/>
+      <c r="T35" s="101">
+        <f>_xlfn.NORM.DIST($T$27,Z12,AD12,TRUE)</f>
         <v>0.37584533679027893</v>
       </c>
-      <c r="U35" s="88">
+      <c r="U35" s="101">
         <f t="shared" si="4"/>
         <v>0.51506861469064869</v>
       </c>
-      <c r="V35" s="88">
+      <c r="V35" s="101">
         <f t="shared" si="5"/>
         <v>0.60792230376456446</v>
       </c>
-      <c r="W35" s="88">
+      <c r="W35" s="101">
         <f t="shared" si="6"/>
-        <v>0.69498667602271957</v>
-      </c>
-      <c r="X35" s="88">
+        <v>0.80626831138166599</v>
+      </c>
+      <c r="X35" s="101">
         <f t="shared" si="7"/>
-        <v>0.30501332397728043</v>
-      </c>
-      <c r="Y35" s="44"/>
-      <c r="Z35" s="71" t="s">
+        <v>0.92710242952401201</v>
+      </c>
+      <c r="Y35" s="101">
+        <f t="shared" si="8"/>
+        <v>0.9795658771957636</v>
+      </c>
+      <c r="Z35" s="101">
+        <f t="shared" si="9"/>
+        <v>0.99579540336422534</v>
+      </c>
+      <c r="AA35" s="101">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="44"/>
+      <c r="AC35" s="71" t="s">
         <v>297</v>
       </c>
-      <c r="AA35" s="88">
-        <f t="shared" si="8"/>
+      <c r="AD35" s="101">
+        <f t="shared" si="10"/>
         <v>8.9754023843298891E-2</v>
       </c>
-      <c r="AB35" s="88">
-        <f t="shared" si="9"/>
+      <c r="AE35" s="101">
+        <f t="shared" si="11"/>
         <v>0.19240027281705166</v>
       </c>
-      <c r="AC35" s="88">
-        <f t="shared" si="10"/>
+      <c r="AF35" s="101">
+        <f t="shared" si="12"/>
         <v>0.28991681177663592</v>
       </c>
-      <c r="AD35" s="88">
-        <f t="shared" si="11"/>
-        <v>0.40587448754231226</v>
-      </c>
-      <c r="AE35" s="88">
-        <f t="shared" si="12"/>
-        <v>0.59412551245768774</v>
-      </c>
-      <c r="AF35" s="44"/>
-      <c r="AG35" s="71" t="s">
+      <c r="AG35" s="101">
+        <f t="shared" si="13"/>
+        <v>0.59290175446950721</v>
+      </c>
+      <c r="AH35" s="101">
+        <f t="shared" si="14"/>
+        <v>0.8470018886690438</v>
+      </c>
+      <c r="AI35" s="101">
+        <f t="shared" si="15"/>
+        <v>0.96503029194003964</v>
+      </c>
+      <c r="AJ35" s="101">
+        <f t="shared" si="16"/>
+        <v>0.99535165071760523</v>
+      </c>
+      <c r="AK35" s="101">
+        <v>0</v>
+      </c>
+      <c r="AL35" s="44"/>
+      <c r="AM35" s="71" t="s">
         <v>297</v>
       </c>
-      <c r="AH35" s="44">
-        <f t="shared" si="13"/>
+      <c r="AN35" s="101">
+        <f t="shared" si="17"/>
         <v>5.6979596817344061E-2</v>
       </c>
-      <c r="AI35" s="44">
-        <f t="shared" si="14"/>
+      <c r="AO35" s="101">
+        <f t="shared" si="18"/>
         <v>0.12698439253107691</v>
       </c>
-      <c r="AJ35" s="44">
-        <f t="shared" si="15"/>
+      <c r="AP35" s="101">
+        <f t="shared" si="19"/>
         <v>0.19835620119859471</v>
       </c>
-      <c r="AK35" s="44">
-        <f t="shared" si="16"/>
-        <v>0.28970312941742804</v>
-      </c>
-      <c r="AL35" s="44">
-        <f t="shared" si="17"/>
-        <v>0.9430204031826559</v>
-      </c>
-      <c r="AM35" s="44"/>
-    </row>
-    <row r="36" spans="2:39" s="44" customFormat="1">
+      <c r="AQ35" s="101">
+        <f t="shared" si="20"/>
+        <v>0.45447244481580307</v>
+      </c>
+      <c r="AR35" s="101">
+        <f t="shared" si="21"/>
+        <v>0.73196550526672355</v>
+      </c>
+      <c r="AS35" s="101">
+        <f t="shared" si="22"/>
+        <v>0.91179733138324648</v>
+      </c>
+      <c r="AT35" s="101">
+        <f t="shared" si="23"/>
+        <v>0.98146734609448394</v>
+      </c>
+      <c r="AU35" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:47" s="44" customFormat="1">
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
@@ -15201,74 +15460,107 @@
       <c r="S36" s="76" t="s">
         <v>301</v>
       </c>
-      <c r="T36" s="88">
+      <c r="T36" s="101">
         <f t="shared" si="3"/>
         <v>0.16552806134367962</v>
       </c>
-      <c r="U36" s="88">
+      <c r="U36" s="101">
         <f t="shared" si="4"/>
         <v>0.29053559209062707</v>
       </c>
-      <c r="V36" s="88">
+      <c r="V36" s="101">
         <f t="shared" si="5"/>
         <v>0.39292301197938029</v>
       </c>
-      <c r="W36" s="88">
+      <c r="W36" s="101">
         <f t="shared" si="6"/>
-        <v>0.50335241668180219</v>
-      </c>
-      <c r="X36" s="88">
+        <v>0.66588242910237538</v>
+      </c>
+      <c r="X36" s="101">
         <f t="shared" si="7"/>
-        <v>0.49664758331819781</v>
-      </c>
-      <c r="Z36" s="76" t="s">
+        <v>0.87051976694100974</v>
+      </c>
+      <c r="Y36" s="101">
+        <f t="shared" si="8"/>
+        <v>0.96631005589236407</v>
+      </c>
+      <c r="Z36" s="101">
+        <f t="shared" si="9"/>
+        <v>0.99428730510778573</v>
+      </c>
+      <c r="AA36" s="101">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="76" t="s">
         <v>301</v>
       </c>
-      <c r="AA36" s="88">
-        <f t="shared" si="8"/>
+      <c r="AD36" s="101">
+        <f t="shared" si="10"/>
         <v>5.0511604601422351E-2</v>
       </c>
-      <c r="AB36" s="88">
-        <f t="shared" si="9"/>
+      <c r="AE36" s="101">
+        <f t="shared" si="11"/>
         <v>9.4333345509310967E-2</v>
       </c>
-      <c r="AC36" s="88">
-        <f t="shared" si="10"/>
+      <c r="AF36" s="101">
+        <f t="shared" si="12"/>
         <v>0.13618656405660809</v>
       </c>
-      <c r="AD36" s="88">
-        <f t="shared" si="11"/>
-        <v>0.18924169383003042</v>
-      </c>
-      <c r="AE36" s="88">
-        <f t="shared" si="12"/>
-        <v>0.81075830616996958</v>
-      </c>
-      <c r="AG36" s="76" t="s">
+      <c r="AG36" s="101">
+        <f t="shared" si="13"/>
+        <v>0.28933976981199794</v>
+      </c>
+      <c r="AH36" s="101">
+        <f t="shared" si="14"/>
+        <v>0.49480783925100147</v>
+      </c>
+      <c r="AI36" s="101">
+        <f t="shared" si="15"/>
+        <v>0.70169583060873153</v>
+      </c>
+      <c r="AJ36" s="101">
+        <f t="shared" si="16"/>
+        <v>0.85804642932382791</v>
+      </c>
+      <c r="AK36" s="101">
+        <v>0</v>
+      </c>
+      <c r="AM36" s="76" t="s">
         <v>301</v>
       </c>
-      <c r="AH36" s="44">
-        <f t="shared" si="13"/>
+      <c r="AN36" s="101">
+        <f t="shared" si="17"/>
         <v>2.8856450394145666E-2</v>
       </c>
-      <c r="AI36" s="44">
-        <f t="shared" si="14"/>
+      <c r="AO36" s="101">
+        <f t="shared" si="18"/>
         <v>5.7199757058308189E-2</v>
       </c>
-      <c r="AJ36" s="44">
-        <f t="shared" si="15"/>
+      <c r="AP36" s="101">
+        <f t="shared" si="19"/>
         <v>8.5976160021217857E-2</v>
       </c>
-      <c r="AK36" s="44">
-        <f t="shared" si="16"/>
-        <v>0.12441589797637952</v>
-      </c>
-      <c r="AL36" s="44">
-        <f t="shared" si="17"/>
-        <v>0.97114354960585436</v>
-      </c>
-    </row>
-    <row r="37" spans="2:39">
+      <c r="AQ36" s="101">
+        <f t="shared" si="20"/>
+        <v>0.20212850255165354</v>
+      </c>
+      <c r="AR36" s="101">
+        <f t="shared" si="21"/>
+        <v>0.38127737390844418</v>
+      </c>
+      <c r="AS36" s="101">
+        <f t="shared" si="22"/>
+        <v>0.5908714474634762</v>
+      </c>
+      <c r="AT36" s="101">
+        <f t="shared" si="23"/>
+        <v>0.77688109740361544</v>
+      </c>
+      <c r="AU36" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:47">
       <c r="L37" s="44"/>
       <c r="M37" s="44"/>
       <c r="O37" s="44"/>
@@ -15278,77 +15570,109 @@
       <c r="S37" s="71" t="s">
         <v>302</v>
       </c>
-      <c r="T37" s="88">
+      <c r="T37" s="101">
         <f t="shared" si="3"/>
         <v>9.1492186931267622E-2</v>
       </c>
-      <c r="U37" s="88">
+      <c r="U37" s="101">
         <f t="shared" si="4"/>
         <v>0.15300882371326033</v>
       </c>
-      <c r="V37" s="88">
+      <c r="V37" s="101">
         <f t="shared" si="5"/>
         <v>0.20660004501142309</v>
       </c>
-      <c r="W37" s="88">
+      <c r="W37" s="101">
         <f t="shared" si="6"/>
-        <v>0.26995921510986137</v>
-      </c>
-      <c r="X37" s="88">
+        <v>0.38021044483571315</v>
+      </c>
+      <c r="X37" s="101">
         <f t="shared" si="7"/>
-        <v>0.73004078489013868</v>
-      </c>
-      <c r="Y37" s="44"/>
-      <c r="Z37" s="71" t="s">
+        <v>0.58254904641534866</v>
+      </c>
+      <c r="Y37" s="101">
+        <f t="shared" si="8"/>
+        <v>0.76478079525417386</v>
+      </c>
+      <c r="Z37" s="101">
+        <f t="shared" si="9"/>
+        <v>0.89160576223881305</v>
+      </c>
+      <c r="AA37" s="101">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="44"/>
+      <c r="AC37" s="71" t="s">
         <v>302</v>
       </c>
-      <c r="AA37" s="88">
-        <f t="shared" si="8"/>
+      <c r="AD37" s="101">
+        <f t="shared" si="10"/>
         <v>3.2210497290905374E-2</v>
       </c>
-      <c r="AB37" s="88">
-        <f t="shared" si="9"/>
+      <c r="AE37" s="101">
+        <f t="shared" si="11"/>
         <v>5.6332486553475364E-2</v>
       </c>
-      <c r="AC37" s="88">
-        <f t="shared" si="10"/>
+      <c r="AF37" s="101">
+        <f t="shared" si="12"/>
         <v>7.9115975834815E-2</v>
       </c>
-      <c r="AD37" s="88">
-        <f t="shared" si="11"/>
-        <v>0.10827424567922854</v>
-      </c>
-      <c r="AE37" s="88">
-        <f t="shared" si="12"/>
-        <v>0.8917257543207715</v>
-      </c>
-      <c r="AF37" s="44"/>
-      <c r="AG37" s="71" t="s">
+      <c r="AG37" s="101">
+        <f t="shared" si="13"/>
+        <v>0.16531868864588461</v>
+      </c>
+      <c r="AH37" s="101">
+        <f t="shared" si="14"/>
+        <v>0.29645675583092174</v>
+      </c>
+      <c r="AI37" s="101">
+        <f t="shared" si="15"/>
+        <v>0.46159880109745322</v>
+      </c>
+      <c r="AJ37" s="101">
+        <f t="shared" si="16"/>
+        <v>0.63375133998904754</v>
+      </c>
+      <c r="AK37" s="101">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="44"/>
+      <c r="AM37" s="71" t="s">
         <v>302</v>
       </c>
-      <c r="AH37" s="44">
-        <f t="shared" si="13"/>
+      <c r="AN37" s="101">
+        <f t="shared" si="17"/>
         <v>7.3325429420576533E-3</v>
       </c>
-      <c r="AI37" s="44">
-        <f t="shared" si="14"/>
+      <c r="AO37" s="101">
+        <f t="shared" si="18"/>
         <v>1.5850994164039133E-2</v>
       </c>
-      <c r="AJ37" s="44">
-        <f t="shared" si="15"/>
+      <c r="AP37" s="101">
+        <f t="shared" si="19"/>
         <v>2.5396980814932565E-2</v>
       </c>
-      <c r="AK37" s="44">
-        <f t="shared" si="16"/>
-        <v>3.9349548301286723E-2</v>
-      </c>
-      <c r="AL37" s="44">
-        <f t="shared" si="17"/>
-        <v>0.99266745705794235</v>
-      </c>
-      <c r="AM37" s="44"/>
-    </row>
-    <row r="38" spans="2:39">
+      <c r="AQ37" s="101">
+        <f t="shared" si="20"/>
+        <v>7.1339545297204487E-2</v>
+      </c>
+      <c r="AR37" s="101">
+        <f t="shared" si="21"/>
+        <v>0.16389933245411942</v>
+      </c>
+      <c r="AS37" s="101">
+        <f t="shared" si="22"/>
+        <v>0.31163257381350196</v>
+      </c>
+      <c r="AT37" s="101">
+        <f t="shared" si="23"/>
+        <v>0.49844467341211474</v>
+      </c>
+      <c r="AU37" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:47">
       <c r="B38" s="7" t="s">
         <v>86</v>
       </c>
@@ -15363,77 +15687,109 @@
       <c r="S38" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="T38" s="88">
+      <c r="T38" s="101">
         <f t="shared" si="3"/>
         <v>3.6630747396996691E-2</v>
       </c>
-      <c r="U38" s="88">
+      <c r="U38" s="101">
         <f t="shared" si="4"/>
         <v>5.4970533940220757E-2</v>
       </c>
-      <c r="V38" s="88">
+      <c r="V38" s="101">
         <f t="shared" si="5"/>
         <v>7.0785662206478708E-2</v>
       </c>
-      <c r="W38" s="88">
+      <c r="W38" s="101">
         <f t="shared" si="6"/>
-        <v>8.9883749084018569E-2</v>
-      </c>
-      <c r="X38" s="88">
+        <v>0.12533343317165579</v>
+      </c>
+      <c r="X38" s="101">
         <f t="shared" si="7"/>
-        <v>0.91011625091598147</v>
-      </c>
-      <c r="Y38" s="44"/>
-      <c r="Z38" s="82" t="s">
+        <v>0.20397754353748057</v>
+      </c>
+      <c r="Y38" s="101">
+        <f t="shared" si="8"/>
+        <v>0.30633564692244153</v>
+      </c>
+      <c r="Z38" s="101">
+        <f t="shared" si="9"/>
+        <v>0.42660254978994411</v>
+      </c>
+      <c r="AA38" s="101">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="44"/>
+      <c r="AC38" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="AA38" s="88">
-        <f t="shared" si="8"/>
+      <c r="AD38" s="101">
+        <f t="shared" si="10"/>
         <v>3.054309712927282E-2</v>
       </c>
-      <c r="AB38" s="88">
-        <f t="shared" si="9"/>
+      <c r="AE38" s="101">
+        <f t="shared" si="11"/>
         <v>4.54767509141593E-2</v>
       </c>
-      <c r="AC38" s="88">
-        <f t="shared" si="10"/>
+      <c r="AF38" s="101">
+        <f t="shared" si="12"/>
         <v>5.8354873920238394E-2</v>
       </c>
-      <c r="AD38" s="88">
-        <f t="shared" si="11"/>
-        <v>7.3937218528355567E-2</v>
-      </c>
-      <c r="AE38" s="88">
-        <f t="shared" si="12"/>
-        <v>0.92606278147164445</v>
-      </c>
-      <c r="AF38" s="44"/>
-      <c r="AG38" s="82" t="s">
+      <c r="AG38" s="101">
+        <f t="shared" si="13"/>
+        <v>0.10300763832828137</v>
+      </c>
+      <c r="AH38" s="101">
+        <f t="shared" si="14"/>
+        <v>0.16841130134712209</v>
+      </c>
+      <c r="AI38" s="101">
+        <f t="shared" si="15"/>
+        <v>0.2558071850950065</v>
+      </c>
+      <c r="AJ38" s="101">
+        <f t="shared" si="16"/>
+        <v>0.362347970092745</v>
+      </c>
+      <c r="AK38" s="101">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="44"/>
+      <c r="AM38" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="AH38" s="44">
-        <f t="shared" si="13"/>
+      <c r="AN38" s="101">
+        <f t="shared" si="17"/>
         <v>3.2086171243230267E-3</v>
       </c>
-      <c r="AI38" s="44">
-        <f t="shared" si="14"/>
+      <c r="AO38" s="101">
+        <f t="shared" si="18"/>
         <v>5.8437278169573741E-3</v>
       </c>
-      <c r="AJ38" s="44">
-        <f t="shared" si="15"/>
+      <c r="AP38" s="101">
+        <f t="shared" si="19"/>
         <v>8.5326893308700167E-3</v>
       </c>
-      <c r="AK38" s="44">
-        <f t="shared" si="16"/>
-        <v>1.2251506395051929E-2</v>
-      </c>
-      <c r="AL38" s="44">
-        <f t="shared" si="17"/>
-        <v>0.99679138287567692</v>
-      </c>
-      <c r="AM38" s="44"/>
-    </row>
-    <row r="39" spans="2:39" ht="15.75" thickBot="1">
+      <c r="AQ38" s="101">
+        <f t="shared" si="20"/>
+        <v>2.0430952713542849E-2</v>
+      </c>
+      <c r="AR38" s="101">
+        <f t="shared" si="21"/>
+        <v>4.4138172035112347E-2</v>
+      </c>
+      <c r="AS38" s="101">
+        <f t="shared" si="22"/>
+        <v>8.6253363635820451E-2</v>
+      </c>
+      <c r="AT38" s="101">
+        <f t="shared" si="23"/>
+        <v>0.15295879709707286</v>
+      </c>
+      <c r="AU38" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:47" ht="15.75" thickBot="1">
       <c r="B39" s="10" t="s">
         <v>12</v>
       </c>
@@ -15492,8 +15848,11 @@
       <c r="AK39" s="44"/>
       <c r="AL39" s="44"/>
       <c r="AM39" s="44"/>
-    </row>
-    <row r="40" spans="2:39">
+      <c r="AN39" s="44"/>
+      <c r="AO39" s="44"/>
+      <c r="AU39" s="101"/>
+    </row>
+    <row r="40" spans="2:47">
       <c r="C40" t="s">
         <v>82</v>
       </c>
@@ -15538,7 +15897,7 @@
       <c r="AL40" s="44"/>
       <c r="AM40" s="44"/>
     </row>
-    <row r="41" spans="2:39">
+    <row r="41" spans="2:47">
       <c r="C41" t="s">
         <v>82</v>
       </c>
@@ -15585,7 +15944,7 @@
       <c r="AL41" s="44"/>
       <c r="AM41" s="44"/>
     </row>
-    <row r="42" spans="2:39" ht="21.75" thickBot="1">
+    <row r="42" spans="2:47" ht="21.75" thickBot="1">
       <c r="B42" s="44"/>
       <c r="C42" s="44" t="s">
         <v>82</v>
@@ -15618,26 +15977,26 @@
       <c r="P42" s="44"/>
       <c r="Q42" s="44"/>
       <c r="R42" s="44"/>
-      <c r="S42" s="100" t="s">
+      <c r="S42" s="98" t="s">
         <v>307</v>
       </c>
-      <c r="T42" s="100"/>
-      <c r="U42" s="100"/>
-      <c r="V42" s="100"/>
+      <c r="T42" s="98"/>
+      <c r="U42" s="98"/>
+      <c r="V42" s="98"/>
       <c r="W42" s="44"/>
-      <c r="X42" s="100" t="s">
+      <c r="X42" s="98" t="s">
         <v>308</v>
       </c>
-      <c r="Y42" s="100"/>
-      <c r="Z42" s="100"/>
-      <c r="AA42" s="100"/>
+      <c r="Y42" s="98"/>
+      <c r="Z42" s="98"/>
+      <c r="AA42" s="98"/>
       <c r="AB42" s="44"/>
-      <c r="AC42" s="100" t="s">
+      <c r="AC42" s="98" t="s">
         <v>309</v>
       </c>
-      <c r="AD42" s="100"/>
-      <c r="AE42" s="100"/>
-      <c r="AF42" s="100"/>
+      <c r="AD42" s="98"/>
+      <c r="AE42" s="98"/>
+      <c r="AF42" s="98"/>
       <c r="AG42" s="44"/>
       <c r="AH42" s="44"/>
       <c r="AI42" s="44"/>
@@ -15646,7 +16005,7 @@
       <c r="AL42" s="44"/>
       <c r="AM42" s="44"/>
     </row>
-    <row r="43" spans="2:39" ht="15.75" thickBot="1">
+    <row r="43" spans="2:47" ht="15.75" thickBot="1">
       <c r="C43" t="s">
         <v>82</v>
       </c>
@@ -15718,7 +16077,7 @@
       <c r="AL43" s="44"/>
       <c r="AM43" s="44"/>
     </row>
-    <row r="44" spans="2:39">
+    <row r="44" spans="2:47">
       <c r="C44" t="s">
         <v>82</v>
       </c>
@@ -15746,15 +16105,15 @@
         <v>287</v>
       </c>
       <c r="T44" s="68">
-        <f t="shared" ref="T44:T52" si="18">U7*T30</f>
+        <f t="shared" ref="T44:T52" si="24">U7*T30</f>
         <v>9417.6380632201017</v>
       </c>
       <c r="U44" s="68">
-        <f t="shared" ref="U44:U52" si="19">V7*AA30</f>
+        <f>V7*AD30</f>
         <v>15372.778652981828</v>
       </c>
       <c r="V44" s="68">
-        <f t="shared" ref="V44:V52" si="20">W7*AH30</f>
+        <f>W7*AN30</f>
         <v>20351.618204054608</v>
       </c>
       <c r="W44" s="44"/>
@@ -15762,15 +16121,15 @@
         <v>287</v>
       </c>
       <c r="Y44" s="68">
-        <f t="shared" ref="Y44:Y52" si="21">U7*U30</f>
+        <f t="shared" ref="Y44:Y52" si="25">U7*U30</f>
         <v>9418.8889686648563</v>
       </c>
       <c r="Z44" s="68">
-        <f t="shared" ref="Z44:Z52" si="22">V7*AB30</f>
+        <f>V7*AE30</f>
         <v>15466.162940366092</v>
       </c>
       <c r="AA44" s="68">
-        <f t="shared" ref="AA44:AA52" si="23">W7*AI30</f>
+        <f>W7*AO30</f>
         <v>20378.602528978172</v>
       </c>
       <c r="AB44" s="44"/>
@@ -15778,15 +16137,15 @@
         <v>287</v>
       </c>
       <c r="AD44" s="68">
-        <f t="shared" ref="AD44:AD52" si="24">U7*V30</f>
+        <f t="shared" ref="AD44:AD52" si="26">U7*V30</f>
         <v>9418.898652143529</v>
       </c>
       <c r="AE44" s="68">
-        <f t="shared" ref="AE44:AE52" si="25">V7*AC30</f>
+        <f>V7*AF30</f>
         <v>15471.469884810578</v>
       </c>
       <c r="AF44" s="68">
-        <f t="shared" ref="AF44:AF52" si="26">W7*AJ30</f>
+        <f>W7*AP30</f>
         <v>20378.705451762668</v>
       </c>
       <c r="AG44" s="44"/>
@@ -15797,7 +16156,7 @@
       <c r="AL44" s="44"/>
       <c r="AM44" s="44"/>
     </row>
-    <row r="45" spans="2:39">
+    <row r="45" spans="2:47">
       <c r="C45" t="s">
         <v>82</v>
       </c>
@@ -15826,15 +16185,15 @@
         <v>289</v>
       </c>
       <c r="T45" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>7226.9569082675025</v>
       </c>
       <c r="U45" s="73">
-        <f t="shared" si="19"/>
+        <f>V8*AD31</f>
         <v>7338.965095745436</v>
       </c>
       <c r="V45" s="73">
-        <f t="shared" si="20"/>
+        <f>W8*AN31</f>
         <v>5783.8602283503142</v>
       </c>
       <c r="W45" s="44"/>
@@ -15842,15 +16201,15 @@
         <v>289</v>
       </c>
       <c r="Y45" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>7439.6406066050522</v>
       </c>
       <c r="Z45" s="73">
-        <f t="shared" si="22"/>
+        <f>V8*AE31</f>
         <v>8783.4591019824566</v>
       </c>
       <c r="AA45" s="73">
-        <f t="shared" si="23"/>
+        <f>W8*AO31</f>
         <v>8286.9859436891857</v>
       </c>
       <c r="AB45" s="44"/>
@@ -15858,15 +16217,15 @@
         <v>289</v>
       </c>
       <c r="AD45" s="73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>7456.845324521013</v>
       </c>
       <c r="AE45" s="73">
-        <f t="shared" si="25"/>
+        <f>V8*AF31</f>
         <v>9238.3388650550733</v>
       </c>
       <c r="AF45" s="73">
-        <f t="shared" si="26"/>
+        <f>W8*AP31</f>
         <v>9058.9611369377526</v>
       </c>
       <c r="AG45" s="44"/>
@@ -15877,7 +16236,7 @@
       <c r="AL45" s="44"/>
       <c r="AM45" s="44"/>
     </row>
-    <row r="46" spans="2:39">
+    <row r="46" spans="2:47">
       <c r="B46" s="44"/>
       <c r="C46" s="44" t="s">
         <v>82</v>
@@ -15911,15 +16270,15 @@
         <v>291</v>
       </c>
       <c r="T46" s="78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>13195.088262110432</v>
       </c>
       <c r="U46" s="78">
-        <f t="shared" si="19"/>
+        <f>V9*AD32</f>
         <v>11116.263088697284</v>
       </c>
       <c r="V46" s="78">
-        <f t="shared" si="20"/>
+        <f>W9*AN32</f>
         <v>6869.9592457318131</v>
       </c>
       <c r="W46" s="44"/>
@@ -15927,15 +16286,15 @@
         <v>291</v>
       </c>
       <c r="Y46" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>13988.85266873088</v>
       </c>
       <c r="Z46" s="78">
-        <f t="shared" si="22"/>
+        <f>V9*AE32</f>
         <v>14752.17189916172</v>
       </c>
       <c r="AA46" s="78">
-        <f t="shared" si="23"/>
+        <f>W9*AO32</f>
         <v>14378.533755727773</v>
       </c>
       <c r="AB46" s="44"/>
@@ -15943,15 +16302,15 @@
         <v>291</v>
       </c>
       <c r="AD46" s="78">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>14037.41695212561</v>
       </c>
       <c r="AE46" s="78">
-        <f t="shared" si="25"/>
+        <f>V9*AF32</f>
         <v>16219.040866463431</v>
       </c>
       <c r="AF46" s="78">
-        <f t="shared" si="26"/>
+        <f>W9*AP32</f>
         <v>17861.884682719923</v>
       </c>
       <c r="AG46" s="44"/>
@@ -15962,7 +16321,7 @@
       <c r="AL46" s="44"/>
       <c r="AM46" s="44"/>
     </row>
-    <row r="47" spans="2:39">
+    <row r="47" spans="2:47">
       <c r="C47" t="s">
         <v>82</v>
       </c>
@@ -15989,15 +16348,15 @@
         <v>293</v>
       </c>
       <c r="T47" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>15278.613097799687</v>
       </c>
       <c r="U47" s="73">
-        <f t="shared" si="19"/>
+        <f>V10*AD33</f>
         <v>24188.71802303115</v>
       </c>
       <c r="V47" s="73">
-        <f t="shared" si="20"/>
+        <f>W10*AN33</f>
         <v>8010.8499729257437</v>
       </c>
       <c r="W47" s="44"/>
@@ -16005,15 +16364,15 @@
         <v>293</v>
       </c>
       <c r="Y47" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>19011.716041964675</v>
       </c>
       <c r="Z47" s="73">
-        <f t="shared" si="22"/>
+        <f>V10*AE33</f>
         <v>37190.201268289908</v>
       </c>
       <c r="AA47" s="73">
-        <f t="shared" si="23"/>
+        <f>W10*AO33</f>
         <v>26228.727973417597</v>
       </c>
       <c r="AB47" s="44"/>
@@ -16021,15 +16380,15 @@
         <v>293</v>
       </c>
       <c r="AD47" s="73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>19724.986233549855</v>
       </c>
       <c r="AE47" s="73">
-        <f t="shared" si="25"/>
+        <f>V10*AF33</f>
         <v>43370.07635953842</v>
       </c>
       <c r="AF47" s="73">
-        <f t="shared" si="26"/>
+        <f>W10*AP33</f>
         <v>39715.1355730949</v>
       </c>
       <c r="AG47" s="44"/>
@@ -16040,7 +16399,7 @@
       <c r="AL47" s="44"/>
       <c r="AM47" s="44"/>
     </row>
-    <row r="48" spans="2:39">
+    <row r="48" spans="2:47">
       <c r="H48" s="39"/>
       <c r="I48" s="39"/>
       <c r="M48" s="44"/>
@@ -16052,15 +16411,15 @@
         <v>295</v>
       </c>
       <c r="T48" s="78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>30270.630926141846</v>
       </c>
       <c r="U48" s="78">
-        <f t="shared" si="19"/>
+        <f>V11*AD34</f>
         <v>71610.298224913975</v>
       </c>
       <c r="V48" s="78">
-        <f t="shared" si="20"/>
+        <f>W11*AN34</f>
         <v>16589.915893594109</v>
       </c>
       <c r="W48" s="44"/>
@@ -16068,15 +16427,15 @@
         <v>295</v>
       </c>
       <c r="Y48" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>41395.59494263638</v>
       </c>
       <c r="Z48" s="78">
-        <f t="shared" si="22"/>
+        <f>V11*AE34</f>
         <v>135553.45700240019</v>
       </c>
       <c r="AA48" s="78">
-        <f t="shared" si="23"/>
+        <f>W11*AO34</f>
         <v>55794.598332264082</v>
       </c>
       <c r="AB48" s="44"/>
@@ -16084,15 +16443,15 @@
         <v>295</v>
       </c>
       <c r="AD48" s="78">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>47489.623833004342</v>
       </c>
       <c r="AE48" s="78">
-        <f t="shared" si="25"/>
+        <f>V11*AF34</f>
         <v>180730.98915856858</v>
       </c>
       <c r="AF48" s="78">
-        <f t="shared" si="26"/>
+        <f>W11*AP34</f>
         <v>98759.017224587151</v>
       </c>
       <c r="AG48" s="44"/>
@@ -16114,15 +16473,15 @@
         <v>297</v>
       </c>
       <c r="T49" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>16439.227593093379</v>
       </c>
       <c r="U49" s="73">
-        <f t="shared" si="19"/>
+        <f>V12*AD35</f>
         <v>16840.280240037471</v>
       </c>
       <c r="V49" s="73">
-        <f t="shared" si="20"/>
+        <f>W12*AN35</f>
         <v>9496.663557138043</v>
       </c>
       <c r="W49" s="44"/>
@@ -16130,15 +16489,15 @@
         <v>297</v>
       </c>
       <c r="Y49" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>22528.762110686101</v>
       </c>
       <c r="Z49" s="73">
-        <f t="shared" si="22"/>
+        <f>V12*AE35</f>
         <v>36099.49029311091</v>
       </c>
       <c r="AA49" s="73">
-        <f t="shared" si="23"/>
+        <f>W12*AO35</f>
         <v>21164.20824704953</v>
       </c>
       <c r="AB49" s="44"/>
@@ -16146,15 +16505,15 @@
         <v>297</v>
       </c>
       <c r="AD49" s="73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>26590.121340469981</v>
       </c>
       <c r="AE49" s="73">
-        <f t="shared" si="25"/>
+        <f>V12*AF35</f>
         <v>54396.228130570431</v>
       </c>
       <c r="AF49" s="73">
-        <f t="shared" si="26"/>
+        <f>W12*AP35</f>
         <v>33059.589966801032</v>
       </c>
       <c r="AG49" s="44"/>
@@ -16180,15 +16539,15 @@
         <v>301</v>
       </c>
       <c r="T50" s="78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>4265.3066374795972</v>
       </c>
       <c r="U50" s="78">
-        <f t="shared" si="19"/>
+        <f>V13*AD36</f>
         <v>5122.8311719375915</v>
       </c>
       <c r="V50" s="78">
-        <f t="shared" si="20"/>
+        <f>W13*AN36</f>
         <v>2348.819777782865</v>
       </c>
       <c r="W50" s="44"/>
@@ -16196,15 +16555,15 @@
         <v>301</v>
       </c>
       <c r="Y50" s="78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>7486.4852479318533</v>
       </c>
       <c r="Z50" s="78">
-        <f t="shared" si="22"/>
+        <f>V13*AE36</f>
         <v>9567.1837539417502</v>
       </c>
       <c r="AA50" s="78">
-        <f t="shared" si="23"/>
+        <f>W13*AO36</f>
         <v>4655.871350351058</v>
       </c>
       <c r="AB50" s="44"/>
@@ -16212,15 +16571,15 @@
         <v>301</v>
       </c>
       <c r="AD50" s="78">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>10124.791635989994</v>
       </c>
       <c r="AE50" s="78">
-        <f t="shared" si="25"/>
+        <f>V13*AF36</f>
         <v>13811.89097145851</v>
       </c>
       <c r="AF50" s="78">
-        <f t="shared" si="26"/>
+        <f>W13*AP36</f>
         <v>6998.1755315487662</v>
       </c>
       <c r="AG50" s="44"/>
@@ -16272,15 +16631,15 @@
         <v>302</v>
       </c>
       <c r="T51" s="73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1128.2060059559165</v>
       </c>
       <c r="U51" s="73">
-        <f t="shared" si="19"/>
+        <f>V14*AD37</f>
         <v>1614.512718252895</v>
       </c>
       <c r="V51" s="73">
-        <f t="shared" si="20"/>
+        <f>W14*AN37</f>
         <v>317.06653161471883</v>
       </c>
       <c r="W51" s="44"/>
@@ -16288,15 +16647,15 @@
         <v>302</v>
       </c>
       <c r="Y51" s="73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>1886.7783104499745</v>
       </c>
       <c r="Z51" s="73">
-        <f t="shared" si="22"/>
+        <f>V14*AE37</f>
         <v>2823.5986290430769</v>
       </c>
       <c r="AA51" s="73">
-        <f t="shared" si="23"/>
+        <f>W14*AO37</f>
         <v>685.4129299959742</v>
       </c>
       <c r="AB51" s="44"/>
@@ -16304,15 +16663,15 @@
         <v>302</v>
       </c>
       <c r="AD51" s="73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>2547.6209437178968</v>
       </c>
       <c r="AE51" s="73">
-        <f t="shared" si="25"/>
+        <f>V14*AF37</f>
         <v>3965.5938264064957</v>
       </c>
       <c r="AF51" s="73">
-        <f t="shared" si="26"/>
+        <f>W14*AP37</f>
         <v>1098.1909937804644</v>
       </c>
       <c r="AG51" s="44"/>
@@ -16350,15 +16709,15 @@
         <v>303</v>
       </c>
       <c r="T52" s="83">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>557.19660693455216</v>
       </c>
       <c r="U52" s="83">
-        <f t="shared" si="19"/>
+        <f>V15*AD38</f>
         <v>1609.8250753795896</v>
       </c>
       <c r="V52" s="83">
-        <f t="shared" si="20"/>
+        <f>W15*AN38</f>
         <v>251.66959576095758</v>
       </c>
       <c r="W52" s="44"/>
@@ -16366,15 +16725,15 @@
         <v>303</v>
       </c>
       <c r="Y52" s="83">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>836.16625838715231</v>
       </c>
       <c r="Z52" s="83">
-        <f t="shared" si="22"/>
+        <f>V15*AE38</f>
         <v>2396.928302933643</v>
       </c>
       <c r="AA52" s="83">
-        <f t="shared" si="23"/>
+        <f>W15*AO38</f>
         <v>458.35590861936208</v>
       </c>
       <c r="AB52" s="44"/>
@@ -16382,15 +16741,15 @@
         <v>303</v>
       </c>
       <c r="AD52" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1076.7328980106768</v>
       </c>
       <c r="AE52" s="83">
-        <f t="shared" si="25"/>
+        <f>V15*AF38</f>
         <v>3075.6913390220689</v>
       </c>
       <c r="AF52" s="83">
-        <f t="shared" si="26"/>
+        <f>W15*AP38</f>
         <v>669.26603937107893</v>
       </c>
       <c r="AG52" s="44"/>
@@ -16506,43 +16865,43 @@
       <c r="Q54" s="44"/>
       <c r="R54" s="44"/>
       <c r="S54" s="44"/>
-      <c r="T54" s="89">
+      <c r="T54" s="88">
         <f>T53/U16</f>
         <v>0.47282104108541512</v>
       </c>
-      <c r="U54" s="89">
+      <c r="U54" s="88">
         <f>U53/V16</f>
         <v>0.20201490784017861</v>
       </c>
-      <c r="V54" s="89">
+      <c r="V54" s="88">
         <f>V53/W16</f>
         <v>9.6655921484074245E-2</v>
       </c>
       <c r="W54" s="44"/>
       <c r="X54" s="44"/>
-      <c r="Y54" s="89">
+      <c r="Y54" s="88">
         <f>Y53/U16</f>
         <v>0.59958198109267813</v>
       </c>
-      <c r="Z54" s="89">
+      <c r="Z54" s="88">
         <f>Z53/V16</f>
         <v>0.34270511306286983</v>
       </c>
-      <c r="AA54" s="89">
+      <c r="AA54" s="88">
         <f>AA53/W16</f>
         <v>0.20986341515823231</v>
       </c>
       <c r="AB54" s="44"/>
       <c r="AC54" s="44"/>
-      <c r="AD54" s="89">
+      <c r="AD54" s="88">
         <f>AD53/U16</f>
         <v>0.66957342547341547</v>
       </c>
-      <c r="AE54" s="89">
+      <c r="AE54" s="88">
         <f>AE53/V16</f>
         <v>0.44402499541316193</v>
       </c>
-      <c r="AF54" s="89">
+      <c r="AF54" s="88">
         <f>AF53/W16</f>
         <v>0.31417667924089815</v>
       </c>
@@ -16625,43 +16984,43 @@
       <c r="Q56" s="44"/>
       <c r="R56" s="44"/>
       <c r="S56" s="44"/>
-      <c r="T56" s="90">
+      <c r="T56" s="89">
         <f>SUM(T44:T50)</f>
         <v>96093.46148811256</v>
       </c>
-      <c r="U56" s="90">
+      <c r="U56" s="89">
         <f t="shared" ref="U56:V56" si="30">SUM(U44:U50)</f>
         <v>151590.13449734473</v>
       </c>
-      <c r="V56" s="90">
+      <c r="V56" s="89">
         <f t="shared" si="30"/>
         <v>69451.686879577494</v>
       </c>
       <c r="W56" s="44"/>
       <c r="X56" s="44"/>
-      <c r="Y56" s="90">
+      <c r="Y56" s="89">
         <f>SUM(Y44:Y50)</f>
         <v>121269.9405872198</v>
       </c>
-      <c r="Z56" s="90">
+      <c r="Z56" s="89">
         <f t="shared" ref="Z56:AA56" si="31">SUM(Z44:Z50)</f>
         <v>257412.12625925304</v>
       </c>
-      <c r="AA56" s="90">
+      <c r="AA56" s="89">
         <f t="shared" si="31"/>
         <v>150887.52813147739</v>
       </c>
       <c r="AB56" s="44"/>
       <c r="AC56" s="44"/>
-      <c r="AD56" s="90">
+      <c r="AD56" s="89">
         <f>SUM(AD44:AD50)</f>
         <v>134842.68397180433</v>
       </c>
-      <c r="AE56" s="90">
+      <c r="AE56" s="89">
         <f t="shared" ref="AE56:AF56" si="32">SUM(AE44:AE50)</f>
         <v>333238.03423646506</v>
       </c>
-      <c r="AF56" s="90">
+      <c r="AF56" s="89">
         <f t="shared" si="32"/>
         <v>225831.46956745218</v>
       </c>
@@ -16697,43 +17056,43 @@
       <c r="Q57" s="44"/>
       <c r="R57" s="44"/>
       <c r="S57" s="44"/>
-      <c r="T57" s="91">
+      <c r="T57" s="90">
         <f>T56/U16</f>
         <v>0.46467108122034878</v>
       </c>
-      <c r="U57" s="91">
+      <c r="U57" s="90">
         <f>U56/V16</f>
         <v>0.19780752145964681</v>
       </c>
-      <c r="V57" s="91">
+      <c r="V57" s="90">
         <f>V56/W16</f>
         <v>9.5870840330432514E-2</v>
       </c>
       <c r="W57" s="44"/>
       <c r="X57" s="44"/>
-      <c r="Y57" s="92">
+      <c r="Y57" s="91">
         <f>Y56/U16</f>
         <v>0.58641486673015575</v>
       </c>
-      <c r="Z57" s="92">
+      <c r="Z57" s="91">
         <f>Z56/V16</f>
         <v>0.33589293167288797</v>
       </c>
-      <c r="AA57" s="92">
+      <c r="AA57" s="91">
         <f>AA56/W16</f>
         <v>0.20828456107090187</v>
       </c>
       <c r="AB57" s="44"/>
       <c r="AC57" s="44"/>
-      <c r="AD57" s="92">
+      <c r="AD57" s="91">
         <f>AD56/U16</f>
         <v>0.65204744199565845</v>
       </c>
-      <c r="AE57" s="92">
+      <c r="AE57" s="91">
         <f>AE56/V16</f>
         <v>0.43483693597194278</v>
       </c>
-      <c r="AF57" s="92">
+      <c r="AF57" s="91">
         <f>AF56/W16</f>
         <v>0.31173688837865487</v>
       </c>
@@ -19377,7 +19736,6 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AH28:AL28"/>
     <mergeCell ref="S42:V42"/>
     <mergeCell ref="X42:AA42"/>
     <mergeCell ref="AC42:AF42"/>
@@ -19386,9 +19744,47 @@
     <mergeCell ref="Z5:AB5"/>
     <mergeCell ref="AD5:AF5"/>
     <mergeCell ref="P12:R12"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="AA28:AE28"/>
+    <mergeCell ref="T28:AA28"/>
+    <mergeCell ref="AM28:AU28"/>
+    <mergeCell ref="AC28:AK28"/>
   </mergeCells>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <conditionalFormatting sqref="T30:AA38">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD30:AK38">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN30:AU38">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update Retrofit selection in #SYS_addational assumptions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A14DDD-5851-4582-9942-264E8727B42D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4B41B6-C091-40C2-86A5-567849B49D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-8145" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="344">
   <si>
     <t>UC_N</t>
   </si>
@@ -1203,7 +1203,37 @@
     <t>None</t>
   </si>
   <si>
-    <t>Add "Y" for suboptimal heatpumps</t>
+    <t>Select HLI for heat pump</t>
+  </si>
+  <si>
+    <t>Apartments</t>
+  </si>
+  <si>
+    <t>R-BLD_Apt_B1</t>
+  </si>
+  <si>
+    <t>R-BLD_Apt_B2</t>
+  </si>
+  <si>
+    <t>R-BLD_Apt_A</t>
+  </si>
+  <si>
+    <t>R-BLD_Att_A</t>
+  </si>
+  <si>
+    <t>R-BLD_Att_B1</t>
+  </si>
+  <si>
+    <t>R-BLD_Att_B2</t>
+  </si>
+  <si>
+    <t>R-BLD_Det_A</t>
+  </si>
+  <si>
+    <t>R-BLD_Det_B1</t>
+  </si>
+  <si>
+    <t>R-BLD_Det_B2</t>
   </si>
 </sst>
 </file>
@@ -2032,6 +2062,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2041,19 +2072,18 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -2455,13 +2485,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>10584</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>10583</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>230717</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -2516,16 +2546,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>407457</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>179916</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>312207</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>129381</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>576771</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>111579</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>598715</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>84365</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2555,8 +2585,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="27525132" y="3561291"/>
-          <a:ext cx="2607714" cy="884163"/>
+          <a:off x="32493100" y="3898560"/>
+          <a:ext cx="2123472" cy="716984"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2577,14 +2607,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>79376</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>153458</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>392642</xdr:colOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>392643</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>136979</xdr:rowOff>
     </xdr:to>
@@ -2638,16 +2668,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>179206</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>111171</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>63499</xdr:rowOff>
+      <xdr:rowOff>90714</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>325315</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>353787</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>20454</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2675,8 +2705,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30344881" y="825499"/>
-          <a:ext cx="3194108" cy="2260600"/>
+          <a:off x="34129028" y="852714"/>
+          <a:ext cx="2079580" cy="1562597"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3449,12 +3479,12 @@
       <c r="Z15" s="46"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="96" t="s">
+      <c r="A16" s="97" t="s">
         <v>253</v>
       </c>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="97"/>
       <c r="E16" s="47"/>
       <c r="F16" s="47"/>
       <c r="G16" s="48"/>
@@ -3538,11 +3568,11 @@
       <c r="A19" s="52" t="s">
         <v>254</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
       <c r="E19" s="53"/>
       <c r="F19" s="53"/>
       <c r="G19" s="54"/>
@@ -3570,11 +3600,11 @@
       <c r="A20" s="52" t="s">
         <v>255</v>
       </c>
-      <c r="B20" s="95" t="s">
+      <c r="B20" s="96" t="s">
         <v>266</v>
       </c>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
       <c r="E20" s="53"/>
       <c r="F20" s="53"/>
       <c r="G20" s="54"/>
@@ -3662,11 +3692,11 @@
       <c r="A23" s="52" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="95" t="s">
+      <c r="B23" s="96" t="s">
         <v>265</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="46"/>
       <c r="F23" s="46"/>
       <c r="G23" s="46"/>
@@ -3752,11 +3782,11 @@
       <c r="A26" s="52" t="s">
         <v>258</v>
       </c>
-      <c r="B26" s="95" t="s">
+      <c r="B26" s="96" t="s">
         <v>265</v>
       </c>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="96"/>
       <c r="E26" s="46"/>
       <c r="F26" s="46"/>
       <c r="G26" s="46"/>
@@ -3872,11 +3902,11 @@
       <c r="A30" s="52" t="s">
         <v>260</v>
       </c>
-      <c r="B30" s="97" t="s">
+      <c r="B30" s="98" t="s">
         <v>261</v>
       </c>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
+      <c r="C30" s="96"/>
+      <c r="D30" s="96"/>
       <c r="E30" s="57"/>
       <c r="F30" s="57"/>
       <c r="G30" s="46"/>
@@ -3904,11 +3934,11 @@
       <c r="A31" s="52" t="s">
         <v>262</v>
       </c>
-      <c r="B31" s="95" t="s">
+      <c r="B31" s="96" t="s">
         <v>263</v>
       </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
+      <c r="C31" s="96"/>
+      <c r="D31" s="96"/>
       <c r="E31" s="57"/>
       <c r="F31" s="57"/>
       <c r="G31" s="46"/>
@@ -13052,10 +13082,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CF89D-3AC9-4E2E-BCF6-79A710F8BD8A}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:AU204"/>
+  <dimension ref="A1:AV204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13068,20 +13098,21 @@
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.7109375" customWidth="1"/>
+    <col min="14" max="14" width="28.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="44" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:40">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:40">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
-      <c r="O2" s="44"/>
       <c r="P2" s="44"/>
       <c r="Q2" s="44"/>
       <c r="R2" s="44"/>
@@ -13106,12 +13137,12 @@
       <c r="AK2" s="44"/>
       <c r="AL2" s="44"/>
       <c r="AM2" s="44"/>
-    </row>
-    <row r="3" spans="1:39">
+      <c r="AN2" s="44"/>
+    </row>
+    <row r="3" spans="1:40">
       <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="44"/>
       <c r="P3" s="44"/>
       <c r="Q3" s="44"/>
       <c r="R3" s="44"/>
@@ -13136,12 +13167,12 @@
       <c r="AK3" s="44"/>
       <c r="AL3" s="44"/>
       <c r="AM3" s="44"/>
-    </row>
-    <row r="4" spans="1:39">
+      <c r="AN3" s="44"/>
+    </row>
+    <row r="4" spans="1:40">
       <c r="I4" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="44"/>
       <c r="P4" s="44"/>
       <c r="Q4" s="44"/>
       <c r="R4" s="44"/>
@@ -13161,15 +13192,16 @@
       <c r="AF4" s="44"/>
       <c r="AG4" s="44"/>
       <c r="AH4" s="44"/>
-      <c r="AI4" s="44" t="s">
+      <c r="AI4" s="44"/>
+      <c r="AJ4" s="44" t="s">
         <v>276</v>
       </c>
-      <c r="AJ4" s="44"/>
       <c r="AK4" s="44"/>
       <c r="AL4" s="44"/>
       <c r="AM4" s="44"/>
-    </row>
-    <row r="5" spans="1:39" ht="21.75" thickBot="1">
+      <c r="AN4" s="44"/>
+    </row>
+    <row r="5" spans="1:40" ht="21.75" thickBot="1">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -13203,41 +13235,44 @@
       <c r="L5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="44"/>
-      <c r="P5" s="100" t="s">
+      <c r="N5" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="99" t="s">
         <v>277</v>
       </c>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="100" t="s">
+      <c r="R5" s="99"/>
+      <c r="S5" s="99"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="99" t="s">
         <v>278</v>
       </c>
-      <c r="U5" s="100"/>
-      <c r="V5" s="100"/>
-      <c r="W5" s="100"/>
-      <c r="X5" s="100"/>
-      <c r="Y5" s="44"/>
-      <c r="Z5" s="100" t="s">
+      <c r="V5" s="99"/>
+      <c r="W5" s="99"/>
+      <c r="X5" s="99"/>
+      <c r="Y5" s="99"/>
+      <c r="Z5" s="44"/>
+      <c r="AA5" s="99" t="s">
         <v>279</v>
       </c>
-      <c r="AA5" s="100"/>
-      <c r="AB5" s="100"/>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="100" t="s">
+      <c r="AB5" s="99"/>
+      <c r="AC5" s="99"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="99" t="s">
         <v>280</v>
       </c>
-      <c r="AE5" s="100"/>
-      <c r="AF5" s="100"/>
-      <c r="AG5" s="44"/>
+      <c r="AF5" s="99"/>
+      <c r="AG5" s="99"/>
       <c r="AH5" s="44"/>
       <c r="AI5" s="44"/>
       <c r="AJ5" s="44"/>
       <c r="AK5" s="44"/>
       <c r="AL5" s="44"/>
       <c r="AM5" s="44"/>
-    </row>
-    <row r="6" spans="1:39" ht="15.75" thickBot="1">
+      <c r="AN5" s="44"/>
+    </row>
+    <row r="6" spans="1:40" ht="15.75" thickBot="1">
       <c r="B6" t="s">
         <v>95</v>
       </c>
@@ -13262,64 +13297,64 @@
       <c r="L6" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="N6" t="s">
-        <v>333</v>
-      </c>
-      <c r="O6" s="44"/>
-      <c r="P6" s="60" t="s">
+      <c r="N6" s="44" t="s">
+        <v>334</v>
+      </c>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="Q6" s="60" t="s">
+      <c r="R6" s="60" t="s">
         <v>282</v>
       </c>
-      <c r="R6" s="60" t="s">
+      <c r="S6" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="S6" s="44"/>
-      <c r="T6" s="61" t="s">
+      <c r="T6" s="44"/>
+      <c r="U6" s="61" t="s">
         <v>284</v>
       </c>
-      <c r="U6" s="60" t="s">
+      <c r="V6" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="V6" s="60" t="s">
+      <c r="W6" s="60" t="s">
         <v>282</v>
       </c>
-      <c r="W6" s="60" t="s">
+      <c r="X6" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="X6" s="62" t="s">
+      <c r="Y6" s="62" t="s">
         <v>285</v>
       </c>
-      <c r="Y6" s="44"/>
-      <c r="Z6" s="63" t="s">
+      <c r="Z6" s="44"/>
+      <c r="AA6" s="63" t="s">
         <v>281</v>
       </c>
-      <c r="AA6" s="64" t="s">
+      <c r="AB6" s="64" t="s">
         <v>282</v>
       </c>
-      <c r="AB6" s="65" t="s">
+      <c r="AC6" s="65" t="s">
         <v>283</v>
       </c>
-      <c r="AC6" s="44"/>
-      <c r="AD6" s="63" t="s">
+      <c r="AD6" s="44"/>
+      <c r="AE6" s="63" t="s">
         <v>281</v>
       </c>
-      <c r="AE6" s="64" t="s">
+      <c r="AF6" s="64" t="s">
         <v>282</v>
       </c>
-      <c r="AF6" s="65" t="s">
+      <c r="AG6" s="65" t="s">
         <v>283</v>
       </c>
-      <c r="AG6" s="44"/>
       <c r="AH6" s="44"/>
       <c r="AI6" s="44"/>
       <c r="AJ6" s="44"/>
       <c r="AK6" s="44"/>
       <c r="AL6" s="44"/>
       <c r="AM6" s="44"/>
-    </row>
-    <row r="7" spans="1:39">
+      <c r="AN6" s="44"/>
+    </row>
+    <row r="7" spans="1:40">
       <c r="D7" s="27" t="s">
         <v>270</v>
       </c>
@@ -13331,69 +13366,71 @@
       </c>
       <c r="I7" s="27"/>
       <c r="J7" s="92">
-        <f>IF(N7="Y",0,-(X33))</f>
-        <v>-0.99999998312382343</v>
+        <f>-INDEX($U$30:$AB$38,MATCH(D7,$T$30:$T$38,0),MATCH($N$7,$U$29:$AB$29,0))</f>
+        <v>0</v>
       </c>
       <c r="K7" s="27"/>
       <c r="L7" s="27"/>
-      <c r="N7" s="102"/>
-      <c r="O7" s="66" t="s">
+      <c r="N7" s="95" t="s">
+        <v>332</v>
+      </c>
+      <c r="P7" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="P7" s="67">
+      <c r="Q7" s="67">
         <v>68452</v>
       </c>
-      <c r="Q7" s="67">
+      <c r="R7" s="67">
         <v>94025</v>
       </c>
-      <c r="R7" s="67">
+      <c r="S7" s="67">
         <v>31885</v>
       </c>
-      <c r="S7" s="44"/>
-      <c r="T7" s="66" t="s">
+      <c r="T7" s="44"/>
+      <c r="U7" s="66" t="s">
         <v>287</v>
       </c>
-      <c r="U7" s="68">
+      <c r="V7" s="68">
         <v>11735.038424732089</v>
       </c>
-      <c r="V7" s="68">
+      <c r="W7" s="68">
         <v>72528.642938868245</v>
       </c>
-      <c r="W7" s="68">
+      <c r="X7" s="68">
         <v>37364.451209178158</v>
       </c>
-      <c r="X7" s="69">
+      <c r="Y7" s="69">
         <v>121628.1325727785</v>
       </c>
-      <c r="Y7" s="44"/>
-      <c r="Z7" s="70">
+      <c r="Z7" s="44"/>
+      <c r="AA7" s="70">
         <v>1.0049999999999999</v>
       </c>
-      <c r="AA7" s="70">
+      <c r="AB7" s="70">
         <v>1.149</v>
       </c>
-      <c r="AB7" s="70">
+      <c r="AC7" s="70">
         <v>1.36</v>
       </c>
-      <c r="AC7" s="44"/>
-      <c r="AD7" s="70">
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="70">
         <v>0.27300000000000002</v>
       </c>
-      <c r="AE7" s="70">
+      <c r="AF7" s="70">
         <v>0.34200000000000003</v>
       </c>
-      <c r="AF7" s="70">
+      <c r="AG7" s="70">
         <v>0.21299999999999999</v>
       </c>
-      <c r="AG7" s="44"/>
       <c r="AH7" s="44"/>
       <c r="AI7" s="44"/>
       <c r="AJ7" s="44"/>
       <c r="AK7" s="44"/>
       <c r="AL7" s="44"/>
       <c r="AM7" s="44"/>
-    </row>
-    <row r="8" spans="1:39" s="44" customFormat="1">
+      <c r="AN7" s="44"/>
+    </row>
+    <row r="8" spans="1:40" s="44" customFormat="1">
       <c r="D8" s="27" t="s">
         <v>271</v>
       </c>
@@ -13405,59 +13442,58 @@
       </c>
       <c r="I8" s="27"/>
       <c r="J8" s="92">
-        <f t="shared" ref="J8:J12" si="0">IF(N8="Y",0,-(X34))</f>
-        <v>-0.99417194789886376</v>
+        <f>-INDEX($U$30:$AB$38,MATCH(D8,$T$30:$T$38,0),MATCH($N$7,$U$29:$AB$29,0))</f>
+        <v>0</v>
       </c>
       <c r="K8" s="27"/>
       <c r="L8" s="27"/>
-      <c r="N8" s="102"/>
-      <c r="O8" s="71" t="s">
+      <c r="P8" s="71" t="s">
         <v>288</v>
       </c>
-      <c r="P8" s="72">
+      <c r="Q8" s="72">
         <v>96213</v>
       </c>
-      <c r="Q8" s="72">
+      <c r="R8" s="72">
         <v>187505</v>
       </c>
-      <c r="R8" s="72">
+      <c r="S8" s="72">
         <v>72100</v>
       </c>
-      <c r="T8" s="71" t="s">
+      <c r="U8" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="U8" s="73">
+      <c r="V8" s="73">
         <v>5197.6132443555907</v>
       </c>
-      <c r="V8" s="73">
+      <c r="W8" s="73">
         <v>6727.4572369101443</v>
       </c>
-      <c r="W8" s="73">
+      <c r="X8" s="73">
         <v>8186.7925913057998</v>
       </c>
-      <c r="X8" s="74">
+      <c r="Y8" s="74">
         <v>20111.863072571534</v>
       </c>
-      <c r="Z8" s="75">
+      <c r="AA8" s="75">
         <v>1.3959999999999999</v>
       </c>
-      <c r="AA8" s="75">
+      <c r="AB8" s="75">
         <v>1.6719999999999999</v>
       </c>
-      <c r="AB8" s="75">
+      <c r="AC8" s="75">
         <v>1.9019999999999999</v>
       </c>
-      <c r="AD8" s="75">
+      <c r="AE8" s="75">
         <v>0.32400000000000001</v>
       </c>
-      <c r="AE8" s="75">
+      <c r="AF8" s="75">
         <v>0.44500000000000001</v>
       </c>
-      <c r="AF8" s="75">
+      <c r="AG8" s="75">
         <v>0.34100000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:39" s="44" customFormat="1">
+    <row r="9" spans="1:40" s="44" customFormat="1">
       <c r="D9" s="27" t="s">
         <v>272</v>
       </c>
@@ -13469,59 +13505,58 @@
       </c>
       <c r="I9" s="27"/>
       <c r="J9" s="92">
-        <f t="shared" si="0"/>
-        <v>-0.92710242952401201</v>
+        <f t="shared" ref="J9:J12" si="0">-INDEX($U$30:$AB$38,MATCH(D9,$T$30:$T$38,0),MATCH($N$7,$U$29:$AB$29,0))</f>
+        <v>0</v>
       </c>
       <c r="K9" s="27"/>
       <c r="L9" s="27"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="76" t="s">
+      <c r="P9" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="P9" s="77">
+      <c r="Q9" s="77">
         <v>109864</v>
       </c>
-      <c r="Q9" s="77">
+      <c r="R9" s="77">
         <v>248054</v>
       </c>
-      <c r="R9" s="77">
+      <c r="S9" s="77">
         <v>106981</v>
       </c>
-      <c r="T9" s="76" t="s">
+      <c r="U9" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="U9" s="78">
+      <c r="V9" s="78">
         <v>13979.419134898935</v>
       </c>
-      <c r="V9" s="78">
+      <c r="W9" s="78">
         <v>14584.48055403824</v>
       </c>
-      <c r="W9" s="78">
+      <c r="X9" s="78">
         <v>18974.694526816245</v>
       </c>
-      <c r="X9" s="79">
+      <c r="Y9" s="79">
         <v>47538.594215753423</v>
       </c>
-      <c r="Z9" s="80">
+      <c r="AA9" s="80">
         <v>1.5840000000000001</v>
       </c>
-      <c r="AA9" s="80">
+      <c r="AB9" s="80">
         <v>1.8440000000000001</v>
       </c>
-      <c r="AB9" s="80">
+      <c r="AC9" s="80">
         <v>2.125</v>
       </c>
-      <c r="AD9" s="80">
+      <c r="AE9" s="80">
         <v>0.26800000000000002</v>
       </c>
-      <c r="AE9" s="80">
+      <c r="AF9" s="80">
         <v>0.45700000000000002</v>
       </c>
-      <c r="AF9" s="80">
+      <c r="AG9" s="80">
         <v>0.307</v>
       </c>
     </row>
-    <row r="10" spans="1:39" s="44" customFormat="1">
+    <row r="10" spans="1:40" s="44" customFormat="1">
       <c r="D10" s="27" t="s">
         <v>273</v>
       </c>
@@ -13534,58 +13569,57 @@
       <c r="I10" s="27"/>
       <c r="J10" s="92">
         <f t="shared" si="0"/>
-        <v>-0.87051976694100974</v>
+        <v>0</v>
       </c>
       <c r="K10" s="27"/>
       <c r="L10" s="27"/>
-      <c r="N10" s="102"/>
-      <c r="O10" s="71" t="s">
+      <c r="P10" s="71" t="s">
         <v>292</v>
       </c>
-      <c r="P10" s="72">
+      <c r="Q10" s="72">
         <v>119296</v>
       </c>
-      <c r="Q10" s="72">
+      <c r="R10" s="72">
         <v>292259</v>
       </c>
-      <c r="R10" s="72">
+      <c r="S10" s="72">
         <v>142753</v>
       </c>
-      <c r="T10" s="71" t="s">
+      <c r="U10" s="71" t="s">
         <v>293</v>
       </c>
-      <c r="U10" s="73">
+      <c r="V10" s="73">
         <v>21709.86153487581</v>
       </c>
-      <c r="V10" s="73">
+      <c r="W10" s="73">
         <v>49420.927051735707</v>
       </c>
-      <c r="W10" s="73">
+      <c r="X10" s="73">
         <v>54549.088898874157</v>
       </c>
-      <c r="X10" s="74">
+      <c r="Y10" s="74">
         <v>125679.87748548566</v>
       </c>
-      <c r="Z10" s="75">
+      <c r="AA10" s="75">
         <v>1.772</v>
       </c>
-      <c r="AA10" s="75">
+      <c r="AB10" s="75">
         <v>2.0150000000000001</v>
       </c>
-      <c r="AB10" s="75">
+      <c r="AC10" s="75">
         <v>2.3069999999999999</v>
       </c>
-      <c r="AD10" s="75">
+      <c r="AE10" s="75">
         <v>0.313</v>
       </c>
-      <c r="AE10" s="75">
+      <c r="AF10" s="75">
         <v>0.42799999999999999</v>
       </c>
-      <c r="AF10" s="75">
+      <c r="AG10" s="75">
         <v>0.29599999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:39" s="44" customFormat="1">
+    <row r="11" spans="1:40" s="44" customFormat="1">
       <c r="D11" s="27" t="s">
         <v>275</v>
       </c>
@@ -13598,58 +13632,57 @@
       <c r="I11" s="27"/>
       <c r="J11" s="92">
         <f t="shared" si="0"/>
-        <v>-0.58254904641534866</v>
+        <v>0</v>
       </c>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
-      <c r="N11" s="102"/>
-      <c r="O11" s="76" t="s">
+      <c r="P11" s="76" t="s">
         <v>294</v>
       </c>
-      <c r="P11" s="77">
+      <c r="Q11" s="77">
         <v>25861</v>
       </c>
-      <c r="Q11" s="77">
+      <c r="R11" s="77">
         <v>158745</v>
       </c>
-      <c r="R11" s="77">
+      <c r="S11" s="77">
         <v>157558</v>
       </c>
-      <c r="T11" s="76" t="s">
+      <c r="U11" s="76" t="s">
         <v>295</v>
       </c>
-      <c r="U11" s="78">
+      <c r="V11" s="78">
         <v>71167.091754613168</v>
       </c>
-      <c r="V11" s="78">
+      <c r="W11" s="78">
         <v>293672.95873330871</v>
       </c>
-      <c r="W11" s="78">
+      <c r="X11" s="78">
         <v>264765.40185365622</v>
       </c>
-      <c r="X11" s="79">
+      <c r="Y11" s="79">
         <v>629605.45234157809</v>
       </c>
-      <c r="Z11" s="80">
+      <c r="AA11" s="80">
         <v>1.9790000000000001</v>
       </c>
-      <c r="AA11" s="80">
+      <c r="AB11" s="80">
         <v>2.3239999999999998</v>
       </c>
-      <c r="AB11" s="80">
+      <c r="AC11" s="80">
         <v>2.61</v>
       </c>
-      <c r="AD11" s="80">
+      <c r="AE11" s="80">
         <v>0.60299999999999998</v>
       </c>
-      <c r="AE11" s="80">
+      <c r="AF11" s="80">
         <v>0.48899999999999999</v>
       </c>
-      <c r="AF11" s="80">
+      <c r="AG11" s="80">
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:39" s="44" customFormat="1" ht="16.5" thickBot="1">
+    <row r="12" spans="1:40" s="44" customFormat="1" ht="16.5" thickBot="1">
       <c r="D12" s="27" t="s">
         <v>274</v>
       </c>
@@ -13662,51 +13695,50 @@
       <c r="I12" s="27"/>
       <c r="J12" s="92">
         <f t="shared" si="0"/>
-        <v>-0.20397754353748057</v>
+        <v>0</v>
       </c>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
-      <c r="N12" s="102"/>
-      <c r="P12" s="101" t="s">
+      <c r="Q12" s="100" t="s">
         <v>296</v>
       </c>
-      <c r="Q12" s="101"/>
-      <c r="R12" s="101"/>
-      <c r="T12" s="71" t="s">
+      <c r="R12" s="100"/>
+      <c r="S12" s="100"/>
+      <c r="U12" s="71" t="s">
         <v>297</v>
       </c>
-      <c r="U12" s="73">
+      <c r="V12" s="73">
         <v>47490.854787158918</v>
       </c>
-      <c r="V12" s="73">
+      <c r="W12" s="73">
         <v>175920.34461876052</v>
       </c>
-      <c r="W12" s="73">
+      <c r="X12" s="73">
         <v>166984.19754801539</v>
       </c>
-      <c r="X12" s="74">
+      <c r="Y12" s="74">
         <v>390395.3969539348</v>
       </c>
-      <c r="Z12" s="75">
+      <c r="AA12" s="75">
         <v>2.2679999999999998</v>
       </c>
-      <c r="AA12" s="75">
+      <c r="AB12" s="75">
         <v>2.851</v>
       </c>
-      <c r="AB12" s="75">
+      <c r="AC12" s="75">
         <v>3.0779999999999998</v>
       </c>
-      <c r="AD12" s="75">
+      <c r="AE12" s="75">
         <v>0.84699999999999998</v>
       </c>
-      <c r="AE12" s="75">
+      <c r="AF12" s="75">
         <v>0.63400000000000001</v>
       </c>
-      <c r="AF12" s="75">
+      <c r="AG12" s="75">
         <v>0.68200000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15.75" thickBot="1">
+    <row r="13" spans="1:40" ht="15.75" thickBot="1">
       <c r="D13" s="27" t="s">
         <v>206</v>
       </c>
@@ -13724,62 +13756,62 @@
       </c>
       <c r="K13" s="27"/>
       <c r="L13" s="27"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="81" t="s">
+      <c r="N13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="81" t="s">
         <v>298</v>
       </c>
-      <c r="Q13" s="81" t="s">
+      <c r="R13" s="81" t="s">
         <v>299</v>
       </c>
-      <c r="R13" s="81" t="s">
+      <c r="S13" s="81" t="s">
         <v>300</v>
       </c>
-      <c r="S13" s="44"/>
-      <c r="T13" s="76" t="s">
+      <c r="T13" s="44"/>
+      <c r="U13" s="76" t="s">
         <v>301</v>
       </c>
-      <c r="U13" s="78">
+      <c r="V13" s="78">
         <v>23790.684938210514</v>
       </c>
-      <c r="V13" s="78">
+      <c r="W13" s="78">
         <v>85755.437936808186</v>
       </c>
-      <c r="W13" s="78">
+      <c r="X13" s="78">
         <v>74836.881491341002</v>
       </c>
-      <c r="X13" s="79">
+      <c r="Y13" s="79">
         <v>184383.0043663597</v>
       </c>
-      <c r="Y13" s="44"/>
-      <c r="Z13" s="80">
+      <c r="Z13" s="44"/>
+      <c r="AA13" s="80">
         <v>2.694</v>
       </c>
-      <c r="AA13" s="80">
+      <c r="AB13" s="80">
         <v>3.512</v>
       </c>
-      <c r="AB13" s="80">
+      <c r="AC13" s="80">
         <v>3.7839999999999998</v>
       </c>
-      <c r="AC13" s="44"/>
-      <c r="AD13" s="80">
+      <c r="AD13" s="44"/>
+      <c r="AE13" s="80">
         <v>0.71399999999999997</v>
       </c>
-      <c r="AE13" s="80">
+      <c r="AF13" s="80">
         <v>0.92200000000000004</v>
       </c>
-      <c r="AF13" s="80">
+      <c r="AG13" s="80">
         <v>0.94</v>
       </c>
-      <c r="AG13" s="44"/>
       <c r="AH13" s="44"/>
       <c r="AI13" s="44"/>
       <c r="AJ13" s="44"/>
       <c r="AK13" s="44"/>
       <c r="AL13" s="44"/>
       <c r="AM13" s="44"/>
-    </row>
-    <row r="14" spans="1:39">
+      <c r="AN13" s="44"/>
+    </row>
+    <row r="14" spans="1:40">
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
@@ -13795,64 +13827,64 @@
         <v>5</v>
       </c>
       <c r="L14" s="28"/>
-      <c r="N14" s="102"/>
-      <c r="O14" s="66" t="s">
+      <c r="N14" s="44"/>
+      <c r="P14" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="P14" s="67">
+      <c r="Q14" s="67">
         <v>64661</v>
       </c>
-      <c r="Q14" s="67">
+      <c r="R14" s="67">
         <v>74932</v>
       </c>
-      <c r="R14" s="67">
+      <c r="S14" s="67">
         <v>19753</v>
       </c>
-      <c r="S14" s="44"/>
-      <c r="T14" s="71" t="s">
+      <c r="T14" s="44"/>
+      <c r="U14" s="71" t="s">
         <v>302</v>
       </c>
-      <c r="U14" s="73">
+      <c r="V14" s="73">
         <v>8010.7993972868508</v>
       </c>
-      <c r="V14" s="73">
+      <c r="W14" s="73">
         <v>38588.997221862926</v>
       </c>
-      <c r="W14" s="73">
+      <c r="X14" s="73">
         <v>37368.747662299225</v>
       </c>
-      <c r="X14" s="74">
+      <c r="Y14" s="74">
         <v>83968.544281448994</v>
       </c>
-      <c r="Y14" s="44"/>
-      <c r="Z14" s="75">
+      <c r="Z14" s="44"/>
+      <c r="AA14" s="75">
         <v>3.2970000000000002</v>
       </c>
-      <c r="AA14" s="75">
+      <c r="AB14" s="75">
         <v>4.1100000000000003</v>
       </c>
-      <c r="AB14" s="75">
+      <c r="AC14" s="75">
         <v>4.5039999999999996</v>
       </c>
-      <c r="AC14" s="44"/>
-      <c r="AD14" s="75">
+      <c r="AD14" s="44"/>
+      <c r="AE14" s="75">
         <v>0.97399999999999998</v>
       </c>
-      <c r="AE14" s="75">
+      <c r="AF14" s="75">
         <v>1.141</v>
       </c>
-      <c r="AF14" s="75">
+      <c r="AG14" s="75">
         <v>1.026</v>
       </c>
-      <c r="AG14" s="44"/>
       <c r="AH14" s="44"/>
       <c r="AI14" s="44"/>
       <c r="AJ14" s="44"/>
       <c r="AK14" s="44"/>
       <c r="AL14" s="44"/>
       <c r="AM14" s="44"/>
-    </row>
-    <row r="15" spans="1:39" ht="15.75" thickBot="1">
+      <c r="AN14" s="44"/>
+    </row>
+    <row r="15" spans="1:40" ht="15.75" thickBot="1">
       <c r="B15" t="s">
         <v>94</v>
       </c>
@@ -13877,64 +13909,67 @@
       <c r="L15" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="O15" s="71" t="s">
+      <c r="N15" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="P15" s="71" t="s">
         <v>288</v>
       </c>
-      <c r="P15" s="72">
+      <c r="Q15" s="72">
         <v>92181</v>
       </c>
-      <c r="Q15" s="72">
+      <c r="R15" s="72">
         <v>167226</v>
       </c>
-      <c r="R15" s="72">
+      <c r="S15" s="72">
         <v>58089</v>
       </c>
-      <c r="S15" s="44"/>
-      <c r="T15" s="82" t="s">
+      <c r="T15" s="44"/>
+      <c r="U15" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="U15" s="83">
+      <c r="V15" s="83">
         <v>8658.126308421115</v>
       </c>
-      <c r="V15" s="83">
+      <c r="W15" s="83">
         <v>38905.107366988203</v>
       </c>
-      <c r="W15" s="83">
+      <c r="X15" s="83">
         <v>66469.176419880765</v>
       </c>
-      <c r="X15" s="79">
+      <c r="Y15" s="79">
         <v>114032.41009529008</v>
       </c>
-      <c r="Y15" s="44"/>
-      <c r="Z15" s="84">
+      <c r="Z15" s="44"/>
+      <c r="AA15" s="84">
         <v>4.7880000000000003</v>
       </c>
-      <c r="AA15" s="84">
+      <c r="AB15" s="84">
         <v>5.0789999999999997</v>
       </c>
-      <c r="AB15" s="84">
+      <c r="AC15" s="84">
         <v>6.0039999999999996</v>
       </c>
-      <c r="AC15" s="44"/>
-      <c r="AD15" s="93">
-        <f>AVERAGE(AE15:AF15)</f>
+      <c r="AD15" s="44"/>
+      <c r="AE15" s="93">
+        <f>AVERAGE(AF15:AG15)</f>
         <v>1.5565</v>
       </c>
-      <c r="AE15" s="84">
+      <c r="AF15" s="84">
         <v>1.6439999999999999</v>
       </c>
-      <c r="AF15" s="84">
+      <c r="AG15" s="84">
         <v>1.4690000000000001</v>
       </c>
-      <c r="AG15" s="44"/>
       <c r="AH15" s="44"/>
       <c r="AI15" s="44"/>
       <c r="AJ15" s="44"/>
       <c r="AK15" s="44"/>
       <c r="AL15" s="44"/>
       <c r="AM15" s="44"/>
-    </row>
-    <row r="16" spans="1:39" ht="15.75" thickBot="1">
+      <c r="AN15" s="44"/>
+    </row>
+    <row r="16" spans="1:40" ht="15.75" thickBot="1">
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
       <c r="D16" s="27" t="s">
@@ -13948,42 +13983,43 @@
       </c>
       <c r="I16" s="27"/>
       <c r="J16" s="92">
-        <f>IF(N16="Y",0,-(AH33))</f>
-        <v>-0.99973940839121955</v>
+        <f>-INDEX($AE$30:$AL$38,MATCH(D16,$AD$30:$AD$38,0),MATCH($N$16,$AE$29:$AL$29,0))</f>
+        <v>0</v>
       </c>
       <c r="K16" s="27"/>
       <c r="L16" s="27"/>
       <c r="M16" s="44"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="76" t="s">
+      <c r="N16" s="95" t="s">
+        <v>332</v>
+      </c>
+      <c r="P16" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="P16" s="77">
+      <c r="Q16" s="77">
         <v>105755</v>
       </c>
-      <c r="Q16" s="77">
+      <c r="R16" s="77">
         <v>227371</v>
       </c>
-      <c r="R16" s="77">
+      <c r="S16" s="77">
         <v>92325</v>
       </c>
-      <c r="S16" s="44"/>
-      <c r="T16" s="85" t="s">
+      <c r="T16" s="44"/>
+      <c r="U16" s="85" t="s">
         <v>304</v>
       </c>
-      <c r="U16" s="86">
+      <c r="V16" s="86">
         <v>211739.48952455298</v>
       </c>
-      <c r="V16" s="86">
+      <c r="W16" s="86">
         <v>776104.35365928081</v>
       </c>
-      <c r="W16" s="86">
+      <c r="X16" s="86">
         <v>729499.43220136687</v>
       </c>
-      <c r="X16" s="87">
+      <c r="Y16" s="87">
         <v>1717343.2753852005</v>
       </c>
-      <c r="Y16" s="44"/>
       <c r="Z16" s="44"/>
       <c r="AA16" s="44"/>
       <c r="AB16" s="44"/>
@@ -13998,8 +14034,9 @@
       <c r="AK16" s="44"/>
       <c r="AL16" s="44"/>
       <c r="AM16" s="44"/>
-    </row>
-    <row r="17" spans="2:47">
+      <c r="AN16" s="44"/>
+    </row>
+    <row r="17" spans="2:48">
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
       <c r="D17" s="27" t="s">
@@ -14013,26 +14050,25 @@
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="92">
-        <f>IF(N17="Y",0,-(AH34))</f>
-        <v>-0.99191173064402915</v>
+        <f t="shared" ref="J17:J21" si="1">-INDEX($AE$30:$AL$38,MATCH(D17,$AD$30:$AD$38,0),MATCH($N$16,$AE$29:$AL$29,0))</f>
+        <v>0</v>
       </c>
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
       <c r="M17" s="44"/>
       <c r="N17" s="44"/>
-      <c r="O17" s="71" t="s">
+      <c r="P17" s="71" t="s">
         <v>292</v>
       </c>
-      <c r="P17" s="72">
+      <c r="Q17" s="72">
         <v>115137</v>
       </c>
-      <c r="Q17" s="72">
+      <c r="R17" s="72">
         <v>271365</v>
       </c>
-      <c r="R17" s="72">
+      <c r="S17" s="72">
         <v>127680</v>
       </c>
-      <c r="S17" s="44"/>
       <c r="T17" s="44"/>
       <c r="U17" s="44"/>
       <c r="V17" s="44"/>
@@ -14053,8 +14089,9 @@
       <c r="AK17" s="44"/>
       <c r="AL17" s="44"/>
       <c r="AM17" s="44"/>
-    </row>
-    <row r="18" spans="2:47">
+      <c r="AN17" s="44"/>
+    </row>
+    <row r="18" spans="2:48">
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
       <c r="D18" s="27" t="s">
@@ -14068,26 +14105,25 @@
       </c>
       <c r="I18" s="27"/>
       <c r="J18" s="92">
-        <f t="shared" ref="J18:J21" si="1">IF(N18="Y",0,-(AH35))</f>
-        <v>-0.8470018886690438</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
       <c r="M18" s="44"/>
       <c r="N18" s="44"/>
-      <c r="O18" s="76" t="s">
+      <c r="P18" s="76" t="s">
         <v>294</v>
       </c>
-      <c r="P18" s="77">
+      <c r="Q18" s="77">
         <v>25764</v>
       </c>
-      <c r="Q18" s="77">
+      <c r="R18" s="77">
         <v>158416</v>
       </c>
-      <c r="R18" s="77">
+      <c r="S18" s="77">
         <v>156690</v>
       </c>
-      <c r="S18" s="44"/>
       <c r="T18" s="44"/>
       <c r="U18" s="44"/>
       <c r="V18" s="44"/>
@@ -14108,8 +14144,9 @@
       <c r="AK18" s="44"/>
       <c r="AL18" s="44"/>
       <c r="AM18" s="44"/>
-    </row>
-    <row r="19" spans="2:47">
+      <c r="AN18" s="44"/>
+    </row>
+    <row r="19" spans="2:48">
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
       <c r="D19" s="27" t="s">
@@ -14124,20 +14161,19 @@
       <c r="I19" s="27"/>
       <c r="J19" s="92">
         <f t="shared" si="1"/>
-        <v>-0.49480783925100147</v>
+        <v>0</v>
       </c>
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
       <c r="M19" s="44"/>
       <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
       <c r="P19" s="44"/>
       <c r="Q19" s="44"/>
       <c r="R19" s="44"/>
-      <c r="S19" s="44" t="s">
+      <c r="S19" s="44"/>
+      <c r="T19" s="44" t="s">
         <v>305</v>
       </c>
-      <c r="T19" s="44"/>
       <c r="U19" s="44"/>
       <c r="V19" s="44"/>
       <c r="W19" s="44"/>
@@ -14157,8 +14193,9 @@
       <c r="AK19" s="44"/>
       <c r="AL19" s="44"/>
       <c r="AM19" s="44"/>
-    </row>
-    <row r="20" spans="2:47">
+      <c r="AN19" s="44"/>
+    </row>
+    <row r="20" spans="2:48">
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
       <c r="D20" s="27" t="s">
@@ -14172,14 +14209,13 @@
       </c>
       <c r="I20" s="27"/>
       <c r="J20" s="92">
-        <f t="shared" si="1"/>
-        <v>-0.29645675583092174</v>
+        <f>-INDEX($AE$30:$AL$38,MATCH(D20,$AD$30:$AD$38,0),MATCH($N$16,$AE$29:$AL$29,0))</f>
+        <v>0</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
       <c r="M20" s="44"/>
       <c r="N20" s="44"/>
-      <c r="O20" s="44"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="44"/>
@@ -14204,8 +14240,9 @@
       <c r="AK20" s="44"/>
       <c r="AL20" s="44"/>
       <c r="AM20" s="44"/>
-    </row>
-    <row r="21" spans="2:47">
+      <c r="AN20" s="44"/>
+    </row>
+    <row r="21" spans="2:48">
       <c r="D21" s="27" t="s">
         <v>317</v>
       </c>
@@ -14218,20 +14255,19 @@
       <c r="I21" s="27"/>
       <c r="J21" s="92">
         <f t="shared" si="1"/>
-        <v>-0.16841130134712209</v>
+        <v>0</v>
       </c>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
       <c r="M21" s="44"/>
       <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
       <c r="P21" s="44"/>
       <c r="Q21" s="44"/>
       <c r="R21" s="44"/>
-      <c r="S21" s="44" t="s">
+      <c r="S21" s="44"/>
+      <c r="T21" s="44" t="s">
         <v>306</v>
       </c>
-      <c r="T21" s="44"/>
       <c r="U21" s="44"/>
       <c r="V21" s="44"/>
       <c r="W21" s="44"/>
@@ -14251,8 +14287,9 @@
       <c r="AK21" s="44"/>
       <c r="AL21" s="44"/>
       <c r="AM21" s="44"/>
-    </row>
-    <row r="22" spans="2:47">
+      <c r="AN21" s="44"/>
+    </row>
+    <row r="22" spans="2:48">
       <c r="D22" s="27" t="s">
         <v>206</v>
       </c>
@@ -14270,7 +14307,6 @@
       </c>
       <c r="K22" s="27"/>
       <c r="L22" s="27"/>
-      <c r="O22" s="44"/>
       <c r="P22" s="44"/>
       <c r="Q22" s="44"/>
       <c r="R22" s="44"/>
@@ -14295,8 +14331,9 @@
       <c r="AK22" s="44"/>
       <c r="AL22" s="44"/>
       <c r="AM22" s="44"/>
-    </row>
-    <row r="23" spans="2:47">
+      <c r="AN22" s="44"/>
+    </row>
+    <row r="23" spans="2:48">
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
@@ -14311,7 +14348,6 @@
       </c>
       <c r="L23" s="28"/>
       <c r="N23" s="44"/>
-      <c r="O23" s="44"/>
       <c r="P23" s="44"/>
       <c r="Q23" s="44"/>
       <c r="R23" s="44"/>
@@ -14336,8 +14372,9 @@
       <c r="AK23" s="44"/>
       <c r="AL23" s="44"/>
       <c r="AM23" s="44"/>
-    </row>
-    <row r="24" spans="2:47">
+      <c r="AN23" s="44"/>
+    </row>
+    <row r="24" spans="2:48">
       <c r="B24" t="s">
         <v>93</v>
       </c>
@@ -14362,8 +14399,9 @@
       <c r="L24" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="N24" s="44"/>
-      <c r="O24" s="44"/>
+      <c r="N24" s="44" t="s">
+        <v>283</v>
+      </c>
       <c r="P24" s="44"/>
       <c r="Q24" s="44"/>
       <c r="R24" s="44"/>
@@ -14388,8 +14426,9 @@
       <c r="AK24" s="44"/>
       <c r="AL24" s="44"/>
       <c r="AM24" s="44"/>
-    </row>
-    <row r="25" spans="2:47">
+      <c r="AN24" s="44"/>
+    </row>
+    <row r="25" spans="2:48">
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="27" t="s">
@@ -14403,14 +14442,15 @@
       </c>
       <c r="I25" s="27"/>
       <c r="J25" s="92">
-        <f>IF(N25="Y",0,-(AR33))</f>
-        <v>-0.99997215963294783</v>
+        <f>-INDEX($AO$30:$AV$38,MATCH(D25,$AN$30:$AN$38,0),MATCH($N$25,$AO$29:$AV$29,0))</f>
+        <v>0</v>
       </c>
       <c r="K25" s="27"/>
       <c r="L25" s="27"/>
       <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
+      <c r="N25" s="95" t="s">
+        <v>332</v>
+      </c>
       <c r="P25" s="44"/>
       <c r="Q25" s="44"/>
       <c r="R25" s="44"/>
@@ -14435,8 +14475,9 @@
       <c r="AK25" s="44"/>
       <c r="AL25" s="44"/>
       <c r="AM25" s="44"/>
-    </row>
-    <row r="26" spans="2:47">
+      <c r="AN25" s="44"/>
+    </row>
+    <row r="26" spans="2:48">
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
       <c r="D26" s="27" t="s">
@@ -14450,14 +14491,13 @@
       </c>
       <c r="I26" s="27"/>
       <c r="J26" s="92">
-        <f t="shared" ref="J26:J30" si="2">IF(N26="Y",0,-(AR34))</f>
-        <v>-0.98600872265415918</v>
+        <f t="shared" ref="J26:J30" si="2">-INDEX($AO$30:$AV$38,MATCH(D26,$AN$30:$AN$38,0),MATCH($N$25,$AO$29:$AV$29,0))</f>
+        <v>0</v>
       </c>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
       <c r="M26" s="44"/>
       <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
       <c r="P26" s="44"/>
       <c r="Q26" s="44"/>
       <c r="R26" s="44"/>
@@ -14482,8 +14522,9 @@
       <c r="AK26" s="44"/>
       <c r="AL26" s="44"/>
       <c r="AM26" s="44"/>
-    </row>
-    <row r="27" spans="2:47">
+      <c r="AN26" s="44"/>
+    </row>
+    <row r="27" spans="2:48">
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
       <c r="D27" s="27" t="s">
@@ -14498,95 +14539,95 @@
       <c r="I27" s="27"/>
       <c r="J27" s="92">
         <f t="shared" si="2"/>
-        <v>-0.73196550526672355</v>
+        <v>0</v>
       </c>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
       <c r="M27" s="44"/>
       <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
       <c r="P27" s="44"/>
       <c r="Q27" s="44"/>
       <c r="R27" s="44"/>
       <c r="S27" s="44"/>
-      <c r="T27" s="44">
+      <c r="T27" s="44"/>
+      <c r="U27" s="44">
         <v>2</v>
       </c>
-      <c r="U27" s="44">
+      <c r="V27" s="44">
         <v>2.2999999999999998</v>
       </c>
-      <c r="V27" s="44">
+      <c r="W27" s="44">
         <v>2.5</v>
       </c>
-      <c r="W27" s="44">
+      <c r="X27" s="44">
         <v>3</v>
       </c>
-      <c r="X27" s="44">
+      <c r="Y27" s="44">
         <v>3.5</v>
       </c>
-      <c r="Y27" s="44">
+      <c r="Z27" s="44">
         <v>4</v>
       </c>
-      <c r="Z27" s="44">
+      <c r="AA27" s="44">
         <v>4.5</v>
       </c>
-      <c r="AA27" s="44">
+      <c r="AB27" s="44">
         <v>0</v>
       </c>
-      <c r="AB27" s="44"/>
       <c r="AC27" s="44"/>
-      <c r="AD27" s="44">
+      <c r="AD27" s="44"/>
+      <c r="AE27" s="44">
         <v>2</v>
       </c>
-      <c r="AE27" s="44">
+      <c r="AF27" s="44">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AF27" s="44">
+      <c r="AG27" s="44">
         <v>2.5</v>
       </c>
-      <c r="AG27" s="44">
+      <c r="AH27" s="44">
         <v>3</v>
       </c>
-      <c r="AH27" s="44">
+      <c r="AI27" s="44">
         <v>3.5</v>
       </c>
-      <c r="AI27" s="44">
+      <c r="AJ27" s="44">
         <v>4</v>
       </c>
-      <c r="AJ27" s="44">
+      <c r="AK27" s="44">
         <v>4.5</v>
       </c>
-      <c r="AK27" s="44">
+      <c r="AL27" s="44">
         <v>0</v>
       </c>
-      <c r="AL27" s="44"/>
       <c r="AM27" s="44"/>
-      <c r="AN27" s="44">
+      <c r="AN27" s="44"/>
+      <c r="AO27" s="44">
         <v>2</v>
       </c>
-      <c r="AO27" s="44">
+      <c r="AP27" s="44">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AP27" s="44">
+      <c r="AQ27" s="44">
         <v>2.5</v>
       </c>
-      <c r="AQ27" s="44">
+      <c r="AR27" s="44">
         <v>3</v>
       </c>
-      <c r="AR27" s="44">
+      <c r="AS27" s="44">
         <v>3.5</v>
       </c>
-      <c r="AS27" s="44">
+      <c r="AT27" s="44">
         <v>4</v>
       </c>
-      <c r="AT27" s="44">
+      <c r="AU27" s="44">
         <v>4.5</v>
       </c>
-      <c r="AU27" s="44">
+      <c r="AV27" s="44">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:47" ht="15.75" thickBot="1">
+    <row r="28" spans="2:48" ht="15.75" thickBot="1">
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
       <c r="D28" s="27" t="s">
@@ -14601,53 +14642,53 @@
       <c r="I28" s="27"/>
       <c r="J28" s="92">
         <f t="shared" si="2"/>
-        <v>-0.38127737390844418</v>
+        <v>0</v>
       </c>
       <c r="K28" s="27"/>
       <c r="L28" s="27"/>
       <c r="M28" s="44"/>
       <c r="N28" s="44"/>
-      <c r="O28" s="44"/>
       <c r="P28" s="44"/>
       <c r="Q28" s="44"/>
       <c r="R28" s="44"/>
       <c r="S28" s="44"/>
-      <c r="T28" s="98" t="s">
+      <c r="T28" s="44"/>
+      <c r="U28" s="101" t="s">
         <v>281</v>
       </c>
-      <c r="U28" s="99"/>
-      <c r="V28" s="99"/>
-      <c r="W28" s="99"/>
-      <c r="X28" s="99"/>
-      <c r="Y28" s="99"/>
-      <c r="Z28" s="99"/>
-      <c r="AA28" s="99"/>
-      <c r="AB28" s="44"/>
-      <c r="AC28" s="99" t="s">
+      <c r="V28" s="102"/>
+      <c r="W28" s="102"/>
+      <c r="X28" s="102"/>
+      <c r="Y28" s="102"/>
+      <c r="Z28" s="102"/>
+      <c r="AA28" s="102"/>
+      <c r="AB28" s="102"/>
+      <c r="AC28" s="44"/>
+      <c r="AD28" s="102" t="s">
         <v>282</v>
       </c>
-      <c r="AD28" s="99"/>
-      <c r="AE28" s="99"/>
-      <c r="AF28" s="99"/>
-      <c r="AG28" s="99"/>
-      <c r="AH28" s="99"/>
-      <c r="AI28" s="99"/>
-      <c r="AJ28" s="99"/>
-      <c r="AK28" s="99"/>
-      <c r="AL28" s="44"/>
-      <c r="AM28" s="98" t="s">
+      <c r="AE28" s="102"/>
+      <c r="AF28" s="102"/>
+      <c r="AG28" s="102"/>
+      <c r="AH28" s="102"/>
+      <c r="AI28" s="102"/>
+      <c r="AJ28" s="102"/>
+      <c r="AK28" s="102"/>
+      <c r="AL28" s="102"/>
+      <c r="AM28" s="44"/>
+      <c r="AN28" s="101" t="s">
         <v>283</v>
       </c>
-      <c r="AN28" s="99"/>
-      <c r="AO28" s="99"/>
-      <c r="AP28" s="99"/>
-      <c r="AQ28" s="99"/>
-      <c r="AR28" s="99"/>
-      <c r="AS28" s="99"/>
-      <c r="AT28" s="99"/>
-      <c r="AU28" s="99"/>
-    </row>
-    <row r="29" spans="2:47" ht="15.75" thickBot="1">
+      <c r="AO28" s="102"/>
+      <c r="AP28" s="102"/>
+      <c r="AQ28" s="102"/>
+      <c r="AR28" s="102"/>
+      <c r="AS28" s="102"/>
+      <c r="AT28" s="102"/>
+      <c r="AU28" s="102"/>
+      <c r="AV28" s="102"/>
+    </row>
+    <row r="29" spans="2:48">
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
       <c r="D29" s="27" t="s">
@@ -14662,94 +14703,94 @@
       <c r="I29" s="27"/>
       <c r="J29" s="92">
         <f t="shared" si="2"/>
-        <v>-0.16389933245411942</v>
+        <v>0</v>
       </c>
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
       <c r="M29" s="44"/>
       <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
       <c r="P29" s="44"/>
       <c r="Q29" s="44"/>
       <c r="R29" s="44"/>
       <c r="S29" s="44"/>
-      <c r="T29" s="66" t="s">
+      <c r="T29" s="44"/>
+      <c r="U29" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="U29" s="71" t="s">
+      <c r="V29" s="71" t="s">
         <v>288</v>
       </c>
-      <c r="V29" s="76" t="s">
+      <c r="W29" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="W29" s="71" t="s">
+      <c r="X29" s="71" t="s">
         <v>331</v>
       </c>
-      <c r="X29" s="71" t="s">
+      <c r="Y29" s="71" t="s">
         <v>328</v>
       </c>
-      <c r="Y29" s="71" t="s">
+      <c r="Z29" s="71" t="s">
         <v>329</v>
       </c>
-      <c r="Z29" s="71" t="s">
+      <c r="AA29" s="71" t="s">
         <v>330</v>
       </c>
-      <c r="AA29" s="71" t="s">
+      <c r="AB29" s="71" t="s">
         <v>332</v>
       </c>
-      <c r="AB29" s="44"/>
       <c r="AC29" s="44"/>
-      <c r="AD29" s="66" t="s">
+      <c r="AD29" s="44"/>
+      <c r="AE29" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="AE29" s="71" t="s">
+      <c r="AF29" s="71" t="s">
         <v>288</v>
       </c>
-      <c r="AF29" s="76" t="s">
+      <c r="AG29" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="AG29" s="71" t="s">
+      <c r="AH29" s="71" t="s">
         <v>331</v>
       </c>
-      <c r="AH29" s="71" t="s">
+      <c r="AI29" s="71" t="s">
         <v>328</v>
       </c>
-      <c r="AI29" s="71" t="s">
+      <c r="AJ29" s="71" t="s">
         <v>329</v>
       </c>
-      <c r="AJ29" s="71" t="s">
+      <c r="AK29" s="71" t="s">
         <v>330</v>
       </c>
-      <c r="AK29" s="71" t="s">
+      <c r="AL29" s="71" t="s">
         <v>332</v>
       </c>
-      <c r="AM29" s="44"/>
-      <c r="AN29" s="66" t="s">
+      <c r="AN29" s="44"/>
+      <c r="AO29" s="66" t="s">
         <v>286</v>
       </c>
-      <c r="AO29" s="71" t="s">
+      <c r="AP29" s="71" t="s">
         <v>288</v>
       </c>
-      <c r="AP29" s="76" t="s">
+      <c r="AQ29" s="76" t="s">
         <v>290</v>
       </c>
-      <c r="AQ29" s="71" t="s">
+      <c r="AR29" s="71" t="s">
         <v>331</v>
       </c>
-      <c r="AR29" s="71" t="s">
+      <c r="AS29" s="71" t="s">
         <v>328</v>
       </c>
-      <c r="AS29" s="71" t="s">
+      <c r="AT29" s="71" t="s">
         <v>329</v>
       </c>
-      <c r="AT29" s="71" t="s">
+      <c r="AU29" s="71" t="s">
         <v>330</v>
       </c>
-      <c r="AU29" s="71" t="s">
+      <c r="AV29" s="71" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="30" spans="2:47">
+    <row r="30" spans="2:48">
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
       <c r="D30" s="27" t="s">
@@ -14764,122 +14805,122 @@
       <c r="I30" s="27"/>
       <c r="J30" s="92">
         <f t="shared" si="2"/>
-        <v>-4.4138172035112347E-2</v>
+        <v>0</v>
       </c>
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
       <c r="M30" s="44"/>
       <c r="N30" s="44"/>
-      <c r="O30" s="44"/>
       <c r="P30" s="44"/>
       <c r="Q30" s="44"/>
       <c r="R30" s="44"/>
-      <c r="S30" s="66" t="s">
-        <v>287</v>
-      </c>
-      <c r="T30" s="94">
-        <f>_xlfn.NORM.DIST($T$27,Z7,AD7,TRUE)</f>
+      <c r="S30" s="44"/>
+      <c r="T30" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="U30" s="94">
+        <f>_xlfn.NORM.DIST($U$27,AA7,AE7,TRUE)</f>
         <v>0.99986614214614677</v>
       </c>
-      <c r="U30" s="94">
-        <f>_xlfn.NORM.DIST($U$27,Z7,AD7,TRUE)</f>
+      <c r="V30" s="94">
+        <f>_xlfn.NORM.DIST($V$27,AA7,AE7,TRUE)</f>
         <v>0.99999895018069218</v>
       </c>
-      <c r="V30" s="94">
-        <f>_xlfn.NORM.DIST($V$27,Z7,AD7,TRUE)</f>
+      <c r="W30" s="94">
+        <f>_xlfn.NORM.DIST($W$27,AA7,AE7,TRUE)</f>
         <v>0.99999997827100517</v>
       </c>
-      <c r="W30" s="94">
-        <f>_xlfn.NORM.DIST($W$27,Z7,AD7,TRUE)</f>
+      <c r="X30" s="94">
+        <f>_xlfn.NORM.DIST($X$27,AA7,AE7,TRUE)</f>
         <v>0.99999999999986411</v>
       </c>
-      <c r="X30" s="94">
-        <f>_xlfn.NORM.DIST($X$27,Z7,AD7,TRUE)</f>
+      <c r="Y30" s="94">
+        <f>_xlfn.NORM.DIST($Y$27,AA7,AE7,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="Y30" s="94">
-        <f>_xlfn.NORM.DIST($Y$27,Z7,AD7,TRUE)</f>
+      <c r="Z30" s="94">
+        <f>_xlfn.NORM.DIST($Z$27,AA7,AE7,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="Z30" s="94">
-        <f>_xlfn.NORM.DIST($Z$27,Z7,AD7,TRUE)</f>
+      <c r="AA30" s="94">
+        <f>_xlfn.NORM.DIST($AA$27,AA7,AE7,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="AA30" s="94">
+      <c r="AB30" s="94">
         <v>0</v>
       </c>
-      <c r="AB30" s="44"/>
-      <c r="AC30" s="66" t="s">
-        <v>287</v>
-      </c>
-      <c r="AD30" s="94">
-        <f>_xlfn.NORM.DIST($AD$27,AA7,AE7,TRUE)</f>
+      <c r="AC30" s="44"/>
+      <c r="AD30" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="AE30" s="94">
+        <f>_xlfn.NORM.DIST($AE$27,AB7,AF7,TRUE)</f>
         <v>0.99358230344905218</v>
       </c>
-      <c r="AE30" s="94">
-        <f>_xlfn.NORM.DIST($AE$27,AA7,AE7,TRUE)</f>
+      <c r="AF30" s="94">
+        <f>_xlfn.NORM.DIST($AF$27,AB7,AF7,TRUE)</f>
         <v>0.99961797061500135</v>
       </c>
-      <c r="AF30" s="94">
-        <f>_xlfn.NORM.DIST($AF$27,AA7,AE7,TRUE)</f>
+      <c r="AG30" s="94">
+        <f>_xlfn.NORM.DIST($AG$27,AB7,AF7,TRUE)</f>
         <v>0.99996097211163748</v>
       </c>
-      <c r="AG30" s="94">
-        <f>_xlfn.NORM.DIST($AG$27,AA7,AE7,TRUE)</f>
+      <c r="AH30" s="94">
+        <f>_xlfn.NORM.DIST($AH$27,AB7,AF7,TRUE)</f>
         <v>0.99999996888648002</v>
       </c>
-      <c r="AH30" s="94">
-        <f>_xlfn.NORM.DIST($AH$27,AA7,AE7,TRUE)</f>
+      <c r="AI30" s="94">
+        <f>_xlfn.NORM.DIST($AI$27,AB7,AF7,TRUE)</f>
         <v>0.9999999999968846</v>
       </c>
-      <c r="AI30" s="94">
-        <f>_xlfn.NORM.DIST($AI$27,AA7,AE7,TRUE)</f>
+      <c r="AJ30" s="94">
+        <f>_xlfn.NORM.DIST($AJ$27,AB7,AF7,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="AJ30" s="94">
-        <f>_xlfn.NORM.DIST($AJ$27,AA7,AE7,TRUE)</f>
+      <c r="AK30" s="94">
+        <f>_xlfn.NORM.DIST($AK$27,AB7,AF7,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="AK30" s="94">
+      <c r="AL30" s="94">
         <v>0</v>
       </c>
-      <c r="AL30" s="44"/>
-      <c r="AM30" s="66" t="s">
-        <v>287</v>
-      </c>
-      <c r="AN30" s="94">
-        <f>_xlfn.NORM.DIST($AN$27,AB7,AF7,TRUE)</f>
+      <c r="AM30" s="44"/>
+      <c r="AN30" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="AO30" s="94">
+        <f>_xlfn.NORM.DIST($AO$27,AC7,AG7,TRUE)</f>
         <v>0.99867076285153633</v>
       </c>
-      <c r="AO30" s="94">
-        <f>_xlfn.NORM.DIST($AO$27,AB7,AF7,TRUE)</f>
+      <c r="AP30" s="94">
+        <f>_xlfn.NORM.DIST($AP$27,AC7,AG7,TRUE)</f>
         <v>0.99999490602709384</v>
       </c>
-      <c r="AP30" s="94">
-        <f>_xlfn.NORM.DIST($AP$27,AB7,AF7,TRUE)</f>
+      <c r="AQ30" s="94">
+        <f>_xlfn.NORM.DIST($AQ$27,AC7,AG7,TRUE)</f>
         <v>0.99999995653338158</v>
       </c>
-      <c r="AQ30" s="94">
-        <f>_xlfn.NORM.DIST($AQ$27,AB7,AF7,TRUE)</f>
+      <c r="AR30" s="94">
+        <f>_xlfn.NORM.DIST($AR$27,AC7,AG7,TRUE)</f>
         <v>0.99999999999999312</v>
       </c>
-      <c r="AR30" s="94">
-        <f>_xlfn.NORM.DIST($AR$27,AB7,AF7,TRUE)</f>
+      <c r="AS30" s="94">
+        <f>_xlfn.NORM.DIST($AS$27,AC7,AG7,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="AS30" s="94">
-        <f>_xlfn.NORM.DIST($AS$27,AB7,AF7,TRUE)</f>
+      <c r="AT30" s="94">
+        <f>_xlfn.NORM.DIST($AT$27,AC7,AG7,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="AT30" s="94">
-        <f>_xlfn.NORM.DIST($AT$27,AB7,AF7,TRUE)</f>
+      <c r="AU30" s="94">
+        <f>_xlfn.NORM.DIST($AU$27,AC7,AG7,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="AU30" s="94">
+      <c r="AV30" s="94">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:47">
+    <row r="31" spans="2:48">
       <c r="D31" s="27" t="s">
         <v>206</v>
       </c>
@@ -14897,116 +14938,116 @@
       </c>
       <c r="K31" s="27"/>
       <c r="L31" s="27"/>
-      <c r="O31" s="44"/>
       <c r="P31" s="44"/>
       <c r="Q31" s="44"/>
       <c r="R31" s="44"/>
-      <c r="S31" s="71" t="s">
-        <v>289</v>
-      </c>
-      <c r="T31" s="94">
-        <f t="shared" ref="T31:T38" si="3">_xlfn.NORM.DIST($T$27,Z8,AD8,TRUE)</f>
+      <c r="S31" s="44"/>
+      <c r="T31" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="U31" s="94">
+        <f t="shared" ref="U31:U38" si="3">_xlfn.NORM.DIST($U$27,AA8,AE8,TRUE)</f>
         <v>0.96885301500182108</v>
       </c>
-      <c r="U31" s="94">
-        <f t="shared" ref="U31:U38" si="4">_xlfn.NORM.DIST($U$27,Z8,AD8,TRUE)</f>
+      <c r="V31" s="94">
+        <f t="shared" ref="V31:V38" si="4">_xlfn.NORM.DIST($V$27,AA8,AE8,TRUE)</f>
         <v>0.99736560266376562</v>
       </c>
-      <c r="V31" s="94">
-        <f t="shared" ref="V31:V38" si="5">_xlfn.NORM.DIST($V$27,Z8,AD8,TRUE)</f>
+      <c r="W31" s="94">
+        <f t="shared" ref="W31:W38" si="5">_xlfn.NORM.DIST($W$27,AA8,AE8,TRUE)</f>
         <v>0.99967208422117826</v>
       </c>
-      <c r="W31" s="94">
-        <f t="shared" ref="W31:W38" si="6">_xlfn.NORM.DIST($W$27,Z8,AD8,TRUE)</f>
+      <c r="X31" s="94">
+        <f t="shared" ref="X31:X38" si="6">_xlfn.NORM.DIST($X$27,AA8,AE8,TRUE)</f>
         <v>0.99999963010770987</v>
       </c>
-      <c r="X31" s="94">
-        <f t="shared" ref="X31:X38" si="7">_xlfn.NORM.DIST($X$27,Z8,AD8,TRUE)</f>
+      <c r="Y31" s="94">
+        <f t="shared" ref="Y31:Y38" si="7">_xlfn.NORM.DIST($Y$27,AA8,AE8,TRUE)</f>
         <v>0.99999999995815858</v>
       </c>
-      <c r="Y31" s="94">
-        <f t="shared" ref="Y31:Y38" si="8">_xlfn.NORM.DIST($Y$27,Z8,AD8,TRUE)</f>
+      <c r="Z31" s="94">
+        <f t="shared" ref="Z31:Z38" si="8">_xlfn.NORM.DIST($Z$27,AA8,AE8,TRUE)</f>
         <v>0.99999999999999956</v>
       </c>
-      <c r="Z31" s="94">
-        <f t="shared" ref="Z31:Z38" si="9">_xlfn.NORM.DIST($Z$27,Z8,AD8,TRUE)</f>
+      <c r="AA31" s="94">
+        <f t="shared" ref="AA31:AA38" si="9">_xlfn.NORM.DIST($AA$27,AA8,AE8,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="AA31" s="94">
+      <c r="AB31" s="94">
         <v>0</v>
       </c>
-      <c r="AB31" s="44"/>
-      <c r="AC31" s="71" t="s">
-        <v>289</v>
-      </c>
-      <c r="AD31" s="94">
-        <f t="shared" ref="AD31:AD38" si="10">_xlfn.NORM.DIST($AD$27,AA8,AE8,TRUE)</f>
+      <c r="AC31" s="44"/>
+      <c r="AD31" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="AE31" s="94">
+        <f t="shared" ref="AE31:AE38" si="10">_xlfn.NORM.DIST($AE$27,AB8,AF8,TRUE)</f>
         <v>0.7694627396275191</v>
       </c>
-      <c r="AE31" s="94">
-        <f t="shared" ref="AE31:AE38" si="11">_xlfn.NORM.DIST($AE$27,AA8,AE8,TRUE)</f>
+      <c r="AF31" s="94">
+        <f t="shared" ref="AF31:AF38" si="11">_xlfn.NORM.DIST($AF$27,AB8,AF8,TRUE)</f>
         <v>0.92091247414921895</v>
       </c>
-      <c r="AF31" s="94">
-        <f t="shared" ref="AF31:AF38" si="12">_xlfn.NORM.DIST($AF$27,AA8,AE8,TRUE)</f>
+      <c r="AG31" s="94">
+        <f t="shared" ref="AG31:AG38" si="12">_xlfn.NORM.DIST($AG$27,AB8,AF8,TRUE)</f>
         <v>0.96860489728090593</v>
       </c>
-      <c r="AG31" s="94">
-        <f t="shared" ref="AG31:AG38" si="13">_xlfn.NORM.DIST($AG$27,AA8,AE8,TRUE)</f>
+      <c r="AH31" s="94">
+        <f t="shared" ref="AH31:AH38" si="13">_xlfn.NORM.DIST($AH$27,AB8,AF8,TRUE)</f>
         <v>0.99857871934570608</v>
       </c>
-      <c r="AH31" s="94">
-        <f t="shared" ref="AH31:AH38" si="14">_xlfn.NORM.DIST($AH$27,AA8,AE8,TRUE)</f>
+      <c r="AI31" s="94">
+        <f t="shared" ref="AI31:AI38" si="14">_xlfn.NORM.DIST($AI$27,AB8,AF8,TRUE)</f>
         <v>0.99998003334500252</v>
       </c>
-      <c r="AI31" s="94">
-        <f t="shared" ref="AI31:AI38" si="15">_xlfn.NORM.DIST($AI$27,AA8,AE8,TRUE)</f>
+      <c r="AJ31" s="94">
+        <f t="shared" ref="AJ31:AJ38" si="15">_xlfn.NORM.DIST($AJ$27,AB8,AF8,TRUE)</f>
         <v>0.99999991591209203</v>
       </c>
-      <c r="AJ31" s="94">
-        <f t="shared" ref="AJ31:AJ38" si="16">_xlfn.NORM.DIST($AJ$27,AA8,AE8,TRUE)</f>
+      <c r="AK31" s="94">
+        <f t="shared" ref="AK31:AK38" si="16">_xlfn.NORM.DIST($AK$27,AB8,AF8,TRUE)</f>
         <v>0.99999999989582478</v>
       </c>
-      <c r="AK31" s="94">
+      <c r="AL31" s="94">
         <v>0</v>
       </c>
-      <c r="AL31" s="44"/>
-      <c r="AM31" s="71" t="s">
-        <v>289</v>
-      </c>
-      <c r="AN31" s="94">
-        <f t="shared" ref="AN31:AN38" si="17">_xlfn.NORM.DIST($AN$27,AB8,AF8,TRUE)</f>
+      <c r="AM31" s="44"/>
+      <c r="AN31" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="AO31" s="94">
+        <f t="shared" ref="AO31:AO38" si="17">_xlfn.NORM.DIST($AO$27,AC8,AG8,TRUE)</f>
         <v>0.6130931526036395</v>
       </c>
-      <c r="AO31" s="94">
-        <f t="shared" ref="AO31:AO38" si="18">_xlfn.NORM.DIST($AO$27,AB8,AF8,TRUE)</f>
+      <c r="AP31" s="94">
+        <f t="shared" ref="AP31:AP38" si="18">_xlfn.NORM.DIST($AP$27,AC8,AG8,TRUE)</f>
         <v>0.87842619586393023</v>
       </c>
-      <c r="AP31" s="94">
-        <f t="shared" ref="AP31:AP38" si="19">_xlfn.NORM.DIST($AP$27,AB8,AF8,TRUE)</f>
+      <c r="AQ31" s="94">
+        <f t="shared" ref="AQ31:AQ38" si="19">_xlfn.NORM.DIST($AQ$27,AC8,AG8,TRUE)</f>
         <v>0.9602560960127382</v>
       </c>
-      <c r="AQ31" s="94">
-        <f t="shared" ref="AQ31:AQ38" si="20">_xlfn.NORM.DIST($AQ$27,AB8,AF8,TRUE)</f>
+      <c r="AR31" s="94">
+        <f t="shared" ref="AR31:AR38" si="20">_xlfn.NORM.DIST($AR$27,AC8,AG8,TRUE)</f>
         <v>0.99935891586967851</v>
       </c>
-      <c r="AR31" s="94">
-        <f t="shared" ref="AR31:AR38" si="21">_xlfn.NORM.DIST($AR$27,AB8,AF8,TRUE)</f>
+      <c r="AS31" s="94">
+        <f t="shared" ref="AS31:AS38" si="21">_xlfn.NORM.DIST($AS$27,AC8,AG8,TRUE)</f>
         <v>0.99999860849411715</v>
       </c>
-      <c r="AS31" s="94">
-        <f t="shared" ref="AS31:AS38" si="22">_xlfn.NORM.DIST($AS$27,AB8,AF8,TRUE)</f>
+      <c r="AT31" s="94">
+        <f t="shared" ref="AT31:AT38" si="22">_xlfn.NORM.DIST($AT$27,AC8,AG8,TRUE)</f>
         <v>0.99999999961862751</v>
       </c>
-      <c r="AT31" s="94">
-        <f t="shared" ref="AT31:AT38" si="23">_xlfn.NORM.DIST($AT$27,AB8,AF8,TRUE)</f>
+      <c r="AU31" s="94">
+        <f t="shared" ref="AU31:AU38" si="23">_xlfn.NORM.DIST($AU$27,AC8,AG8,TRUE)</f>
         <v>0.99999999999998723</v>
       </c>
-      <c r="AU31" s="94">
+      <c r="AV31" s="94">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:47" s="44" customFormat="1">
+    <row r="32" spans="2:48" s="44" customFormat="1">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32" s="28"/>
@@ -15025,442 +15066,442 @@
       </c>
       <c r="L32" s="28"/>
       <c r="M32"/>
-      <c r="S32" s="76" t="s">
-        <v>291</v>
-      </c>
-      <c r="T32" s="94">
+      <c r="T32" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="U32" s="94">
         <f t="shared" si="3"/>
         <v>0.93969745300565943</v>
       </c>
-      <c r="U32" s="94">
+      <c r="V32" s="94">
         <f t="shared" si="4"/>
         <v>0.99622594121059427</v>
       </c>
-      <c r="V32" s="94">
+      <c r="W32" s="94">
         <f t="shared" si="5"/>
         <v>0.99968448066910742</v>
       </c>
-      <c r="W32" s="94">
+      <c r="X32" s="94">
         <f t="shared" si="6"/>
         <v>0.99999993665897058</v>
       </c>
-      <c r="X32" s="94">
+      <c r="Y32" s="94">
         <f t="shared" si="7"/>
         <v>0.99999999999956379</v>
       </c>
-      <c r="Y32" s="94">
+      <c r="Z32" s="94">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="Z32" s="94">
+      <c r="AA32" s="94">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="AA32" s="94">
+      <c r="AB32" s="94">
         <v>0</v>
       </c>
-      <c r="AC32" s="76" t="s">
-        <v>291</v>
-      </c>
-      <c r="AD32" s="94">
+      <c r="AD32" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="AE32" s="94">
         <f t="shared" si="10"/>
         <v>0.63358245624321075</v>
       </c>
-      <c r="AE32" s="94">
+      <c r="AF32" s="94">
         <f t="shared" si="11"/>
         <v>0.84081469035187228</v>
       </c>
-      <c r="AF32" s="94">
+      <c r="AG32" s="94">
         <f t="shared" si="12"/>
         <v>0.92442034414706997</v>
       </c>
-      <c r="AG32" s="94">
+      <c r="AH32" s="94">
         <f t="shared" si="13"/>
         <v>0.99428940010152511</v>
       </c>
-      <c r="AH32" s="94">
+      <c r="AI32" s="94">
         <f t="shared" si="14"/>
         <v>0.99985475279512115</v>
       </c>
-      <c r="AI32" s="94">
+      <c r="AJ32" s="94">
         <f t="shared" si="15"/>
         <v>0.99999880751297388</v>
       </c>
-      <c r="AJ32" s="94">
+      <c r="AK32" s="94">
         <f t="shared" si="16"/>
         <v>0.99999999691006625</v>
       </c>
-      <c r="AK32" s="94">
+      <c r="AL32" s="94">
         <v>0</v>
       </c>
-      <c r="AM32" s="76" t="s">
-        <v>291</v>
-      </c>
-      <c r="AN32" s="94">
+      <c r="AN32" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="AO32" s="94">
         <f t="shared" si="17"/>
         <v>0.34194299028735675</v>
       </c>
-      <c r="AO32" s="94">
+      <c r="AP32" s="94">
         <f t="shared" si="18"/>
         <v>0.71567219724569331</v>
       </c>
-      <c r="AP32" s="94">
+      <c r="AQ32" s="94">
         <f t="shared" si="19"/>
         <v>0.88905130905570107</v>
       </c>
-      <c r="AQ32" s="94">
+      <c r="AR32" s="94">
         <f t="shared" si="20"/>
         <v>0.99781515762844886</v>
       </c>
-      <c r="AR32" s="94">
+      <c r="AS32" s="94">
         <f t="shared" si="21"/>
         <v>0.99999624728992065</v>
       </c>
-      <c r="AS32" s="94">
+      <c r="AT32" s="94">
         <f t="shared" si="22"/>
         <v>0.99999999949395513</v>
       </c>
-      <c r="AT32" s="94">
+      <c r="AU32" s="94">
         <f t="shared" si="23"/>
         <v>0.99999999999999489</v>
       </c>
-      <c r="AU32" s="94">
+      <c r="AV32" s="94">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:47">
-      <c r="O33" s="44"/>
+    <row r="33" spans="2:48">
       <c r="P33" s="44"/>
       <c r="Q33" s="44"/>
       <c r="R33" s="44"/>
-      <c r="S33" s="71" t="s">
-        <v>293</v>
-      </c>
-      <c r="T33" s="94">
+      <c r="S33" s="44"/>
+      <c r="T33" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="U33" s="94">
         <f t="shared" si="3"/>
         <v>0.76682617615099935</v>
       </c>
-      <c r="U33" s="94">
+      <c r="V33" s="94">
         <f t="shared" si="4"/>
         <v>0.95418880111755022</v>
       </c>
-      <c r="V33" s="94">
+      <c r="W33" s="94">
         <f t="shared" si="5"/>
         <v>0.98998748585906793</v>
       </c>
-      <c r="W33" s="94">
+      <c r="X33" s="94">
         <f t="shared" si="6"/>
         <v>0.99995633197497646</v>
       </c>
-      <c r="X33" s="94">
+      <c r="Y33" s="94">
         <f t="shared" si="7"/>
         <v>0.99999998312382343</v>
       </c>
-      <c r="Y33" s="94">
+      <c r="Z33" s="94">
         <f t="shared" si="8"/>
         <v>0.99999999999945333</v>
       </c>
-      <c r="Z33" s="94">
+      <c r="AA33" s="94">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="AA33" s="94">
+      <c r="AB33" s="94">
         <v>0</v>
       </c>
-      <c r="AB33" s="44"/>
-      <c r="AC33" s="71" t="s">
-        <v>293</v>
-      </c>
-      <c r="AD33" s="94">
+      <c r="AC33" s="44"/>
+      <c r="AD33" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="AE33" s="94">
         <f t="shared" si="10"/>
         <v>0.48602123970467664</v>
       </c>
-      <c r="AE33" s="94">
+      <c r="AF33" s="94">
         <f t="shared" si="11"/>
         <v>0.74725860659793841</v>
       </c>
-      <c r="AF33" s="94">
+      <c r="AG33" s="94">
         <f t="shared" si="12"/>
         <v>0.87143015426775872</v>
       </c>
-      <c r="AG33" s="94">
+      <c r="AH33" s="94">
         <f t="shared" si="13"/>
         <v>0.98931553681492335</v>
       </c>
-      <c r="AH33" s="94">
+      <c r="AI33" s="94">
         <f t="shared" si="14"/>
         <v>0.99973940839121955</v>
       </c>
-      <c r="AI33" s="94">
+      <c r="AJ33" s="94">
         <f t="shared" si="15"/>
         <v>0.99999823974334678</v>
       </c>
-      <c r="AJ33" s="94">
+      <c r="AK33" s="94">
         <f t="shared" si="16"/>
         <v>0.99999999680227936</v>
       </c>
-      <c r="AK33" s="94">
+      <c r="AL33" s="94">
         <v>0</v>
       </c>
-      <c r="AL33" s="44"/>
-      <c r="AM33" s="71" t="s">
-        <v>293</v>
-      </c>
-      <c r="AN33" s="94">
+      <c r="AM33" s="44"/>
+      <c r="AN33" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="AO33" s="94">
         <f t="shared" si="17"/>
         <v>0.14983014442834014</v>
       </c>
-      <c r="AO33" s="94">
+      <c r="AP33" s="94">
         <f t="shared" si="18"/>
         <v>0.49056643348839696</v>
       </c>
-      <c r="AP33" s="94">
+      <c r="AQ33" s="94">
         <f t="shared" si="19"/>
         <v>0.74280813134921952</v>
       </c>
-      <c r="AQ33" s="94">
+      <c r="AR33" s="94">
         <f t="shared" si="20"/>
         <v>0.9903894839477374</v>
       </c>
-      <c r="AR33" s="94">
+      <c r="AS33" s="94">
         <f t="shared" si="21"/>
         <v>0.99997215963294783</v>
       </c>
-      <c r="AS33" s="94">
+      <c r="AT33" s="94">
         <f t="shared" si="22"/>
         <v>0.99999999466107425</v>
       </c>
-      <c r="AT33" s="94">
+      <c r="AU33" s="94">
         <f t="shared" si="23"/>
         <v>0.99999999999993627</v>
       </c>
-      <c r="AU33" s="94">
+      <c r="AV33" s="94">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:47">
+    <row r="34" spans="2:48">
       <c r="L34" s="44"/>
-      <c r="O34" s="44"/>
       <c r="P34" s="44"/>
       <c r="Q34" s="44"/>
       <c r="R34" s="44"/>
-      <c r="S34" s="76" t="s">
-        <v>295</v>
-      </c>
-      <c r="T34" s="94">
+      <c r="S34" s="44"/>
+      <c r="T34" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="U34" s="94">
         <f t="shared" si="3"/>
         <v>0.5138907043261417</v>
       </c>
-      <c r="U34" s="94">
+      <c r="V34" s="94">
         <f t="shared" si="4"/>
         <v>0.70275414783970647</v>
       </c>
-      <c r="V34" s="94">
+      <c r="W34" s="94">
         <f t="shared" si="5"/>
         <v>0.80620969874302539</v>
       </c>
-      <c r="W34" s="94">
+      <c r="X34" s="94">
         <f t="shared" si="6"/>
         <v>0.95479136080813631</v>
       </c>
-      <c r="X34" s="94">
+      <c r="Y34" s="94">
         <f t="shared" si="7"/>
         <v>0.99417194789886376</v>
       </c>
-      <c r="Y34" s="94">
+      <c r="Z34" s="94">
         <f t="shared" si="8"/>
         <v>0.99959823430951478</v>
       </c>
-      <c r="Z34" s="94">
+      <c r="AA34" s="94">
         <f t="shared" si="9"/>
         <v>0.99998547336263233</v>
       </c>
-      <c r="AA34" s="94">
+      <c r="AB34" s="94">
         <v>0</v>
       </c>
-      <c r="AB34" s="44"/>
-      <c r="AC34" s="76" t="s">
-        <v>295</v>
-      </c>
-      <c r="AD34" s="94">
+      <c r="AC34" s="44"/>
+      <c r="AD34" s="27" t="s">
+        <v>313</v>
+      </c>
+      <c r="AE34" s="94">
         <f t="shared" si="10"/>
         <v>0.25380085256173046</v>
       </c>
-      <c r="AE34" s="94">
+      <c r="AF34" s="94">
         <f t="shared" si="11"/>
         <v>0.48042786872418958</v>
       </c>
-      <c r="AF34" s="94">
+      <c r="AG34" s="94">
         <f t="shared" si="12"/>
         <v>0.64054584703308814</v>
       </c>
-      <c r="AG34" s="94">
+      <c r="AH34" s="94">
         <f t="shared" si="13"/>
         <v>0.91657755012121211</v>
       </c>
-      <c r="AH34" s="94">
+      <c r="AI34" s="94">
         <f t="shared" si="14"/>
         <v>0.99191173064402915</v>
       </c>
-      <c r="AI34" s="94">
+      <c r="AJ34" s="94">
         <f t="shared" si="15"/>
         <v>0.99969530786128746</v>
       </c>
-      <c r="AJ34" s="94">
+      <c r="AK34" s="94">
         <f t="shared" si="16"/>
         <v>0.9999957044409139</v>
       </c>
-      <c r="AK34" s="94">
+      <c r="AL34" s="94">
         <v>0</v>
       </c>
-      <c r="AL34" s="44"/>
-      <c r="AM34" s="76" t="s">
-        <v>295</v>
-      </c>
-      <c r="AN34" s="94">
+      <c r="AM34" s="44"/>
+      <c r="AN34" s="27" t="s">
+        <v>320</v>
+      </c>
+      <c r="AO34" s="94">
         <f t="shared" si="17"/>
         <v>6.6011404930960929E-2</v>
       </c>
-      <c r="AO34" s="94">
+      <c r="AP34" s="94">
         <f t="shared" si="18"/>
         <v>0.22200714259760385</v>
       </c>
-      <c r="AP34" s="94">
+      <c r="AQ34" s="94">
         <f t="shared" si="19"/>
         <v>0.39296290098211079</v>
       </c>
-      <c r="AQ34" s="94">
+      <c r="AR34" s="94">
         <f t="shared" si="20"/>
         <v>0.83221694488457221</v>
       </c>
-      <c r="AR34" s="94">
+      <c r="AS34" s="94">
         <f t="shared" si="21"/>
         <v>0.98600872265415918</v>
       </c>
-      <c r="AS34" s="94">
+      <c r="AT34" s="94">
         <f t="shared" si="22"/>
         <v>0.99970053530100189</v>
       </c>
-      <c r="AT34" s="94">
+      <c r="AU34" s="94">
         <f t="shared" si="23"/>
         <v>0.99999846937326342</v>
       </c>
-      <c r="AU34" s="94">
+      <c r="AV34" s="94">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:47">
+    <row r="35" spans="2:48">
       <c r="L35" s="44"/>
-      <c r="O35" s="44"/>
       <c r="P35" s="44"/>
       <c r="Q35" s="44"/>
       <c r="R35" s="44"/>
-      <c r="S35" s="71" t="s">
-        <v>297</v>
-      </c>
-      <c r="T35" s="94">
-        <f>_xlfn.NORM.DIST($T$27,Z12,AD12,TRUE)</f>
+      <c r="S35" s="44"/>
+      <c r="T35" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="U35" s="94">
+        <f>_xlfn.NORM.DIST($U$27,AA12,AE12,TRUE)</f>
         <v>0.37584533679027893</v>
       </c>
-      <c r="U35" s="94">
+      <c r="V35" s="94">
         <f t="shared" si="4"/>
         <v>0.51506861469064869</v>
       </c>
-      <c r="V35" s="94">
+      <c r="W35" s="94">
         <f t="shared" si="5"/>
         <v>0.60792230376456446</v>
       </c>
-      <c r="W35" s="94">
+      <c r="X35" s="94">
         <f t="shared" si="6"/>
         <v>0.80626831138166599</v>
       </c>
-      <c r="X35" s="94">
+      <c r="Y35" s="94">
         <f t="shared" si="7"/>
         <v>0.92710242952401201</v>
       </c>
-      <c r="Y35" s="94">
+      <c r="Z35" s="94">
         <f t="shared" si="8"/>
         <v>0.9795658771957636</v>
       </c>
-      <c r="Z35" s="94">
+      <c r="AA35" s="94">
         <f t="shared" si="9"/>
         <v>0.99579540336422534</v>
       </c>
-      <c r="AA35" s="94">
+      <c r="AB35" s="94">
         <v>0</v>
       </c>
-      <c r="AB35" s="44"/>
-      <c r="AC35" s="71" t="s">
-        <v>297</v>
-      </c>
-      <c r="AD35" s="94">
+      <c r="AC35" s="44"/>
+      <c r="AD35" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="AE35" s="94">
         <f t="shared" si="10"/>
         <v>8.9754023843298891E-2</v>
       </c>
-      <c r="AE35" s="94">
+      <c r="AF35" s="94">
         <f t="shared" si="11"/>
         <v>0.19240027281705166</v>
       </c>
-      <c r="AF35" s="94">
+      <c r="AG35" s="94">
         <f t="shared" si="12"/>
         <v>0.28991681177663592</v>
       </c>
-      <c r="AG35" s="94">
+      <c r="AH35" s="94">
         <f t="shared" si="13"/>
         <v>0.59290175446950721</v>
       </c>
-      <c r="AH35" s="94">
+      <c r="AI35" s="94">
         <f t="shared" si="14"/>
         <v>0.8470018886690438</v>
       </c>
-      <c r="AI35" s="94">
+      <c r="AJ35" s="94">
         <f t="shared" si="15"/>
         <v>0.96503029194003964</v>
       </c>
-      <c r="AJ35" s="94">
+      <c r="AK35" s="94">
         <f t="shared" si="16"/>
         <v>0.99535165071760523</v>
       </c>
-      <c r="AK35" s="94">
+      <c r="AL35" s="94">
         <v>0</v>
       </c>
-      <c r="AL35" s="44"/>
-      <c r="AM35" s="71" t="s">
-        <v>297</v>
-      </c>
-      <c r="AN35" s="94">
+      <c r="AM35" s="44"/>
+      <c r="AN35" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="AO35" s="94">
         <f t="shared" si="17"/>
         <v>5.6979596817344061E-2</v>
       </c>
-      <c r="AO35" s="94">
+      <c r="AP35" s="94">
         <f t="shared" si="18"/>
         <v>0.12698439253107691</v>
       </c>
-      <c r="AP35" s="94">
+      <c r="AQ35" s="94">
         <f t="shared" si="19"/>
         <v>0.19835620119859471</v>
       </c>
-      <c r="AQ35" s="94">
+      <c r="AR35" s="94">
         <f t="shared" si="20"/>
         <v>0.45447244481580307</v>
       </c>
-      <c r="AR35" s="94">
+      <c r="AS35" s="94">
         <f t="shared" si="21"/>
         <v>0.73196550526672355</v>
       </c>
-      <c r="AS35" s="94">
+      <c r="AT35" s="94">
         <f t="shared" si="22"/>
         <v>0.91179733138324648</v>
       </c>
-      <c r="AT35" s="94">
+      <c r="AU35" s="94">
         <f t="shared" si="23"/>
         <v>0.98146734609448394</v>
       </c>
-      <c r="AU35" s="94">
+      <c r="AV35" s="94">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:47" s="44" customFormat="1">
+    <row r="36" spans="2:48" s="44" customFormat="1">
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
@@ -15471,222 +15512,222 @@
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>
-      <c r="S36" s="76" t="s">
-        <v>301</v>
-      </c>
-      <c r="T36" s="94">
+      <c r="T36" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="U36" s="94">
         <f t="shared" si="3"/>
         <v>0.16552806134367962</v>
       </c>
-      <c r="U36" s="94">
+      <c r="V36" s="94">
         <f t="shared" si="4"/>
         <v>0.29053559209062707</v>
       </c>
-      <c r="V36" s="94">
+      <c r="W36" s="94">
         <f t="shared" si="5"/>
         <v>0.39292301197938029</v>
       </c>
-      <c r="W36" s="94">
+      <c r="X36" s="94">
         <f t="shared" si="6"/>
         <v>0.66588242910237538</v>
       </c>
-      <c r="X36" s="94">
+      <c r="Y36" s="94">
         <f t="shared" si="7"/>
         <v>0.87051976694100974</v>
       </c>
-      <c r="Y36" s="94">
+      <c r="Z36" s="94">
         <f t="shared" si="8"/>
         <v>0.96631005589236407</v>
       </c>
-      <c r="Z36" s="94">
+      <c r="AA36" s="94">
         <f t="shared" si="9"/>
         <v>0.99428730510778573</v>
       </c>
-      <c r="AA36" s="94">
+      <c r="AB36" s="94">
         <v>0</v>
       </c>
-      <c r="AC36" s="76" t="s">
-        <v>301</v>
-      </c>
-      <c r="AD36" s="94">
+      <c r="AD36" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="AE36" s="94">
         <f t="shared" si="10"/>
         <v>5.0511604601422351E-2</v>
       </c>
-      <c r="AE36" s="94">
+      <c r="AF36" s="94">
         <f t="shared" si="11"/>
         <v>9.4333345509310967E-2</v>
       </c>
-      <c r="AF36" s="94">
+      <c r="AG36" s="94">
         <f t="shared" si="12"/>
         <v>0.13618656405660809</v>
       </c>
-      <c r="AG36" s="94">
+      <c r="AH36" s="94">
         <f t="shared" si="13"/>
         <v>0.28933976981199794</v>
       </c>
-      <c r="AH36" s="94">
+      <c r="AI36" s="94">
         <f t="shared" si="14"/>
         <v>0.49480783925100147</v>
       </c>
-      <c r="AI36" s="94">
+      <c r="AJ36" s="94">
         <f t="shared" si="15"/>
         <v>0.70169583060873153</v>
       </c>
-      <c r="AJ36" s="94">
+      <c r="AK36" s="94">
         <f t="shared" si="16"/>
         <v>0.85804642932382791</v>
       </c>
-      <c r="AK36" s="94">
+      <c r="AL36" s="94">
         <v>0</v>
       </c>
-      <c r="AM36" s="76" t="s">
-        <v>301</v>
-      </c>
-      <c r="AN36" s="94">
+      <c r="AN36" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="AO36" s="94">
         <f t="shared" si="17"/>
         <v>2.8856450394145666E-2</v>
       </c>
-      <c r="AO36" s="94">
+      <c r="AP36" s="94">
         <f t="shared" si="18"/>
         <v>5.7199757058308189E-2</v>
       </c>
-      <c r="AP36" s="94">
+      <c r="AQ36" s="94">
         <f t="shared" si="19"/>
         <v>8.5976160021217857E-2</v>
       </c>
-      <c r="AQ36" s="94">
+      <c r="AR36" s="94">
         <f t="shared" si="20"/>
         <v>0.20212850255165354</v>
       </c>
-      <c r="AR36" s="94">
+      <c r="AS36" s="94">
         <f t="shared" si="21"/>
         <v>0.38127737390844418</v>
       </c>
-      <c r="AS36" s="94">
+      <c r="AT36" s="94">
         <f t="shared" si="22"/>
         <v>0.5908714474634762</v>
       </c>
-      <c r="AT36" s="94">
+      <c r="AU36" s="94">
         <f t="shared" si="23"/>
         <v>0.77688109740361544</v>
       </c>
-      <c r="AU36" s="94">
+      <c r="AV36" s="94">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:47">
+    <row r="37" spans="2:48">
       <c r="L37" s="44"/>
       <c r="M37" s="44"/>
-      <c r="O37" s="44"/>
       <c r="P37" s="44"/>
       <c r="Q37" s="44"/>
       <c r="R37" s="44"/>
-      <c r="S37" s="71" t="s">
-        <v>302</v>
-      </c>
-      <c r="T37" s="94">
+      <c r="S37" s="44"/>
+      <c r="T37" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="U37" s="94">
         <f t="shared" si="3"/>
         <v>9.1492186931267622E-2</v>
       </c>
-      <c r="U37" s="94">
+      <c r="V37" s="94">
         <f t="shared" si="4"/>
         <v>0.15300882371326033</v>
       </c>
-      <c r="V37" s="94">
+      <c r="W37" s="94">
         <f t="shared" si="5"/>
         <v>0.20660004501142309</v>
       </c>
-      <c r="W37" s="94">
+      <c r="X37" s="94">
         <f t="shared" si="6"/>
         <v>0.38021044483571315</v>
       </c>
-      <c r="X37" s="94">
+      <c r="Y37" s="94">
         <f t="shared" si="7"/>
         <v>0.58254904641534866</v>
       </c>
-      <c r="Y37" s="94">
+      <c r="Z37" s="94">
         <f t="shared" si="8"/>
         <v>0.76478079525417386</v>
       </c>
-      <c r="Z37" s="94">
+      <c r="AA37" s="94">
         <f t="shared" si="9"/>
         <v>0.89160576223881305</v>
       </c>
-      <c r="AA37" s="94">
+      <c r="AB37" s="94">
         <v>0</v>
       </c>
-      <c r="AB37" s="44"/>
-      <c r="AC37" s="71" t="s">
-        <v>302</v>
-      </c>
-      <c r="AD37" s="94">
+      <c r="AC37" s="44"/>
+      <c r="AD37" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="AE37" s="94">
         <f t="shared" si="10"/>
         <v>3.2210497290905374E-2</v>
       </c>
-      <c r="AE37" s="94">
+      <c r="AF37" s="94">
         <f t="shared" si="11"/>
         <v>5.6332486553475364E-2</v>
       </c>
-      <c r="AF37" s="94">
+      <c r="AG37" s="94">
         <f t="shared" si="12"/>
         <v>7.9115975834815E-2</v>
       </c>
-      <c r="AG37" s="94">
+      <c r="AH37" s="94">
         <f t="shared" si="13"/>
         <v>0.16531868864588461</v>
       </c>
-      <c r="AH37" s="94">
+      <c r="AI37" s="94">
         <f t="shared" si="14"/>
         <v>0.29645675583092174</v>
       </c>
-      <c r="AI37" s="94">
+      <c r="AJ37" s="94">
         <f t="shared" si="15"/>
         <v>0.46159880109745322</v>
       </c>
-      <c r="AJ37" s="94">
+      <c r="AK37" s="94">
         <f t="shared" si="16"/>
         <v>0.63375133998904754</v>
       </c>
-      <c r="AK37" s="94">
+      <c r="AL37" s="94">
         <v>0</v>
       </c>
-      <c r="AL37" s="44"/>
-      <c r="AM37" s="71" t="s">
-        <v>302</v>
-      </c>
-      <c r="AN37" s="94">
+      <c r="AM37" s="44"/>
+      <c r="AN37" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="AO37" s="94">
         <f t="shared" si="17"/>
         <v>7.3325429420576533E-3</v>
       </c>
-      <c r="AO37" s="94">
+      <c r="AP37" s="94">
         <f t="shared" si="18"/>
         <v>1.5850994164039133E-2</v>
       </c>
-      <c r="AP37" s="94">
+      <c r="AQ37" s="94">
         <f t="shared" si="19"/>
         <v>2.5396980814932565E-2</v>
       </c>
-      <c r="AQ37" s="94">
+      <c r="AR37" s="94">
         <f t="shared" si="20"/>
         <v>7.1339545297204487E-2</v>
       </c>
-      <c r="AR37" s="94">
+      <c r="AS37" s="94">
         <f t="shared" si="21"/>
         <v>0.16389933245411942</v>
       </c>
-      <c r="AS37" s="94">
+      <c r="AT37" s="94">
         <f t="shared" si="22"/>
         <v>0.31163257381350196</v>
       </c>
-      <c r="AT37" s="94">
+      <c r="AU37" s="94">
         <f t="shared" si="23"/>
         <v>0.49844467341211474</v>
       </c>
-      <c r="AU37" s="94">
+      <c r="AV37" s="94">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:47">
+    <row r="38" spans="2:48">
       <c r="B38" s="7" t="s">
         <v>86</v>
       </c>
@@ -15694,116 +15735,116 @@
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="M38" s="44"/>
-      <c r="O38" s="44"/>
       <c r="P38" s="44"/>
       <c r="Q38" s="44"/>
       <c r="R38" s="44"/>
-      <c r="S38" s="82" t="s">
-        <v>303</v>
-      </c>
-      <c r="T38" s="94">
+      <c r="S38" s="44"/>
+      <c r="T38" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="U38" s="94">
         <f t="shared" si="3"/>
         <v>3.6630747396996691E-2</v>
       </c>
-      <c r="U38" s="94">
+      <c r="V38" s="94">
         <f t="shared" si="4"/>
         <v>5.4970533940220757E-2</v>
       </c>
-      <c r="V38" s="94">
+      <c r="W38" s="94">
         <f t="shared" si="5"/>
         <v>7.0785662206478708E-2</v>
       </c>
-      <c r="W38" s="94">
+      <c r="X38" s="94">
         <f t="shared" si="6"/>
         <v>0.12533343317165579</v>
       </c>
-      <c r="X38" s="94">
+      <c r="Y38" s="94">
         <f t="shared" si="7"/>
         <v>0.20397754353748057</v>
       </c>
-      <c r="Y38" s="94">
+      <c r="Z38" s="94">
         <f t="shared" si="8"/>
         <v>0.30633564692244153</v>
       </c>
-      <c r="Z38" s="94">
+      <c r="AA38" s="94">
         <f t="shared" si="9"/>
         <v>0.42660254978994411</v>
       </c>
-      <c r="AA38" s="94">
+      <c r="AB38" s="94">
         <v>0</v>
       </c>
-      <c r="AB38" s="44"/>
-      <c r="AC38" s="82" t="s">
-        <v>303</v>
-      </c>
-      <c r="AD38" s="94">
+      <c r="AC38" s="44"/>
+      <c r="AD38" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="AE38" s="94">
         <f t="shared" si="10"/>
         <v>3.054309712927282E-2</v>
       </c>
-      <c r="AE38" s="94">
+      <c r="AF38" s="94">
         <f t="shared" si="11"/>
         <v>4.54767509141593E-2</v>
       </c>
-      <c r="AF38" s="94">
+      <c r="AG38" s="94">
         <f t="shared" si="12"/>
         <v>5.8354873920238394E-2</v>
       </c>
-      <c r="AG38" s="94">
+      <c r="AH38" s="94">
         <f t="shared" si="13"/>
         <v>0.10300763832828137</v>
       </c>
-      <c r="AH38" s="94">
+      <c r="AI38" s="94">
         <f t="shared" si="14"/>
         <v>0.16841130134712209</v>
       </c>
-      <c r="AI38" s="94">
+      <c r="AJ38" s="94">
         <f t="shared" si="15"/>
         <v>0.2558071850950065</v>
       </c>
-      <c r="AJ38" s="94">
+      <c r="AK38" s="94">
         <f t="shared" si="16"/>
         <v>0.362347970092745</v>
       </c>
-      <c r="AK38" s="94">
+      <c r="AL38" s="94">
         <v>0</v>
       </c>
-      <c r="AL38" s="44"/>
-      <c r="AM38" s="82" t="s">
-        <v>303</v>
-      </c>
-      <c r="AN38" s="94">
+      <c r="AM38" s="44"/>
+      <c r="AN38" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="AO38" s="94">
         <f t="shared" si="17"/>
         <v>3.2086171243230267E-3</v>
       </c>
-      <c r="AO38" s="94">
+      <c r="AP38" s="94">
         <f t="shared" si="18"/>
         <v>5.8437278169573741E-3</v>
       </c>
-      <c r="AP38" s="94">
+      <c r="AQ38" s="94">
         <f t="shared" si="19"/>
         <v>8.5326893308700167E-3</v>
       </c>
-      <c r="AQ38" s="94">
+      <c r="AR38" s="94">
         <f t="shared" si="20"/>
         <v>2.0430952713542849E-2</v>
       </c>
-      <c r="AR38" s="94">
+      <c r="AS38" s="94">
         <f t="shared" si="21"/>
         <v>4.4138172035112347E-2</v>
       </c>
-      <c r="AS38" s="94">
+      <c r="AT38" s="94">
         <f t="shared" si="22"/>
         <v>8.6253363635820451E-2</v>
       </c>
-      <c r="AT38" s="94">
+      <c r="AU38" s="94">
         <f t="shared" si="23"/>
         <v>0.15295879709707286</v>
       </c>
-      <c r="AU38" s="94">
+      <c r="AV38" s="94">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:47" ht="15.75" thickBot="1">
+    <row r="39" spans="2:48" ht="15.75" thickBot="1">
       <c r="B39" s="10" t="s">
         <v>12</v>
       </c>
@@ -15835,7 +15876,6 @@
         <v>3</v>
       </c>
       <c r="M39" s="44"/>
-      <c r="O39" s="44"/>
       <c r="P39" s="44"/>
       <c r="Q39" s="44"/>
       <c r="R39" s="44"/>
@@ -15862,9 +15902,10 @@
       <c r="AM39" s="44"/>
       <c r="AN39" s="44"/>
       <c r="AO39" s="44"/>
-      <c r="AU39" s="94"/>
-    </row>
-    <row r="40" spans="2:47">
+      <c r="AP39" s="44"/>
+      <c r="AV39" s="94"/>
+    </row>
+    <row r="40" spans="2:48">
       <c r="C40" t="s">
         <v>82</v>
       </c>
@@ -15881,7 +15922,6 @@
       <c r="K40" t="s">
         <v>222</v>
       </c>
-      <c r="O40" s="44"/>
       <c r="P40" s="44"/>
       <c r="Q40" s="44"/>
       <c r="R40" s="44"/>
@@ -15906,8 +15946,9 @@
       <c r="AK40" s="44"/>
       <c r="AL40" s="44"/>
       <c r="AM40" s="44"/>
-    </row>
-    <row r="41" spans="2:47">
+      <c r="AN40" s="44"/>
+    </row>
+    <row r="41" spans="2:48">
       <c r="C41" t="s">
         <v>82</v>
       </c>
@@ -15925,7 +15966,6 @@
       <c r="K41" t="s">
         <v>222</v>
       </c>
-      <c r="O41" s="44"/>
       <c r="P41" s="44"/>
       <c r="Q41" s="44"/>
       <c r="R41" s="44"/>
@@ -15950,8 +15990,9 @@
       <c r="AK41" s="44"/>
       <c r="AL41" s="44"/>
       <c r="AM41" s="44"/>
-    </row>
-    <row r="42" spans="2:47" ht="21.75" thickBot="1">
+      <c r="AN41" s="44"/>
+    </row>
+    <row r="42" spans="2:48" ht="21.75" thickBot="1">
       <c r="B42" s="44"/>
       <c r="C42" s="44" t="s">
         <v>82</v>
@@ -15977,39 +16018,39 @@
       <c r="M42" s="25">
         <v>0.5</v>
       </c>
-      <c r="O42" s="44"/>
       <c r="P42" s="44"/>
       <c r="Q42" s="44"/>
       <c r="R42" s="44"/>
-      <c r="S42" s="100" t="s">
+      <c r="S42" s="44"/>
+      <c r="T42" s="99" t="s">
         <v>307</v>
       </c>
-      <c r="T42" s="100"/>
-      <c r="U42" s="100"/>
-      <c r="V42" s="100"/>
-      <c r="W42" s="44"/>
-      <c r="X42" s="100" t="s">
+      <c r="U42" s="99"/>
+      <c r="V42" s="99"/>
+      <c r="W42" s="99"/>
+      <c r="X42" s="44"/>
+      <c r="Y42" s="99" t="s">
         <v>308</v>
       </c>
-      <c r="Y42" s="100"/>
-      <c r="Z42" s="100"/>
-      <c r="AA42" s="100"/>
-      <c r="AB42" s="44"/>
-      <c r="AC42" s="100" t="s">
+      <c r="Z42" s="99"/>
+      <c r="AA42" s="99"/>
+      <c r="AB42" s="99"/>
+      <c r="AC42" s="44"/>
+      <c r="AD42" s="99" t="s">
         <v>309</v>
       </c>
-      <c r="AD42" s="100"/>
-      <c r="AE42" s="100"/>
-      <c r="AF42" s="100"/>
-      <c r="AG42" s="44"/>
+      <c r="AE42" s="99"/>
+      <c r="AF42" s="99"/>
+      <c r="AG42" s="99"/>
       <c r="AH42" s="44"/>
       <c r="AI42" s="44"/>
       <c r="AJ42" s="44"/>
       <c r="AK42" s="44"/>
       <c r="AL42" s="44"/>
       <c r="AM42" s="44"/>
-    </row>
-    <row r="43" spans="2:47" ht="15.75" thickBot="1">
+      <c r="AN42" s="44"/>
+    </row>
+    <row r="43" spans="2:48" ht="15.75" thickBot="1">
       <c r="C43" t="s">
         <v>82</v>
       </c>
@@ -16029,57 +16070,57 @@
       <c r="M43" s="25">
         <v>0.1</v>
       </c>
-      <c r="O43" s="44"/>
       <c r="P43" s="44"/>
       <c r="Q43" s="44"/>
       <c r="R43" s="44"/>
-      <c r="S43" s="61" t="s">
+      <c r="S43" s="44"/>
+      <c r="T43" s="61" t="s">
         <v>284</v>
       </c>
-      <c r="T43" s="60" t="s">
+      <c r="U43" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="U43" s="60" t="s">
+      <c r="V43" s="60" t="s">
         <v>282</v>
       </c>
-      <c r="V43" s="60" t="s">
+      <c r="W43" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="W43" s="44"/>
-      <c r="X43" s="61" t="s">
+      <c r="X43" s="44"/>
+      <c r="Y43" s="61" t="s">
         <v>284</v>
       </c>
-      <c r="Y43" s="60" t="s">
+      <c r="Z43" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="Z43" s="60" t="s">
+      <c r="AA43" s="60" t="s">
         <v>282</v>
       </c>
-      <c r="AA43" s="60" t="s">
+      <c r="AB43" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="AB43" s="44"/>
-      <c r="AC43" s="61" t="s">
+      <c r="AC43" s="44"/>
+      <c r="AD43" s="61" t="s">
         <v>284</v>
       </c>
-      <c r="AD43" s="60" t="s">
+      <c r="AE43" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="AE43" s="60" t="s">
+      <c r="AF43" s="60" t="s">
         <v>282</v>
       </c>
-      <c r="AF43" s="60" t="s">
+      <c r="AG43" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="AG43" s="44"/>
       <c r="AH43" s="44"/>
       <c r="AI43" s="44"/>
       <c r="AJ43" s="44"/>
       <c r="AK43" s="44"/>
       <c r="AL43" s="44"/>
       <c r="AM43" s="44"/>
-    </row>
-    <row r="44" spans="2:47">
+      <c r="AN43" s="44"/>
+    </row>
+    <row r="44" spans="2:48">
       <c r="C44" t="s">
         <v>82</v>
       </c>
@@ -16097,66 +16138,66 @@
         <v>231</v>
       </c>
       <c r="M44" s="44"/>
-      <c r="O44" s="44"/>
       <c r="P44" s="44"/>
       <c r="Q44" s="44"/>
       <c r="R44" s="44"/>
-      <c r="S44" s="66" t="s">
+      <c r="S44" s="44"/>
+      <c r="T44" s="66" t="s">
         <v>287</v>
       </c>
-      <c r="T44" s="68">
-        <f t="shared" ref="T44:T52" si="24">U7*T30</f>
+      <c r="U44" s="68">
+        <f t="shared" ref="U44:U52" si="24">V7*U30</f>
         <v>11733.467597673669</v>
       </c>
-      <c r="U44" s="68">
-        <f t="shared" ref="U44:U52" si="25">V7*AD30</f>
+      <c r="V44" s="68">
+        <f t="shared" ref="V44:V52" si="25">W7*AE30</f>
         <v>72063.176117234543</v>
       </c>
-      <c r="V44" s="68">
-        <f t="shared" ref="V44:V52" si="26">W7*AN30</f>
+      <c r="W44" s="68">
+        <f t="shared" ref="W44:W52" si="26">X7*AO30</f>
         <v>37314.784992598958</v>
       </c>
-      <c r="W44" s="44"/>
-      <c r="X44" s="66" t="s">
+      <c r="X44" s="44"/>
+      <c r="Y44" s="66" t="s">
         <v>287</v>
       </c>
-      <c r="Y44" s="68">
-        <f t="shared" ref="Y44:Y52" si="27">U7*U30</f>
+      <c r="Z44" s="68">
+        <f t="shared" ref="Z44:Z52" si="27">V7*V30</f>
         <v>11735.026105062172</v>
       </c>
-      <c r="Z44" s="68">
-        <f t="shared" ref="Z44:Z52" si="28">V7*AE30</f>
+      <c r="AA44" s="68">
+        <f t="shared" ref="AA44:AA52" si="28">W7*AF30</f>
         <v>72500.934866011521</v>
       </c>
-      <c r="AA44" s="68">
-        <f t="shared" ref="AA44:AA52" si="29">W7*AO30</f>
+      <c r="AB44" s="68">
+        <f t="shared" ref="AB44:AB52" si="29">X7*AP30</f>
         <v>37364.260875676046</v>
       </c>
-      <c r="AB44" s="44"/>
-      <c r="AC44" s="66" t="s">
+      <c r="AC44" s="44"/>
+      <c r="AD44" s="66" t="s">
         <v>287</v>
       </c>
-      <c r="AD44" s="68">
-        <f t="shared" ref="AD44:AD52" si="30">U7*V30</f>
+      <c r="AE44" s="68">
+        <f t="shared" ref="AE44:AE52" si="30">V7*W30</f>
         <v>11735.0381697415</v>
       </c>
-      <c r="AE44" s="68">
-        <f t="shared" ref="AE44:AE52" si="31">V7*AF30</f>
+      <c r="AF44" s="68">
+        <f t="shared" ref="AF44:AF52" si="31">W7*AG30</f>
         <v>72525.812299088546</v>
       </c>
-      <c r="AF44" s="68">
-        <f t="shared" ref="AF44:AF52" si="32">W7*AP30</f>
+      <c r="AG44" s="68">
+        <f t="shared" ref="AG44:AG52" si="32">X7*AQ30</f>
         <v>37364.449585071816</v>
       </c>
-      <c r="AG44" s="44"/>
       <c r="AH44" s="44"/>
       <c r="AI44" s="44"/>
       <c r="AJ44" s="44"/>
       <c r="AK44" s="44"/>
       <c r="AL44" s="44"/>
       <c r="AM44" s="44"/>
-    </row>
-    <row r="45" spans="2:47">
+      <c r="AN44" s="44"/>
+    </row>
+    <row r="45" spans="2:48">
       <c r="C45" t="s">
         <v>82</v>
       </c>
@@ -16174,66 +16215,66 @@
       <c r="K45" t="s">
         <v>231</v>
       </c>
-      <c r="O45" s="44"/>
       <c r="P45" s="44"/>
       <c r="Q45" s="44"/>
       <c r="R45" s="44"/>
-      <c r="S45" s="71" t="s">
+      <c r="S45" s="44"/>
+      <c r="T45" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="T45" s="73">
+      <c r="U45" s="73">
         <f t="shared" si="24"/>
         <v>5035.723262607311</v>
       </c>
-      <c r="U45" s="73">
+      <c r="V45" s="73">
         <f t="shared" si="25"/>
         <v>5176.5276762398598</v>
       </c>
-      <c r="V45" s="73">
+      <c r="W45" s="73">
         <f t="shared" si="26"/>
         <v>5019.2664795157916</v>
       </c>
-      <c r="W45" s="44"/>
-      <c r="X45" s="71" t="s">
+      <c r="X45" s="44"/>
+      <c r="Y45" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="Y45" s="73">
+      <c r="Z45" s="73">
         <f t="shared" si="27"/>
         <v>5183.920665869884</v>
       </c>
-      <c r="Z45" s="73">
+      <c r="AA45" s="73">
         <f t="shared" si="28"/>
         <v>6195.3992887759896</v>
       </c>
-      <c r="AA45" s="73">
+      <c r="AB45" s="73">
         <f t="shared" si="29"/>
         <v>7191.4930723077614</v>
       </c>
-      <c r="AB45" s="44"/>
-      <c r="AC45" s="71" t="s">
+      <c r="AC45" s="44"/>
+      <c r="AD45" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="AD45" s="73">
+      <c r="AE45" s="73">
         <f t="shared" si="30"/>
         <v>5195.9088649605537</v>
       </c>
-      <c r="AE45" s="73">
+      <c r="AF45" s="73">
         <f t="shared" si="31"/>
         <v>6516.2480259190379</v>
       </c>
-      <c r="AF45" s="73">
+      <c r="AG45" s="73">
         <f t="shared" si="32"/>
         <v>7861.4174925933157</v>
       </c>
-      <c r="AG45" s="44"/>
       <c r="AH45" s="44"/>
       <c r="AI45" s="44"/>
       <c r="AJ45" s="44"/>
       <c r="AK45" s="44"/>
       <c r="AL45" s="44"/>
       <c r="AM45" s="44"/>
-    </row>
-    <row r="46" spans="2:47">
+      <c r="AN45" s="44"/>
+    </row>
+    <row r="46" spans="2:48">
       <c r="B46" s="44"/>
       <c r="C46" s="44" t="s">
         <v>82</v>
@@ -16256,66 +16297,66 @@
         <v>231</v>
       </c>
       <c r="L46" s="44"/>
-      <c r="O46" s="44"/>
       <c r="P46" s="44"/>
       <c r="Q46" s="44"/>
       <c r="R46" s="44"/>
-      <c r="S46" s="76" t="s">
+      <c r="S46" s="44"/>
+      <c r="T46" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="T46" s="78">
+      <c r="U46" s="78">
         <f t="shared" si="24"/>
         <v>13136.424555563108</v>
       </c>
-      <c r="U46" s="78">
+      <c r="V46" s="78">
         <f t="shared" si="25"/>
         <v>9240.471012458891</v>
       </c>
-      <c r="V46" s="78">
+      <c r="W46" s="78">
         <f t="shared" si="26"/>
         <v>6488.2637862886886</v>
       </c>
-      <c r="W46" s="44"/>
-      <c r="X46" s="76" t="s">
+      <c r="X46" s="44"/>
+      <c r="Y46" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="Y46" s="78">
+      <c r="Z46" s="78">
         <f t="shared" si="27"/>
         <v>13926.659985242084</v>
       </c>
-      <c r="Z46" s="78">
+      <c r="AA46" s="78">
         <f t="shared" si="28"/>
         <v>12262.845500986567</v>
       </c>
-      <c r="AA46" s="78">
+      <c r="AB46" s="78">
         <f t="shared" si="29"/>
         <v>13579.661324072413</v>
       </c>
-      <c r="AB46" s="44"/>
-      <c r="AC46" s="76" t="s">
+      <c r="AC46" s="44"/>
+      <c r="AD46" s="76" t="s">
         <v>291</v>
       </c>
-      <c r="AD46" s="78">
+      <c r="AE46" s="78">
         <f t="shared" si="30"/>
         <v>13975.008357927225</v>
       </c>
-      <c r="AE46" s="78">
+      <c r="AF46" s="78">
         <f t="shared" si="31"/>
         <v>13482.19053297028</v>
       </c>
-      <c r="AF46" s="78">
+      <c r="AG46" s="78">
         <f t="shared" si="32"/>
         <v>16869.47700799803</v>
       </c>
-      <c r="AG46" s="44"/>
       <c r="AH46" s="44"/>
       <c r="AI46" s="44"/>
       <c r="AJ46" s="44"/>
       <c r="AK46" s="44"/>
       <c r="AL46" s="44"/>
       <c r="AM46" s="44"/>
-    </row>
-    <row r="47" spans="2:47">
+      <c r="AN46" s="44"/>
+    </row>
+    <row r="47" spans="2:48">
       <c r="C47" t="s">
         <v>82</v>
       </c>
@@ -16332,66 +16373,66 @@
       <c r="K47" t="s">
         <v>231</v>
       </c>
-      <c r="O47" s="44"/>
       <c r="P47" s="44"/>
       <c r="Q47" s="44"/>
       <c r="R47" s="44"/>
-      <c r="S47" s="71" t="s">
+      <c r="S47" s="44"/>
+      <c r="T47" s="71" t="s">
         <v>293</v>
       </c>
-      <c r="T47" s="73">
+      <c r="U47" s="73">
         <f t="shared" si="24"/>
         <v>16647.690105556485</v>
       </c>
-      <c r="U47" s="73">
+      <c r="V47" s="73">
         <f t="shared" si="25"/>
         <v>24019.620233038979</v>
       </c>
-      <c r="V47" s="73">
+      <c r="W47" s="73">
         <f t="shared" si="26"/>
         <v>8173.0978681526803</v>
       </c>
-      <c r="W47" s="44"/>
-      <c r="X47" s="71" t="s">
+      <c r="X47" s="44"/>
+      <c r="Y47" s="71" t="s">
         <v>293</v>
       </c>
-      <c r="Y47" s="73">
+      <c r="Z47" s="73">
         <f t="shared" si="27"/>
         <v>20715.30675039117</v>
       </c>
-      <c r="Z47" s="73">
+      <c r="AA47" s="73">
         <f t="shared" si="28"/>
         <v>36930.213085458388</v>
       </c>
-      <c r="AA47" s="73">
+      <c r="AB47" s="73">
         <f t="shared" si="29"/>
         <v>26759.951991162201</v>
       </c>
-      <c r="AB47" s="44"/>
-      <c r="AC47" s="71" t="s">
+      <c r="AC47" s="44"/>
+      <c r="AD47" s="71" t="s">
         <v>293</v>
       </c>
-      <c r="AD47" s="73">
+      <c r="AE47" s="73">
         <f t="shared" si="30"/>
         <v>21492.491239260187</v>
       </c>
-      <c r="AE47" s="73">
+      <c r="AF47" s="73">
         <f t="shared" si="31"/>
         <v>43066.886084749698</v>
       </c>
-      <c r="AF47" s="73">
+      <c r="AG47" s="73">
         <f t="shared" si="32"/>
         <v>40519.506791775166</v>
       </c>
-      <c r="AG47" s="44"/>
       <c r="AH47" s="44"/>
       <c r="AI47" s="44"/>
       <c r="AJ47" s="44"/>
       <c r="AK47" s="44"/>
       <c r="AL47" s="44"/>
       <c r="AM47" s="44"/>
-    </row>
-    <row r="48" spans="2:47">
+      <c r="AN47" s="44"/>
+    </row>
+    <row r="48" spans="2:48">
       <c r="B48" s="44"/>
       <c r="C48" s="44"/>
       <c r="D48" s="44"/>
@@ -16403,66 +16444,66 @@
       <c r="J48" s="44"/>
       <c r="K48" s="44"/>
       <c r="M48" s="44"/>
-      <c r="O48" s="44"/>
       <c r="P48" s="44"/>
       <c r="Q48" s="44"/>
       <c r="R48" s="44"/>
-      <c r="S48" s="76" t="s">
+      <c r="S48" s="44"/>
+      <c r="T48" s="76" t="s">
         <v>295</v>
       </c>
-      <c r="T48" s="78">
+      <c r="U48" s="78">
         <f t="shared" si="24"/>
         <v>36572.106906621309</v>
       </c>
-      <c r="U48" s="78">
+      <c r="V48" s="78">
         <f t="shared" si="25"/>
         <v>74534.447300839645</v>
       </c>
-      <c r="V48" s="78">
+      <c r="W48" s="78">
         <f t="shared" si="26"/>
         <v>17477.536153470293</v>
       </c>
-      <c r="W48" s="44"/>
-      <c r="X48" s="76" t="s">
+      <c r="X48" s="44"/>
+      <c r="Y48" s="76" t="s">
         <v>295</v>
       </c>
-      <c r="Y48" s="78">
+      <c r="Z48" s="78">
         <f t="shared" si="27"/>
         <v>50012.96892024338</v>
       </c>
-      <c r="Z48" s="78">
+      <c r="AA48" s="78">
         <f t="shared" si="28"/>
         <v>141088.67366617039</v>
       </c>
-      <c r="AA48" s="78">
+      <c r="AB48" s="78">
         <f t="shared" si="29"/>
         <v>58779.81032423654</v>
       </c>
-      <c r="AB48" s="44"/>
-      <c r="AC48" s="76" t="s">
+      <c r="AC48" s="44"/>
+      <c r="AD48" s="76" t="s">
         <v>295</v>
       </c>
-      <c r="AD48" s="78">
+      <c r="AE48" s="78">
         <f t="shared" si="30"/>
         <v>57375.599603903931</v>
       </c>
-      <c r="AE48" s="78">
+      <c r="AF48" s="78">
         <f t="shared" si="31"/>
         <v>188110.99410254037</v>
       </c>
-      <c r="AF48" s="78">
+      <c r="AG48" s="78">
         <f t="shared" si="32"/>
         <v>104042.98039210709</v>
       </c>
-      <c r="AG48" s="44"/>
       <c r="AH48" s="44"/>
       <c r="AI48" s="44"/>
       <c r="AJ48" s="44"/>
       <c r="AK48" s="44"/>
       <c r="AL48" s="44"/>
       <c r="AM48" s="44"/>
-    </row>
-    <row r="49" spans="2:39">
+      <c r="AN48" s="44"/>
+    </row>
+    <row r="49" spans="2:40">
       <c r="B49" s="44"/>
       <c r="C49" s="44"/>
       <c r="D49" s="44"/>
@@ -16473,66 +16514,66 @@
       <c r="I49" s="39"/>
       <c r="J49" s="44"/>
       <c r="K49" s="44"/>
-      <c r="O49" s="44"/>
       <c r="P49" s="44"/>
       <c r="Q49" s="44"/>
       <c r="R49" s="44"/>
-      <c r="S49" s="71" t="s">
+      <c r="S49" s="44"/>
+      <c r="T49" s="71" t="s">
         <v>297</v>
       </c>
-      <c r="T49" s="73">
+      <c r="U49" s="73">
         <f t="shared" si="24"/>
         <v>17849.216311937973</v>
       </c>
-      <c r="U49" s="73">
+      <c r="V49" s="73">
         <f t="shared" si="25"/>
         <v>15789.558805433589</v>
       </c>
-      <c r="V49" s="73">
+      <c r="W49" s="73">
         <f t="shared" si="26"/>
         <v>9514.6922511536504</v>
       </c>
-      <c r="W49" s="44"/>
-      <c r="X49" s="71" t="s">
+      <c r="X49" s="44"/>
+      <c r="Y49" s="71" t="s">
         <v>297</v>
       </c>
-      <c r="Y49" s="73">
+      <c r="Z49" s="73">
         <f t="shared" si="27"/>
         <v>24461.048785696705</v>
       </c>
-      <c r="Z49" s="73">
+      <c r="AA49" s="73">
         <f t="shared" si="28"/>
         <v>33847.122298719267</v>
       </c>
-      <c r="AA49" s="73">
+      <c r="AB49" s="73">
         <f t="shared" si="29"/>
         <v>21204.386887924076</v>
       </c>
-      <c r="AB49" s="44"/>
-      <c r="AC49" s="71" t="s">
+      <c r="AC49" s="44"/>
+      <c r="AD49" s="71" t="s">
         <v>297</v>
       </c>
-      <c r="AD49" s="73">
+      <c r="AE49" s="73">
         <f t="shared" si="30"/>
         <v>28870.749849958043</v>
       </c>
-      <c r="AE49" s="73">
+      <c r="AF49" s="73">
         <f t="shared" si="31"/>
         <v>51002.265438518116</v>
       </c>
-      <c r="AF49" s="73">
+      <c r="AG49" s="73">
         <f t="shared" si="32"/>
         <v>33122.351085820024</v>
       </c>
-      <c r="AG49" s="44"/>
       <c r="AH49" s="44"/>
       <c r="AI49" s="44"/>
       <c r="AJ49" s="44"/>
       <c r="AK49" s="44"/>
       <c r="AL49" s="44"/>
       <c r="AM49" s="44"/>
-    </row>
-    <row r="50" spans="2:39">
+      <c r="AN49" s="44"/>
+    </row>
+    <row r="50" spans="2:40">
       <c r="B50" s="44"/>
       <c r="C50" s="44"/>
       <c r="D50" s="44"/>
@@ -16543,66 +16584,66 @@
       <c r="I50" s="39"/>
       <c r="J50" s="44"/>
       <c r="K50" s="44"/>
-      <c r="O50" s="44"/>
       <c r="P50" s="44"/>
       <c r="Q50" s="44"/>
       <c r="R50" s="44"/>
-      <c r="S50" s="76" t="s">
+      <c r="S50" s="44"/>
+      <c r="T50" s="76" t="s">
         <v>301</v>
       </c>
-      <c r="T50" s="78">
+      <c r="U50" s="78">
         <f t="shared" si="24"/>
         <v>3938.0259558602647</v>
       </c>
-      <c r="U50" s="78">
+      <c r="V50" s="78">
         <f t="shared" si="25"/>
         <v>4331.6447734858693</v>
       </c>
-      <c r="V50" s="78">
+      <c r="W50" s="78">
         <f t="shared" si="26"/>
         <v>2159.5267584074395</v>
       </c>
-      <c r="W50" s="44"/>
-      <c r="X50" s="76" t="s">
+      <c r="X50" s="44"/>
+      <c r="Y50" s="76" t="s">
         <v>301</v>
       </c>
-      <c r="Y50" s="78">
+      <c r="Z50" s="78">
         <f t="shared" si="27"/>
         <v>6912.0407347645551</v>
       </c>
-      <c r="Z50" s="78">
+      <c r="AA50" s="78">
         <f t="shared" si="28"/>
         <v>8089.5973561951996</v>
       </c>
-      <c r="AA50" s="78">
+      <c r="AB50" s="78">
         <f t="shared" si="29"/>
         <v>4280.6514403061055</v>
       </c>
-      <c r="AB50" s="44"/>
-      <c r="AC50" s="76" t="s">
+      <c r="AC50" s="44"/>
+      <c r="AD50" s="76" t="s">
         <v>301</v>
       </c>
-      <c r="AD50" s="78">
+      <c r="AE50" s="78">
         <f t="shared" si="30"/>
         <v>9347.9075829741523</v>
       </c>
-      <c r="AE50" s="78">
+      <c r="AF50" s="78">
         <f t="shared" si="31"/>
         <v>11678.738441783607</v>
       </c>
-      <c r="AF50" s="78">
+      <c r="AG50" s="78">
         <f t="shared" si="32"/>
         <v>6434.187698588451</v>
       </c>
-      <c r="AG50" s="44"/>
       <c r="AH50" s="44"/>
       <c r="AI50" s="44"/>
       <c r="AJ50" s="44"/>
       <c r="AK50" s="44"/>
       <c r="AL50" s="44"/>
       <c r="AM50" s="44"/>
-    </row>
-    <row r="51" spans="2:39">
+      <c r="AN50" s="44"/>
+    </row>
+    <row r="51" spans="2:40">
       <c r="B51" s="44"/>
       <c r="C51" s="44"/>
       <c r="D51" s="44"/>
@@ -16613,190 +16654,190 @@
       <c r="I51" s="39"/>
       <c r="J51" s="44"/>
       <c r="K51" s="44"/>
-      <c r="O51" s="44"/>
       <c r="P51" s="44"/>
       <c r="Q51" s="44"/>
       <c r="R51" s="44"/>
-      <c r="S51" s="71" t="s">
+      <c r="S51" s="44"/>
+      <c r="T51" s="71" t="s">
         <v>302</v>
       </c>
-      <c r="T51" s="73">
+      <c r="U51" s="73">
         <f t="shared" si="24"/>
         <v>732.92555592545455</v>
       </c>
-      <c r="U51" s="73">
+      <c r="V51" s="73">
         <f t="shared" si="25"/>
         <v>1242.9707904735708</v>
       </c>
-      <c r="V51" s="73">
+      <c r="W51" s="73">
         <f t="shared" si="26"/>
         <v>274.00794692472562</v>
       </c>
-      <c r="W51" s="44"/>
-      <c r="X51" s="71" t="s">
+      <c r="X51" s="44"/>
+      <c r="Y51" s="71" t="s">
         <v>302</v>
       </c>
-      <c r="Y51" s="73">
+      <c r="Z51" s="73">
         <f t="shared" si="27"/>
         <v>1225.7229927817559</v>
       </c>
-      <c r="Z51" s="73">
+      <c r="AA51" s="73">
         <f t="shared" si="28"/>
         <v>2173.8141671126914</v>
       </c>
-      <c r="AA51" s="73">
+      <c r="AB51" s="73">
         <f t="shared" si="29"/>
         <v>592.33180111255604</v>
       </c>
-      <c r="AB51" s="44"/>
-      <c r="AC51" s="71" t="s">
+      <c r="AC51" s="44"/>
+      <c r="AD51" s="71" t="s">
         <v>302</v>
       </c>
-      <c r="AD51" s="73">
+      <c r="AE51" s="73">
         <f t="shared" si="30"/>
         <v>1655.0315160569444</v>
       </c>
-      <c r="AE51" s="73">
+      <c r="AF51" s="73">
         <f t="shared" si="31"/>
         <v>3053.0061716946507</v>
       </c>
-      <c r="AF51" s="73">
+      <c r="AG51" s="73">
         <f t="shared" si="32"/>
         <v>949.05336745746956</v>
       </c>
-      <c r="AG51" s="44"/>
       <c r="AH51" s="44"/>
       <c r="AI51" s="44"/>
       <c r="AJ51" s="44"/>
       <c r="AK51" s="44"/>
       <c r="AL51" s="44"/>
       <c r="AM51" s="44"/>
-    </row>
-    <row r="52" spans="2:39" ht="15.75" thickBot="1">
+      <c r="AN51" s="44"/>
+    </row>
+    <row r="52" spans="2:40" ht="15.75" thickBot="1">
       <c r="H52" s="39"/>
       <c r="I52" s="39"/>
-      <c r="O52" s="44"/>
       <c r="P52" s="44"/>
       <c r="Q52" s="44"/>
       <c r="R52" s="44"/>
-      <c r="S52" s="82" t="s">
+      <c r="S52" s="44"/>
+      <c r="T52" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="T52" s="83">
+      <c r="U52" s="83">
         <f t="shared" si="24"/>
         <v>317.15363773506533</v>
       </c>
-      <c r="U52" s="83">
+      <c r="V52" s="83">
         <f t="shared" si="25"/>
         <v>1188.2824731347082</v>
       </c>
-      <c r="V52" s="83">
+      <c r="W52" s="83">
         <f t="shared" si="26"/>
         <v>213.27413770047775</v>
       </c>
-      <c r="W52" s="44"/>
-      <c r="X52" s="82" t="s">
+      <c r="X52" s="44"/>
+      <c r="Y52" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="Y52" s="83">
+      <c r="Z52" s="83">
         <f t="shared" si="27"/>
         <v>475.94182609578115</v>
       </c>
-      <c r="Z52" s="83">
+      <c r="AA52" s="83">
         <f t="shared" si="28"/>
         <v>1769.2778770171465</v>
       </c>
-      <c r="AA52" s="83">
+      <c r="AB52" s="83">
         <f t="shared" si="29"/>
         <v>388.42777521510436</v>
       </c>
-      <c r="AB52" s="44"/>
-      <c r="AC52" s="82" t="s">
+      <c r="AC52" s="44"/>
+      <c r="AD52" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="AD52" s="83">
+      <c r="AE52" s="83">
         <f t="shared" si="30"/>
         <v>612.87120420892359</v>
       </c>
-      <c r="AE52" s="83">
+      <c r="AF52" s="83">
         <f t="shared" si="31"/>
         <v>2270.3026352539346</v>
       </c>
-      <c r="AF52" s="83">
+      <c r="AG52" s="83">
         <f t="shared" si="32"/>
         <v>567.16083246963353</v>
       </c>
-      <c r="AG52" s="44"/>
       <c r="AH52" s="44"/>
       <c r="AI52" s="44"/>
       <c r="AJ52" s="44"/>
       <c r="AK52" s="44"/>
       <c r="AL52" s="44"/>
       <c r="AM52" s="44"/>
-    </row>
-    <row r="53" spans="2:39" ht="15.75" thickBot="1">
+      <c r="AN52" s="44"/>
+    </row>
+    <row r="53" spans="2:40" ht="15.75" thickBot="1">
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
-      <c r="O53" s="44"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="44"/>
       <c r="R53" s="44"/>
-      <c r="S53" s="85" t="s">
+      <c r="S53" s="44"/>
+      <c r="T53" s="85" t="s">
         <v>304</v>
       </c>
-      <c r="T53" s="86">
-        <f>SUM(T44:T52)</f>
+      <c r="U53" s="86">
+        <f>SUM(U44:U52)</f>
         <v>105962.73388948065</v>
       </c>
-      <c r="U53" s="86">
-        <f t="shared" ref="U53:V53" si="33">SUM(U44:U52)</f>
+      <c r="V53" s="86">
+        <f t="shared" ref="V53:W53" si="33">SUM(V44:V52)</f>
         <v>207586.69918233968</v>
       </c>
-      <c r="V53" s="86">
+      <c r="W53" s="86">
         <f t="shared" si="33"/>
         <v>86634.450374212713</v>
       </c>
-      <c r="W53" s="44"/>
-      <c r="X53" s="85" t="s">
+      <c r="X53" s="44"/>
+      <c r="Y53" s="85" t="s">
         <v>304</v>
       </c>
-      <c r="Y53" s="86">
-        <f>SUM(Y44:Y52)</f>
+      <c r="Z53" s="86">
+        <f>SUM(Z44:Z52)</f>
         <v>134648.63676614748</v>
       </c>
-      <c r="Z53" s="86">
-        <f t="shared" ref="Z53:AA53" si="34">SUM(Z44:Z52)</f>
+      <c r="AA53" s="86">
+        <f t="shared" ref="AA53:AB53" si="34">SUM(AA44:AA52)</f>
         <v>314857.87810644717</v>
       </c>
-      <c r="AA53" s="86">
+      <c r="AB53" s="86">
         <f t="shared" si="34"/>
         <v>170140.9754920128</v>
       </c>
-      <c r="AB53" s="44"/>
-      <c r="AC53" s="85" t="s">
+      <c r="AC53" s="44"/>
+      <c r="AD53" s="85" t="s">
         <v>304</v>
       </c>
-      <c r="AD53" s="86">
-        <f>SUM(AD44:AD52)</f>
+      <c r="AE53" s="86">
+        <f>SUM(AE44:AE52)</f>
         <v>150260.60638899147</v>
       </c>
-      <c r="AE53" s="86">
-        <f t="shared" ref="AE53:AF53" si="35">SUM(AE44:AE52)</f>
+      <c r="AF53" s="86">
+        <f t="shared" ref="AF53:AG53" si="35">SUM(AF44:AF52)</f>
         <v>391706.44373251824</v>
       </c>
-      <c r="AF53" s="86">
+      <c r="AG53" s="86">
         <f t="shared" si="35"/>
         <v>247730.58425388101</v>
       </c>
-      <c r="AG53" s="44"/>
       <c r="AH53" s="44"/>
       <c r="AI53" s="44"/>
       <c r="AJ53" s="44"/>
       <c r="AK53" s="44"/>
       <c r="AL53" s="44"/>
       <c r="AM53" s="44"/>
-    </row>
-    <row r="54" spans="2:39">
+      <c r="AN53" s="44"/>
+    </row>
+    <row r="54" spans="2:40">
       <c r="B54" s="7" t="s">
         <v>86</v>
       </c>
@@ -16806,60 +16847,60 @@
       <c r="M54" s="25">
         <v>0.5</v>
       </c>
-      <c r="O54" s="44"/>
       <c r="P54" s="44"/>
       <c r="Q54" s="44"/>
       <c r="R54" s="44"/>
       <c r="S54" s="44"/>
-      <c r="T54" s="88">
-        <f>T53/U16</f>
-        <v>0.50043916761777862</v>
-      </c>
+      <c r="T54" s="44"/>
       <c r="U54" s="88">
         <f>U53/V16</f>
-        <v>0.26747266421529797</v>
+        <v>0.50043916761777862</v>
       </c>
       <c r="V54" s="88">
         <f>V53/W16</f>
+        <v>0.26747266421529797</v>
+      </c>
+      <c r="W54" s="88">
+        <f>W53/X16</f>
         <v>0.11875876326974115</v>
       </c>
-      <c r="W54" s="44"/>
       <c r="X54" s="44"/>
-      <c r="Y54" s="88">
-        <f>Y53/U16</f>
-        <v>0.63591650791494814</v>
-      </c>
+      <c r="Y54" s="44"/>
       <c r="Z54" s="88">
         <f>Z53/V16</f>
-        <v>0.40569013254714142</v>
+        <v>0.63591650791494814</v>
       </c>
       <c r="AA54" s="88">
         <f>AA53/W16</f>
+        <v>0.40569013254714142</v>
+      </c>
+      <c r="AB54" s="88">
+        <f>AB53/X16</f>
         <v>0.23322975725777956</v>
       </c>
-      <c r="AB54" s="44"/>
       <c r="AC54" s="44"/>
-      <c r="AD54" s="88">
-        <f>AD53/U16</f>
-        <v>0.70964847760043115</v>
-      </c>
+      <c r="AD54" s="44"/>
       <c r="AE54" s="88">
         <f>AE53/V16</f>
-        <v>0.50470847365518334</v>
+        <v>0.70964847760043115</v>
       </c>
       <c r="AF54" s="88">
         <f>AF53/W16</f>
+        <v>0.50470847365518334</v>
+      </c>
+      <c r="AG54" s="88">
+        <f>AG53/X16</f>
         <v>0.3395898246367639</v>
       </c>
-      <c r="AG54" s="44"/>
       <c r="AH54" s="44"/>
       <c r="AI54" s="44"/>
       <c r="AJ54" s="44"/>
       <c r="AK54" s="44"/>
       <c r="AL54" s="44"/>
       <c r="AM54" s="44"/>
-    </row>
-    <row r="55" spans="2:39" ht="15.75" thickBot="1">
+      <c r="AN54" s="44"/>
+    </row>
+    <row r="55" spans="2:40" ht="15.75" thickBot="1">
       <c r="B55" s="10" t="s">
         <v>12</v>
       </c>
@@ -16890,15 +16931,14 @@
       <c r="K55" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O55" s="44"/>
       <c r="P55" s="44"/>
       <c r="Q55" s="44"/>
       <c r="R55" s="44"/>
       <c r="S55" s="44"/>
-      <c r="T55" s="44" t="s">
+      <c r="T55" s="44"/>
+      <c r="U55" s="44" t="s">
         <v>310</v>
       </c>
-      <c r="U55" s="44"/>
       <c r="V55" s="44"/>
       <c r="W55" s="44"/>
       <c r="X55" s="44"/>
@@ -16917,8 +16957,9 @@
       <c r="AK55" s="44"/>
       <c r="AL55" s="44"/>
       <c r="AM55" s="44"/>
-    </row>
-    <row r="56" spans="2:39">
+      <c r="AN55" s="44"/>
+    </row>
+    <row r="56" spans="2:40">
       <c r="C56" t="s">
         <v>203</v>
       </c>
@@ -16937,60 +16978,60 @@
       <c r="K56" t="s">
         <v>103</v>
       </c>
-      <c r="O56" s="44"/>
       <c r="P56" s="44"/>
       <c r="Q56" s="44"/>
       <c r="R56" s="44"/>
       <c r="S56" s="44"/>
-      <c r="T56" s="89">
-        <f>SUM(T44:T50)</f>
+      <c r="T56" s="44"/>
+      <c r="U56" s="89">
+        <f>SUM(U44:U50)</f>
         <v>104912.65469582012</v>
       </c>
-      <c r="U56" s="89">
-        <f t="shared" ref="U56:V56" si="36">SUM(U44:U50)</f>
+      <c r="V56" s="89">
+        <f t="shared" ref="V56:W56" si="36">SUM(V44:V50)</f>
         <v>205155.44591873139</v>
       </c>
-      <c r="V56" s="89">
+      <c r="W56" s="89">
         <f t="shared" si="36"/>
         <v>86147.168289587513</v>
       </c>
-      <c r="W56" s="44"/>
       <c r="X56" s="44"/>
-      <c r="Y56" s="89">
-        <f>SUM(Y44:Y50)</f>
+      <c r="Y56" s="44"/>
+      <c r="Z56" s="89">
+        <f>SUM(Z44:Z50)</f>
         <v>132946.97194726995</v>
       </c>
-      <c r="Z56" s="89">
-        <f t="shared" ref="Z56:AA56" si="37">SUM(Z44:Z50)</f>
+      <c r="AA56" s="89">
+        <f t="shared" ref="AA56:AB56" si="37">SUM(AA44:AA50)</f>
         <v>310914.78606231732</v>
       </c>
-      <c r="AA56" s="89">
+      <c r="AB56" s="89">
         <f t="shared" si="37"/>
         <v>169160.21591568514</v>
       </c>
-      <c r="AB56" s="44"/>
       <c r="AC56" s="44"/>
-      <c r="AD56" s="89">
-        <f>SUM(AD44:AD50)</f>
+      <c r="AD56" s="44"/>
+      <c r="AE56" s="89">
+        <f>SUM(AE44:AE50)</f>
         <v>147992.70366872559</v>
       </c>
-      <c r="AE56" s="89">
-        <f t="shared" ref="AE56:AF56" si="38">SUM(AE44:AE50)</f>
+      <c r="AF56" s="89">
+        <f t="shared" ref="AF56:AG56" si="38">SUM(AF44:AF50)</f>
         <v>386383.13492556964</v>
       </c>
-      <c r="AF56" s="89">
+      <c r="AG56" s="89">
         <f t="shared" si="38"/>
         <v>246214.3700539539</v>
       </c>
-      <c r="AG56" s="44"/>
       <c r="AH56" s="44"/>
       <c r="AI56" s="44"/>
       <c r="AJ56" s="44"/>
       <c r="AK56" s="44"/>
       <c r="AL56" s="44"/>
       <c r="AM56" s="44"/>
-    </row>
-    <row r="57" spans="2:39">
+      <c r="AN56" s="44"/>
+    </row>
+    <row r="57" spans="2:40">
       <c r="C57" t="s">
         <v>203</v>
       </c>
@@ -17009,60 +17050,60 @@
         <f>RSDAFC!C2</f>
         <v>R-HC_Apt_ELC_HPN1</v>
       </c>
-      <c r="O57" s="44"/>
       <c r="P57" s="44"/>
       <c r="Q57" s="44"/>
       <c r="R57" s="44"/>
       <c r="S57" s="44"/>
-      <c r="T57" s="90">
-        <f>T56/U16</f>
-        <v>0.49547986977485658</v>
-      </c>
+      <c r="T57" s="44"/>
       <c r="U57" s="90">
         <f>U56/V16</f>
-        <v>0.26434002715155119</v>
+        <v>0.49547986977485658</v>
       </c>
       <c r="V57" s="90">
         <f>V56/W16</f>
+        <v>0.26434002715155119</v>
+      </c>
+      <c r="W57" s="90">
+        <f>W56/X16</f>
         <v>0.11809079553307718</v>
       </c>
-      <c r="W57" s="44"/>
       <c r="X57" s="44"/>
-      <c r="Y57" s="91">
-        <f>Y56/U16</f>
-        <v>0.6278799115167113</v>
-      </c>
+      <c r="Y57" s="44"/>
       <c r="Z57" s="91">
         <f>Z56/V16</f>
-        <v>0.40060951159000024</v>
+        <v>0.6278799115167113</v>
       </c>
       <c r="AA57" s="91">
         <f>AA56/W16</f>
+        <v>0.40060951159000024</v>
+      </c>
+      <c r="AB57" s="91">
+        <f>AB56/X16</f>
         <v>0.23188532910193016</v>
       </c>
-      <c r="AB57" s="44"/>
       <c r="AC57" s="44"/>
-      <c r="AD57" s="91">
-        <f>AD56/U16</f>
-        <v>0.69893766156248616</v>
-      </c>
+      <c r="AD57" s="44"/>
       <c r="AE57" s="91">
         <f>AE56/V16</f>
-        <v>0.49784946200056557</v>
+        <v>0.69893766156248616</v>
       </c>
       <c r="AF57" s="91">
         <f>AF56/W16</f>
+        <v>0.49784946200056557</v>
+      </c>
+      <c r="AG57" s="91">
+        <f>AG56/X16</f>
         <v>0.33751139368397792</v>
       </c>
-      <c r="AG57" s="44"/>
       <c r="AH57" s="44"/>
       <c r="AI57" s="44"/>
       <c r="AJ57" s="44"/>
       <c r="AK57" s="44"/>
       <c r="AL57" s="44"/>
       <c r="AM57" s="44"/>
-    </row>
-    <row r="58" spans="2:39">
+      <c r="AN57" s="44"/>
+    </row>
+    <row r="58" spans="2:40">
       <c r="C58" t="s">
         <v>203</v>
       </c>
@@ -17082,7 +17123,7 @@
         <v>R-HC_Apt_ELC_HPN1</v>
       </c>
     </row>
-    <row r="59" spans="2:39">
+    <row r="59" spans="2:40">
       <c r="C59" t="s">
         <v>203</v>
       </c>
@@ -17102,7 +17143,7 @@
         <v>R-HC_Apt_ELC_HPN2*</v>
       </c>
     </row>
-    <row r="60" spans="2:39">
+    <row r="60" spans="2:40">
       <c r="C60" t="s">
         <v>203</v>
       </c>
@@ -17122,7 +17163,7 @@
         <v>R-HC_Apt_ELC_HPN2*</v>
       </c>
     </row>
-    <row r="61" spans="2:39">
+    <row r="61" spans="2:40">
       <c r="C61" t="s">
         <v>203</v>
       </c>
@@ -17142,7 +17183,7 @@
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="62" spans="2:39">
+    <row r="62" spans="2:40">
       <c r="C62" t="s">
         <v>203</v>
       </c>
@@ -17162,7 +17203,7 @@
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
     </row>
-    <row r="63" spans="2:39">
+    <row r="63" spans="2:40">
       <c r="C63" t="s">
         <v>203</v>
       </c>
@@ -17182,7 +17223,7 @@
         <v>R-HC_Att_ELC_HPN2*</v>
       </c>
     </row>
-    <row r="64" spans="2:39">
+    <row r="64" spans="2:40">
       <c r="C64" t="s">
         <v>203</v>
       </c>
@@ -19774,20 +19815,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="AD5:AF5"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="AM28:AU28"/>
-    <mergeCell ref="AC28:AK28"/>
-    <mergeCell ref="S42:V42"/>
-    <mergeCell ref="X42:AA42"/>
-    <mergeCell ref="AC42:AF42"/>
-    <mergeCell ref="T28:AA28"/>
+    <mergeCell ref="AN28:AV28"/>
+    <mergeCell ref="AD28:AL28"/>
+    <mergeCell ref="T42:W42"/>
+    <mergeCell ref="Y42:AB42"/>
+    <mergeCell ref="AD42:AG42"/>
+    <mergeCell ref="U28:AB28"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="U5:Y5"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="Q12:S12"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
-  <conditionalFormatting sqref="T30:AA38">
+  <conditionalFormatting sqref="U30:AB38">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -19799,7 +19840,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD30:AK38">
+  <conditionalFormatting sqref="AE30:AL38">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -19811,7 +19852,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AN30:AU38">
+  <conditionalFormatting sqref="AO30:AV38">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -19823,6 +19864,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7" xr:uid="{1FE2C46E-0F36-449A-A690-A40D9B93D41C}">
+      <formula1>$U$29:$AB$29</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N16" xr:uid="{F5BBB0D6-0F4A-4840-87F3-D7F0F3620D9B}">
+      <formula1>$AE$29:$AL$29</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N25" xr:uid="{8EE695F0-4138-4A4C-AF1B-02E028BC3519}">
+      <formula1>$AO$29:$AV$29</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Lo constraints on regions removed
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4B41B6-C091-40C2-86A5-567849B49D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469DB7BF-4E8C-46B7-B79F-38555D6F1CC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8145" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -2072,16 +2072,16 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="21" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -13085,7 +13085,7 @@
   <dimension ref="A1:AV204"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13239,31 +13239,31 @@
         <v>333</v>
       </c>
       <c r="P5" s="44"/>
-      <c r="Q5" s="99" t="s">
+      <c r="Q5" s="101" t="s">
         <v>277</v>
       </c>
-      <c r="R5" s="99"/>
-      <c r="S5" s="99"/>
+      <c r="R5" s="101"/>
+      <c r="S5" s="101"/>
       <c r="T5" s="44"/>
-      <c r="U5" s="99" t="s">
+      <c r="U5" s="101" t="s">
         <v>278</v>
       </c>
-      <c r="V5" s="99"/>
-      <c r="W5" s="99"/>
-      <c r="X5" s="99"/>
-      <c r="Y5" s="99"/>
+      <c r="V5" s="101"/>
+      <c r="W5" s="101"/>
+      <c r="X5" s="101"/>
+      <c r="Y5" s="101"/>
       <c r="Z5" s="44"/>
-      <c r="AA5" s="99" t="s">
+      <c r="AA5" s="101" t="s">
         <v>279</v>
       </c>
-      <c r="AB5" s="99"/>
-      <c r="AC5" s="99"/>
+      <c r="AB5" s="101"/>
+      <c r="AC5" s="101"/>
       <c r="AD5" s="44"/>
-      <c r="AE5" s="99" t="s">
+      <c r="AE5" s="101" t="s">
         <v>280</v>
       </c>
-      <c r="AF5" s="99"/>
-      <c r="AG5" s="99"/>
+      <c r="AF5" s="101"/>
+      <c r="AG5" s="101"/>
       <c r="AH5" s="44"/>
       <c r="AI5" s="44"/>
       <c r="AJ5" s="44"/>
@@ -13699,11 +13699,11 @@
       </c>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
-      <c r="Q12" s="100" t="s">
+      <c r="Q12" s="102" t="s">
         <v>296</v>
       </c>
-      <c r="R12" s="100"/>
-      <c r="S12" s="100"/>
+      <c r="R12" s="102"/>
+      <c r="S12" s="102"/>
       <c r="U12" s="71" t="s">
         <v>297</v>
       </c>
@@ -14653,40 +14653,40 @@
       <c r="R28" s="44"/>
       <c r="S28" s="44"/>
       <c r="T28" s="44"/>
-      <c r="U28" s="101" t="s">
+      <c r="U28" s="99" t="s">
         <v>281</v>
       </c>
-      <c r="V28" s="102"/>
-      <c r="W28" s="102"/>
-      <c r="X28" s="102"/>
-      <c r="Y28" s="102"/>
-      <c r="Z28" s="102"/>
-      <c r="AA28" s="102"/>
-      <c r="AB28" s="102"/>
+      <c r="V28" s="100"/>
+      <c r="W28" s="100"/>
+      <c r="X28" s="100"/>
+      <c r="Y28" s="100"/>
+      <c r="Z28" s="100"/>
+      <c r="AA28" s="100"/>
+      <c r="AB28" s="100"/>
       <c r="AC28" s="44"/>
-      <c r="AD28" s="102" t="s">
+      <c r="AD28" s="100" t="s">
         <v>282</v>
       </c>
-      <c r="AE28" s="102"/>
-      <c r="AF28" s="102"/>
-      <c r="AG28" s="102"/>
-      <c r="AH28" s="102"/>
-      <c r="AI28" s="102"/>
-      <c r="AJ28" s="102"/>
-      <c r="AK28" s="102"/>
-      <c r="AL28" s="102"/>
+      <c r="AE28" s="100"/>
+      <c r="AF28" s="100"/>
+      <c r="AG28" s="100"/>
+      <c r="AH28" s="100"/>
+      <c r="AI28" s="100"/>
+      <c r="AJ28" s="100"/>
+      <c r="AK28" s="100"/>
+      <c r="AL28" s="100"/>
       <c r="AM28" s="44"/>
-      <c r="AN28" s="101" t="s">
+      <c r="AN28" s="99" t="s">
         <v>283</v>
       </c>
-      <c r="AO28" s="102"/>
-      <c r="AP28" s="102"/>
-      <c r="AQ28" s="102"/>
-      <c r="AR28" s="102"/>
-      <c r="AS28" s="102"/>
-      <c r="AT28" s="102"/>
-      <c r="AU28" s="102"/>
-      <c r="AV28" s="102"/>
+      <c r="AO28" s="100"/>
+      <c r="AP28" s="100"/>
+      <c r="AQ28" s="100"/>
+      <c r="AR28" s="100"/>
+      <c r="AS28" s="100"/>
+      <c r="AT28" s="100"/>
+      <c r="AU28" s="100"/>
+      <c r="AV28" s="100"/>
     </row>
     <row r="29" spans="2:48">
       <c r="B29" s="44"/>
@@ -15864,7 +15864,7 @@
         <v>14</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="I39" s="11" t="s">
         <v>242</v>
@@ -16022,26 +16022,26 @@
       <c r="Q42" s="44"/>
       <c r="R42" s="44"/>
       <c r="S42" s="44"/>
-      <c r="T42" s="99" t="s">
+      <c r="T42" s="101" t="s">
         <v>307</v>
       </c>
-      <c r="U42" s="99"/>
-      <c r="V42" s="99"/>
-      <c r="W42" s="99"/>
+      <c r="U42" s="101"/>
+      <c r="V42" s="101"/>
+      <c r="W42" s="101"/>
       <c r="X42" s="44"/>
-      <c r="Y42" s="99" t="s">
+      <c r="Y42" s="101" t="s">
         <v>308</v>
       </c>
-      <c r="Z42" s="99"/>
-      <c r="AA42" s="99"/>
-      <c r="AB42" s="99"/>
+      <c r="Z42" s="101"/>
+      <c r="AA42" s="101"/>
+      <c r="AB42" s="101"/>
       <c r="AC42" s="44"/>
-      <c r="AD42" s="99" t="s">
+      <c r="AD42" s="101" t="s">
         <v>309</v>
       </c>
-      <c r="AE42" s="99"/>
-      <c r="AF42" s="99"/>
-      <c r="AG42" s="99"/>
+      <c r="AE42" s="101"/>
+      <c r="AF42" s="101"/>
+      <c r="AG42" s="101"/>
       <c r="AH42" s="44"/>
       <c r="AI42" s="44"/>
       <c r="AJ42" s="44"/>
@@ -19815,17 +19815,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="U5:Y5"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="Q12:S12"/>
     <mergeCell ref="AN28:AV28"/>
     <mergeCell ref="AD28:AL28"/>
     <mergeCell ref="T42:W42"/>
     <mergeCell ref="Y42:AB42"/>
     <mergeCell ref="AD42:AG42"/>
     <mergeCell ref="U28:AB28"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="U5:Y5"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="Q12:S12"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <conditionalFormatting sqref="U30:AB38">

</xml_diff>

<commit_message>
Add PWRAHT commodity, limit existing DH
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E72B7F-BB02-464D-AA4B-E0DCF6E2BA42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616C1B0C-ED6C-4D7B-8FF8-DE3F6C532E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="344">
   <si>
     <t>UC_N</t>
   </si>
@@ -1235,15 +1235,12 @@
   <si>
     <t>HET-GRID</t>
   </si>
-  <si>
-    <t>FT-RSDHET_X,FT-SRVHET_X,</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1251,7 +1248,6 @@
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="173" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1846,9 +1842,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2077,19 +2073,18 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -12320,7 +12315,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12720,24 +12715,20 @@
         <v>2018</v>
       </c>
       <c r="F26">
-        <v>0.35</v>
+        <v>0.6</v>
       </c>
       <c r="G26">
         <f>F26</f>
-        <v>0.35</v>
-      </c>
-      <c r="H26" s="103" t="s">
-        <v>344</v>
-      </c>
-      <c r="I26" s="103" t="s">
+        <v>0.6</v>
+      </c>
+      <c r="H26" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="I26" s="44" t="s">
         <v>343</v>
       </c>
-      <c r="L26" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="M26" s="44" t="s">
-        <v>343</v>
-      </c>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
     </row>
     <row r="27" spans="2:13">
       <c r="C27" t="str">
@@ -12758,18 +12749,14 @@
         <f>F27</f>
         <v>5</v>
       </c>
-      <c r="H27" s="103" t="s">
-        <v>344</v>
-      </c>
-      <c r="I27" s="103" t="s">
+      <c r="H27" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="I27" s="44" t="s">
         <v>343</v>
       </c>
-      <c r="L27" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="M27" s="44" t="s">
-        <v>343</v>
-      </c>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
     </row>
     <row r="28" spans="2:13">
       <c r="C28" t="s">
@@ -13257,31 +13244,31 @@
         <v>332</v>
       </c>
       <c r="P5" s="44"/>
-      <c r="Q5" s="101" t="s">
+      <c r="Q5" s="99" t="s">
         <v>276</v>
       </c>
-      <c r="R5" s="101"/>
-      <c r="S5" s="101"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="99"/>
       <c r="T5" s="44"/>
-      <c r="U5" s="101" t="s">
+      <c r="U5" s="99" t="s">
         <v>277</v>
       </c>
-      <c r="V5" s="101"/>
-      <c r="W5" s="101"/>
-      <c r="X5" s="101"/>
-      <c r="Y5" s="101"/>
+      <c r="V5" s="99"/>
+      <c r="W5" s="99"/>
+      <c r="X5" s="99"/>
+      <c r="Y5" s="99"/>
       <c r="Z5" s="44"/>
-      <c r="AA5" s="101" t="s">
+      <c r="AA5" s="99" t="s">
         <v>278</v>
       </c>
-      <c r="AB5" s="101"/>
-      <c r="AC5" s="101"/>
+      <c r="AB5" s="99"/>
+      <c r="AC5" s="99"/>
       <c r="AD5" s="44"/>
-      <c r="AE5" s="101" t="s">
+      <c r="AE5" s="99" t="s">
         <v>279</v>
       </c>
-      <c r="AF5" s="101"/>
-      <c r="AG5" s="101"/>
+      <c r="AF5" s="99"/>
+      <c r="AG5" s="99"/>
       <c r="AH5" s="44"/>
       <c r="AI5" s="44"/>
       <c r="AJ5" s="44"/>
@@ -13717,11 +13704,11 @@
       </c>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
-      <c r="Q12" s="102" t="s">
+      <c r="Q12" s="100" t="s">
         <v>295</v>
       </c>
-      <c r="R12" s="102"/>
-      <c r="S12" s="102"/>
+      <c r="R12" s="100"/>
+      <c r="S12" s="100"/>
       <c r="U12" s="71" t="s">
         <v>296</v>
       </c>
@@ -14671,40 +14658,40 @@
       <c r="R28" s="44"/>
       <c r="S28" s="44"/>
       <c r="T28" s="44"/>
-      <c r="U28" s="99" t="s">
+      <c r="U28" s="101" t="s">
         <v>280</v>
       </c>
-      <c r="V28" s="100"/>
-      <c r="W28" s="100"/>
-      <c r="X28" s="100"/>
-      <c r="Y28" s="100"/>
-      <c r="Z28" s="100"/>
-      <c r="AA28" s="100"/>
-      <c r="AB28" s="100"/>
+      <c r="V28" s="102"/>
+      <c r="W28" s="102"/>
+      <c r="X28" s="102"/>
+      <c r="Y28" s="102"/>
+      <c r="Z28" s="102"/>
+      <c r="AA28" s="102"/>
+      <c r="AB28" s="102"/>
       <c r="AC28" s="44"/>
-      <c r="AD28" s="100" t="s">
+      <c r="AD28" s="102" t="s">
         <v>281</v>
       </c>
-      <c r="AE28" s="100"/>
-      <c r="AF28" s="100"/>
-      <c r="AG28" s="100"/>
-      <c r="AH28" s="100"/>
-      <c r="AI28" s="100"/>
-      <c r="AJ28" s="100"/>
-      <c r="AK28" s="100"/>
-      <c r="AL28" s="100"/>
+      <c r="AE28" s="102"/>
+      <c r="AF28" s="102"/>
+      <c r="AG28" s="102"/>
+      <c r="AH28" s="102"/>
+      <c r="AI28" s="102"/>
+      <c r="AJ28" s="102"/>
+      <c r="AK28" s="102"/>
+      <c r="AL28" s="102"/>
       <c r="AM28" s="44"/>
-      <c r="AN28" s="99" t="s">
+      <c r="AN28" s="101" t="s">
         <v>282</v>
       </c>
-      <c r="AO28" s="100"/>
-      <c r="AP28" s="100"/>
-      <c r="AQ28" s="100"/>
-      <c r="AR28" s="100"/>
-      <c r="AS28" s="100"/>
-      <c r="AT28" s="100"/>
-      <c r="AU28" s="100"/>
-      <c r="AV28" s="100"/>
+      <c r="AO28" s="102"/>
+      <c r="AP28" s="102"/>
+      <c r="AQ28" s="102"/>
+      <c r="AR28" s="102"/>
+      <c r="AS28" s="102"/>
+      <c r="AT28" s="102"/>
+      <c r="AU28" s="102"/>
+      <c r="AV28" s="102"/>
     </row>
     <row r="29" spans="2:48">
       <c r="B29" s="44"/>
@@ -16040,26 +16027,26 @@
       <c r="Q42" s="44"/>
       <c r="R42" s="44"/>
       <c r="S42" s="44"/>
-      <c r="T42" s="101" t="s">
+      <c r="T42" s="99" t="s">
         <v>306</v>
       </c>
-      <c r="U42" s="101"/>
-      <c r="V42" s="101"/>
-      <c r="W42" s="101"/>
+      <c r="U42" s="99"/>
+      <c r="V42" s="99"/>
+      <c r="W42" s="99"/>
       <c r="X42" s="44"/>
-      <c r="Y42" s="101" t="s">
+      <c r="Y42" s="99" t="s">
         <v>307</v>
       </c>
-      <c r="Z42" s="101"/>
-      <c r="AA42" s="101"/>
-      <c r="AB42" s="101"/>
+      <c r="Z42" s="99"/>
+      <c r="AA42" s="99"/>
+      <c r="AB42" s="99"/>
       <c r="AC42" s="44"/>
-      <c r="AD42" s="101" t="s">
+      <c r="AD42" s="99" t="s">
         <v>308</v>
       </c>
-      <c r="AE42" s="101"/>
-      <c r="AF42" s="101"/>
-      <c r="AG42" s="101"/>
+      <c r="AE42" s="99"/>
+      <c r="AF42" s="99"/>
+      <c r="AG42" s="99"/>
       <c r="AH42" s="44"/>
       <c r="AI42" s="44"/>
       <c r="AJ42" s="44"/>
@@ -19833,17 +19820,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="U5:Y5"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="Q12:S12"/>
     <mergeCell ref="AN28:AV28"/>
     <mergeCell ref="AD28:AL28"/>
     <mergeCell ref="T42:W42"/>
     <mergeCell ref="Y42:AB42"/>
     <mergeCell ref="AD42:AG42"/>
     <mergeCell ref="U28:AB28"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="U5:Y5"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="Q12:S12"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <conditionalFormatting sqref="U30:AB38">

</xml_diff>

<commit_message>
Set maximum solar capacity bound at 5.5 GW
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D0A763-C3EF-4CFC-BC62-3660EFE3BBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695E09F2-2837-485A-8C73-50ABCCCE0369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="336">
   <si>
     <t>UC_N</t>
   </si>
@@ -1200,6 +1200,15 @@
   </si>
   <si>
     <t>P-RNW-SOL-CSP*</t>
+  </si>
+  <si>
+    <t>Maximum solar PV capacity</t>
+  </si>
+  <si>
+    <t>UC_Max_PV_Cap</t>
+  </si>
+  <si>
+    <t>P*SOL-PV*</t>
   </si>
 </sst>
 </file>
@@ -2011,16 +2020,16 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="12" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -11721,280 +11730,375 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:M17"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C2:D2)</f>
+        <v xml:space="preserve">~UC_Sets: R_E: </v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="F6" s="31">
+        <v>2030</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="31">
+        <v>5.5</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="F7" s="31">
+        <v>0</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="K8" s="31"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="11" t="str">
+      <c r="F11" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G3" s="11" t="str">
+      <c r="G11" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J11" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>84</v>
       </c>
-      <c r="F4">
+      <c r="F12">
         <v>5</v>
       </c>
-      <c r="G4">
-        <f t="shared" ref="G4" si="0">F4</f>
+      <c r="G12">
+        <f t="shared" ref="G12" si="0">F12</f>
         <v>5</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I12" t="s">
         <v>83</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L12" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>147</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C13" t="s">
         <v>81</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D13" t="s">
         <v>209</v>
       </c>
-      <c r="E5">
+      <c r="E13">
         <v>2025</v>
       </c>
-      <c r="F5">
+      <c r="F13">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G13">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I13" t="s">
         <v>239</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L13" s="19" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>147</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C14" t="s">
         <v>81</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D14" t="s">
         <v>209</v>
       </c>
-      <c r="E6">
+      <c r="E14">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F14">
         <v>5</v>
       </c>
-      <c r="G6">
+      <c r="G14">
         <v>5</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I14" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="11" t="str">
+      <c r="F18" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G10" s="11" t="str">
+      <c r="G18" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J18" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>78</v>
       </c>
-      <c r="F11">
+      <c r="F19">
         <v>2035</v>
       </c>
-      <c r="G11">
-        <f>F11</f>
+      <c r="G19">
+        <f t="shared" ref="G19:G25" si="1">F19</f>
         <v>2035</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I19" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
         <v>78</v>
       </c>
-      <c r="F12">
+      <c r="F20">
         <v>2026</v>
       </c>
-      <c r="G12">
-        <f>F12</f>
+      <c r="G20">
+        <f t="shared" si="1"/>
         <v>2026</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I20" t="s">
         <v>321</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L20" s="19" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
         <v>78</v>
       </c>
-      <c r="F13">
+      <c r="F21">
         <v>2100</v>
       </c>
-      <c r="G13">
-        <f>F13</f>
+      <c r="G21">
+        <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I21" t="s">
         <v>324</v>
       </c>
-      <c r="L13" s="19" t="s">
+      <c r="L21" s="19" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>78</v>
       </c>
-      <c r="F14">
+      <c r="F22">
         <v>2100</v>
       </c>
-      <c r="G14">
-        <f>F14</f>
+      <c r="G22">
+        <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I22" t="s">
         <v>325</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L22" s="19" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
         <v>78</v>
       </c>
-      <c r="F15">
+      <c r="F23">
         <v>2100</v>
       </c>
-      <c r="G15">
-        <f>F15</f>
+      <c r="G23">
+        <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I23" t="s">
         <v>332</v>
       </c>
-      <c r="L15" s="19" t="s">
+      <c r="L23" s="19" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
         <v>78</v>
       </c>
-      <c r="F16">
+      <c r="F24">
         <v>2100</v>
       </c>
-      <c r="G16">
-        <f>F16</f>
+      <c r="G24">
+        <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I24" t="s">
         <v>329</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="L24" s="19" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
         <v>78</v>
       </c>
-      <c r="F17">
+      <c r="F25">
         <v>2035</v>
       </c>
-      <c r="G17">
-        <f>F17</f>
+      <c r="G25">
+        <f t="shared" si="1"/>
         <v>2035</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I25" t="s">
         <v>83</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L25" s="19" t="s">
         <v>323</v>
       </c>
     </row>
@@ -12084,8 +12188,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12892,28 +12996,28 @@
       <c r="L5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="88" t="s">
+      <c r="P5" s="86" t="s">
         <v>265</v>
       </c>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="T5" s="88" t="s">
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="T5" s="86" t="s">
         <v>266</v>
       </c>
-      <c r="U5" s="88"/>
-      <c r="V5" s="88"/>
-      <c r="W5" s="88"/>
-      <c r="X5" s="88"/>
-      <c r="Z5" s="88" t="s">
+      <c r="U5" s="86"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="86"/>
+      <c r="X5" s="86"/>
+      <c r="Z5" s="86" t="s">
         <v>267</v>
       </c>
-      <c r="AA5" s="88"/>
-      <c r="AB5" s="88"/>
-      <c r="AD5" s="88" t="s">
+      <c r="AA5" s="86"/>
+      <c r="AB5" s="86"/>
+      <c r="AD5" s="86" t="s">
         <v>268</v>
       </c>
-      <c r="AE5" s="88"/>
-      <c r="AF5" s="88"/>
+      <c r="AE5" s="86"/>
+      <c r="AF5" s="86"/>
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -13276,11 +13380,11 @@
         <f t="shared" si="0"/>
         <v>-0.20397754353748057</v>
       </c>
-      <c r="P12" s="89" t="s">
+      <c r="P12" s="87" t="s">
         <v>284</v>
       </c>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="89"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="87"/>
       <c r="T12" s="59" t="s">
         <v>285</v>
       </c>
@@ -13808,38 +13912,38 @@
         <f t="shared" si="2"/>
         <v>-0.38127737390844418</v>
       </c>
-      <c r="T28" s="86" t="s">
+      <c r="T28" s="88" t="s">
         <v>269</v>
       </c>
-      <c r="U28" s="87"/>
-      <c r="V28" s="87"/>
-      <c r="W28" s="87"/>
-      <c r="X28" s="87"/>
-      <c r="Y28" s="87"/>
-      <c r="Z28" s="87"/>
-      <c r="AA28" s="87"/>
-      <c r="AC28" s="87" t="s">
+      <c r="U28" s="89"/>
+      <c r="V28" s="89"/>
+      <c r="W28" s="89"/>
+      <c r="X28" s="89"/>
+      <c r="Y28" s="89"/>
+      <c r="Z28" s="89"/>
+      <c r="AA28" s="89"/>
+      <c r="AC28" s="89" t="s">
         <v>270</v>
       </c>
-      <c r="AD28" s="87"/>
-      <c r="AE28" s="87"/>
-      <c r="AF28" s="87"/>
-      <c r="AG28" s="87"/>
-      <c r="AH28" s="87"/>
-      <c r="AI28" s="87"/>
-      <c r="AJ28" s="87"/>
-      <c r="AK28" s="87"/>
-      <c r="AM28" s="86" t="s">
+      <c r="AD28" s="89"/>
+      <c r="AE28" s="89"/>
+      <c r="AF28" s="89"/>
+      <c r="AG28" s="89"/>
+      <c r="AH28" s="89"/>
+      <c r="AI28" s="89"/>
+      <c r="AJ28" s="89"/>
+      <c r="AK28" s="89"/>
+      <c r="AM28" s="88" t="s">
         <v>271</v>
       </c>
-      <c r="AN28" s="87"/>
-      <c r="AO28" s="87"/>
-      <c r="AP28" s="87"/>
-      <c r="AQ28" s="87"/>
-      <c r="AR28" s="87"/>
-      <c r="AS28" s="87"/>
-      <c r="AT28" s="87"/>
-      <c r="AU28" s="87"/>
+      <c r="AN28" s="89"/>
+      <c r="AO28" s="89"/>
+      <c r="AP28" s="89"/>
+      <c r="AQ28" s="89"/>
+      <c r="AR28" s="89"/>
+      <c r="AS28" s="89"/>
+      <c r="AT28" s="89"/>
+      <c r="AU28" s="89"/>
     </row>
     <row r="29" spans="2:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
@@ -15005,24 +15109,24 @@
       <c r="M42" s="25">
         <v>0.5</v>
       </c>
-      <c r="S42" s="88" t="s">
+      <c r="S42" s="86" t="s">
         <v>295</v>
       </c>
-      <c r="T42" s="88"/>
-      <c r="U42" s="88"/>
-      <c r="V42" s="88"/>
-      <c r="X42" s="88" t="s">
+      <c r="T42" s="86"/>
+      <c r="U42" s="86"/>
+      <c r="V42" s="86"/>
+      <c r="X42" s="86" t="s">
         <v>296</v>
       </c>
-      <c r="Y42" s="88"/>
-      <c r="Z42" s="88"/>
-      <c r="AA42" s="88"/>
-      <c r="AC42" s="88" t="s">
+      <c r="Y42" s="86"/>
+      <c r="Z42" s="86"/>
+      <c r="AA42" s="86"/>
+      <c r="AC42" s="86" t="s">
         <v>297</v>
       </c>
-      <c r="AD42" s="88"/>
-      <c r="AE42" s="88"/>
-      <c r="AF42" s="88"/>
+      <c r="AD42" s="86"/>
+      <c r="AE42" s="86"/>
+      <c r="AF42" s="86"/>
     </row>
     <row r="43" spans="2:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
@@ -18539,17 +18643,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="AD5:AF5"/>
-    <mergeCell ref="P12:R12"/>
     <mergeCell ref="AM28:AU28"/>
     <mergeCell ref="AC28:AK28"/>
     <mergeCell ref="S42:V42"/>
     <mergeCell ref="X42:AA42"/>
     <mergeCell ref="AC42:AF42"/>
     <mergeCell ref="T28:AA28"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="AD5:AF5"/>
+    <mergeCell ref="P12:R12"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="T30:AA38">

</xml_diff>

<commit_message>
Set max net import
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695E09F2-2837-485A-8C73-50ABCCCE0369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA45B021-BD93-4BAC-8457-94FCC3E025D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="348">
   <si>
     <t>UC_N</t>
   </si>
@@ -1209,6 +1209,42 @@
   </si>
   <si>
     <t>P*SOL-PV*</t>
+  </si>
+  <si>
+    <t>UC_MaxNetELCCImport</t>
+  </si>
+  <si>
+    <t>Maximum net electricity import</t>
+  </si>
+  <si>
+    <t>UC_IRE</t>
+  </si>
+  <si>
+    <t>*Units</t>
+  </si>
+  <si>
+    <t>*Pja</t>
+  </si>
+  <si>
+    <t>Other_indexes</t>
+  </si>
+  <si>
+    <t>imp</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>ELCC</t>
+  </si>
+  <si>
+    <t>IRE</t>
+  </si>
+  <si>
+    <t>IMPELC*</t>
+  </si>
+  <si>
+    <t>EXPELC*</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1846,7 @@
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2011,6 +2047,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3426,12 +3464,12 @@
       <c r="Z15" s="34"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="84" t="s">
+      <c r="A16" s="86" t="s">
         <v>241</v>
       </c>
-      <c r="B16" s="84"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
       <c r="G16" s="36"/>
@@ -3515,11 +3553,11 @@
       <c r="A19" s="40" t="s">
         <v>242</v>
       </c>
-      <c r="B19" s="83" t="s">
+      <c r="B19" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
       <c r="G19" s="42"/>
@@ -3547,11 +3585,11 @@
       <c r="A20" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="85" t="s">
         <v>254</v>
       </c>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
       <c r="G20" s="42"/>
@@ -3639,11 +3677,11 @@
       <c r="A23" s="40" t="s">
         <v>245</v>
       </c>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="85" t="s">
         <v>253</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -3729,11 +3767,11 @@
       <c r="A26" s="40" t="s">
         <v>246</v>
       </c>
-      <c r="B26" s="83" t="s">
+      <c r="B26" s="85" t="s">
         <v>253</v>
       </c>
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
       <c r="G26" s="34"/>
@@ -3849,11 +3887,11 @@
       <c r="A30" s="40" t="s">
         <v>248</v>
       </c>
-      <c r="B30" s="85" t="s">
+      <c r="B30" s="87" t="s">
         <v>249</v>
       </c>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="85"/>
       <c r="E30" s="45"/>
       <c r="F30" s="45"/>
       <c r="G30" s="34"/>
@@ -3881,11 +3919,11 @@
       <c r="A31" s="40" t="s">
         <v>250</v>
       </c>
-      <c r="B31" s="83" t="s">
+      <c r="B31" s="85" t="s">
         <v>251</v>
       </c>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="85"/>
       <c r="E31" s="45"/>
       <c r="F31" s="45"/>
       <c r="G31" s="34"/>
@@ -11732,7 +11770,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
@@ -12186,10 +12224,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12197,109 +12235,107 @@
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" customWidth="1"/>
+    <col min="12" max="12" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I5" t="s">
         <v>235</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="31" t="s">
         <v>234</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="H6" s="31">
+      <c r="G6" s="31">
         <v>2025</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="H6" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="J6">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="K6" s="31">
+      <c r="J6" s="31">
         <v>0</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="K6" s="31" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="31"/>
       <c r="D7" s="32"/>
-      <c r="H7" s="31">
+      <c r="G7" s="31">
         <v>0</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="H7" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="31">
+      <c r="J7" s="31">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="31" t="s">
         <v>238</v>
       </c>
@@ -12307,384 +12343,546 @@
         <v>236</v>
       </c>
       <c r="E8" s="31"/>
-      <c r="H8" s="31">
+      <c r="G8" s="31">
         <v>2020</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="H8" s="31" t="s">
         <v>81</v>
       </c>
+      <c r="I8" s="31">
+        <v>1</v>
+      </c>
       <c r="J8" s="31">
-        <v>1</v>
-      </c>
-      <c r="K8" s="31">
         <v>7.3689999999999998</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="K8" s="31" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
       <c r="D9" s="32" t="s">
         <v>236</v>
       </c>
       <c r="E9" s="31"/>
-      <c r="H9" s="31">
+      <c r="G9" s="31">
         <v>2030</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="H9" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31">
+      <c r="I9" s="31"/>
+      <c r="J9" s="31">
         <v>24.074100000000001</v>
       </c>
-      <c r="L9" s="31"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
       <c r="D10" s="32" t="s">
         <v>236</v>
       </c>
       <c r="E10" s="31"/>
-      <c r="H10" s="31">
+      <c r="G10" s="31">
         <v>2040</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="H10" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31">
+      <c r="I10" s="31"/>
+      <c r="J10" s="31">
         <v>48.148200000000003</v>
       </c>
-      <c r="L10" s="31"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
       <c r="D11" s="32" t="s">
         <v>236</v>
       </c>
       <c r="E11" s="31"/>
-      <c r="H11" s="31">
+      <c r="G11" s="31">
         <v>2050</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="H11" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31">
+      <c r="I11" s="31"/>
+      <c r="J11" s="31">
         <v>96.296400000000006</v>
       </c>
-      <c r="L11" s="31"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="31"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
       <c r="D12" s="32" t="s">
         <v>236</v>
       </c>
       <c r="E12" s="31"/>
-      <c r="H12" s="31">
+      <c r="G12" s="31">
         <v>0</v>
       </c>
-      <c r="I12" s="31" t="s">
+      <c r="H12" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31">
+      <c r="I12" s="31"/>
+      <c r="J12" s="31">
         <v>15</v>
       </c>
-      <c r="L12" s="31"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="31"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="32"/>
+      <c r="E13" s="31"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
-      <c r="M13" s="31"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="E14" s="31"/>
       <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
       <c r="J14" s="31"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="I16" s="83" t="s">
+        <v>338</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="K17" s="84"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="31" t="s">
+        <v>336</v>
+      </c>
+      <c r="C18" t="s">
+        <v>344</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="E18" t="s">
+        <v>346</v>
+      </c>
+      <c r="F18" s="31">
+        <v>2022</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" t="s">
+        <v>342</v>
+      </c>
+      <c r="I18" s="31">
+        <v>1</v>
+      </c>
+      <c r="J18" s="31">
+        <v>6</v>
+      </c>
+      <c r="K18" t="s">
+        <v>337</v>
+      </c>
+      <c r="M18" s="31"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="31"/>
+      <c r="C19" t="s">
+        <v>344</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="E19" t="s">
+        <v>347</v>
+      </c>
+      <c r="F19" s="31">
+        <v>2022</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" t="s">
+        <v>343</v>
+      </c>
+      <c r="I19" s="31">
+        <v>-1</v>
+      </c>
+      <c r="J19" s="31"/>
+      <c r="M19" s="31"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="31"/>
+      <c r="D20" s="32"/>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31">
+        <v>5</v>
+      </c>
+      <c r="M20" s="31"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="M21" s="31"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="31"/>
+      <c r="D22" s="32"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="M22" s="31"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="31"/>
+      <c r="D23" s="32"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="M23" s="31"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="J24" s="31"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="11" t="str">
+      <c r="F27" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G17" s="11" t="str">
+      <c r="G27" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I27" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J27" s="12" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>81</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D28" t="s">
         <v>209</v>
       </c>
-      <c r="E18">
+      <c r="E28">
         <v>2025</v>
       </c>
-      <c r="F18">
+      <c r="F28">
         <v>0</v>
       </c>
-      <c r="G18">
-        <f>F18</f>
+      <c r="G28">
+        <f>F28</f>
         <v>0</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I28" t="s">
         <v>213</v>
       </c>
-      <c r="J18">
+      <c r="J28">
         <v>0</v>
       </c>
-      <c r="M18" s="19" t="s">
+      <c r="L28" s="19" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C19" t="str">
-        <f>C18</f>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C29" t="str">
+        <f>C28</f>
         <v>UP</v>
       </c>
-      <c r="D19" t="str">
-        <f t="shared" ref="D19" si="0">D18</f>
+      <c r="D29" t="str">
+        <f t="shared" ref="D29" si="0">D28</f>
         <v>ACT_BND</v>
       </c>
-      <c r="E19">
+      <c r="E29">
         <v>0</v>
       </c>
-      <c r="F19">
+      <c r="F29">
         <v>5</v>
       </c>
-      <c r="G19">
-        <f>F19</f>
+      <c r="G29">
+        <f>F29</f>
         <v>5</v>
       </c>
-      <c r="I19" t="str">
-        <f>I18</f>
+      <c r="I29" t="str">
+        <f>I28</f>
         <v>IMPBIO*1G*2,IMPBIO*1G*3,IMPBIO*1G*4</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E33" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="11" t="str">
+      <c r="F33" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G23" s="11" t="str">
+      <c r="G33" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H33" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="I33" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>81</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D34" t="s">
         <v>209</v>
       </c>
-      <c r="E24">
+      <c r="E34">
         <v>2018</v>
       </c>
-      <c r="F24">
+      <c r="F34">
         <v>0.35</v>
       </c>
-      <c r="G24">
-        <f>F24</f>
+      <c r="G34">
+        <f>F34</f>
         <v>0.35</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H34" t="s">
         <v>212</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I34" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C25" t="str">
-        <f>C24</f>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C35" t="str">
+        <f>C34</f>
         <v>UP</v>
       </c>
-      <c r="D25" t="str">
-        <f t="shared" ref="D25:D27" si="1">D24</f>
+      <c r="D35" t="str">
+        <f t="shared" ref="D35:D37" si="1">D34</f>
         <v>ACT_BND</v>
       </c>
-      <c r="E25">
+      <c r="E35">
         <v>0</v>
       </c>
-      <c r="F25">
+      <c r="F35">
         <v>5</v>
       </c>
-      <c r="G25">
-        <f>F25</f>
+      <c r="G35">
+        <f>F35</f>
         <v>5</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H35" t="s">
         <v>212</v>
       </c>
-      <c r="I25" t="str">
-        <f>I24</f>
+      <c r="I35" t="str">
+        <f>I34</f>
         <v>*GRID</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>81</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D36" t="s">
         <v>209</v>
       </c>
-      <c r="E26">
+      <c r="E36">
         <v>2030</v>
       </c>
-      <c r="F26">
+      <c r="F36">
         <v>0</v>
       </c>
-      <c r="G26">
-        <f>F26</f>
+      <c r="G36">
+        <f>F36</f>
         <v>0</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I36" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C27" t="str">
-        <f>C26</f>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C37" t="str">
+        <f>C36</f>
         <v>UP</v>
       </c>
-      <c r="D27" t="str">
+      <c r="D37" t="str">
         <f t="shared" si="1"/>
         <v>ACT_BND</v>
       </c>
-      <c r="E27">
+      <c r="E37">
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F37">
         <v>5</v>
       </c>
-      <c r="G27">
-        <f>F27</f>
+      <c r="G37">
+        <f>F37</f>
         <v>5</v>
       </c>
-      <c r="I27" t="str">
-        <f>I26</f>
+      <c r="I37" t="str">
+        <f>I36</f>
         <v>IMPH2G</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-    </row>
-    <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="10" t="s">
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C41" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D41" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E41" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="11" t="str">
+      <c r="F41" s="11" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G31" s="11" t="str">
+      <c r="G41" s="11" t="str">
         <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H41" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="I41" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
         <v>78</v>
       </c>
-      <c r="F32">
+      <c r="F42">
         <v>2018</v>
       </c>
-      <c r="G32">
+      <c r="G42">
         <v>2018</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I42" t="s">
         <v>79</v>
       </c>
-      <c r="M32" s="19" t="s">
+      <c r="M42" s="19" t="s">
         <v>80</v>
       </c>
     </row>
@@ -12996,28 +13194,28 @@
       <c r="L5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="86" t="s">
+      <c r="P5" s="88" t="s">
         <v>265</v>
       </c>
-      <c r="Q5" s="86"/>
-      <c r="R5" s="86"/>
-      <c r="T5" s="86" t="s">
+      <c r="Q5" s="88"/>
+      <c r="R5" s="88"/>
+      <c r="T5" s="88" t="s">
         <v>266</v>
       </c>
-      <c r="U5" s="86"/>
-      <c r="V5" s="86"/>
-      <c r="W5" s="86"/>
-      <c r="X5" s="86"/>
-      <c r="Z5" s="86" t="s">
+      <c r="U5" s="88"/>
+      <c r="V5" s="88"/>
+      <c r="W5" s="88"/>
+      <c r="X5" s="88"/>
+      <c r="Z5" s="88" t="s">
         <v>267</v>
       </c>
-      <c r="AA5" s="86"/>
-      <c r="AB5" s="86"/>
-      <c r="AD5" s="86" t="s">
+      <c r="AA5" s="88"/>
+      <c r="AB5" s="88"/>
+      <c r="AD5" s="88" t="s">
         <v>268</v>
       </c>
-      <c r="AE5" s="86"/>
-      <c r="AF5" s="86"/>
+      <c r="AE5" s="88"/>
+      <c r="AF5" s="88"/>
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -13380,11 +13578,11 @@
         <f t="shared" si="0"/>
         <v>-0.20397754353748057</v>
       </c>
-      <c r="P12" s="87" t="s">
+      <c r="P12" s="89" t="s">
         <v>284</v>
       </c>
-      <c r="Q12" s="87"/>
-      <c r="R12" s="87"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="89"/>
       <c r="T12" s="59" t="s">
         <v>285</v>
       </c>
@@ -13912,38 +14110,38 @@
         <f t="shared" si="2"/>
         <v>-0.38127737390844418</v>
       </c>
-      <c r="T28" s="88" t="s">
+      <c r="T28" s="90" t="s">
         <v>269</v>
       </c>
-      <c r="U28" s="89"/>
-      <c r="V28" s="89"/>
-      <c r="W28" s="89"/>
-      <c r="X28" s="89"/>
-      <c r="Y28" s="89"/>
-      <c r="Z28" s="89"/>
-      <c r="AA28" s="89"/>
-      <c r="AC28" s="89" t="s">
+      <c r="U28" s="91"/>
+      <c r="V28" s="91"/>
+      <c r="W28" s="91"/>
+      <c r="X28" s="91"/>
+      <c r="Y28" s="91"/>
+      <c r="Z28" s="91"/>
+      <c r="AA28" s="91"/>
+      <c r="AC28" s="91" t="s">
         <v>270</v>
       </c>
-      <c r="AD28" s="89"/>
-      <c r="AE28" s="89"/>
-      <c r="AF28" s="89"/>
-      <c r="AG28" s="89"/>
-      <c r="AH28" s="89"/>
-      <c r="AI28" s="89"/>
-      <c r="AJ28" s="89"/>
-      <c r="AK28" s="89"/>
-      <c r="AM28" s="88" t="s">
+      <c r="AD28" s="91"/>
+      <c r="AE28" s="91"/>
+      <c r="AF28" s="91"/>
+      <c r="AG28" s="91"/>
+      <c r="AH28" s="91"/>
+      <c r="AI28" s="91"/>
+      <c r="AJ28" s="91"/>
+      <c r="AK28" s="91"/>
+      <c r="AM28" s="90" t="s">
         <v>271</v>
       </c>
-      <c r="AN28" s="89"/>
-      <c r="AO28" s="89"/>
-      <c r="AP28" s="89"/>
-      <c r="AQ28" s="89"/>
-      <c r="AR28" s="89"/>
-      <c r="AS28" s="89"/>
-      <c r="AT28" s="89"/>
-      <c r="AU28" s="89"/>
+      <c r="AN28" s="91"/>
+      <c r="AO28" s="91"/>
+      <c r="AP28" s="91"/>
+      <c r="AQ28" s="91"/>
+      <c r="AR28" s="91"/>
+      <c r="AS28" s="91"/>
+      <c r="AT28" s="91"/>
+      <c r="AU28" s="91"/>
     </row>
     <row r="29" spans="2:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
@@ -15109,24 +15307,24 @@
       <c r="M42" s="25">
         <v>0.5</v>
       </c>
-      <c r="S42" s="86" t="s">
+      <c r="S42" s="88" t="s">
         <v>295</v>
       </c>
-      <c r="T42" s="86"/>
-      <c r="U42" s="86"/>
-      <c r="V42" s="86"/>
-      <c r="X42" s="86" t="s">
+      <c r="T42" s="88"/>
+      <c r="U42" s="88"/>
+      <c r="V42" s="88"/>
+      <c r="X42" s="88" t="s">
         <v>296</v>
       </c>
-      <c r="Y42" s="86"/>
-      <c r="Z42" s="86"/>
-      <c r="AA42" s="86"/>
-      <c r="AC42" s="86" t="s">
+      <c r="Y42" s="88"/>
+      <c r="Z42" s="88"/>
+      <c r="AA42" s="88"/>
+      <c r="AC42" s="88" t="s">
         <v>297</v>
       </c>
-      <c r="AD42" s="86"/>
-      <c r="AE42" s="86"/>
-      <c r="AF42" s="86"/>
+      <c r="AD42" s="88"/>
+      <c r="AE42" s="88"/>
+      <c r="AF42" s="88"/>
     </row>
     <row r="43" spans="2:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" t="s">

</xml_diff>

<commit_message>
Allow CCS in industry from 2029
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A0A0BF-8B01-4296-9DB1-AD7DC804AAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA9640F-3162-4D89-8C41-A3D4EB6D2A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
     <sheet name="Regions" sheetId="15" r:id="rId2"/>
-    <sheet name="PWR" sheetId="19" r:id="rId3"/>
-    <sheet name="SYS" sheetId="28" r:id="rId4"/>
-    <sheet name="SUP" sheetId="11" r:id="rId5"/>
-    <sheet name="SRV" sheetId="26" r:id="rId6"/>
-    <sheet name="TRA" sheetId="27" r:id="rId7"/>
+    <sheet name="Study" sheetId="30" r:id="rId3"/>
+    <sheet name="PWR" sheetId="19" r:id="rId4"/>
+    <sheet name="SYS" sheetId="28" r:id="rId5"/>
+    <sheet name="SUP" sheetId="11" r:id="rId6"/>
+    <sheet name="SRV" sheetId="26" r:id="rId7"/>
+    <sheet name="TRA" sheetId="27" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
@@ -140,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
   <si>
     <t>UC_N</t>
   </si>
@@ -648,13 +649,16 @@
   <si>
     <t>EXPELC*</t>
   </si>
+  <si>
+    <t>I-DMD-ONM-N1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -971,7 +975,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5325,12 +5329,78 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6ED70B-9A96-4A29-B1C4-70A9797AA7C3}">
+  <dimension ref="B3:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9" t="str">
+        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G4" s="9" t="str">
+        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5">
+        <v>2029</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5" si="0">F5</f>
+        <v>2029</v>
+      </c>
+      <c r="I5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5704,7 +5774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE4666E-C19A-4073-8183-3ACBB585B13C}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:J4"/>
@@ -5780,7 +5850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M42"/>
@@ -6450,7 +6520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F532AC2E-E047-4124-A56C-AD8CA9B97A1E}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B3:I12"/>
@@ -6673,7 +6743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FB1178-AF9A-473D-9FB3-41C2F896D89C}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B3:K5"/>

</xml_diff>

<commit_message>
Exclude BECCS by default
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA9640F-3162-4D89-8C41-A3D4EB6D2A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3620F4F-80C9-4F9D-87BA-840BEE36E2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="166">
   <si>
     <t>UC_N</t>
   </si>
@@ -651,6 +651,15 @@
   </si>
   <si>
     <t>I-DMD-ONM-N1</t>
+  </si>
+  <si>
+    <t>P-RNW-ST-BIO-CCS05</t>
+  </si>
+  <si>
+    <t>PWRBIO</t>
+  </si>
+  <si>
+    <t>- no new BECCS during the modelling horizon</t>
   </si>
 </sst>
 </file>
@@ -5332,8 +5341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6ED70B-9A96-4A29-B1C4-70A9797AA7C3}">
   <dimension ref="B3:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5397,10 +5406,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE79BAD-EA44-47F0-A194-320DE6C9FB50}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:M25"/>
+  <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5643,7 +5652,7 @@
         <v>3</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
@@ -5654,7 +5663,7 @@
         <v>2035</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:G25" si="1">F19</f>
+        <f t="shared" ref="G19:G26" si="1">F19</f>
         <v>2035</v>
       </c>
       <c r="I19" t="s">
@@ -5767,6 +5776,27 @@
       </c>
       <c r="L25" s="17" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26">
+        <v>2100</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="I26" t="s">
+        <v>163</v>
+      </c>
+      <c r="J26" t="s">
+        <v>164</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SRV and RSD Biomass, No CCS before 2040 and slower growth
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A0A0BF-8B01-4296-9DB1-AD7DC804AAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183C5468-7561-4F59-9A47-EC2FB4036430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -574,9 +574,6 @@
     <t>- no new offshore before 2026</t>
   </si>
   <si>
-    <t>- no CCS before 2035</t>
-  </si>
-  <si>
     <t>P*HY*DAM*</t>
   </si>
   <si>
@@ -647,6 +644,9 @@
   </si>
   <si>
     <t>EXPELC*</t>
+  </si>
+  <si>
+    <t>- no CCS before 2040</t>
   </si>
 </sst>
 </file>
@@ -654,7 +654,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -971,7 +971,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5330,7 +5330,7 @@
   <dimension ref="B2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5388,10 +5388,10 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>148</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>149</v>
       </c>
       <c r="F6" s="19">
         <v>2030</v>
@@ -5406,7 +5406,7 @@
         <v>5.5</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -5488,7 +5488,7 @@
         <v>83</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -5621,10 +5621,10 @@
         <v>2100</v>
       </c>
       <c r="I21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
@@ -5639,10 +5639,10 @@
         <v>2100</v>
       </c>
       <c r="I22" t="s">
+        <v>138</v>
+      </c>
+      <c r="L22" s="17" t="s">
         <v>139</v>
-      </c>
-      <c r="L22" s="17" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
@@ -5657,10 +5657,10 @@
         <v>2100</v>
       </c>
       <c r="I23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
@@ -5675,10 +5675,10 @@
         <v>2100</v>
       </c>
       <c r="I24" t="s">
+        <v>142</v>
+      </c>
+      <c r="L24" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="L24" s="17" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
@@ -5686,17 +5686,17 @@
         <v>78</v>
       </c>
       <c r="F25">
-        <v>2035</v>
+        <v>2040</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>2035</v>
+        <v>2040</v>
       </c>
       <c r="I25" t="s">
         <v>83</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -6041,10 +6041,10 @@
         <v>9</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>17</v>
@@ -6055,7 +6055,7 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
@@ -6065,22 +6065,22 @@
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K17" s="37"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="E18" t="s">
         <v>159</v>
-      </c>
-      <c r="E18" t="s">
-        <v>160</v>
       </c>
       <c r="F18" s="19">
         <v>2022</v>
@@ -6089,7 +6089,7 @@
         <v>81</v>
       </c>
       <c r="H18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I18" s="19">
         <v>1</v>
@@ -6098,27 +6098,27 @@
         <v>6</v>
       </c>
       <c r="K18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M18" s="19"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="D19" s="20" t="s">
-        <v>159</v>
-      </c>
       <c r="E19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F19" s="19">
         <v>2022</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I19" s="19">
         <v>-1</v>

</xml_diff>

<commit_message>
CCS start 2035 with slow growth
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183C5468-7561-4F59-9A47-EC2FB4036430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0E284B-81A3-4749-8BF0-7318AE403EA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-16080" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -5329,8 +5329,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5686,11 +5686,11 @@
         <v>78</v>
       </c>
       <c r="F25">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="I25" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
No RSD CBs & Kerosen reduce by 90%
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0E284B-81A3-4749-8BF0-7318AE403EA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0959413-7CB3-4A1B-9264-D4B6512AF697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-16080" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -18,9 +18,13 @@
     <sheet name="PWR" sheetId="19" r:id="rId3"/>
     <sheet name="SYS" sheetId="28" r:id="rId4"/>
     <sheet name="SUP" sheetId="11" r:id="rId5"/>
-    <sheet name="SRV" sheetId="26" r:id="rId6"/>
-    <sheet name="TRA" sheetId="27" r:id="rId7"/>
+    <sheet name="RSD" sheetId="30" r:id="rId6"/>
+    <sheet name="SRV" sheetId="26" r:id="rId7"/>
+    <sheet name="TRA" sheetId="27" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -117,6 +121,29 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gary Goldstein</author>
+  </authors>
+  <commentList>
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{EB6B86EC-8D33-4238-9030-229E5D9011CC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
@@ -140,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="163">
   <si>
     <t>UC_N</t>
   </si>
@@ -648,6 +675,9 @@
   <si>
     <t>- no CCS before 2040</t>
   </si>
+  <si>
+    <t>FT-RSDKER</t>
+  </si>
 </sst>
 </file>
 
@@ -656,7 +686,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -774,6 +804,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -900,12 +942,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -994,11 +1037,16 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{B2F64745-2C6D-45FB-A556-9D42C8713F7A}"/>
+    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="3" xr:uid="{ED86729C-4FFD-40F0-9032-437159C0D370}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1389,6 +1437,48 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Regions"/>
+      <sheetName val="PWR"/>
+      <sheetName val="SYS"/>
+      <sheetName val="SUP"/>
+      <sheetName val="SUP_biogas"/>
+      <sheetName val="SRV"/>
+      <sheetName val="RSD"/>
+      <sheetName val="TRA"/>
+      <sheetName val="DataFill"/>
+      <sheetName val="RSDAFC"/>
+      <sheetName val="RSDAFA"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>IE</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>National</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5329,7 +5419,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -6451,6 +6541,144 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2BA889-3E0F-432B-9A75-59D73B919502}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="42" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="41"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="9" t="str">
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="I6" s="9" t="str">
+        <f>IF([1]Regions!D$3&lt;&gt;"",[1]Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7">
+        <v>2030</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8">
+        <v>2050</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F532AC2E-E047-4124-A56C-AD8CA9B97A1E}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B3:I12"/>
@@ -6673,7 +6901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FB1178-AF9A-473D-9FB3-41C2F896D89C}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B3:K5"/>

</xml_diff>

<commit_message>
RSD CBs, No Adittional Assumption, Max Growth Rate
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B0A126-D64A-4B4A-BCAC-BB26DED09657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A558D6-BD76-4B20-BAB0-97BAD4377B7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -6548,7 +6548,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6573,10 +6573,12 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>82</v>
-      </c>
       <c r="I5" s="38"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -6703,13 +6705,13 @@
         <v>89</v>
       </c>
       <c r="E11">
-        <v>2040</v>
+        <v>2050</v>
       </c>
       <c r="H11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K11" t="s">
         <v>163</v>

</xml_diff>

<commit_message>
RSD GAS Additional Assump
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536E2620-E6F4-42A5-B903-129571A8AF90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1009827-B4AA-4D9E-A2B8-742D103D3A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="-14385" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="165">
   <si>
     <t>UC_N</t>
   </si>
@@ -5882,7 +5882,7 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6551,7 +6551,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6577,9 +6577,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>82</v>
-      </c>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I5" s="38"/>
@@ -6741,9 +6739,10 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>82</v>
       </c>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
@@ -6780,53 +6779,53 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>89</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>2030</v>
       </c>
       <c r="H19">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I19">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K19" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>81</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>89</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>2050</v>
       </c>
       <c r="H20">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I20">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>89</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>0</v>
       </c>
       <c r="H21">

</xml_diff>

<commit_message>
Tweak Max Growth, Gas degrowth rate, and FX
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314C0560-DB5B-478F-A9F1-1B5C5DCA629D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DE5CF2-8ECC-4968-A4CB-EF4E6C3B904C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -4617,7 +4617,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -6508,8 +6508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2BA889-3E0F-432B-9A75-59D73B919502}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6693,10 +6693,12 @@
         <v>163</v>
       </c>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>82</v>
-      </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
COal 2030 cap, fix UCs and WH Elc growth
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D684D64-024E-48D6-AD8B-1217543A5B24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7825D592-FDF4-468E-8793-ECE157FC876E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="165">
   <si>
     <t>UC_N</t>
   </si>
@@ -671,9 +671,6 @@
   </si>
   <si>
     <t>- no CCS before 2040</t>
-  </si>
-  <si>
-    <t>FT-RSDKER</t>
   </si>
   <si>
     <t>FT-RSDCOA</t>
@@ -6506,10 +6503,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2BA889-3E0F-432B-9A75-59D73B919502}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6525,7 +6522,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -6537,7 +6534,9 @@
       <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="I5" s="38"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -6585,10 +6584,10 @@
         <v>2030</v>
       </c>
       <c r="H7">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="K7" t="s">
         <v>162</v>
@@ -6605,10 +6604,10 @@
         <v>2050</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K8" t="s">
         <v>162</v>
@@ -6634,162 +6633,102 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>81</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D16" t="s">
         <v>89</v>
       </c>
-      <c r="E10">
+      <c r="E16">
         <v>2030</v>
       </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="H16">
+        <v>17</v>
+      </c>
+      <c r="I16">
+        <v>17</v>
+      </c>
+      <c r="K16" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>81</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D17" t="s">
         <v>89</v>
       </c>
-      <c r="E11">
+      <c r="E17">
         <v>2050</v>
       </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="K17" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>81</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D18" t="s">
         <v>89</v>
       </c>
-      <c r="E12">
+      <c r="E18">
         <v>0</v>
       </c>
-      <c r="H12">
+      <c r="H18">
         <v>5</v>
       </c>
-      <c r="I12">
+      <c r="I18">
         <v>5</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K18" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19">
-        <v>2030</v>
-      </c>
-      <c r="H19">
-        <v>17</v>
-      </c>
-      <c r="I19">
-        <v>17</v>
-      </c>
-      <c r="K19" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20">
-        <v>2050</v>
-      </c>
-      <c r="H20">
-        <v>10</v>
-      </c>
-      <c r="I20">
-        <v>10</v>
-      </c>
-      <c r="K20" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>5</v>
-      </c>
-      <c r="I21">
-        <v>5</v>
-      </c>
-      <c r="K21" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addittions to the calibration
New techs later and car stock
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
+++ b/SuppXLS/Scen_B_SYS_Additional_Assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\times-ireland-model-main\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\TIM_Carbon Budget\TIM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE54422-0FF8-44F5-8B5F-C14F082C6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AEBF9A-348E-45D0-92B0-34BB55379A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="29" r:id="rId1"/>
@@ -127,7 +127,7 @@
     <author>tc={5F60B11B-92F4-4362-8C85-12A98901D200}</author>
   </authors>
   <commentList>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{39F88E30-94DE-4149-8FC0-41BD81F323F5}">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{39F88E30-94DE-4149-8FC0-41BD81F323F5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -135,7 +135,7 @@
     CAP 2023</t>
       </text>
     </comment>
-    <comment ref="I7" authorId="1" shapeId="0" xr:uid="{EB3DCB1B-8982-4D24-8304-DBCBE04F3479}">
+    <comment ref="I8" authorId="1" shapeId="0" xr:uid="{EB3DCB1B-8982-4D24-8304-DBCBE04F3479}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -144,7 +144,7 @@
 CAP23, Page 129</t>
       </text>
     </comment>
-    <comment ref="I53" authorId="2" shapeId="0" xr:uid="{C3394AD6-E865-4488-B7C2-96AE6AE9F254}">
+    <comment ref="I41" authorId="2" shapeId="0" xr:uid="{C3394AD6-E865-4488-B7C2-96AE6AE9F254}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -152,7 +152,7 @@
     CAP 2023</t>
       </text>
     </comment>
-    <comment ref="I54" authorId="3" shapeId="0" xr:uid="{122B1FEC-CDFA-43B1-9578-EE77FA507220}">
+    <comment ref="I42" authorId="3" shapeId="0" xr:uid="{122B1FEC-CDFA-43B1-9578-EE77FA507220}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -160,7 +160,7 @@
     CAP 2023</t>
       </text>
     </comment>
-    <comment ref="I55" authorId="4" shapeId="0" xr:uid="{5F60B11B-92F4-4362-8C85-12A98901D200}">
+    <comment ref="I43" authorId="4" shapeId="0" xr:uid="{5F60B11B-92F4-4362-8C85-12A98901D200}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="182">
   <si>
     <t>UC_N</t>
   </si>
@@ -568,197 +568,199 @@
     <t>UC_BIOIMPORTS_LIMIT</t>
   </si>
   <si>
+    <t>- no coal from 2025</t>
+  </si>
+  <si>
+    <t>TIMES-Ireland Model</t>
+  </si>
+  <si>
+    <t>Document type:</t>
+  </si>
+  <si>
+    <t>Sector(s):</t>
+  </si>
+  <si>
+    <t>Purpose:</t>
+  </si>
+  <si>
+    <t>Original developer(s):</t>
+  </si>
+  <si>
+    <t>Current maintainer(s):</t>
+  </si>
+  <si>
+    <t>Part of TIM version:</t>
+  </si>
+  <si>
+    <t>Model repository:</t>
+  </si>
+  <si>
+    <t>https://github.com/MaREI-EPMG/TIMES-Ireland-model</t>
+  </si>
+  <si>
+    <t>Licence:</t>
+  </si>
+  <si>
+    <t>CC BY-NC-SA 4.0 (unless specified otherwise)</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>Olexandr Balyk (UCC, olexandr.balyk@ucc.ie)</t>
+  </si>
+  <si>
+    <t>All sectors</t>
+  </si>
+  <si>
+    <t>Specify various assumptions to reflect current policies</t>
+  </si>
+  <si>
+    <t>Hannah Daly (UCC, h.daly@ucc.ie)</t>
+  </si>
+  <si>
+    <t>P*W*OF*</t>
+  </si>
+  <si>
+    <t>- no CCS before 2035</t>
+  </si>
+  <si>
+    <t>P*HY*DAM*</t>
+  </si>
+  <si>
+    <t>P*HY*ROR*</t>
+  </si>
+  <si>
+    <t>- no new hydro (ror) during the modelling horizon</t>
+  </si>
+  <si>
+    <t>- no new hydro (dam) during the modelling horizon</t>
+  </si>
+  <si>
+    <t>- no new CSP during the modelling horizon</t>
+  </si>
+  <si>
+    <t>P-RNW-GEO*</t>
+  </si>
+  <si>
+    <t>- no new GEO during the modelling horizon</t>
+  </si>
+  <si>
+    <t>- 5-year lead time for CCS</t>
+  </si>
+  <si>
+    <t>P-RNW-SOL-CSP*</t>
+  </si>
+  <si>
+    <t>Maximum solar PV capacity</t>
+  </si>
+  <si>
+    <t>UC_Max_PV_Cap</t>
+  </si>
+  <si>
+    <t>P*SOL-PV*</t>
+  </si>
+  <si>
+    <t>UC_MaxNetELCCImport</t>
+  </si>
+  <si>
+    <t>Maximum net electricity import</t>
+  </si>
+  <si>
+    <t>UC_IRE</t>
+  </si>
+  <si>
+    <t>*Units</t>
+  </si>
+  <si>
+    <t>*Pja</t>
+  </si>
+  <si>
+    <t>Other_indexes</t>
+  </si>
+  <si>
+    <t>imp</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>ELCC</t>
+  </si>
+  <si>
+    <t>IRE</t>
+  </si>
+  <si>
+    <t>IMPELC*</t>
+  </si>
+  <si>
+    <t>EXPELC*</t>
+  </si>
+  <si>
+    <t>- no new offshore before 2025</t>
+  </si>
+  <si>
+    <t>UC_Max_WIN-Off_Cap</t>
+  </si>
+  <si>
+    <t>P*WIN*OF*</t>
+  </si>
+  <si>
+    <t>UC_Max_WIN-On_Cap</t>
+  </si>
+  <si>
+    <t>P*WIN*ON*</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>Maximum Wind Onshore Capacity</t>
+  </si>
+  <si>
+    <t>Source: CLIMATE ACTION PLAN 2023, CAP23</t>
+  </si>
+  <si>
+    <t>Minimum solar PV capacity</t>
+  </si>
+  <si>
+    <t>Max Wind Offshore Capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~UC_Sets: R_E: </t>
+  </si>
+  <si>
     <t>P*COA*,P*PEA*</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>- no coal from 2025</t>
-  </si>
-  <si>
-    <t>TIMES-Ireland Model</t>
-  </si>
-  <si>
-    <t>Document type:</t>
-  </si>
-  <si>
-    <t>Sector(s):</t>
-  </si>
-  <si>
-    <t>Purpose:</t>
-  </si>
-  <si>
-    <t>Original developer(s):</t>
-  </si>
-  <si>
-    <t>Current maintainer(s):</t>
-  </si>
-  <si>
-    <t>Part of TIM version:</t>
-  </si>
-  <si>
-    <t>Model repository:</t>
-  </si>
-  <si>
-    <t>https://github.com/MaREI-EPMG/TIMES-Ireland-model</t>
-  </si>
-  <si>
-    <t>Licence:</t>
-  </si>
-  <si>
-    <t>CC BY-NC-SA 4.0 (unless specified otherwise)</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
-  </si>
-  <si>
-    <t>Olexandr Balyk (UCC, olexandr.balyk@ucc.ie)</t>
-  </si>
-  <si>
-    <t>All sectors</t>
-  </si>
-  <si>
-    <t>Specify various assumptions to reflect current policies</t>
-  </si>
-  <si>
-    <t>Hannah Daly (UCC, h.daly@ucc.ie)</t>
-  </si>
-  <si>
-    <t>P*W*OF*</t>
-  </si>
-  <si>
-    <t>- no CCS before 2035</t>
-  </si>
-  <si>
-    <t>P*HY*DAM*</t>
-  </si>
-  <si>
-    <t>P*HY*ROR*</t>
-  </si>
-  <si>
-    <t>- no new hydro (ror) during the modelling horizon</t>
-  </si>
-  <si>
-    <t>- no new hydro (dam) during the modelling horizon</t>
-  </si>
-  <si>
-    <t>- no new CSP during the modelling horizon</t>
-  </si>
-  <si>
-    <t>P-RNW-GEO*</t>
-  </si>
-  <si>
-    <t>- no new GEO during the modelling horizon</t>
-  </si>
-  <si>
-    <t>- 5-year lead time for CCS</t>
-  </si>
-  <si>
-    <t>P-RNW-SOL-CSP*</t>
-  </si>
-  <si>
-    <t>Maximum solar PV capacity</t>
-  </si>
-  <si>
-    <t>UC_Max_PV_Cap</t>
-  </si>
-  <si>
-    <t>P*SOL-PV*</t>
-  </si>
-  <si>
-    <t>UC_MaxNetELCCImport</t>
-  </si>
-  <si>
-    <t>Maximum net electricity import</t>
-  </si>
-  <si>
-    <t>UC_IRE</t>
-  </si>
-  <si>
-    <t>*Units</t>
-  </si>
-  <si>
-    <t>*Pja</t>
-  </si>
-  <si>
-    <t>Other_indexes</t>
-  </si>
-  <si>
-    <t>imp</t>
-  </si>
-  <si>
-    <t>exp</t>
-  </si>
-  <si>
-    <t>ELCC</t>
-  </si>
-  <si>
-    <t>IRE</t>
-  </si>
-  <si>
-    <t>IMPELC*</t>
-  </si>
-  <si>
-    <t>EXPELC*</t>
-  </si>
-  <si>
-    <t>- no new offshore before 2025</t>
-  </si>
-  <si>
-    <t>UC_Max_WIN-Off_Cap</t>
-  </si>
-  <si>
-    <t>P*WIN*OF*</t>
-  </si>
-  <si>
-    <t>UC_Max_WIN-On_Cap</t>
-  </si>
-  <si>
-    <t>P*WIN*ON*</t>
-  </si>
-  <si>
-    <t>LO</t>
-  </si>
-  <si>
-    <t>Maximum Wind Onshore Capacity</t>
+  </si>
+  <si>
+    <t>- limit on coal power generation from 2023</t>
+  </si>
+  <si>
+    <t>FT-PWRDIS</t>
+  </si>
+  <si>
+    <t>- limit on oil-based power generation</t>
+  </si>
+  <si>
+    <t>FT-PWRHFO</t>
+  </si>
+  <si>
+    <t>FT-PWRDIS,FT-PWRHFO</t>
+  </si>
+  <si>
+    <t>- no oil-based power generation</t>
+  </si>
+  <si>
+    <t>P-TH*DIS*,P-TH*HFO*</t>
+  </si>
+  <si>
+    <t>FT-PWRGAS</t>
+  </si>
+  <si>
+    <t>- limit on gas-based power generation</t>
   </si>
   <si>
     <t>Minimum Wind Offshore Capacity</t>
-  </si>
-  <si>
-    <t>Source: CLIMATE ACTION PLAN 2023, CAP23</t>
-  </si>
-  <si>
-    <t>Minimum solar PV capacity</t>
-  </si>
-  <si>
-    <t>- limit on coal power generation from 2023</t>
-  </si>
-  <si>
-    <t>- no oil-based power generation</t>
-  </si>
-  <si>
-    <t>Max Wind Offshore Capacity</t>
-  </si>
-  <si>
-    <t>FT-PWRDIS</t>
-  </si>
-  <si>
-    <t>FT-PWRDIS,FT-PWRHFO</t>
-  </si>
-  <si>
-    <t>FT-PWRHFO</t>
-  </si>
-  <si>
-    <t>- limit on oil-based power generation</t>
-  </si>
-  <si>
-    <t>P-TH*DIS*,P-TH*HFO*</t>
-  </si>
-  <si>
-    <t>FT-PWRGAS</t>
-  </si>
-  <si>
-    <t>- limit on gas-based power generation</t>
   </si>
 </sst>
 </file>
@@ -895,7 +897,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1030,7 +1033,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1124,6 +1127,7 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1469,7 +1473,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>21771</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1532,7 +1536,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>133718</xdr:rowOff>
+      <xdr:rowOff>133717</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1861,20 +1865,20 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I6" dT="2023-10-03T14:05:42.13" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{39F88E30-94DE-4149-8FC0-41BD81F323F5}">
+  <threadedComment ref="I7" dT="2023-10-03T14:05:42.13" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{39F88E30-94DE-4149-8FC0-41BD81F323F5}">
     <text>CAP 2023</text>
   </threadedComment>
-  <threadedComment ref="I7" dT="2023-10-03T14:04:21.81" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{EB3DCB1B-8982-4D24-8304-DBCBE04F3479}">
+  <threadedComment ref="I8" dT="2023-10-03T14:04:21.81" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{EB3DCB1B-8982-4D24-8304-DBCBE04F3479}">
     <text>CLIMATE ACTION PLAN 2023
 CAP23, Page 129</text>
   </threadedComment>
-  <threadedComment ref="I53" dT="2023-10-03T14:51:58.12" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{C3394AD6-E865-4488-B7C2-96AE6AE9F254}">
+  <threadedComment ref="I41" dT="2023-10-03T14:51:58.12" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{C3394AD6-E865-4488-B7C2-96AE6AE9F254}">
     <text>CAP 2023</text>
   </threadedComment>
-  <threadedComment ref="I54" dT="2023-10-03T14:52:11.99" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{122B1FEC-CDFA-43B1-9578-EE77FA507220}">
+  <threadedComment ref="I42" dT="2023-10-03T14:52:11.99" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{122B1FEC-CDFA-43B1-9578-EE77FA507220}">
     <text>CAP 2023</text>
   </threadedComment>
-  <threadedComment ref="I55" dT="2023-10-03T14:52:20.09" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{5F60B11B-92F4-4362-8C85-12A98901D200}">
+  <threadedComment ref="I43" dT="2023-10-03T14:52:20.09" personId="{4A3ACF47-1851-4D1B-9F96-7F3B13E0B2BE}" id="{5F60B11B-92F4-4362-8C85-12A98901D200}">
     <text>CAP 2023</text>
   </threadedComment>
 </ThreadedComments>
@@ -1887,20 +1891,20 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
-    <col min="8" max="10" width="8.109375" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" customWidth="1"/>
+    <col min="1" max="4" width="21.69140625" customWidth="1"/>
+    <col min="5" max="6" width="14.07421875" customWidth="1"/>
+    <col min="7" max="7" width="12.07421875" customWidth="1"/>
+    <col min="8" max="10" width="8.07421875" customWidth="1"/>
+    <col min="11" max="11" width="9.69140625" customWidth="1"/>
+    <col min="12" max="12" width="8.07421875" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11.4609375" customWidth="1"/>
+    <col min="15" max="15" width="13.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="21"/>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -1928,7 +1932,7 @@
       <c r="Y1" s="22"/>
       <c r="Z1" s="22"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -1956,7 +1960,7 @@
       <c r="Y2" s="22"/>
       <c r="Z2" s="22"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1984,7 +1988,7 @@
       <c r="Y3" s="22"/>
       <c r="Z3" s="22"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -2012,7 +2016,7 @@
       <c r="Y4" s="22"/>
       <c r="Z4" s="22"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -2040,7 +2044,7 @@
       <c r="Y5" s="22"/>
       <c r="Z5" s="22"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -2068,7 +2072,7 @@
       <c r="Y6" s="22"/>
       <c r="Z6" s="22"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -2096,7 +2100,7 @@
       <c r="Y7" s="22"/>
       <c r="Z7" s="22"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -2124,7 +2128,7 @@
       <c r="Y8" s="22"/>
       <c r="Z8" s="22"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -2152,7 +2156,7 @@
       <c r="Y9" s="22"/>
       <c r="Z9" s="22"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -2180,7 +2184,7 @@
       <c r="Y10" s="22"/>
       <c r="Z10" s="22"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -2208,7 +2212,7 @@
       <c r="Y11" s="22"/>
       <c r="Z11" s="22"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
@@ -2236,7 +2240,7 @@
       <c r="Y12" s="22"/>
       <c r="Z12" s="22"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -2264,7 +2268,7 @@
       <c r="Y13" s="22"/>
       <c r="Z13" s="22"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -2292,7 +2296,7 @@
       <c r="Y14" s="22"/>
       <c r="Z14" s="22"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -2320,9 +2324,9 @@
       <c r="Y15" s="22"/>
       <c r="Z15" s="22"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="42"/>
@@ -2350,7 +2354,7 @@
       <c r="Y16" s="22"/>
       <c r="Z16" s="22"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -2378,7 +2382,7 @@
       <c r="Y17" s="22"/>
       <c r="Z17" s="22"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -2406,9 +2410,9 @@
       <c r="Y18" s="22"/>
       <c r="Z18" s="22"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" s="41" t="s">
         <v>86</v>
@@ -2438,12 +2442,12 @@
       <c r="Y19" s="22"/>
       <c r="Z19" s="22"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="41"/>
@@ -2470,12 +2474,12 @@
       <c r="Y20" s="22"/>
       <c r="Z20" s="22"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
@@ -2502,7 +2506,7 @@
       <c r="Y21" s="22"/>
       <c r="Z21" s="22"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="28"/>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
@@ -2530,12 +2534,12 @@
       <c r="Y22" s="22"/>
       <c r="Z22" s="22"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
@@ -2562,10 +2566,10 @@
       <c r="Y23" s="22"/>
       <c r="Z23" s="22"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="28"/>
       <c r="B24" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
@@ -2592,7 +2596,7 @@
       <c r="Y24" s="22"/>
       <c r="Z24" s="22"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="28"/>
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
@@ -2620,12 +2624,12 @@
       <c r="Y25" s="22"/>
       <c r="Z25" s="22"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
@@ -2652,7 +2656,7 @@
       <c r="Y26" s="22"/>
       <c r="Z26" s="22"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="28"/>
       <c r="B27" s="31"/>
       <c r="C27" s="31"/>
@@ -2680,7 +2684,7 @@
       <c r="Y27" s="22"/>
       <c r="Z27" s="22"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="28"/>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -2708,9 +2712,9 @@
       <c r="Y28" s="22"/>
       <c r="Z28" s="22"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B29" s="32">
         <v>1</v>
@@ -2740,12 +2744,12 @@
       <c r="Y29" s="22"/>
       <c r="Z29" s="22"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="43" t="s">
         <v>126</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>127</v>
       </c>
       <c r="C30" s="41"/>
       <c r="D30" s="41"/>
@@ -2772,12 +2776,12 @@
       <c r="Y30" s="22"/>
       <c r="Z30" s="22"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="41" t="s">
         <v>128</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>129</v>
       </c>
       <c r="C31" s="41"/>
       <c r="D31" s="41"/>
@@ -2804,10 +2808,10 @@
       <c r="Y31" s="22"/>
       <c r="Z31" s="22"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="34"/>
       <c r="B32" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="34"/>
@@ -2834,7 +2838,7 @@
       <c r="Y32" s="22"/>
       <c r="Z32" s="22"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -2862,7 +2866,7 @@
       <c r="Y33" s="22"/>
       <c r="Z33" s="22"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -2890,7 +2894,7 @@
       <c r="Y34" s="22"/>
       <c r="Z34" s="22"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -2918,7 +2922,7 @@
       <c r="Y35" s="22"/>
       <c r="Z35" s="22"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A36" s="21"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
@@ -2946,7 +2950,7 @@
       <c r="Y36" s="22"/>
       <c r="Z36" s="22"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -2974,7 +2978,7 @@
       <c r="Y37" s="22"/>
       <c r="Z37" s="22"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -3002,7 +3006,7 @@
       <c r="Y38" s="22"/>
       <c r="Z38" s="22"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -3030,7 +3034,7 @@
       <c r="Y39" s="22"/>
       <c r="Z39" s="22"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
@@ -3058,7 +3062,7 @@
       <c r="Y40" s="22"/>
       <c r="Z40" s="22"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -3086,7 +3090,7 @@
       <c r="Y41" s="22"/>
       <c r="Z41" s="22"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A42" s="21"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -3114,7 +3118,7 @@
       <c r="Y42" s="22"/>
       <c r="Z42" s="22"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A43" s="22"/>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
@@ -3142,7 +3146,7 @@
       <c r="Y43" s="22"/>
       <c r="Z43" s="22"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A44" s="22"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
@@ -3170,7 +3174,7 @@
       <c r="Y44" s="22"/>
       <c r="Z44" s="22"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A45" s="22"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
@@ -3198,7 +3202,7 @@
       <c r="Y45" s="22"/>
       <c r="Z45" s="22"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A46" s="22"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
@@ -3226,7 +3230,7 @@
       <c r="Y46" s="22"/>
       <c r="Z46" s="22"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A47" s="22"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
@@ -3254,7 +3258,7 @@
       <c r="Y47" s="22"/>
       <c r="Z47" s="22"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A48" s="22"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
@@ -3282,7 +3286,7 @@
       <c r="Y48" s="22"/>
       <c r="Z48" s="22"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A49" s="22"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
@@ -3310,7 +3314,7 @@
       <c r="Y49" s="22"/>
       <c r="Z49" s="22"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A50" s="22"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
@@ -3338,7 +3342,7 @@
       <c r="Y50" s="22"/>
       <c r="Z50" s="22"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A51" s="22"/>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
@@ -3366,7 +3370,7 @@
       <c r="Y51" s="22"/>
       <c r="Z51" s="22"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A52" s="22"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
@@ -3394,7 +3398,7 @@
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A53" s="22"/>
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
@@ -3422,7 +3426,7 @@
       <c r="Y53" s="22"/>
       <c r="Z53" s="22"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A54" s="22"/>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
@@ -3450,7 +3454,7 @@
       <c r="Y54" s="22"/>
       <c r="Z54" s="22"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A55" s="22"/>
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
@@ -3478,7 +3482,7 @@
       <c r="Y55" s="22"/>
       <c r="Z55" s="22"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A56" s="22"/>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
@@ -3506,7 +3510,7 @@
       <c r="Y56" s="22"/>
       <c r="Z56" s="22"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A57" s="22"/>
       <c r="B57" s="22"/>
       <c r="C57" s="22"/>
@@ -3534,7 +3538,7 @@
       <c r="Y57" s="22"/>
       <c r="Z57" s="22"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A58" s="22"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
@@ -3562,7 +3566,7 @@
       <c r="Y58" s="22"/>
       <c r="Z58" s="22"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A59" s="22"/>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
@@ -3590,7 +3594,7 @@
       <c r="Y59" s="22"/>
       <c r="Z59" s="22"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A60" s="22"/>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
@@ -3618,7 +3622,7 @@
       <c r="Y60" s="22"/>
       <c r="Z60" s="22"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A61" s="22"/>
       <c r="B61" s="22"/>
       <c r="C61" s="22"/>
@@ -3646,7 +3650,7 @@
       <c r="Y61" s="22"/>
       <c r="Z61" s="22"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A62" s="22"/>
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
@@ -3674,7 +3678,7 @@
       <c r="Y62" s="22"/>
       <c r="Z62" s="22"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A63" s="22"/>
       <c r="B63" s="22"/>
       <c r="C63" s="22"/>
@@ -3702,7 +3706,7 @@
       <c r="Y63" s="22"/>
       <c r="Z63" s="22"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A64" s="22"/>
       <c r="B64" s="22"/>
       <c r="C64" s="22"/>
@@ -3730,7 +3734,7 @@
       <c r="Y64" s="22"/>
       <c r="Z64" s="22"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A65" s="22"/>
       <c r="B65" s="22"/>
       <c r="C65" s="22"/>
@@ -3758,7 +3762,7 @@
       <c r="Y65" s="22"/>
       <c r="Z65" s="22"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A66" s="22"/>
       <c r="B66" s="22"/>
       <c r="C66" s="22"/>
@@ -3786,7 +3790,7 @@
       <c r="Y66" s="22"/>
       <c r="Z66" s="22"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A67" s="22"/>
       <c r="B67" s="22"/>
       <c r="C67" s="22"/>
@@ -3814,7 +3818,7 @@
       <c r="Y67" s="22"/>
       <c r="Z67" s="22"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A68" s="22"/>
       <c r="B68" s="22"/>
       <c r="C68" s="22"/>
@@ -3842,7 +3846,7 @@
       <c r="Y68" s="22"/>
       <c r="Z68" s="22"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A69" s="22"/>
       <c r="B69" s="22"/>
       <c r="C69" s="22"/>
@@ -3870,7 +3874,7 @@
       <c r="Y69" s="22"/>
       <c r="Z69" s="22"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A70" s="22"/>
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
@@ -3898,7 +3902,7 @@
       <c r="Y70" s="22"/>
       <c r="Z70" s="22"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A71" s="22"/>
       <c r="B71" s="22"/>
       <c r="C71" s="22"/>
@@ -3926,7 +3930,7 @@
       <c r="Y71" s="22"/>
       <c r="Z71" s="22"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A72" s="22"/>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
@@ -3954,7 +3958,7 @@
       <c r="Y72" s="22"/>
       <c r="Z72" s="22"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A73" s="22"/>
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
@@ -3982,7 +3986,7 @@
       <c r="Y73" s="22"/>
       <c r="Z73" s="22"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A74" s="22"/>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
@@ -4010,7 +4014,7 @@
       <c r="Y74" s="22"/>
       <c r="Z74" s="22"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A75" s="22"/>
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
@@ -4038,7 +4042,7 @@
       <c r="Y75" s="22"/>
       <c r="Z75" s="22"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A76" s="22"/>
       <c r="B76" s="22"/>
       <c r="C76" s="22"/>
@@ -4066,7 +4070,7 @@
       <c r="Y76" s="22"/>
       <c r="Z76" s="22"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A77" s="22"/>
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
@@ -4094,7 +4098,7 @@
       <c r="Y77" s="22"/>
       <c r="Z77" s="22"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A78" s="22"/>
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
@@ -4122,7 +4126,7 @@
       <c r="Y78" s="22"/>
       <c r="Z78" s="22"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A79" s="22"/>
       <c r="B79" s="22"/>
       <c r="C79" s="22"/>
@@ -4150,7 +4154,7 @@
       <c r="Y79" s="22"/>
       <c r="Z79" s="22"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A80" s="22"/>
       <c r="B80" s="22"/>
       <c r="C80" s="22"/>
@@ -4178,7 +4182,7 @@
       <c r="Y80" s="22"/>
       <c r="Z80" s="22"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A81" s="22"/>
       <c r="B81" s="22"/>
       <c r="C81" s="22"/>
@@ -4206,7 +4210,7 @@
       <c r="Y81" s="22"/>
       <c r="Z81" s="22"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A82" s="22"/>
       <c r="B82" s="22"/>
       <c r="C82" s="22"/>
@@ -4234,7 +4238,7 @@
       <c r="Y82" s="22"/>
       <c r="Z82" s="22"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A83" s="22"/>
       <c r="B83" s="22"/>
       <c r="C83" s="22"/>
@@ -4262,7 +4266,7 @@
       <c r="Y83" s="22"/>
       <c r="Z83" s="22"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A84" s="22"/>
       <c r="B84" s="22"/>
       <c r="C84" s="22"/>
@@ -4290,7 +4294,7 @@
       <c r="Y84" s="22"/>
       <c r="Z84" s="22"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A85" s="22"/>
       <c r="B85" s="22"/>
       <c r="C85" s="22"/>
@@ -4318,7 +4322,7 @@
       <c r="Y85" s="22"/>
       <c r="Z85" s="22"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A86" s="22"/>
       <c r="B86" s="22"/>
       <c r="C86" s="22"/>
@@ -4346,7 +4350,7 @@
       <c r="Y86" s="22"/>
       <c r="Z86" s="22"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A87" s="22"/>
       <c r="B87" s="22"/>
       <c r="C87" s="22"/>
@@ -4374,7 +4378,7 @@
       <c r="Y87" s="22"/>
       <c r="Z87" s="22"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A88" s="22"/>
       <c r="B88" s="22"/>
       <c r="C88" s="22"/>
@@ -4402,7 +4406,7 @@
       <c r="Y88" s="22"/>
       <c r="Z88" s="22"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A89" s="22"/>
       <c r="B89" s="22"/>
       <c r="C89" s="22"/>
@@ -4430,7 +4434,7 @@
       <c r="Y89" s="22"/>
       <c r="Z89" s="22"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A90" s="22"/>
       <c r="B90" s="22"/>
       <c r="C90" s="22"/>
@@ -4458,7 +4462,7 @@
       <c r="Y90" s="22"/>
       <c r="Z90" s="22"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A91" s="22"/>
       <c r="B91" s="22"/>
       <c r="C91" s="22"/>
@@ -4486,7 +4490,7 @@
       <c r="Y91" s="22"/>
       <c r="Z91" s="22"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A92" s="22"/>
       <c r="B92" s="22"/>
       <c r="C92" s="22"/>
@@ -4514,7 +4518,7 @@
       <c r="Y92" s="22"/>
       <c r="Z92" s="22"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A93" s="22"/>
       <c r="B93" s="22"/>
       <c r="C93" s="22"/>
@@ -4542,7 +4546,7 @@
       <c r="Y93" s="22"/>
       <c r="Z93" s="22"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A94" s="22"/>
       <c r="B94" s="22"/>
       <c r="C94" s="22"/>
@@ -4570,7 +4574,7 @@
       <c r="Y94" s="22"/>
       <c r="Z94" s="22"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A95" s="22"/>
       <c r="B95" s="22"/>
       <c r="C95" s="22"/>
@@ -4598,7 +4602,7 @@
       <c r="Y95" s="22"/>
       <c r="Z95" s="22"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A96" s="22"/>
       <c r="B96" s="22"/>
       <c r="C96" s="22"/>
@@ -4626,7 +4630,7 @@
       <c r="Y96" s="22"/>
       <c r="Z96" s="22"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A97" s="22"/>
       <c r="B97" s="22"/>
       <c r="C97" s="22"/>
@@ -4654,7 +4658,7 @@
       <c r="Y97" s="22"/>
       <c r="Z97" s="22"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A98" s="22"/>
       <c r="B98" s="22"/>
       <c r="C98" s="22"/>
@@ -4682,7 +4686,7 @@
       <c r="Y98" s="22"/>
       <c r="Z98" s="22"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A99" s="22"/>
       <c r="B99" s="22"/>
       <c r="C99" s="22"/>
@@ -4739,39 +4743,39 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5546875" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.07421875" customWidth="1"/>
+    <col min="2" max="2" width="11.69140625" customWidth="1"/>
+    <col min="3" max="3" width="3.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.4609375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.69140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.53515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.07421875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.69140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.53515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.69140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.07421875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.69140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.53515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.84375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.69140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.84375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.53515625" customWidth="1"/>
+    <col min="25" max="25" width="6.69140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.07421875" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.69140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
       <c r="C3" s="11" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -4885,12 +4889,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -5005,7 +5009,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -5122,7 +5126,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -5239,7 +5243,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="13" t="s">
         <v>23</v>
       </c>
@@ -5247,7 +5251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -5255,7 +5259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A12" s="15" t="s">
         <v>27</v>
       </c>
@@ -5263,7 +5267,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A13" s="15" t="s">
         <v>29</v>
       </c>
@@ -5271,7 +5275,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A14" s="15" t="s">
         <v>31</v>
       </c>
@@ -5279,7 +5283,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
         <v>33</v>
       </c>
@@ -5287,7 +5291,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A16" s="15" t="s">
         <v>35</v>
       </c>
@@ -5295,7 +5299,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="15" t="s">
         <v>37</v>
       </c>
@@ -5303,7 +5307,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" s="15" t="s">
         <v>39</v>
       </c>
@@ -5311,7 +5315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" s="15" t="s">
         <v>41</v>
       </c>
@@ -5319,7 +5323,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="15" t="s">
         <v>43</v>
       </c>
@@ -5327,7 +5331,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" s="15" t="s">
         <v>45</v>
       </c>
@@ -5335,7 +5339,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" s="15" t="s">
         <v>47</v>
       </c>
@@ -5343,7 +5347,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" s="15" t="s">
         <v>49</v>
       </c>
@@ -5351,7 +5355,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" s="15" t="s">
         <v>51</v>
       </c>
@@ -5359,7 +5363,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" s="15" t="s">
         <v>53</v>
       </c>
@@ -5367,7 +5371,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" s="15" t="s">
         <v>55</v>
       </c>
@@ -5375,7 +5379,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" s="15" t="s">
         <v>57</v>
       </c>
@@ -5383,7 +5387,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" s="15" t="s">
         <v>59</v>
       </c>
@@ -5391,7 +5395,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" s="15" t="s">
         <v>61</v>
       </c>
@@ -5399,7 +5403,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" s="15" t="s">
         <v>63</v>
       </c>
@@ -5407,7 +5411,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" s="15" t="s">
         <v>65</v>
       </c>
@@ -5415,7 +5419,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" s="15" t="s">
         <v>67</v>
       </c>
@@ -5423,7 +5427,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" s="15" t="s">
         <v>69</v>
       </c>
@@ -5431,7 +5435,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" s="15" t="s">
         <v>71</v>
       </c>
@@ -5439,7 +5443,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" s="15" t="s">
         <v>73</v>
       </c>
@@ -5447,7 +5451,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" s="15" t="s">
         <v>75</v>
       </c>
@@ -5455,7 +5459,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" s="16" t="s">
         <v>77</v>
       </c>
@@ -5481,7 +5485,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:colOff>21771</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -5501,35 +5505,34 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.4609375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="str">
-        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C2:D2)</f>
-        <v xml:space="preserve">~UC_Sets: R_E: </v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B2" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.4">
       <c r="G4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -5558,18 +5561,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B6" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>147</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>148</v>
       </c>
       <c r="F6" s="19">
         <v>2023</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -5578,15 +5581,15 @@
         <v>0.9</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B7" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>147</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>148</v>
       </c>
       <c r="F7" s="19">
         <v>2025</v>
@@ -5601,15 +5604,15 @@
         <v>5</v>
       </c>
       <c r="J7" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B8" s="19" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="D8" s="20" t="s">
         <v>147</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>148</v>
       </c>
       <c r="F8" s="19">
         <v>2030</v>
@@ -5624,15 +5627,15 @@
         <v>8</v>
       </c>
       <c r="J8" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B9" s="19" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="19" t="s">
+      <c r="D9" s="20" t="s">
         <v>147</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>148</v>
       </c>
       <c r="F9" s="19">
         <v>2040</v>
@@ -5647,10 +5650,10 @@
         <v>10</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B10" s="19"/>
       <c r="D10" s="20"/>
       <c r="F10" s="19">
@@ -5663,41 +5666,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B11" s="19"/>
       <c r="D11" s="20"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="I11" s="38"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B12" s="19"/>
       <c r="D12" s="20"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="I12" s="38"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B13" s="19"/>
       <c r="D13" s="20"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B14" s="19"/>
       <c r="D14" s="20"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B15" s="6" t="s">
         <v>82</v>
       </c>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -5710,13 +5713,11 @@
       <c r="E16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="9" t="str">
-        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
-        <v>IE</v>
-      </c>
-      <c r="G16" s="9" t="str">
-        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
-        <v>National</v>
+      <c r="F16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>4</v>
@@ -5728,7 +5729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D17" t="s">
         <v>84</v>
       </c>
@@ -5736,17 +5737,16 @@
         <v>5</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17" si="0">F17</f>
         <v>5</v>
       </c>
       <c r="I17" t="s">
         <v>83</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B18" s="39" t="s">
         <v>88</v>
       </c>
@@ -5767,15 +5767,15 @@
       </c>
       <c r="H18" s="39"/>
       <c r="I18" s="39" t="s">
-        <v>117</v>
+        <v>171</v>
       </c>
       <c r="J18" s="39"/>
       <c r="K18" s="39"/>
       <c r="L18" s="40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>88</v>
       </c>
@@ -5795,13 +5795,13 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
+        <v>171</v>
+      </c>
+      <c r="L19" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="L19" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>88</v>
       </c>
@@ -5821,15 +5821,33 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="I21" s="39"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="I22" s="39"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B23" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="8" t="s">
         <v>12</v>
       </c>
@@ -5842,13 +5860,11 @@
       <c r="E24" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="9" t="str">
-        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
-        <v>IE</v>
-      </c>
-      <c r="G24" s="9" t="str">
-        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
-        <v>National</v>
+      <c r="F24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>4</v>
@@ -5860,7 +5876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B25" s="39" t="s">
         <v>88</v>
       </c>
@@ -5880,13 +5896,13 @@
         <v>1.5</v>
       </c>
       <c r="I25" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="L25" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="L25" s="40" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B26" s="39" t="s">
         <v>88</v>
       </c>
@@ -5906,13 +5922,13 @@
         <v>13.8</v>
       </c>
       <c r="I26" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L26" s="40" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B27" s="39" t="s">
         <v>88</v>
       </c>
@@ -5922,8 +5938,8 @@
       <c r="D27" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="39">
-        <v>2025</v>
+      <c r="E27" s="44">
+        <v>2026</v>
       </c>
       <c r="F27" s="39">
         <v>0</v>
@@ -5932,13 +5948,13 @@
         <v>0</v>
       </c>
       <c r="I27" s="39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L27" s="40" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B28" s="39" t="s">
         <v>88</v>
       </c>
@@ -5958,10 +5974,10 @@
         <v>5</v>
       </c>
       <c r="I28" s="39" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B29" s="39" t="s">
         <v>88</v>
       </c>
@@ -5985,7 +6001,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B30" s="39" t="s">
         <v>88</v>
       </c>
@@ -6009,7 +6025,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B31" s="39" t="s">
         <v>88</v>
       </c>
@@ -6036,7 +6052,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B32" s="39" t="s">
         <v>88</v>
       </c>
@@ -6063,7 +6079,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B33" s="39" t="s">
         <v>88</v>
       </c>
@@ -6087,7 +6103,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
       <c r="D34" s="39"/>
@@ -6096,12 +6112,12 @@
       <c r="G34" s="39"/>
       <c r="I34" s="39"/>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B36" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B37" s="8" t="s">
         <v>12</v>
       </c>
@@ -6114,13 +6130,11 @@
       <c r="E37" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="9" t="str">
-        <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
-        <v>IE</v>
-      </c>
-      <c r="G37" s="9" t="str">
-        <f>IF(Regions!D$3&lt;&gt;"",Regions!D$3,"*")</f>
-        <v>National</v>
+      <c r="F37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="H37" s="10" t="s">
         <v>4</v>
@@ -6132,7 +6146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D38" t="s">
         <v>78</v>
       </c>
@@ -6140,14 +6154,13 @@
         <v>2035</v>
       </c>
       <c r="G38">
-        <f t="shared" ref="G38:G44" si="1">F38</f>
         <v>2035</v>
       </c>
       <c r="I38" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D39" t="s">
         <v>78</v>
       </c>
@@ -6158,13 +6171,13 @@
         <v>2025</v>
       </c>
       <c r="I39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L39" s="17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D40" t="s">
         <v>78</v>
       </c>
@@ -6172,17 +6185,16 @@
         <v>2100</v>
       </c>
       <c r="G40">
-        <f t="shared" si="1"/>
         <v>2100</v>
       </c>
       <c r="I40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D41" t="s">
         <v>78</v>
       </c>
@@ -6190,17 +6202,16 @@
         <v>2100</v>
       </c>
       <c r="G41">
-        <f t="shared" si="1"/>
         <v>2100</v>
       </c>
       <c r="I41" t="s">
+        <v>137</v>
+      </c>
+      <c r="L41" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="L41" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D42" t="s">
         <v>78</v>
       </c>
@@ -6208,17 +6219,16 @@
         <v>2100</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
         <v>2100</v>
       </c>
       <c r="I42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L42" s="17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D43" t="s">
         <v>78</v>
       </c>
@@ -6226,17 +6236,16 @@
         <v>2100</v>
       </c>
       <c r="G43">
-        <f t="shared" si="1"/>
         <v>2100</v>
       </c>
       <c r="I43" t="s">
+        <v>141</v>
+      </c>
+      <c r="L43" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="L43" s="17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D44" t="s">
         <v>78</v>
       </c>
@@ -6244,22 +6253,36 @@
         <v>2035</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
         <v>2035</v>
       </c>
       <c r="I44" t="s">
         <v>83</v>
       </c>
       <c r="L44" s="17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="I45" s="38"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="I46" s="38"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="I47" s="38"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.4">
       <c r="G48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B49" s="3" t="s">
         <v>0</v>
       </c>
@@ -6288,12 +6311,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B50" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" s="20" t="s">
         <v>162</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>163</v>
       </c>
       <c r="F50" s="19">
         <v>2027</v>
@@ -6308,15 +6331,15 @@
         <v>0.2</v>
       </c>
       <c r="J50" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B51" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="20" t="s">
         <v>162</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>163</v>
       </c>
       <c r="F51" s="19">
         <v>2028</v>
@@ -6331,15 +6354,15 @@
         <v>1.5</v>
       </c>
       <c r="J51" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B52" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52" s="20" t="s">
         <v>162</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>163</v>
       </c>
       <c r="F52" s="19">
         <v>2029</v>
@@ -6354,21 +6377,21 @@
         <v>3</v>
       </c>
       <c r="J52" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B53" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D53" s="20" t="s">
         <v>162</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>163</v>
       </c>
       <c r="F53" s="19">
         <v>2030</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -6377,15 +6400,15 @@
         <v>5</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B54" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D54" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>165</v>
       </c>
       <c r="F54" s="19">
         <v>2025</v>
@@ -6400,15 +6423,15 @@
         <v>6</v>
       </c>
       <c r="J54" s="19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B55" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D55" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>165</v>
       </c>
       <c r="F55" s="19">
         <v>2030</v>
@@ -6423,15 +6446,15 @@
         <v>9</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B56" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D56" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>165</v>
       </c>
       <c r="F56" s="19">
         <v>2050</v>
@@ -6446,10 +6469,10 @@
         <v>30.6</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.4">
       <c r="F57" s="19">
         <v>0</v>
       </c>
@@ -6460,16 +6483,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -6482,13 +6505,13 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
@@ -6496,7 +6519,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
@@ -6527,7 +6550,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
       <c r="D4" t="s">
         <v>78</v>
       </c>
@@ -6558,44 +6581,44 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.69140625" customWidth="1"/>
+    <col min="3" max="3" width="8.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.84375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.84375" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" customWidth="1"/>
-    <col min="12" max="12" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.3046875" customWidth="1"/>
+    <col min="12" max="12" width="44.69140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="H4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -6627,7 +6650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B6" s="19" t="s">
         <v>112</v>
       </c>
@@ -6650,7 +6673,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B7" s="19"/>
       <c r="D7" s="20"/>
       <c r="G7" s="19">
@@ -6663,7 +6686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B8" s="19" t="s">
         <v>116</v>
       </c>
@@ -6687,7 +6710,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
@@ -6706,7 +6729,7 @@
       </c>
       <c r="K9" s="19"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20" t="s">
@@ -6725,7 +6748,7 @@
       </c>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20" t="s">
@@ -6744,7 +6767,7 @@
       </c>
       <c r="K11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20" t="s">
@@ -6763,7 +6786,7 @@
       </c>
       <c r="K12" s="19"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
@@ -6774,7 +6797,7 @@
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
@@ -6785,12 +6808,12 @@
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="H15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
@@ -6810,10 +6833,10 @@
         <v>9</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>17</v>
@@ -6822,9 +6845,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B17" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
@@ -6834,22 +6857,22 @@
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K17" s="37"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B18" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="E18" t="s">
         <v>158</v>
-      </c>
-      <c r="E18" t="s">
-        <v>159</v>
       </c>
       <c r="F18" s="19">
         <v>2022</v>
@@ -6858,7 +6881,7 @@
         <v>81</v>
       </c>
       <c r="H18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I18" s="19">
         <v>1</v>
@@ -6867,27 +6890,27 @@
         <v>6</v>
       </c>
       <c r="K18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M18" s="19"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B19" s="19"/>
       <c r="C19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="D19" s="20" t="s">
-        <v>158</v>
-      </c>
       <c r="E19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F19" s="19">
         <v>2022</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I19" s="19">
         <v>-1</v>
@@ -6895,7 +6918,7 @@
       <c r="J19" s="19"/>
       <c r="M19" s="19"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B20" s="19"/>
       <c r="D20" s="20"/>
       <c r="F20">
@@ -6911,28 +6934,28 @@
       </c>
       <c r="M20" s="19"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B21" s="19"/>
       <c r="D21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
       <c r="M21" s="19"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B22" s="19"/>
       <c r="D22" s="20"/>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
       <c r="M22" s="19"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B23" s="19"/>
       <c r="D23" s="20"/>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
       <c r="M23" s="19"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
@@ -6940,7 +6963,7 @@
       <c r="H24" s="19"/>
       <c r="J24" s="19"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B26" s="6" t="s">
         <v>82</v>
       </c>
@@ -6948,7 +6971,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B27" s="8" t="s">
         <v>12</v>
       </c>
@@ -6979,7 +7002,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
         <v>81</v>
       </c>
@@ -7006,7 +7029,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C29" t="str">
         <f>C28</f>
         <v>UP</v>
@@ -7030,14 +7053,14 @@
         <v>IMPBIO*1G*2,IMPBIO*1G*3,IMPBIO*1G*4</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B32" s="6" t="s">
         <v>82</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B33" s="8" t="s">
         <v>12</v>
       </c>
@@ -7065,7 +7088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C34" t="s">
         <v>81</v>
       </c>
@@ -7089,7 +7112,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C35" t="str">
         <f>C34</f>
         <v>UP</v>
@@ -7116,7 +7139,7 @@
         <v>*GRID</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C36" t="s">
         <v>81</v>
       </c>
@@ -7137,7 +7160,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C37" t="str">
         <f>C36</f>
         <v>UP</v>
@@ -7161,7 +7184,7 @@
         <v>IMPH2G</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B40" s="6" t="s">
         <v>15</v>
       </c>
@@ -7169,7 +7192,7 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
     </row>
-    <row r="41" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B41" s="8" t="s">
         <v>12</v>
       </c>
@@ -7197,7 +7220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.4">
       <c r="D42" t="s">
         <v>78</v>
       </c>
@@ -7228,20 +7251,20 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>82</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -7269,7 +7292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C5" t="s">
         <v>81</v>
       </c>
@@ -7290,7 +7313,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
         <v>81</v>
       </c>
@@ -7311,7 +7334,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
         <v>81</v>
       </c>
@@ -7332,7 +7355,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
         <v>81</v>
       </c>
@@ -7353,7 +7376,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
         <v>81</v>
       </c>
@@ -7374,7 +7397,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
         <v>81</v>
       </c>
@@ -7395,7 +7418,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C11" t="s">
         <v>81</v>
       </c>
@@ -7416,7 +7439,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
         <v>81</v>
       </c>
@@ -7451,20 +7474,20 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.53515625" customWidth="1"/>
+    <col min="6" max="6" width="11.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -7498,7 +7521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
       <c r="D5" t="s">
         <v>104</v>
       </c>

</xml_diff>